<commit_message>
Added Table 5 and completed section about development stage
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="4" r:id="rId1"/>
     <sheet name="Table 2" sheetId="5" r:id="rId2"/>
     <sheet name="Table 3" sheetId="6" r:id="rId3"/>
     <sheet name="Table 4" sheetId="7" r:id="rId4"/>
-    <sheet name="Figure 1" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
+    <sheet name="Table 5" sheetId="8" r:id="rId5"/>
+    <sheet name="Figure 1" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="120">
   <si>
     <t>Total</t>
   </si>
@@ -429,6 +430,38 @@
   </si>
   <si>
     <t>The demonstration of a new 'fuzzy logic' approach to avionics consisting of tests of the algorithms in a partially computer-based, partially bench-top component (e.g., fiber optic gyros) in a controls laboratory using simulated vehicle inputs.</t>
+  </si>
+  <si>
+    <t>Table 5</t>
+  </si>
+  <si>
+    <t>Readiness Level Scales</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nolte, W., &amp; Kruse, R. (2011). Readiness level proliferation. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Air Force Research Laboratory, Tech. Rep. 88ABW-2011-5501</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved from https://ndiastorage.blob.core.usgovcloudapi.net/ndia/2011/system/13132_NolteWednesday.pdf</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -552,7 +585,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -670,6 +703,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -4277,7 +4319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5009,44 +5051,44 @@
       <c r="F19" s="29"/>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
     </row>
     <row r="21" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="30"/>
@@ -5131,7 +5173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5262,28 +5304,28 @@
       <c r="D19" s="32"/>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
     </row>
     <row r="21" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
     </row>
     <row r="22" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
     </row>
     <row r="23" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="30"/>
@@ -5634,27 +5676,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -5744,6 +5786,192 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+    </row>
+    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+    </row>
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+    </row>
+    <row r="20" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+    </row>
+    <row r="21" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+    </row>
+    <row r="22" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+    </row>
+    <row r="23" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="37"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A20:C20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
@@ -6202,7 +6430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -6457,7 +6685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added table of contents, list of tables, and list of figures
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="183">
   <si>
     <t>Total</t>
   </si>
@@ -435,7 +435,218 @@
     <t>Table 5</t>
   </si>
   <si>
-    <t>Readiness Level Scales</t>
+    <t>Strategic Readiness Levels</t>
+  </si>
+  <si>
+    <t>Programmatic Readiness Levels</t>
+  </si>
+  <si>
+    <t>Security Readiness Levels</t>
+  </si>
+  <si>
+    <t>Fuel Readiness Levels</t>
+  </si>
+  <si>
+    <t>Fire Readiness Levels</t>
+  </si>
+  <si>
+    <t>Reading Readiness Levels</t>
+  </si>
+  <si>
+    <t>Community Readiness Levels</t>
+  </si>
+  <si>
+    <t>Operational Readiness Levels</t>
+  </si>
+  <si>
+    <t>Condition of Readiness Levels</t>
+  </si>
+  <si>
+    <t>Tropical Storm Readiness Levels</t>
+  </si>
+  <si>
+    <t>Defense Readiness Condition (DEFCON) Levels</t>
+  </si>
+  <si>
+    <t>People’s “Task” Readiness Levels</t>
+  </si>
+  <si>
+    <t>Football Readiness Levels</t>
+  </si>
+  <si>
+    <t>Tactical Readiness Levels</t>
+  </si>
+  <si>
+    <t>Problem Solving Readiness Levels</t>
+  </si>
+  <si>
+    <t>Survival Readiness Levels</t>
+  </si>
+  <si>
+    <t>Extreme Heat Readiness Levels</t>
+  </si>
+  <si>
+    <t>Learning Readiness Levels</t>
+  </si>
+  <si>
+    <t>Love Readiness Levels</t>
+  </si>
+  <si>
+    <t>Internet Marketing Readiness Levels</t>
+  </si>
+  <si>
+    <t>Continuity Readiness Levels</t>
+  </si>
+  <si>
+    <t>Follower Readiness Levels</t>
+  </si>
+  <si>
+    <t>Business Readiness Levels</t>
+  </si>
+  <si>
+    <t>Physical Readiness Levels</t>
+  </si>
+  <si>
+    <t>TQM Readiness Levels</t>
+  </si>
+  <si>
+    <t>Defence Readiness Levels</t>
+  </si>
+  <si>
+    <t>Change Readiness Levels</t>
+  </si>
+  <si>
+    <t>Material Operational Readiness Levels</t>
+  </si>
+  <si>
+    <t>E-Procurement Readiness Levels</t>
+  </si>
+  <si>
+    <t>Venture Readiness Levels</t>
+  </si>
+  <si>
+    <t>Entrepreneurship Readiness Levels</t>
+  </si>
+  <si>
+    <t>Partner Readiness Levels</t>
+  </si>
+  <si>
+    <t>Bilingualism Test Readiness Levels</t>
+  </si>
+  <si>
+    <t>Performance Readiness Levels</t>
+  </si>
+  <si>
+    <t>Disaster Readiness Levels</t>
+  </si>
+  <si>
+    <t>Human Effects Readiness Levels</t>
+  </si>
+  <si>
+    <t>Earthquake Readiness Levels</t>
+  </si>
+  <si>
+    <t>Primary Mental Abilities Readiness Levels</t>
+  </si>
+  <si>
+    <t>Technical Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Manufacturing Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Logistics Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Innovation Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Integration Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Direct Manufacturing Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Sustainment Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Software Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Risk Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Human Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Engineering &amp; Manufacturing Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Technology Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Reuse Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Demand Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Funding Readiness Levels*</t>
+  </si>
+  <si>
+    <t>System Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Supportability Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Countermeasures Readiness Levels*</t>
+  </si>
+  <si>
+    <t>Accreditation Readiness Levels*</t>
+  </si>
+  <si>
+    <t>University Technology Transfer Readiness Levels*</t>
+  </si>
+  <si>
+    <t>* indicates related to technology maturity per Nolte &amp; Kruse (2011).</t>
+  </si>
+  <si>
+    <t>Investement Readiness Levels</t>
+  </si>
+  <si>
+    <t>Investor Readiness Levels</t>
+  </si>
+  <si>
+    <t>Alternative Readiness Level Scales</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fellnhofer, K. (2015). Literature review: investment readiness level of small and medium sized 
+companies. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>International Journal of Managerial and Financial Accounting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 7(3/4), 268-284. Retrieved from 
+https://www.researchgate.net/profile/Katharina_Fellnhofer/publication/291670426_Literature_Review_Investment_Readiness_Level_of_Small_and_Medium_Sized_Companies/links/57e80d2908ae9e5e4558c179/Literature-Review-Investment-Readiness-Level-of-Small-and-Medium-Sized-Companies.pdf</t>
+    </r>
   </si>
   <si>
     <r>
@@ -444,7 +655,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="11"/>
+        <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -454,13 +665,39 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>. Retrieved from https://ndiastorage.blob.core.usgovcloudapi.net/ndia/2011/system/13132_NolteWednesday.pdf</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Westerik, F. H. (2014). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Investor readiness-Increasing the measurability of investor readiness</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Master's thesis, University of Twente). Retrieved from https://essay.utwente.nl/64605/1/Westerik_MA_MB.pdf</t>
     </r>
   </si>
 </sst>
@@ -472,7 +709,7 @@
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -533,6 +770,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -585,7 +837,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -706,11 +958,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4340,21 +4625,21 @@
       <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
       <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4776,7 +5061,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4794,7 +5081,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="49" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5051,44 +5338,44 @@
       <c r="F19" s="29"/>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
     </row>
     <row r="21" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
     </row>
     <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="30"/>
@@ -5173,7 +5460,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5189,7 +5478,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="49" t="s">
         <v>68</v>
       </c>
     </row>
@@ -5304,28 +5593,28 @@
       <c r="D19" s="32"/>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
     </row>
     <row r="21" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
     </row>
     <row r="22" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
+      <c r="A22" s="51"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
     </row>
     <row r="23" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
+      <c r="A23" s="51"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="30"/>
@@ -5417,7 +5706,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="49" t="s">
         <v>112</v>
       </c>
     </row>
@@ -5676,27 +5965,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
+      <c r="A17" s="51"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
+      <c r="A18" s="51"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
+      <c r="A19" s="51"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -5787,15 +6076,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5804,167 +6096,408 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+    </row>
+    <row r="3" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="44"/>
+      <c r="C5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="44"/>
+      <c r="C6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="44"/>
+      <c r="C7" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="44"/>
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="44"/>
+      <c r="C11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="44"/>
+      <c r="C12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="44"/>
+      <c r="C13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" s="44"/>
+      <c r="C14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="44"/>
+      <c r="C15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" s="44"/>
+      <c r="C16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="44"/>
+      <c r="C17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" s="44"/>
+      <c r="C18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="44"/>
+      <c r="C19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="37"/>
+      <c r="C21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="37"/>
+      <c r="C22" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-    </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-    </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-    </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-    </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-    </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-    </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-    </row>
-    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" s="37"/>
+      <c r="C23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="37"/>
+      <c r="C24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="37"/>
+      <c r="C25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" s="37"/>
+      <c r="C26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" s="37"/>
+      <c r="C29" s="23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="37"/>
+      <c r="C30" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" s="37"/>
+      <c r="C31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>177</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>178</v>
+      </c>
+      <c r="B33" s="37"/>
+      <c r="C33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="36"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="53"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-    </row>
-    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="54"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-    </row>
-    <row r="20" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-    </row>
-    <row r="21" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-    </row>
-    <row r="22" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-    </row>
-    <row r="23" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="54"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+    </row>
+    <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="55" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" s="55"/>
+      <c r="C42" s="55"/>
+    </row>
+    <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="B43" s="56"/>
+      <c r="C43" s="56"/>
+    </row>
+    <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="55" t="s">
+        <v>182</v>
+      </c>
+      <c r="B44" s="55"/>
+      <c r="C44" s="55"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="51"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="51"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="37"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="37"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="37"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="37"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="37"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="37"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
     </row>
   </sheetData>
+  <sortState ref="F1:F58">
+    <sortCondition ref="F58"/>
+  </sortState>
   <mergeCells count="4">
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A43:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added content to section on the valley of death and updated Table 2 on policies
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="187">
   <si>
     <t>Total</t>
   </si>
@@ -699,6 +699,21 @@
       </rPr>
       <t xml:space="preserve"> (Master's thesis, University of Twente). Retrieved from https://essay.utwente.nl/64605/1/Westerik_MA_MB.pdf</t>
     </r>
+  </si>
+  <si>
+    <t>Pub.L. 112-29
+Leahy-Smith America Invents Act</t>
+  </si>
+  <si>
+    <t>Free rider problems
+Incomplete markets</t>
+  </si>
+  <si>
+    <t>H.R.1249 - Leahy-Smith America Invents Act. (n.d.). Congress.gov. Retrieved May 20, 2020 from
+https://www.congress.gov/bill/112th-congress/house-bill/1249</t>
+  </si>
+  <si>
+    <t>Reformed patent laws and instituted "first inventor to file" patent registration system.</t>
   </si>
 </sst>
 </file>
@@ -837,7 +852,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -979,9 +994,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -991,10 +1003,22 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4604,7 +4628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5059,10 +5083,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5294,42 +5318,48 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35">
+      <c r="A16" s="57">
         <v>2000</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36" t="s">
+      <c r="C16" s="38"/>
+      <c r="D16" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36" t="s">
+      <c r="E16" s="38"/>
+      <c r="F16" s="38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-    </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
+    <row r="17" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="57">
+        <v>2011</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="58"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
@@ -5338,60 +5368,64 @@
       <c r="F19" s="29"/>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-    </row>
-    <row r="21" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51" t="s">
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+    </row>
+    <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+    </row>
+    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-    </row>
-    <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="51" t="s">
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+    </row>
+    <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-    </row>
-    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="51" t="s">
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+    </row>
+    <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -5441,15 +5475,32 @@
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
     </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="30"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+    </row>
   </sheetData>
   <sortState ref="A2:D28">
     <sortCondition ref="A1"/>
   </sortState>
-  <mergeCells count="4">
-    <mergeCell ref="A20:F20"/>
+  <mergeCells count="5">
     <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
     <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5593,28 +5644,28 @@
       <c r="D19" s="32"/>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
     </row>
     <row r="21" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
     </row>
     <row r="22" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
+      <c r="A22" s="54"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
     </row>
     <row r="23" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="51"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="30"/>
@@ -5965,27 +6016,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
+      <c r="A18" s="54"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -6388,40 +6439,40 @@
       <c r="C35" s="37"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="B36" s="53"/>
-      <c r="C36" s="53"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="53"/>
-      <c r="B37" s="53"/>
-      <c r="C37" s="53"/>
+      <c r="A37" s="52"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="52"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="52"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="54"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
+      <c r="A39" s="53"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="52"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="54"/>
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
+      <c r="A41" s="53"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="55" t="s">
@@ -6445,9 +6496,9 @@
       <c r="C44" s="55"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="51"/>
-      <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
+      <c r="A45" s="54"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="54"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>

</xml_diff>

<commit_message>
Added Table of Org Studies
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="775" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 1" sheetId="4" r:id="rId1"/>
-    <sheet name="Table 2" sheetId="5" r:id="rId2"/>
-    <sheet name="Table 3" sheetId="6" r:id="rId3"/>
-    <sheet name="Table 4" sheetId="7" r:id="rId4"/>
-    <sheet name="Table 5" sheetId="8" r:id="rId5"/>
-    <sheet name="Figure 1" sheetId="3" r:id="rId6"/>
-    <sheet name="Figure 1a" sheetId="1" r:id="rId7"/>
-    <sheet name="Figure 1b" sheetId="2" r:id="rId8"/>
-    <sheet name="Figure 2" sheetId="9" r:id="rId9"/>
+    <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
+    <sheet name="Table - Tech Tran Policies" sheetId="5" r:id="rId2"/>
+    <sheet name="Table - Determinants" sheetId="6" r:id="rId3"/>
+    <sheet name="Table - Org Studies" sheetId="10" r:id="rId4"/>
+    <sheet name="Table - NASA TRL Scale" sheetId="7" r:id="rId5"/>
+    <sheet name="Table - Alt Readiness Scales" sheetId="8" r:id="rId6"/>
+    <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId7"/>
+    <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId8"/>
+    <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId9"/>
+    <sheet name="Figure - Causal Diagram" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="224">
   <si>
     <t>Total</t>
   </si>
@@ -715,6 +716,157 @@
   </si>
   <si>
     <t>Reformed patent laws and instituted "first inventor to file" patent registration system.</t>
+  </si>
+  <si>
+    <t>Perspective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table </t>
+  </si>
+  <si>
+    <t>Focus of Study</t>
+  </si>
+  <si>
+    <t>Classical</t>
+  </si>
+  <si>
+    <t>Modern</t>
+  </si>
+  <si>
+    <t>Symbolic-Interpretive</t>
+  </si>
+  <si>
+    <t>Postmodern</t>
+  </si>
+  <si>
+    <t>Observation
+Historical analysis
+Reflection on personal experience</t>
+  </si>
+  <si>
+    <t>Emperical measurement
+Correlation among measures</t>
+  </si>
+  <si>
+    <t>Participant observation
+Ethnography</t>
+  </si>
+  <si>
+    <t>Typologies
+Theoretical frameworks
+Prescriptions for management practice</t>
+  </si>
+  <si>
+    <t>Comparative studies
+Statistical analyses</t>
+  </si>
+  <si>
+    <t>Case studies
+Organizational ethnographies</t>
+  </si>
+  <si>
+    <t>Reflexive accounts</t>
+  </si>
+  <si>
+    <t>Typical Types of Research Output</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hatch, M. J. (1997). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Organization theory: Modern, symbolic interpretivism, and postmodern perspectives </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(p. 49). New York, NY: Oxford University Press.</t>
+    </r>
+  </si>
+  <si>
+    <t>Methods of Study</t>
+  </si>
+  <si>
+    <t>Deconstruction of theories and practices
+Negation of assumptions
+Reflexivity</t>
+  </si>
+  <si>
+    <t>Schools of Thought</t>
+  </si>
+  <si>
+    <t>Epistemological Approach</t>
+  </si>
+  <si>
+    <t>Even if there is an objective reality, all knowledge is filtered by the experience of the observer.  The organization is a subject whose meaning is to be understood and appreciated.</t>
+  </si>
+  <si>
+    <t>Comparison of Perspectives and Schools of Thought in Organization Studies</t>
+  </si>
+  <si>
+    <t>How organizations affect society.
+How organization activities are coordinated.</t>
+  </si>
+  <si>
+    <t>How to maximize the rationality and efficiency organization activities.</t>
+  </si>
+  <si>
+    <t>How subjective perceptions affect the behavior of organizations.</t>
+  </si>
+  <si>
+    <t>How theory and theorizing practices affect our understanding of organizations.</t>
+  </si>
+  <si>
+    <t>There is an objective reality independent of the observer that can only be known through reasoned and logical analysis of data and information gathered from sensory experience. The organization is an object that can be measured and analyzed.</t>
+  </si>
+  <si>
+    <t>Human relations management</t>
+  </si>
+  <si>
+    <t>There is an objective reality independent of the observer.  The organization is a kind of  sociological process that both affects and is affected by society.</t>
+  </si>
+  <si>
+    <t>Key Metaphors</t>
+  </si>
+  <si>
+    <t>Since all knowledge is filtered by the experience of the observer, all distinctions used to describe reality are arbitrary and semantic in origin.  The organization is an abstraction that is best understood by revealing and comprehending the underlying assumptions used to construct it.</t>
+  </si>
+  <si>
+    <t>Scientific management
+Econometric
+Open systems</t>
+  </si>
+  <si>
+    <t>The organization is a pattern of meanings that created through human interaction that produces shared values, traditions, and customs (i.e., a culture).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The organization is a machine that management designs, constructs, and maintains to achieve specific goals and objectives.
+The organization is a living organism comprised of systems that perform the functions necessary for its survival. </t>
+  </si>
+  <si>
+    <t>The organization is a machine that management designs, constructs, and maintains to achieve specific goals and objectives.</t>
+  </si>
+  <si>
+    <t>The abstraction we call the organization is a collage composed of bits of knowledge and understanding that form a new perspective when rearranged.
+The organization is a text, a narrative, and a discourse.</t>
+  </si>
+  <si>
+    <t>Bureacratic management
+Administrative management
+Scientific management</t>
   </si>
 </sst>
 </file>
@@ -853,7 +1005,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1016,6 +1168,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1137,7 +1298,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Figure 1'!$A$35:$A$54</c:f>
+              <c:f>'Figure - R&amp;D Funding 1967-2019'!$A$35:$A$54</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -1205,7 +1366,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Figure 1'!$B$35:$B$54</c:f>
+              <c:f>'Figure - R&amp;D Funding 1967-2019'!$B$35:$B$54</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0_);\("$"#,##0\)</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1634,7 +1795,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Figure 1a'!$B$1</c:f>
+              <c:f>'Figure - R&amp;D Funding 1990-2015'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1655,7 +1816,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Figure 1a'!$A$12:$A$27</c:f>
+              <c:f>'Figure - R&amp;D Funding 1990-2015'!$A$12:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1712,7 +1873,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Figure 1a'!$B$12:$B$27</c:f>
+              <c:f>'Figure - R&amp;D Funding 1990-2015'!$B$12:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0_);\("$"#,##0\)</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2152,7 +2313,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Figure 1b'!$A$51:$A$70</c:f>
+              <c:f>'Figure - R&amp;D Funding 1951-2019'!$A$51:$A$70</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -2220,7 +2381,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Figure 1b'!$B$51:$B$70</c:f>
+              <c:f>'Figure - R&amp;D Funding 1951-2019'!$B$51:$B$70</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0_);\("$"#,##0\)</c:formatCode>
                 <c:ptCount val="20"/>
@@ -5909,6 +6070,19 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
@@ -6206,54 +6380,54 @@
       <c r="F20" s="29"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="57" t="s">
+      <c r="A22" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
     </row>
     <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -6472,28 +6646,28 @@
       <c r="D19" s="32"/>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
+      <c r="A20" s="59"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
     </row>
     <row r="21" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="56"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
+      <c r="A21" s="59"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
     </row>
     <row r="22" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="56"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
+      <c r="A22" s="59"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
     </row>
     <row r="23" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="30"/>
@@ -6556,6 +6730,416 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
+    <col min="10" max="10" width="40.7109375" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" customWidth="1"/>
+    <col min="12" max="12" width="40.7109375" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" customWidth="1"/>
+    <col min="14" max="14" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="57"/>
+      <c r="B4" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56" t="s">
+        <v>209</v>
+      </c>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58" t="s">
+        <v>221</v>
+      </c>
+      <c r="I4" s="58"/>
+      <c r="J4" s="56" t="s">
+        <v>194</v>
+      </c>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56" t="s">
+        <v>197</v>
+      </c>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="57"/>
+      <c r="B5" s="56" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56" t="s">
+        <v>210</v>
+      </c>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58" t="s">
+        <v>213</v>
+      </c>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58" t="s">
+        <v>220</v>
+      </c>
+      <c r="I5" s="58"/>
+      <c r="J5" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56" t="s">
+        <v>198</v>
+      </c>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="57"/>
+      <c r="B6" s="56" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="I6" s="58"/>
+      <c r="J6" s="56" t="s">
+        <v>196</v>
+      </c>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
+      <c r="B7" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="57"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+    </row>
+    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+    </row>
+    <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+    </row>
+    <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="56"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="56"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="56"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="57"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="57"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="57"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="57"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="56"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="57"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="57"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="57"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="57"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="44" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
@@ -6844,27 +7428,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
+      <c r="A17" s="59"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="56"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
+      <c r="A18" s="59"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
+      <c r="A19" s="59"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -6953,7 +7537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
@@ -7303,30 +7887,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="58" t="s">
+      <c r="A42" s="61" t="s">
         <v>180</v>
       </c>
-      <c r="B42" s="58"/>
-      <c r="C42" s="58"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="59" t="s">
+      <c r="A43" s="62" t="s">
         <v>181</v>
       </c>
-      <c r="B43" s="59"/>
-      <c r="C43" s="59"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="62"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="58" t="s">
+      <c r="A44" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="B44" s="58"/>
-      <c r="C44" s="58"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="61"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="56"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
+      <c r="A45" s="59"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>
@@ -7383,7 +7967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
@@ -7842,7 +8426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -8099,7 +8683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
@@ -8682,17 +9266,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Created tables about determinants of tech transfer outcomes
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
     <sheet name="Table - Tech Tran Policies" sheetId="5" r:id="rId2"/>
     <sheet name="Table - Determinants" sheetId="6" r:id="rId3"/>
-    <sheet name="Table - Org Studies" sheetId="10" r:id="rId4"/>
-    <sheet name="Table - NASA TRL Scale" sheetId="7" r:id="rId5"/>
-    <sheet name="Table - Alt Readiness Scales" sheetId="8" r:id="rId6"/>
-    <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId7"/>
-    <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId8"/>
-    <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId9"/>
-    <sheet name="Figure - Causal Diagram" sheetId="9" r:id="rId10"/>
+    <sheet name="Table - Determinants No Assoc" sheetId="11" r:id="rId4"/>
+    <sheet name="Table - Org Studies" sheetId="10" r:id="rId5"/>
+    <sheet name="Table - NASA TRL Scale" sheetId="7" r:id="rId6"/>
+    <sheet name="Table - Alt Readiness Scales" sheetId="8" r:id="rId7"/>
+    <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId8"/>
+    <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId9"/>
+    <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId10"/>
+    <sheet name="Figure - Causal Diagram" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="258">
   <si>
     <t>Total</t>
   </si>
@@ -84,9 +85,6 @@
   </si>
   <si>
     <t>Fiscal Year</t>
-  </si>
-  <si>
-    <t>Table 1</t>
   </si>
   <si>
     <t>Federal Obligations to Universities for 
@@ -235,9 +233,6 @@
     <t>Lee, Y. S. (1997). Technology transfer and economic development: A framework for policy analysis. In Y. S. Lee (Ed.), Technology Transfer and Public Policy (pp. 3-20). Quorum Books.</t>
   </si>
   <si>
-    <t>Table 2</t>
-  </si>
-  <si>
     <t>Federal Legislation and Executive Action Relevant to University Technology Transfer</t>
   </si>
   <si>
@@ -259,13 +254,7 @@
     <t>(Millions of Nominal U.S. Dollars)</t>
   </si>
   <si>
-    <t>Table 3</t>
-  </si>
-  <si>
     <t>Determinants of Technology Transfer Outcomes Found in the Literature</t>
-  </si>
-  <si>
-    <t>Response Variables</t>
   </si>
   <si>
     <t>Determinants</t>
@@ -724,9 +713,6 @@
     <t xml:space="preserve">Table </t>
   </si>
   <si>
-    <t>Focus of Study</t>
-  </si>
-  <si>
     <t>Classical</t>
   </si>
   <si>
@@ -797,20 +783,11 @@
     </r>
   </si>
   <si>
-    <t>Methods of Study</t>
-  </si>
-  <si>
     <t>Deconstruction of theories and practices
 Negation of assumptions
 Reflexivity</t>
   </si>
   <si>
-    <t>Schools of Thought</t>
-  </si>
-  <si>
-    <t>Epistemological Approach</t>
-  </si>
-  <si>
     <t>Even if there is an objective reality, all knowledge is filtered by the experience of the observer.  The organization is a subject whose meaning is to be understood and appreciated.</t>
   </si>
   <si>
@@ -845,28 +822,201 @@
     <t>Since all knowledge is filtered by the experience of the observer, all distinctions used to describe reality are arbitrary and semantic in origin.  The organization is an abstraction that is best understood by revealing and comprehending the underlying assumptions used to construct it.</t>
   </si>
   <si>
+    <t>The organization is a pattern of meanings that created through human interaction that produces shared values, traditions, and customs (i.e., a culture).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The organization is a machine that management designs, constructs, and maintains to achieve specific goals and objectives.
+The organization is a living organism comprised of systems that perform the functions necessary for its survival. </t>
+  </si>
+  <si>
+    <t>The organization is a machine that management designs, constructs, and maintains to achieve specific goals and objectives.</t>
+  </si>
+  <si>
+    <t>The abstraction we call the organization is a collage composed of bits of knowledge and understanding that form a new perspective when rearranged.
+The organization is a text, a narrative, and a discourse.</t>
+  </si>
+  <si>
+    <t>Supply-Side</t>
+  </si>
+  <si>
+    <t>Demand-Side</t>
+  </si>
+  <si>
+    <t>Economic Perspective</t>
+  </si>
+  <si>
+    <t>Studies</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Theories and Schools of Thought</t>
+  </si>
+  <si>
+    <t>Bureacracy theory
+Administrative theory
+Scientific management</t>
+  </si>
+  <si>
     <t>Scientific management
 Econometric
-Open systems</t>
-  </si>
-  <si>
-    <t>The organization is a pattern of meanings that created through human interaction that produces shared values, traditions, and customs (i.e., a culture).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The organization is a machine that management designs, constructs, and maintains to achieve specific goals and objectives.
-The organization is a living organism comprised of systems that perform the functions necessary for its survival. </t>
-  </si>
-  <si>
-    <t>The organization is a machine that management designs, constructs, and maintains to achieve specific goals and objectives.</t>
-  </si>
-  <si>
-    <t>The abstraction we call the organization is a collage composed of bits of knowledge and understanding that form a new perspective when rearranged.
-The organization is a text, a narrative, and a discourse.</t>
-  </si>
-  <si>
-    <t>Bureacratic management
-Administrative management
-Scientific management</t>
+Open systems theory</t>
+  </si>
+  <si>
+    <t>Autopoietic systems theory
+Discourse theory</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Miller, H. T., &amp; Fox, C. J. (2015). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Postmodern Public Administration. New York, NY:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Taylor &amp; Francis.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Luhmann, N. (2018). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Organization and decision</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (R. Barrett, Trans. D. Baecker Ed.). Cambridge, United Kingdom: Cambridge University Press.</t>
+    </r>
+  </si>
+  <si>
+    <t>Primary Focus of Study</t>
+  </si>
+  <si>
+    <t>Typical Methods of Study</t>
+  </si>
+  <si>
+    <t>General Epistemological Approach</t>
+  </si>
+  <si>
+    <t>Technology Transfer Proxies</t>
+  </si>
+  <si>
+    <t>Markman, Gianiodis, &amp; Phan (2009)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Licensing revenue</t>
+  </si>
+  <si>
+    <t>Firm creation</t>
+  </si>
+  <si>
+    <t>Public or private status of university</t>
+  </si>
+  <si>
+    <t>Quality of university faculty</t>
+  </si>
+  <si>
+    <t>Presence of university-affiliated incubator</t>
+  </si>
+  <si>
+    <t>High-autonomy of technology transfer operation</t>
+  </si>
+  <si>
+    <t>Low-autonomy of technology transfer operation</t>
+  </si>
+  <si>
+    <t>Age of technology transfer operation</t>
+  </si>
+  <si>
+    <t>Size of technology transfer operation (FTEs)</t>
+  </si>
+  <si>
+    <t>Level of technology transfer-related compensation to faculty</t>
+  </si>
+  <si>
+    <t>Level of technology transfer-related compensation to faculty departments</t>
+  </si>
+  <si>
+    <t>Level of technology transfer-related compensation to TTO staff</t>
+  </si>
+  <si>
+    <t>Use of sponsored research agreements</t>
+  </si>
+  <si>
+    <t>Use of licensing agreements</t>
+  </si>
+  <si>
+    <t>Factors Found Not to be Associated with Technology Transfer Outcomes</t>
+  </si>
+  <si>
+    <t>Number of professional schools at the university</t>
+  </si>
+  <si>
+    <t>Presence of a medical school at the university</t>
+  </si>
+  <si>
+    <t>Amount of the research budget for the university</t>
+  </si>
+  <si>
+    <t>Quality of the university</t>
+  </si>
+  <si>
+    <t>Number of high quality research universities within 100 miles of the university</t>
+  </si>
+  <si>
+    <t>Concentration of high-tech industries within the region</t>
+  </si>
+  <si>
+    <t>Cost of living where the univrsity is located</t>
+  </si>
+  <si>
+    <t>Level of local venture capital activity in the region where the university is located</t>
+  </si>
+  <si>
+    <t>Number of patents assigned to the university</t>
+  </si>
+  <si>
+    <t>Use of equity as compensation in licensing agreements</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>Table</t>
   </si>
 </sst>
 </file>
@@ -962,7 +1112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -999,13 +1149,159 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1177,11 +1473,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5632,14 +6009,14 @@
   <sheetData>
     <row r="1" spans="1:8" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>17</v>
+        <v>184</v>
       </c>
       <c r="E1" s="22"/>
       <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="48"/>
       <c r="C2" s="48"/>
@@ -5648,7 +6025,7 @@
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="48"/>
       <c r="C3" s="48"/>
@@ -6041,27 +6418,27 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -6071,6 +6448,591 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D70"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>1951</v>
+      </c>
+      <c r="B2" s="15">
+        <v>1851571</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1952</v>
+      </c>
+      <c r="B3" s="15">
+        <v>2216848</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>1953</v>
+      </c>
+      <c r="B4" s="15">
+        <v>2167456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>1954</v>
+      </c>
+      <c r="B5" s="15">
+        <v>1918046</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>1955</v>
+      </c>
+      <c r="B6" s="15">
+        <v>2251894</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>1956</v>
+      </c>
+      <c r="B7" s="15">
+        <v>3266903</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>1957</v>
+      </c>
+      <c r="B8" s="15">
+        <v>4389237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>1958</v>
+      </c>
+      <c r="B9" s="15">
+        <v>4906015</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>1959</v>
+      </c>
+      <c r="B10" s="15">
+        <v>7122610</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>1960</v>
+      </c>
+      <c r="B11" s="15">
+        <v>8080015</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>1961</v>
+      </c>
+      <c r="B12" s="15">
+        <v>9607023</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>1962</v>
+      </c>
+      <c r="B13" s="15">
+        <v>11069059</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>1963</v>
+      </c>
+      <c r="B14" s="15">
+        <v>13662879</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>1964</v>
+      </c>
+      <c r="B15" s="15">
+        <v>15323870</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>1965</v>
+      </c>
+      <c r="B16" s="15">
+        <v>15745852</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>1966</v>
+      </c>
+      <c r="B17" s="15">
+        <v>16178640</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>1967</v>
+      </c>
+      <c r="B18" s="15">
+        <v>17149186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>1968</v>
+      </c>
+      <c r="B19" s="15">
+        <v>16525038</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>1969</v>
+      </c>
+      <c r="B20" s="15">
+        <v>16309900</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>1970</v>
+      </c>
+      <c r="B21" s="15">
+        <v>15863385</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>1971</v>
+      </c>
+      <c r="B22" s="15">
+        <v>16153756</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>1972</v>
+      </c>
+      <c r="B23" s="15">
+        <v>17097951</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>1973</v>
+      </c>
+      <c r="B24" s="15">
+        <v>17574486</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>1974</v>
+      </c>
+      <c r="B25" s="15">
+        <v>18176457</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>1975</v>
+      </c>
+      <c r="B26" s="15">
+        <v>19859548</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>1976</v>
+      </c>
+      <c r="B27" s="15">
+        <v>21616382</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>1977</v>
+      </c>
+      <c r="B28" s="15">
+        <v>24817577</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>1978</v>
+      </c>
+      <c r="B29" s="15">
+        <v>27140849</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>1979</v>
+      </c>
+      <c r="B30" s="15">
+        <v>29620597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>1980</v>
+      </c>
+      <c r="B31" s="15">
+        <v>31386095</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>1981</v>
+      </c>
+      <c r="B32" s="15">
+        <v>34589634</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>1982</v>
+      </c>
+      <c r="B33" s="15">
+        <v>37822363</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>1983</v>
+      </c>
+      <c r="B34" s="15">
+        <v>40009032</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
+        <v>1984</v>
+      </c>
+      <c r="B35" s="15">
+        <v>44012149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>1985</v>
+      </c>
+      <c r="B36" s="15">
+        <v>50180369</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>1986</v>
+      </c>
+      <c r="B37" s="15">
+        <v>52951181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="14">
+        <v>1987</v>
+      </c>
+      <c r="B38" s="15">
+        <v>57099656</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="14">
+        <v>1988</v>
+      </c>
+      <c r="B39" s="15">
+        <v>58826512</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
+        <v>1989</v>
+      </c>
+      <c r="B40" s="15">
+        <v>63571605</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="14">
+        <v>1990</v>
+      </c>
+      <c r="B41" s="15">
+        <v>65831189</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
+        <v>1991</v>
+      </c>
+      <c r="B42" s="15">
+        <v>64147951</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="14">
+        <v>1992</v>
+      </c>
+      <c r="B43" s="15">
+        <v>68577184</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="14">
+        <v>1993</v>
+      </c>
+      <c r="B44" s="15">
+        <v>70414697</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
+        <v>1994</v>
+      </c>
+      <c r="B45" s="15">
+        <v>69450776</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
+        <v>1995</v>
+      </c>
+      <c r="B46" s="15">
+        <v>70442935</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
+        <v>1996</v>
+      </c>
+      <c r="B47" s="15">
+        <v>69399164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="14">
+        <v>1997</v>
+      </c>
+      <c r="B48" s="15">
+        <v>71753430</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="14">
+        <v>1998</v>
+      </c>
+      <c r="B49" s="15">
+        <v>73913988</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="14">
+        <v>1999</v>
+      </c>
+      <c r="B50" s="15">
+        <v>77386368</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="14">
+        <v>2000</v>
+      </c>
+      <c r="B51" s="15">
+        <v>80403169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="14">
+        <v>2001</v>
+      </c>
+      <c r="B52" s="15">
+        <v>88562350</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="14">
+        <v>2002</v>
+      </c>
+      <c r="B53" s="15">
+        <v>98013347</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="14">
+        <v>2003</v>
+      </c>
+      <c r="B54" s="15">
+        <v>107794188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="14">
+        <v>2004</v>
+      </c>
+      <c r="B55" s="15">
+        <v>116068604</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="14">
+        <v>2005</v>
+      </c>
+      <c r="B56" s="15">
+        <v>122619584</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="14">
+        <v>2006</v>
+      </c>
+      <c r="B57" s="15">
+        <v>123854731</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="14">
+        <v>2007</v>
+      </c>
+      <c r="B58" s="15">
+        <v>129431246</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="14">
+        <v>2008</v>
+      </c>
+      <c r="B59" s="15">
+        <v>129049945.3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="14">
+        <v>2009</v>
+      </c>
+      <c r="B60" s="15">
+        <v>144758102.69999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="14">
+        <v>2010</v>
+      </c>
+      <c r="B61" s="15">
+        <v>146967799.90000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="14">
+        <v>2011</v>
+      </c>
+      <c r="B62" s="15">
+        <v>139703255.59999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="14">
+        <v>2012</v>
+      </c>
+      <c r="B63" s="15">
+        <v>140670243.09999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="14">
+        <v>2013</v>
+      </c>
+      <c r="B64" s="15">
+        <v>127625543.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="14">
+        <v>2014</v>
+      </c>
+      <c r="B65" s="15">
+        <v>132778961.59999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="14">
+        <v>2015</v>
+      </c>
+      <c r="B66" s="15">
+        <v>131578340.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="14">
+        <v>2016</v>
+      </c>
+      <c r="B67" s="15">
+        <v>118273783.59999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="14">
+        <v>2017</v>
+      </c>
+      <c r="B68" s="15">
+        <v>121626565</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="12">
+        <v>2018</v>
+      </c>
+      <c r="B69" s="13">
+        <v>133277539.59999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" s="13">
+        <v>146076729.90000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6087,8 +7049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6103,12 +7065,12 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>61</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6116,15 +7078,15 @@
         <v>1</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="34"/>
       <c r="F3" s="34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -6132,15 +7094,15 @@
         <v>1980</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6148,15 +7110,15 @@
         <v>1980</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="29"/>
       <c r="F5" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -6164,15 +7126,15 @@
         <v>1982</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="29"/>
       <c r="F6" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -6180,15 +7142,15 @@
         <v>1984</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="29"/>
       <c r="F7" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6196,15 +7158,15 @@
         <v>1986</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="29"/>
       <c r="F8" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6212,15 +7174,15 @@
         <v>1987</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="29"/>
       <c r="F9" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6228,15 +7190,15 @@
         <v>1987</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="29"/>
       <c r="F10" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6244,15 +7206,15 @@
         <v>1988</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6260,15 +7222,15 @@
         <v>1989</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -6276,15 +7238,15 @@
         <v>1991</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6292,15 +7254,15 @@
         <v>1993</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6308,15 +7270,15 @@
         <v>1995</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="29"/>
       <c r="F15" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -6324,15 +7286,15 @@
         <v>2000</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="38"/>
       <c r="F16" s="38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6340,15 +7302,15 @@
         <v>2011</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C17" s="38"/>
       <c r="D17" s="38" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E17" s="38"/>
       <c r="F17" s="38" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -6361,7 +7323,7 @@
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
@@ -6371,7 +7333,7 @@
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -6380,54 +7342,54 @@
       <c r="F20" s="29"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="59" t="s">
+      <c r="A21" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+    </row>
+    <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+    </row>
+    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-    </row>
-    <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="60" t="s">
-        <v>185</v>
-      </c>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-    </row>
-    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="59" t="s">
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+    </row>
+    <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-    </row>
-    <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="59" t="s">
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+    </row>
+    <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-    </row>
-    <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -6511,218 +7473,571 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="75.7109375" customWidth="1"/>
     <col min="3" max="3" width="2.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" style="88" customWidth="1"/>
+    <col min="6" max="9" width="10.7109375" style="88" customWidth="1"/>
+    <col min="10" max="10" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+    </row>
+    <row r="2" spans="1:10" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+    </row>
+    <row r="3" spans="1:10" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="66" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="67"/>
+      <c r="F3" s="81" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="79"/>
+    </row>
+    <row r="4" spans="1:10" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="73"/>
+      <c r="B4" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="74"/>
+      <c r="D4" s="71" t="s">
+        <v>214</v>
+      </c>
+      <c r="E4" s="72" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>231</v>
+      </c>
+      <c r="G4" s="68" t="s">
+        <v>232</v>
+      </c>
+      <c r="H4" s="68" t="s">
+        <v>218</v>
+      </c>
+      <c r="I4" s="68" t="s">
+        <v>218</v>
+      </c>
+      <c r="J4" s="78" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30"/>
-      <c r="B5" s="32"/>
+      <c r="B5" s="32" t="s">
+        <v>238</v>
+      </c>
       <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" s="84"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
-      <c r="B6" s="32"/>
+      <c r="B6" s="32" t="s">
+        <v>239</v>
+      </c>
       <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" s="84"/>
+      <c r="F6" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="G6" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
-      <c r="B7" s="32"/>
+      <c r="B7" s="32" t="s">
+        <v>233</v>
+      </c>
       <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E7" s="84"/>
+      <c r="F7" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
-      <c r="B8" s="32"/>
+      <c r="B8" s="32" t="s">
+        <v>234</v>
+      </c>
       <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E8" s="84"/>
+      <c r="F8" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="G8" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
-      <c r="B9" s="32"/>
+      <c r="B9" s="32" t="s">
+        <v>243</v>
+      </c>
       <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" s="84"/>
+      <c r="F9" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
-      <c r="B10" s="32"/>
+      <c r="B10" s="32" t="s">
+        <v>244</v>
+      </c>
       <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" s="84"/>
+      <c r="F10" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
-      <c r="B11" s="32"/>
+      <c r="B11" s="32" t="s">
+        <v>237</v>
+      </c>
       <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E11" s="84"/>
+      <c r="F11" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30"/>
-      <c r="B12" s="32"/>
+      <c r="B12" s="32" t="s">
+        <v>236</v>
+      </c>
       <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12" s="84"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="60"/>
+      <c r="B13" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="C13" s="59"/>
+      <c r="D13" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E13" s="84"/>
+      <c r="F13" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="G13" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="60"/>
+      <c r="B14" s="59" t="s">
+        <v>241</v>
+      </c>
+      <c r="C14" s="59"/>
+      <c r="D14" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" s="84"/>
+      <c r="F14" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="G14" s="87"/>
+      <c r="H14" s="87"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="60"/>
+      <c r="B15" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="C15" s="59"/>
+      <c r="D15" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E15" s="84"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="30"/>
+      <c r="B16" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E16" s="84"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87" t="s">
+        <v>230</v>
+      </c>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-    </row>
-    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>23</v>
-      </c>
+      <c r="D17" s="83"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="69"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-    </row>
-    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
-        <v>56</v>
-      </c>
+      <c r="D18" s="83"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="69"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="30"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-    </row>
-    <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-    </row>
-    <row r="21" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-    </row>
-    <row r="22" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-    </row>
-    <row r="23" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="83"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
+      <c r="H19" s="87"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="69"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="89"/>
+      <c r="J20" s="70"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="30"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="87"/>
+      <c r="J21" s="59"/>
+    </row>
+    <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="59"/>
+    </row>
+    <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="87"/>
+      <c r="J23" s="59"/>
+    </row>
+    <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="61"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="87"/>
+    </row>
+    <row r="25" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="61"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="87"/>
+      <c r="I25" s="87"/>
+    </row>
+    <row r="26" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="61"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="87"/>
+    </row>
+    <row r="27" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="61"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="30"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="87"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="59"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="30"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="59"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="30"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="87"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="59"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="30"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="87"/>
+      <c r="F31" s="87"/>
+      <c r="G31" s="87"/>
+      <c r="H31" s="87"/>
+      <c r="I31" s="87"/>
+      <c r="J31" s="59"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="59"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="30"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="87"/>
+      <c r="E33" s="87"/>
+      <c r="F33" s="87"/>
+      <c r="G33" s="87"/>
+      <c r="H33" s="87"/>
+      <c r="I33" s="87"/>
+      <c r="J33" s="59"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="30"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="87"/>
+      <c r="I34" s="87"/>
+      <c r="J34" s="59"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="30"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="87"/>
+      <c r="E35" s="87"/>
+      <c r="F35" s="87"/>
+      <c r="G35" s="87"/>
+      <c r="H35" s="87"/>
+      <c r="I35" s="87"/>
+      <c r="J35" s="59"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
+  <mergeCells count="6">
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6731,12 +8046,391 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="75.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" style="88" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+    </row>
+    <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+    </row>
+    <row r="3" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="66" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="67"/>
+      <c r="F3" s="79"/>
+    </row>
+    <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="73"/>
+      <c r="B4" s="74" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="74"/>
+      <c r="D4" s="71" t="s">
+        <v>214</v>
+      </c>
+      <c r="E4" s="72" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="78" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="60"/>
+      <c r="B5" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" s="59"/>
+      <c r="D5" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" s="84"/>
+      <c r="F5" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="60"/>
+      <c r="B6" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" s="59"/>
+      <c r="D6" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" s="84"/>
+      <c r="F6" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="60"/>
+      <c r="B7" s="59" t="s">
+        <v>248</v>
+      </c>
+      <c r="C7" s="59"/>
+      <c r="D7" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E7" s="84"/>
+      <c r="F7" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="60"/>
+      <c r="B8" s="59" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E8" s="84"/>
+      <c r="F8" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="60"/>
+      <c r="B9" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" s="59"/>
+      <c r="D9" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" s="84"/>
+      <c r="F9" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="60"/>
+      <c r="B10" s="59" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" s="59"/>
+      <c r="D10" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" s="84"/>
+      <c r="F10" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="60"/>
+      <c r="B11" s="59" t="s">
+        <v>252</v>
+      </c>
+      <c r="C11" s="59"/>
+      <c r="D11" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E11" s="84"/>
+      <c r="F11" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="60"/>
+      <c r="B12" s="59" t="s">
+        <v>253</v>
+      </c>
+      <c r="C12" s="59"/>
+      <c r="D12" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12" s="84"/>
+      <c r="F12" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="60"/>
+      <c r="B13" s="59" t="s">
+        <v>254</v>
+      </c>
+      <c r="C13" s="59"/>
+      <c r="D13" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E13" s="84"/>
+      <c r="F13" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="60"/>
+      <c r="B14" s="59" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" s="59"/>
+      <c r="D14" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" s="84"/>
+      <c r="F14" s="69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="60"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="69"/>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="60"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="69"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="60"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="69"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="60"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="69"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="60"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="69"/>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="70"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="60"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="59"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="59"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="59"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="61"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+    </row>
+    <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="61"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+    </row>
+    <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="61"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+    </row>
+    <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="61"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="60"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="59"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="60"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="59"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="60"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="59"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="60"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="87"/>
+      <c r="F31" s="59"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="60"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="59"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="60"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="87"/>
+      <c r="E33" s="87"/>
+      <c r="F33" s="59"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="60"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="59"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="60"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="87"/>
+      <c r="E35" s="87"/>
+      <c r="F35" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -6763,161 +8457,163 @@
   <sheetData>
     <row r="1" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
       <c r="B3" s="34" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="E3" s="34"/>
       <c r="F3" s="34" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="34" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I3" s="34"/>
       <c r="J3" s="34" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="K3" s="34"/>
       <c r="L3" s="34" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="M3" s="34"/>
       <c r="N3" s="34" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="57"/>
       <c r="B4" s="56" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C4" s="56"/>
       <c r="D4" s="56" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="58" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="58" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="I4" s="58"/>
       <c r="J4" s="56" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="K4" s="56"/>
       <c r="L4" s="56" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="M4" s="56"/>
       <c r="N4" s="56" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="57"/>
       <c r="B5" s="56" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C5" s="56"/>
       <c r="D5" s="56" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="58" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="G5" s="58"/>
       <c r="H5" s="58" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="I5" s="58"/>
       <c r="J5" s="56" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="K5" s="56"/>
       <c r="L5" s="56" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="M5" s="56"/>
       <c r="N5" s="56" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="57"/>
       <c r="B6" s="56" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C6" s="56"/>
       <c r="D6" s="56" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E6" s="58"/>
       <c r="F6" s="58" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="G6" s="58"/>
       <c r="H6" s="58" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="I6" s="58"/>
       <c r="J6" s="56" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="K6" s="56"/>
       <c r="L6" s="56" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="M6" s="56"/>
       <c r="N6" s="56" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35"/>
       <c r="B7" s="36" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="36" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E7" s="36"/>
       <c r="F7" s="36" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="G7" s="36"/>
       <c r="H7" s="36" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="I7" s="36"/>
       <c r="J7" s="36" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="K7" s="36"/>
       <c r="L7" s="36" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
+      <c r="N7" s="36" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="57"/>
@@ -6937,7 +8633,7 @@
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="56"/>
       <c r="C9" s="56"/>
@@ -6955,7 +8651,7 @@
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="56"/>
       <c r="C10" s="56"/>
@@ -6973,7 +8669,7 @@
     </row>
     <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -6981,16 +8677,20 @@
       <c r="M11" s="23"/>
       <c r="N11" s="23"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="56"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
+    <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>223</v>
+      </c>
       <c r="B13" s="56"/>
       <c r="C13" s="56"/>
       <c r="D13" s="56"/>
@@ -7006,18 +8706,10 @@
       <c r="N14" s="56"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="56"/>
       <c r="C15" s="56"/>
       <c r="D15" s="56"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="56"/>
       <c r="M15" s="56"/>
       <c r="N15" s="56"/>
     </row>
@@ -7133,13 +8825,29 @@
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
     </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="57"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
@@ -7165,222 +8873,222 @@
   <sheetData>
     <row r="1" spans="1:9" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="27" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D3" s="39"/>
       <c r="E3" s="39" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F3" s="39"/>
       <c r="G3" s="40" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H3" s="39"/>
       <c r="I3" s="40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="23" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B4" s="32"/>
       <c r="C4" s="32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="32" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="23" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B5" s="32"/>
       <c r="C5" s="32" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="32" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F5" s="32"/>
       <c r="G5" s="32" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="32" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="23" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B6" s="32"/>
       <c r="C6" s="32" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="32" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="32" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="23" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B7" s="32"/>
       <c r="C7" s="32" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="32" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="32" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H7" s="32"/>
       <c r="I7" s="32" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="23" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B8" s="32"/>
       <c r="C8" s="32" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H8" s="32"/>
       <c r="I8" s="32" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="23" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="32" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="32" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H9" s="32"/>
       <c r="I9" s="32" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="23" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="32" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H10" s="32"/>
       <c r="I10" s="32" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="23" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="32" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H11" s="32"/>
       <c r="I11" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="23" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B12" s="36"/>
       <c r="C12" s="36" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="38" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="32" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -7396,7 +9104,7 @@
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -7407,7 +9115,7 @@
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -7418,7 +9126,7 @@
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -7428,27 +9136,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -7537,7 +9245,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
@@ -7555,12 +9263,12 @@
   <sheetData>
     <row r="1" spans="1:3" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="45"/>
@@ -7572,272 +9280,272 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B4" s="44"/>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B5" s="44"/>
       <c r="C5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B6" s="44"/>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B7" s="44"/>
       <c r="C7" s="23" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B8" s="44"/>
       <c r="C8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B9" s="44"/>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B10" s="44"/>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B11" s="44"/>
       <c r="C11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B12" s="44"/>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B13" s="44"/>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B14" s="44"/>
       <c r="C14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B15" s="44"/>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B18" s="44"/>
       <c r="C18" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B19" s="44"/>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B20" s="44"/>
       <c r="C20" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B21" s="37"/>
       <c r="C21" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B22" s="37"/>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B23" s="37"/>
       <c r="C23" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B25" s="37"/>
       <c r="C25" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B26" s="37"/>
       <c r="C26" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B27" s="37"/>
       <c r="C27" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B28" s="37"/>
       <c r="C28" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B29" s="37"/>
       <c r="C29" s="23" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B30" s="37"/>
       <c r="C30" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B31" s="37"/>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B32" s="43"/>
       <c r="C32" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B33" s="37"/>
       <c r="C33" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -7852,7 +9560,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="51" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B36" s="52"/>
       <c r="C36" s="52"/>
@@ -7864,7 +9572,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B38" s="52"/>
       <c r="C38" s="52"/>
@@ -7876,7 +9584,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" s="52"/>
       <c r="C40" s="52"/>
@@ -7887,30 +9595,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="61" t="s">
-        <v>180</v>
-      </c>
-      <c r="B42" s="61"/>
-      <c r="C42" s="61"/>
+      <c r="A42" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="B42" s="63"/>
+      <c r="C42" s="63"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="62" t="s">
-        <v>181</v>
-      </c>
-      <c r="B43" s="62"/>
-      <c r="C43" s="62"/>
+      <c r="A43" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="B43" s="64"/>
+      <c r="C43" s="64"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="61" t="s">
-        <v>182</v>
-      </c>
-      <c r="B44" s="61"/>
-      <c r="C44" s="61"/>
+      <c r="A44" s="63" t="s">
+        <v>178</v>
+      </c>
+      <c r="B44" s="63"/>
+      <c r="C44" s="63"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="59"/>
-      <c r="B45" s="59"/>
-      <c r="C45" s="59"/>
+      <c r="A45" s="61"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="61"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>
@@ -7967,7 +9675,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
@@ -8426,7 +10134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -8681,589 +10389,4 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D70"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
-        <v>1951</v>
-      </c>
-      <c r="B2" s="15">
-        <v>1851571</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
-        <v>1952</v>
-      </c>
-      <c r="B3" s="15">
-        <v>2216848</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
-        <v>1953</v>
-      </c>
-      <c r="B4" s="15">
-        <v>2167456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
-        <v>1954</v>
-      </c>
-      <c r="B5" s="15">
-        <v>1918046</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
-        <v>1955</v>
-      </c>
-      <c r="B6" s="15">
-        <v>2251894</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
-        <v>1956</v>
-      </c>
-      <c r="B7" s="15">
-        <v>3266903</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>1957</v>
-      </c>
-      <c r="B8" s="15">
-        <v>4389237</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
-        <v>1958</v>
-      </c>
-      <c r="B9" s="15">
-        <v>4906015</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
-        <v>1959</v>
-      </c>
-      <c r="B10" s="15">
-        <v>7122610</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>1960</v>
-      </c>
-      <c r="B11" s="15">
-        <v>8080015</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
-        <v>1961</v>
-      </c>
-      <c r="B12" s="15">
-        <v>9607023</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
-        <v>1962</v>
-      </c>
-      <c r="B13" s="15">
-        <v>11069059</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <v>1963</v>
-      </c>
-      <c r="B14" s="15">
-        <v>13662879</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>1964</v>
-      </c>
-      <c r="B15" s="15">
-        <v>15323870</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
-        <v>1965</v>
-      </c>
-      <c r="B16" s="15">
-        <v>15745852</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
-        <v>1966</v>
-      </c>
-      <c r="B17" s="15">
-        <v>16178640</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
-        <v>1967</v>
-      </c>
-      <c r="B18" s="15">
-        <v>17149186</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
-        <v>1968</v>
-      </c>
-      <c r="B19" s="15">
-        <v>16525038</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
-        <v>1969</v>
-      </c>
-      <c r="B20" s="15">
-        <v>16309900</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
-        <v>1970</v>
-      </c>
-      <c r="B21" s="15">
-        <v>15863385</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
-        <v>1971</v>
-      </c>
-      <c r="B22" s="15">
-        <v>16153756</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
-        <v>1972</v>
-      </c>
-      <c r="B23" s="15">
-        <v>17097951</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
-        <v>1973</v>
-      </c>
-      <c r="B24" s="15">
-        <v>17574486</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
-        <v>1974</v>
-      </c>
-      <c r="B25" s="15">
-        <v>18176457</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
-        <v>1975</v>
-      </c>
-      <c r="B26" s="15">
-        <v>19859548</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
-        <v>1976</v>
-      </c>
-      <c r="B27" s="15">
-        <v>21616382</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
-        <v>1977</v>
-      </c>
-      <c r="B28" s="15">
-        <v>24817577</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
-        <v>1978</v>
-      </c>
-      <c r="B29" s="15">
-        <v>27140849</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
-        <v>1979</v>
-      </c>
-      <c r="B30" s="15">
-        <v>29620597</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
-        <v>1980</v>
-      </c>
-      <c r="B31" s="15">
-        <v>31386095</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="14">
-        <v>1981</v>
-      </c>
-      <c r="B32" s="15">
-        <v>34589634</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
-        <v>1982</v>
-      </c>
-      <c r="B33" s="15">
-        <v>37822363</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
-        <v>1983</v>
-      </c>
-      <c r="B34" s="15">
-        <v>40009032</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
-        <v>1984</v>
-      </c>
-      <c r="B35" s="15">
-        <v>44012149</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
-        <v>1985</v>
-      </c>
-      <c r="B36" s="15">
-        <v>50180369</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="14">
-        <v>1986</v>
-      </c>
-      <c r="B37" s="15">
-        <v>52951181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="14">
-        <v>1987</v>
-      </c>
-      <c r="B38" s="15">
-        <v>57099656</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="14">
-        <v>1988</v>
-      </c>
-      <c r="B39" s="15">
-        <v>58826512</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
-        <v>1989</v>
-      </c>
-      <c r="B40" s="15">
-        <v>63571605</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="14">
-        <v>1990</v>
-      </c>
-      <c r="B41" s="15">
-        <v>65831189</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="14">
-        <v>1991</v>
-      </c>
-      <c r="B42" s="15">
-        <v>64147951</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="14">
-        <v>1992</v>
-      </c>
-      <c r="B43" s="15">
-        <v>68577184</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="14">
-        <v>1993</v>
-      </c>
-      <c r="B44" s="15">
-        <v>70414697</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="14">
-        <v>1994</v>
-      </c>
-      <c r="B45" s="15">
-        <v>69450776</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="14">
-        <v>1995</v>
-      </c>
-      <c r="B46" s="15">
-        <v>70442935</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="14">
-        <v>1996</v>
-      </c>
-      <c r="B47" s="15">
-        <v>69399164</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="14">
-        <v>1997</v>
-      </c>
-      <c r="B48" s="15">
-        <v>71753430</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="14">
-        <v>1998</v>
-      </c>
-      <c r="B49" s="15">
-        <v>73913988</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="14">
-        <v>1999</v>
-      </c>
-      <c r="B50" s="15">
-        <v>77386368</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="14">
-        <v>2000</v>
-      </c>
-      <c r="B51" s="15">
-        <v>80403169</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="14">
-        <v>2001</v>
-      </c>
-      <c r="B52" s="15">
-        <v>88562350</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="14">
-        <v>2002</v>
-      </c>
-      <c r="B53" s="15">
-        <v>98013347</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="14">
-        <v>2003</v>
-      </c>
-      <c r="B54" s="15">
-        <v>107794188</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="14">
-        <v>2004</v>
-      </c>
-      <c r="B55" s="15">
-        <v>116068604</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="14">
-        <v>2005</v>
-      </c>
-      <c r="B56" s="15">
-        <v>122619584</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="14">
-        <v>2006</v>
-      </c>
-      <c r="B57" s="15">
-        <v>123854731</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="14">
-        <v>2007</v>
-      </c>
-      <c r="B58" s="15">
-        <v>129431246</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="14">
-        <v>2008</v>
-      </c>
-      <c r="B59" s="15">
-        <v>129049945.3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="14">
-        <v>2009</v>
-      </c>
-      <c r="B60" s="15">
-        <v>144758102.69999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="14">
-        <v>2010</v>
-      </c>
-      <c r="B61" s="15">
-        <v>146967799.90000001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="14">
-        <v>2011</v>
-      </c>
-      <c r="B62" s="15">
-        <v>139703255.59999999</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="14">
-        <v>2012</v>
-      </c>
-      <c r="B63" s="15">
-        <v>140670243.09999999</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="14">
-        <v>2013</v>
-      </c>
-      <c r="B64" s="15">
-        <v>127625543.8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="14">
-        <v>2014</v>
-      </c>
-      <c r="B65" s="15">
-        <v>132778961.59999999</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="14">
-        <v>2015</v>
-      </c>
-      <c r="B66" s="15">
-        <v>131578340.7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="14">
-        <v>2016</v>
-      </c>
-      <c r="B67" s="15">
-        <v>118273783.59999999</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="14">
-        <v>2017</v>
-      </c>
-      <c r="B68" s="15">
-        <v>121626565</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="12">
-        <v>2018</v>
-      </c>
-      <c r="B69" s="13">
-        <v>133277539.59999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B70" s="13">
-        <v>146076729.90000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Began discussion of the method of agreement
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -810,9 +810,6 @@
     <t>There is an objective reality independent of the observer that can only be known through reasoned and logical analysis of data and information gathered from sensory experience. The organization is an object that can be measured and analyzed.</t>
   </si>
   <si>
-    <t>Human relations management</t>
-  </si>
-  <si>
     <t>There is an objective reality independent of the observer.  The organization is a kind of  sociological process that both affects and is affected by society.</t>
   </si>
   <si>
@@ -820,9 +817,6 @@
   </si>
   <si>
     <t>Since all knowledge is filtered by the experience of the observer, all distinctions used to describe reality are arbitrary and semantic in origin.  The organization is an abstraction that is best understood by revealing and comprehending the underlying assumptions used to construct it.</t>
-  </si>
-  <si>
-    <t>The organization is a pattern of meanings that created through human interaction that produces shared values, traditions, and customs (i.e., a culture).</t>
   </si>
   <si>
     <t xml:space="preserve">The organization is a machine that management designs, constructs, and maintains to achieve specific goals and objectives.
@@ -849,9 +843,6 @@
   </si>
   <si>
     <t>Variable</t>
-  </si>
-  <si>
-    <t>Theories and Schools of Thought</t>
   </si>
   <si>
     <t>Bureacracy theory
@@ -1018,6 +1009,17 @@
   <si>
     <t>Table</t>
   </si>
+  <si>
+    <t>The organization is a pattern of meanings that created through human interaction that produces shared values, traditions, and customs (i.e., a culture).
+The organization is a political arena</t>
+  </si>
+  <si>
+    <t>Modeles, Theories, and Schools of Thought</t>
+  </si>
+  <si>
+    <t>Human relations management
+Garbage can model</t>
+  </si>
 </sst>
 </file>
 
@@ -1027,7 +1029,7 @@
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1098,6 +1100,21 @@
     <font>
       <i/>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1301,7 +1318,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1474,25 +1491,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
@@ -1530,15 +1529,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1559,6 +1549,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7065,7 +7097,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7342,54 +7374,54 @@
       <c r="F20" s="29"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="61" t="s">
+      <c r="A21" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="82" t="s">
         <v>181</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
     </row>
     <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="61" t="s">
+      <c r="A23" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="81"/>
     </row>
     <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="61" t="s">
+      <c r="A25" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -7475,7 +7507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
@@ -7485,8 +7517,8 @@
     <col min="1" max="1" width="2.7109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="75.7109375" customWidth="1"/>
     <col min="3" max="3" width="2.7109375" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" style="88" customWidth="1"/>
-    <col min="6" max="9" width="10.7109375" style="88" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" style="79" customWidth="1"/>
+    <col min="6" max="9" width="10.7109375" style="79" customWidth="1"/>
     <col min="10" max="10" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7494,372 +7526,372 @@
       <c r="A1" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
     </row>
     <row r="2" spans="1:10" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:10" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="66" t="s">
+      <c r="A3" s="69"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="83" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85" t="s">
+        <v>225</v>
+      </c>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="73"/>
+    </row>
+    <row r="4" spans="1:10" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67"/>
+      <c r="B4" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="68"/>
+      <c r="D4" s="65" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>213</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4" s="62" t="s">
+        <v>229</v>
+      </c>
+      <c r="H4" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="81" t="s">
-        <v>228</v>
-      </c>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="79"/>
-    </row>
-    <row r="4" spans="1:10" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="73"/>
-      <c r="B4" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="71" t="s">
-        <v>214</v>
-      </c>
-      <c r="E4" s="72" t="s">
+      <c r="I4" s="62" t="s">
+        <v>216</v>
+      </c>
+      <c r="J4" s="72" t="s">
         <v>215</v>
-      </c>
-      <c r="F4" s="68" t="s">
-        <v>231</v>
-      </c>
-      <c r="G4" s="68" t="s">
-        <v>232</v>
-      </c>
-      <c r="H4" s="68" t="s">
-        <v>218</v>
-      </c>
-      <c r="I4" s="68" t="s">
-        <v>218</v>
-      </c>
-      <c r="J4" s="78" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30"/>
       <c r="B5" s="32" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C5" s="32"/>
-      <c r="D5" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E5" s="84"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="69" t="s">
-        <v>229</v>
+      <c r="D5" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E5" s="75"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
       <c r="B6" s="32" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C6" s="32"/>
-      <c r="D6" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="G6" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="69" t="s">
-        <v>229</v>
+      <c r="D6" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E6" s="75"/>
+      <c r="F6" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="G6" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
       <c r="B7" s="32" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C7" s="32"/>
-      <c r="D7" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E7" s="84"/>
-      <c r="F7" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="69" t="s">
-        <v>229</v>
+      <c r="D7" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" s="75"/>
+      <c r="F7" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
       <c r="B8" s="32" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C8" s="32"/>
-      <c r="D8" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E8" s="84"/>
-      <c r="F8" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="G8" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="H8" s="87"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="69" t="s">
-        <v>229</v>
+      <c r="D8" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E8" s="75"/>
+      <c r="F8" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="G8" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
       <c r="B9" s="32" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C9" s="32"/>
-      <c r="D9" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E9" s="84"/>
-      <c r="F9" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="69" t="s">
-        <v>229</v>
+      <c r="D9" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E9" s="75"/>
+      <c r="F9" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
       <c r="B10" s="32" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C10" s="32"/>
-      <c r="D10" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E10" s="84"/>
-      <c r="F10" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="G10" s="87"/>
-      <c r="H10" s="87"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="69" t="s">
-        <v>229</v>
+      <c r="D10" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E10" s="75"/>
+      <c r="F10" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
       <c r="B11" s="32" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C11" s="32"/>
-      <c r="D11" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="G11" s="87"/>
-      <c r="H11" s="87"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="69" t="s">
-        <v>229</v>
+      <c r="D11" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" s="75"/>
+      <c r="F11" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30"/>
       <c r="B12" s="32" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C12" s="32"/>
-      <c r="D12" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E12" s="84"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="69" t="s">
-        <v>229</v>
+      <c r="D12" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E12" s="75"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="59" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C13" s="59"/>
-      <c r="D13" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E13" s="84"/>
-      <c r="F13" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="G13" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="69" t="s">
-        <v>229</v>
+      <c r="D13" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E13" s="75"/>
+      <c r="F13" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="G13" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="59" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C14" s="59"/>
-      <c r="D14" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E14" s="84"/>
-      <c r="F14" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="G14" s="87"/>
-      <c r="H14" s="87"/>
-      <c r="I14" s="87"/>
-      <c r="J14" s="69" t="s">
-        <v>229</v>
+      <c r="D14" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E14" s="75"/>
+      <c r="F14" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="G14" s="78"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
       <c r="B15" s="59" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C15" s="59"/>
-      <c r="D15" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E15" s="84"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="H15" s="87"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="69" t="s">
-        <v>229</v>
+      <c r="D15" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E15" s="75"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="H15" s="78"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30"/>
       <c r="B16" s="32" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C16" s="32"/>
-      <c r="D16" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E16" s="84"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87" t="s">
-        <v>230</v>
-      </c>
-      <c r="H16" s="87"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="69" t="s">
-        <v>229</v>
+      <c r="D16" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E16" s="75"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="87"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="69"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="63"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="69"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="63"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="69"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="63"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="89"/>
-      <c r="J20" s="70"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="64"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="87"/>
-      <c r="H21" s="87"/>
-      <c r="I21" s="87"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="78"/>
       <c r="J21" s="59"/>
     </row>
     <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7868,12 +7900,12 @@
       </c>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="87"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="78"/>
       <c r="J22" s="59"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7882,152 +7914,152 @@
       </c>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="78"/>
       <c r="J23" s="59"/>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="78"/>
     </row>
     <row r="25" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="87"/>
+      <c r="A25" s="81"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
     </row>
     <row r="26" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="61"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="87"/>
-      <c r="I26" s="87"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="81"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
     </row>
     <row r="27" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="61"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
+      <c r="A27" s="81"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="78"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="30"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="87"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="78"/>
       <c r="J28" s="59"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="30"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
-      <c r="I29" s="87"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="78"/>
       <c r="J29" s="59"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="30"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87"/>
-      <c r="I30" s="87"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="78"/>
       <c r="J30" s="59"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="30"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="87"/>
-      <c r="I31" s="87"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="78"/>
+      <c r="G31" s="78"/>
+      <c r="H31" s="78"/>
+      <c r="I31" s="78"/>
       <c r="J31" s="59"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
-      <c r="D32" s="87"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="87"/>
-      <c r="I32" s="87"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="78"/>
+      <c r="H32" s="78"/>
+      <c r="I32" s="78"/>
       <c r="J32" s="59"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="32"/>
       <c r="C33" s="32"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="87"/>
-      <c r="H33" s="87"/>
-      <c r="I33" s="87"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="78"/>
+      <c r="H33" s="78"/>
+      <c r="I33" s="78"/>
       <c r="J33" s="59"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="30"/>
       <c r="B34" s="32"/>
       <c r="C34" s="32"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="87"/>
-      <c r="I34" s="87"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="78"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="78"/>
       <c r="J34" s="59"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="30"/>
       <c r="B35" s="32"/>
       <c r="C35" s="32"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="87"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="87"/>
-      <c r="I35" s="87"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="78"/>
+      <c r="I35" s="78"/>
       <c r="J35" s="59"/>
     </row>
   </sheetData>
@@ -8058,244 +8090,244 @@
     <col min="1" max="1" width="2.7109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="75.7109375" customWidth="1"/>
     <col min="3" max="3" width="2.7109375" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" style="88" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" style="79" customWidth="1"/>
     <col min="6" max="6" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>257</v>
-      </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
+        <v>254</v>
+      </c>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>245</v>
-      </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
+        <v>242</v>
+      </c>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="66" t="s">
-        <v>216</v>
-      </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="79"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="83" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3" s="84"/>
+      <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="73"/>
-      <c r="B4" s="74" t="s">
-        <v>256</v>
-      </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="71" t="s">
-        <v>214</v>
-      </c>
-      <c r="E4" s="72" t="s">
+      <c r="A4" s="67"/>
+      <c r="B4" s="68" t="s">
+        <v>253</v>
+      </c>
+      <c r="C4" s="68"/>
+      <c r="D4" s="65" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>213</v>
+      </c>
+      <c r="F4" s="72" t="s">
         <v>215</v>
-      </c>
-      <c r="F4" s="78" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60"/>
       <c r="B5" s="59" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C5" s="59"/>
-      <c r="D5" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E5" s="84"/>
-      <c r="F5" s="69" t="s">
-        <v>229</v>
+      <c r="D5" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E5" s="75"/>
+      <c r="F5" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60"/>
       <c r="B6" s="59" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C6" s="59"/>
-      <c r="D6" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="69" t="s">
-        <v>229</v>
+      <c r="D6" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E6" s="75"/>
+      <c r="F6" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>
       <c r="B7" s="59" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C7" s="59"/>
-      <c r="D7" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E7" s="84"/>
-      <c r="F7" s="69" t="s">
-        <v>229</v>
+      <c r="D7" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" s="75"/>
+      <c r="F7" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
       <c r="B8" s="59" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C8" s="59"/>
-      <c r="D8" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E8" s="84"/>
-      <c r="F8" s="69" t="s">
-        <v>229</v>
+      <c r="D8" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E8" s="75"/>
+      <c r="F8" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60"/>
       <c r="B9" s="59" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C9" s="59"/>
-      <c r="D9" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E9" s="84"/>
-      <c r="F9" s="69" t="s">
-        <v>229</v>
+      <c r="D9" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E9" s="75"/>
+      <c r="F9" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="60"/>
       <c r="B10" s="59" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C10" s="59"/>
-      <c r="D10" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E10" s="84"/>
-      <c r="F10" s="69" t="s">
-        <v>229</v>
+      <c r="D10" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E10" s="75"/>
+      <c r="F10" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="60"/>
       <c r="B11" s="59" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C11" s="59"/>
-      <c r="D11" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="69" t="s">
-        <v>229</v>
+      <c r="D11" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" s="75"/>
+      <c r="F11" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60"/>
       <c r="B12" s="59" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C12" s="59"/>
-      <c r="D12" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E12" s="84"/>
-      <c r="F12" s="69" t="s">
-        <v>229</v>
+      <c r="D12" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E12" s="75"/>
+      <c r="F12" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="59" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C13" s="59"/>
-      <c r="D13" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E13" s="84"/>
-      <c r="F13" s="69" t="s">
-        <v>229</v>
+      <c r="D13" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E13" s="75"/>
+      <c r="F13" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="59" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C14" s="59"/>
-      <c r="D14" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E14" s="84"/>
-      <c r="F14" s="69" t="s">
-        <v>229</v>
+      <c r="D14" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="E14" s="75"/>
+      <c r="F14" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
       <c r="B15" s="59"/>
       <c r="C15" s="59"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="69"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="63"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
       <c r="B16" s="59"/>
       <c r="C16" s="59"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="69"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="63"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="60"/>
       <c r="B17" s="59"/>
       <c r="C17" s="59"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="69"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="63"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="60"/>
       <c r="B18" s="59"/>
       <c r="C18" s="59"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="69"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="63"/>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="60"/>
       <c r="B19" s="59"/>
       <c r="C19" s="59"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="69"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="63"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="70"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="64"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="60"/>
       <c r="B21" s="59"/>
       <c r="C21" s="59"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
       <c r="F21" s="59"/>
     </row>
     <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -8304,8 +8336,8 @@
       </c>
       <c r="B22" s="59"/>
       <c r="C22" s="59"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
       <c r="F22" s="59"/>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -8314,100 +8346,100 @@
       </c>
       <c r="B23" s="59"/>
       <c r="C23" s="59"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
+      <c r="A25" s="81"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="61"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="61"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
+      <c r="A27" s="81"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
       <c r="B28" s="59"/>
       <c r="C28" s="59"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
       <c r="F28" s="59"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="60"/>
       <c r="B29" s="59"/>
       <c r="C29" s="59"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
       <c r="F29" s="59"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="60"/>
       <c r="B30" s="59"/>
       <c r="C30" s="59"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="87"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
       <c r="F30" s="59"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="60"/>
       <c r="B31" s="59"/>
       <c r="C31" s="59"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
       <c r="F31" s="59"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="60"/>
       <c r="B32" s="59"/>
       <c r="C32" s="59"/>
-      <c r="D32" s="87"/>
-      <c r="E32" s="87"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="78"/>
       <c r="F32" s="59"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="60"/>
       <c r="B33" s="59"/>
       <c r="C33" s="59"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
       <c r="F33" s="59"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="60"/>
       <c r="B34" s="59"/>
       <c r="C34" s="59"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
       <c r="F34" s="59"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="60"/>
       <c r="B35" s="59"/>
       <c r="C35" s="59"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="87"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
       <c r="F35" s="59"/>
     </row>
   </sheetData>
@@ -8430,7 +8462,7 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -8452,47 +8484,47 @@
     <col min="11" max="11" width="2.7109375" customWidth="1"/>
     <col min="12" max="12" width="40.7109375" customWidth="1"/>
     <col min="13" max="13" width="2.7109375" customWidth="1"/>
-    <col min="14" max="14" width="30.7109375" customWidth="1"/>
+    <col min="14" max="14" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="92" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="93" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="34" t="s">
+      <c r="A3" s="94"/>
+      <c r="B3" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39" t="s">
+        <v>207</v>
+      </c>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39" t="s">
         <v>196</v>
       </c>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34" t="s">
-        <v>219</v>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8506,11 +8538,11 @@
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="58" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="58" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I4" s="58"/>
       <c r="J4" s="56" t="s">
@@ -8522,97 +8554,97 @@
       </c>
       <c r="M4" s="56"/>
       <c r="N4" s="56" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="56" t="s">
+      <c r="A5" s="90"/>
+      <c r="B5" s="91" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56" t="s">
+      <c r="C5" s="91"/>
+      <c r="D5" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58" t="s">
+      <c r="E5" s="91"/>
+      <c r="F5" s="91" t="s">
         <v>205</v>
       </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58" t="s">
+      <c r="G5" s="91"/>
+      <c r="H5" s="91" t="s">
+        <v>209</v>
+      </c>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91" t="s">
+        <v>190</v>
+      </c>
+      <c r="K5" s="91"/>
+      <c r="L5" s="91" t="s">
+        <v>193</v>
+      </c>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="90"/>
+      <c r="B6" s="91" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91" t="s">
+        <v>203</v>
+      </c>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91" t="s">
+        <v>199</v>
+      </c>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91" t="s">
+        <v>255</v>
+      </c>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91" t="s">
+        <v>191</v>
+      </c>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91" t="s">
+        <v>194</v>
+      </c>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="90"/>
+      <c r="B7" s="91" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="91"/>
+      <c r="D7" s="91" t="s">
+        <v>204</v>
+      </c>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91" t="s">
+        <v>208</v>
+      </c>
+      <c r="G7" s="91"/>
+      <c r="H7" s="91" t="s">
         <v>211</v>
       </c>
-      <c r="I5" s="58"/>
-      <c r="J5" s="56" t="s">
-        <v>190</v>
-      </c>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56" t="s">
-        <v>193</v>
-      </c>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57"/>
-      <c r="B6" s="56" t="s">
-        <v>187</v>
-      </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56" t="s">
-        <v>203</v>
-      </c>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58" t="s">
-        <v>199</v>
-      </c>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58" t="s">
-        <v>210</v>
-      </c>
-      <c r="I6" s="58"/>
-      <c r="J6" s="56" t="s">
-        <v>191</v>
-      </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56" t="s">
-        <v>194</v>
-      </c>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36" t="s">
-        <v>204</v>
-      </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36" t="s">
-        <v>209</v>
-      </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36" t="s">
-        <v>213</v>
-      </c>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36" t="s">
+      <c r="I7" s="91"/>
+      <c r="J7" s="91" t="s">
         <v>198</v>
       </c>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36" t="s">
+      <c r="K7" s="91"/>
+      <c r="L7" s="91" t="s">
         <v>195</v>
       </c>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36" t="s">
-        <v>222</v>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -8679,7 +8711,7 @@
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -8689,7 +8721,7 @@
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B13" s="56"/>
       <c r="C13" s="56"/>
@@ -8843,7 +8875,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="44" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="43" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9136,27 +9168,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="61"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
+      <c r="A19" s="81"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -9595,30 +9627,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="63" t="s">
+      <c r="A42" s="88" t="s">
         <v>176</v>
       </c>
-      <c r="B42" s="63"/>
-      <c r="C42" s="63"/>
+      <c r="B42" s="88"/>
+      <c r="C42" s="88"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="64" t="s">
+      <c r="A43" s="89" t="s">
         <v>177</v>
       </c>
-      <c r="B43" s="64"/>
-      <c r="C43" s="64"/>
+      <c r="B43" s="89"/>
+      <c r="C43" s="89"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="63" t="s">
+      <c r="A44" s="88" t="s">
         <v>178</v>
       </c>
-      <c r="B44" s="63"/>
-      <c r="C44" s="63"/>
+      <c r="B44" s="88"/>
+      <c r="C44" s="88"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="61"/>
-      <c r="B45" s="61"/>
-      <c r="C45" s="61"/>
+      <c r="A45" s="81"/>
+      <c r="B45" s="81"/>
+      <c r="C45" s="81"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>

</xml_diff>

<commit_message>
Added York & Ahn (2012) and Wu, Welch, & Huang (2015) to tables on determinants
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="287">
   <si>
     <t>Total</t>
   </si>
@@ -920,9 +920,6 @@
     <t>General Epistemological Approach</t>
   </si>
   <si>
-    <t>Technology Transfer Proxies</t>
-  </si>
-  <si>
     <t>Markman, Gianiodis, &amp; Phan (2009)</t>
   </si>
   <si>
@@ -1019,6 +1016,96 @@
   <si>
     <t>Human relations management
 Garbage can model</t>
+  </si>
+  <si>
+    <t>Patent effectiveness</t>
+  </si>
+  <si>
+    <t>Licensing agreements</t>
+  </si>
+  <si>
+    <t>York &amp; Ahn (2012)</t>
+  </si>
+  <si>
+    <t>Markman, Gianiodis, &amp; Phan (2009); York &amp; Ahn (2012)</t>
+  </si>
+  <si>
+    <t>Sponsored research funding</t>
+  </si>
+  <si>
+    <t>Reimbursement of legal fees</t>
+  </si>
+  <si>
+    <t>Patent applications</t>
+  </si>
+  <si>
+    <t>Patent allowances</t>
+  </si>
+  <si>
+    <t>Service agreements</t>
+  </si>
+  <si>
+    <t>Business acumen of TTO staff</t>
+  </si>
+  <si>
+    <t>Breadth of intellectual property protection pursued</t>
+  </si>
+  <si>
+    <t>Degree of patent protection selectivity</t>
+  </si>
+  <si>
+    <t>Stage when patent protection pursued</t>
+  </si>
+  <si>
+    <t>Emphasis on revenue generation</t>
+  </si>
+  <si>
+    <t>Relationship with local business community</t>
+  </si>
+  <si>
+    <t>Degree of institutional support for technology transfer activities</t>
+  </si>
+  <si>
+    <t>Degree of process specialization of TTO staff</t>
+  </si>
+  <si>
+    <t>Degree of website functionality</t>
+  </si>
+  <si>
+    <t>Researcher attitude towards technology transfer</t>
+  </si>
+  <si>
+    <t>Percent of university research funding received from industry</t>
+  </si>
+  <si>
+    <t>Researcher perception of TTO effectiveness</t>
+  </si>
+  <si>
+    <t>Wu, Welch, &amp; Huang (2015)</t>
+  </si>
+  <si>
+    <t>Researcher gender</t>
+  </si>
+  <si>
+    <t>Discipline of research that produced the technology</t>
+  </si>
+  <si>
+    <t>Performance of additional research during patent prosecution</t>
+  </si>
+  <si>
+    <t>Participation of industry researchers in the research that produced the technology</t>
+  </si>
+  <si>
+    <t>Researcher belief that a potential licensee must be identified for patent prosecution</t>
+  </si>
+  <si>
+    <t>Researcher belief that the university covers all patent expenses</t>
+  </si>
+  <si>
+    <t>Tenure status of researcher</t>
+  </si>
+  <si>
+    <t>Operationalizations of Technology Transfer</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1216,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1249,19 +1336,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1318,7 +1392,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1496,10 +1570,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1520,13 +1594,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1556,26 +1630,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1591,6 +1647,42 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7097,7 +7189,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7374,54 +7466,54 @@
       <c r="F20" s="29"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="81"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="89"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="90" t="s">
         <v>181</v>
       </c>
-      <c r="B22" s="82"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="82"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
     </row>
     <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="81" t="s">
+      <c r="A23" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="81"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
     </row>
     <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="81"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="81" t="s">
+      <c r="A25" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="81"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -7505,11 +7597,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7518,11 +7613,11 @@
     <col min="2" max="2" width="75.7109375" customWidth="1"/>
     <col min="3" max="3" width="2.7109375" customWidth="1"/>
     <col min="4" max="5" width="12.7109375" style="79" customWidth="1"/>
-    <col min="6" max="9" width="10.7109375" style="79" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" customWidth="1"/>
+    <col min="6" max="14" width="5.7109375" style="79" customWidth="1"/>
+    <col min="15" max="15" width="40.7109375" style="96" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>184</v>
       </c>
@@ -7532,8 +7627,14 @@
       <c r="G1" s="61"/>
       <c r="H1" s="61"/>
       <c r="I1" s="61"/>
-    </row>
-    <row r="2" spans="1:10" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="81"/>
+    </row>
+    <row r="2" spans="1:15" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>65</v>
       </c>
@@ -7543,24 +7644,35 @@
       <c r="G2" s="61"/>
       <c r="H2" s="61"/>
       <c r="I2" s="61"/>
-    </row>
-    <row r="3" spans="1:10" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="81"/>
+    </row>
+    <row r="3" spans="1:15" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="91" t="s">
         <v>214</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="85" t="s">
-        <v>225</v>
-      </c>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="73"/>
-    </row>
-    <row r="4" spans="1:10" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="92"/>
+      <c r="F3" s="100" t="s">
+        <v>286</v>
+      </c>
+      <c r="G3" s="83"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="95"/>
+    </row>
+    <row r="4" spans="1:15" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="68" t="s">
         <v>66</v>
@@ -7573,506 +7685,1113 @@
         <v>213</v>
       </c>
       <c r="F4" s="62" t="s">
+        <v>263</v>
+      </c>
+      <c r="G4" s="62" t="s">
+        <v>264</v>
+      </c>
+      <c r="H4" s="62" t="s">
+        <v>227</v>
+      </c>
+      <c r="I4" s="62" t="s">
+        <v>258</v>
+      </c>
+      <c r="J4" s="62" t="s">
+        <v>265</v>
+      </c>
+      <c r="K4" s="62" t="s">
         <v>228</v>
       </c>
-      <c r="G4" s="62" t="s">
-        <v>229</v>
-      </c>
-      <c r="H4" s="62" t="s">
+      <c r="L4" s="62" t="s">
+        <v>261</v>
+      </c>
+      <c r="M4" s="62" t="s">
+        <v>262</v>
+      </c>
+      <c r="N4" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="I4" s="62" t="s">
-        <v>216</v>
-      </c>
-      <c r="J4" s="72" t="s">
+      <c r="O4" s="72" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="30"/>
       <c r="B5" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E5" s="75"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78" t="s">
-        <v>227</v>
-      </c>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
       <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="63" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
       <c r="B6" s="32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E6" s="75"/>
-      <c r="F6" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="G6" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="H6" s="78"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="78" t="s">
+        <v>226</v>
+      </c>
       <c r="I6" s="78"/>
-      <c r="J6" s="63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="78"/>
+      <c r="K6" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="63" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
       <c r="B7" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E7" s="75"/>
-      <c r="F7" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="78" t="s">
+        <v>226</v>
+      </c>
       <c r="I7" s="78"/>
-      <c r="J7" s="63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="78"/>
+      <c r="N7" s="78"/>
+      <c r="O7" s="63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
       <c r="B8" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C8" s="32"/>
       <c r="D8" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E8" s="75"/>
-      <c r="F8" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="G8" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="H8" s="78"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="78" t="s">
+        <v>226</v>
+      </c>
       <c r="I8" s="78"/>
-      <c r="J8" s="63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="78"/>
+      <c r="K8" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L8" s="78"/>
+      <c r="M8" s="78"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
       <c r="B9" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E9" s="75"/>
-      <c r="F9" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="78" t="s">
+        <v>226</v>
+      </c>
       <c r="I9" s="78"/>
-      <c r="J9" s="63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
       <c r="B10" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E10" s="75"/>
-      <c r="F10" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="G10" s="78"/>
-      <c r="H10" s="78"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="78" t="s">
+        <v>226</v>
+      </c>
       <c r="I10" s="78"/>
-      <c r="J10" s="63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
       <c r="B11" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E11" s="75"/>
-      <c r="F11" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="78" t="s">
+        <v>226</v>
+      </c>
       <c r="I11" s="78"/>
-      <c r="J11" s="63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="78"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="78"/>
+      <c r="O11" s="63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30"/>
       <c r="B12" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E12" s="75"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78" t="s">
-        <v>227</v>
-      </c>
+      <c r="F12" s="97"/>
+      <c r="G12" s="97"/>
       <c r="H12" s="78"/>
       <c r="I12" s="78"/>
-      <c r="J12" s="63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="78"/>
+      <c r="K12" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L12" s="78"/>
+      <c r="M12" s="78"/>
+      <c r="N12" s="78"/>
+      <c r="O12" s="63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="59" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E13" s="75"/>
-      <c r="F13" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="G13" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="H13" s="78"/>
+      <c r="F13" s="97"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="78" t="s">
+        <v>226</v>
+      </c>
       <c r="I13" s="78"/>
-      <c r="J13" s="63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="78"/>
+      <c r="K13" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L13" s="78"/>
+      <c r="M13" s="78"/>
+      <c r="N13" s="78"/>
+      <c r="O13" s="63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="59" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E14" s="75"/>
-      <c r="F14" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="78" t="s">
+        <v>226</v>
+      </c>
       <c r="I14" s="78"/>
-      <c r="J14" s="63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78"/>
+      <c r="M14" s="78"/>
+      <c r="N14" s="78"/>
+      <c r="O14" s="63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
       <c r="B15" s="59" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E15" s="75"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78" t="s">
-        <v>227</v>
-      </c>
+      <c r="F15" s="97"/>
+      <c r="G15" s="97"/>
       <c r="H15" s="78"/>
       <c r="I15" s="78"/>
-      <c r="J15" s="63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="78"/>
+      <c r="K15" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L15" s="78"/>
+      <c r="M15" s="78"/>
+      <c r="N15" s="78"/>
+      <c r="O15" s="63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30"/>
       <c r="B16" s="32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C16" s="32"/>
       <c r="D16" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E16" s="75"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78" t="s">
-        <v>227</v>
-      </c>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
       <c r="H16" s="78"/>
       <c r="I16" s="78"/>
-      <c r="J16" s="63" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="78"/>
+      <c r="K16" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L16" s="78"/>
+      <c r="M16" s="78"/>
+      <c r="N16" s="78"/>
+      <c r="O16" s="63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
-      <c r="B17" s="32"/>
+      <c r="B17" s="32" t="s">
+        <v>257</v>
+      </c>
       <c r="C17" s="32"/>
-      <c r="D17" s="74"/>
+      <c r="D17" s="74" t="s">
+        <v>226</v>
+      </c>
       <c r="E17" s="75"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="63"/>
-    </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="74"/>
+      <c r="F17" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="G17" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="H17" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="I17" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J17" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="K17" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L17" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="M17" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="N17" s="78"/>
+      <c r="O17" s="63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="82"/>
+      <c r="B18" s="81" t="s">
+        <v>266</v>
+      </c>
+      <c r="C18" s="81"/>
+      <c r="D18" s="74" t="s">
+        <v>226</v>
+      </c>
       <c r="E18" s="75"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
-      <c r="J18" s="63"/>
-    </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="74"/>
+      <c r="F18" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="G18" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="H18" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="I18" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J18" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="K18" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L18" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="M18" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="N18" s="78"/>
+      <c r="O18" s="63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="82"/>
+      <c r="B19" s="81" t="s">
+        <v>267</v>
+      </c>
+      <c r="C19" s="81"/>
+      <c r="D19" s="74" t="s">
+        <v>226</v>
+      </c>
       <c r="E19" s="75"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="78"/>
-      <c r="J19" s="63"/>
-    </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="64"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="G19" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="H19" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="I19" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J19" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="K19" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L19" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="M19" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="N19" s="78"/>
+      <c r="O19" s="63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="82"/>
+      <c r="B20" s="81" t="s">
+        <v>268</v>
+      </c>
+      <c r="C20" s="81"/>
+      <c r="D20" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E20" s="75"/>
+      <c r="F20" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="G20" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="H20" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="I20" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J20" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="K20" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L20" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="M20" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="N20" s="78"/>
+      <c r="O20" s="63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
-      <c r="B21" s="32"/>
+      <c r="B21" s="32" t="s">
+        <v>269</v>
+      </c>
       <c r="C21" s="32"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="59"/>
-    </row>
-    <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="32"/>
+      <c r="D21" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E21" s="75"/>
+      <c r="F21" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="G21" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="H21" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="I21" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J21" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="K21" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L21" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="M21" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="N21" s="78"/>
+      <c r="O21" s="63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="30"/>
+      <c r="B22" s="32" t="s">
+        <v>270</v>
+      </c>
       <c r="C22" s="32"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="59"/>
-    </row>
-    <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="59"/>
-    </row>
-    <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="81"/>
-      <c r="B24" s="81"/>
+      <c r="D22" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E22" s="75"/>
+      <c r="F22" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="G22" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="H22" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="I22" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J22" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="K22" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L22" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="M22" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="N22" s="78"/>
+      <c r="O22" s="63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="82"/>
+      <c r="B23" s="81" t="s">
+        <v>271</v>
+      </c>
+      <c r="C23" s="81"/>
+      <c r="D23" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E23" s="75"/>
+      <c r="F23" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="G23" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="H23" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="I23" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J23" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="K23" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L23" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="M23" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="N23" s="78"/>
+      <c r="O23" s="63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="82"/>
+      <c r="B24" s="81" t="s">
+        <v>272</v>
+      </c>
       <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-    </row>
-    <row r="25" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="81"/>
-      <c r="B25" s="81"/>
+      <c r="D24" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E24" s="75"/>
+      <c r="F24" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="G24" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="H24" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="I24" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J24" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="K24" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L24" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="M24" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="N24" s="78"/>
+      <c r="O24" s="63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="82"/>
+      <c r="B25" s="81" t="s">
+        <v>273</v>
+      </c>
       <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="78"/>
-    </row>
-    <row r="26" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="81"/>
-      <c r="B26" s="81"/>
+      <c r="D25" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E25" s="75"/>
+      <c r="F25" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="G25" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="H25" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="I25" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J25" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="K25" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L25" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="M25" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="N25" s="78"/>
+      <c r="O25" s="63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="82"/>
+      <c r="B26" s="81" t="s">
+        <v>274</v>
+      </c>
       <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78"/>
-    </row>
-    <row r="27" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="81"/>
-      <c r="B27" s="81"/>
+      <c r="D26" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E26" s="75"/>
+      <c r="F26" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="G26" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="H26" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="I26" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J26" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="K26" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="L26" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="M26" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="N26" s="78"/>
+      <c r="O26" s="63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="82"/>
+      <c r="B27" s="81" t="s">
+        <v>275</v>
+      </c>
       <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="78"/>
+      <c r="D27" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E27" s="75"/>
+      <c r="F27" s="97"/>
+      <c r="G27" s="97"/>
       <c r="H27" s="78"/>
-      <c r="I27" s="78"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
+      <c r="I27" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J27" s="78"/>
+      <c r="K27" s="78"/>
+      <c r="L27" s="78"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="78"/>
+      <c r="O27" s="63" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="82"/>
+      <c r="B28" s="81" t="s">
+        <v>281</v>
+      </c>
+      <c r="C28" s="81"/>
+      <c r="D28" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E28" s="75"/>
+      <c r="F28" s="97"/>
+      <c r="G28" s="97"/>
       <c r="H28" s="78"/>
-      <c r="I28" s="78"/>
-      <c r="J28" s="59"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
+      <c r="I28" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J28" s="78"/>
+      <c r="K28" s="78"/>
+      <c r="L28" s="78"/>
+      <c r="M28" s="78"/>
+      <c r="N28" s="78"/>
+      <c r="O28" s="63" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="82"/>
+      <c r="B29" s="81" t="s">
+        <v>282</v>
+      </c>
+      <c r="C29" s="81"/>
+      <c r="D29" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E29" s="75"/>
+      <c r="F29" s="97"/>
+      <c r="G29" s="97"/>
       <c r="H29" s="78"/>
-      <c r="I29" s="78"/>
-      <c r="J29" s="59"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
+      <c r="I29" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J29" s="78"/>
+      <c r="K29" s="78"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="78"/>
+      <c r="O29" s="63" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="82"/>
+      <c r="B30" s="81" t="s">
+        <v>283</v>
+      </c>
+      <c r="C30" s="81"/>
+      <c r="D30" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E30" s="75"/>
+      <c r="F30" s="97"/>
+      <c r="G30" s="97"/>
       <c r="H30" s="78"/>
-      <c r="I30" s="78"/>
-      <c r="J30" s="59"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
+      <c r="I30" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J30" s="78"/>
+      <c r="K30" s="78"/>
+      <c r="L30" s="78"/>
+      <c r="M30" s="78"/>
+      <c r="N30" s="78"/>
+      <c r="O30" s="63" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="82"/>
+      <c r="B31" s="81" t="s">
+        <v>284</v>
+      </c>
+      <c r="C31" s="81"/>
+      <c r="D31" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E31" s="75"/>
+      <c r="F31" s="97"/>
+      <c r="G31" s="97"/>
       <c r="H31" s="78"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="59"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
+      <c r="I31" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J31" s="78"/>
+      <c r="K31" s="78"/>
+      <c r="L31" s="78"/>
+      <c r="M31" s="78"/>
+      <c r="N31" s="78"/>
+      <c r="O31" s="63" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="82"/>
+      <c r="B32" s="81" t="s">
+        <v>280</v>
+      </c>
+      <c r="C32" s="81"/>
+      <c r="D32" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E32" s="75"/>
+      <c r="F32" s="97"/>
+      <c r="G32" s="97"/>
       <c r="H32" s="78"/>
-      <c r="I32" s="78"/>
-      <c r="J32" s="59"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="78"/>
+      <c r="I32" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="J32" s="78"/>
+      <c r="K32" s="78"/>
+      <c r="L32" s="78"/>
+      <c r="M32" s="78"/>
+      <c r="N32" s="78"/>
+      <c r="O32" s="63" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="82"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="97"/>
+      <c r="G33" s="97"/>
       <c r="H33" s="78"/>
       <c r="I33" s="78"/>
-      <c r="J33" s="59"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
+      <c r="J33" s="78"/>
+      <c r="K33" s="78"/>
+      <c r="L33" s="78"/>
+      <c r="M33" s="78"/>
+      <c r="N33" s="78"/>
+      <c r="O33" s="63"/>
+    </row>
+    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="82"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="97"/>
       <c r="H34" s="78"/>
       <c r="I34" s="78"/>
-      <c r="J34" s="59"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
+      <c r="J34" s="78"/>
+      <c r="K34" s="78"/>
+      <c r="L34" s="78"/>
+      <c r="M34" s="78"/>
+      <c r="N34" s="78"/>
+      <c r="O34" s="63"/>
+    </row>
+    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="82"/>
+      <c r="B35" s="81"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="74"/>
+      <c r="E35" s="75"/>
+      <c r="F35" s="97"/>
+      <c r="G35" s="97"/>
       <c r="H35" s="78"/>
       <c r="I35" s="78"/>
-      <c r="J35" s="59"/>
+      <c r="J35" s="78"/>
+      <c r="K35" s="78"/>
+      <c r="L35" s="78"/>
+      <c r="M35" s="78"/>
+      <c r="N35" s="78"/>
+      <c r="O35" s="63"/>
+    </row>
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="35"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="80"/>
+      <c r="L36" s="80"/>
+      <c r="M36" s="80"/>
+      <c r="N36" s="80"/>
+      <c r="O36" s="64"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="30"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78"/>
+      <c r="G37" s="78"/>
+      <c r="H37" s="78"/>
+      <c r="I37" s="78"/>
+      <c r="J37" s="78"/>
+      <c r="K37" s="78"/>
+      <c r="L37" s="78"/>
+      <c r="M37" s="78"/>
+      <c r="N37" s="78"/>
+      <c r="O37" s="81"/>
+    </row>
+    <row r="38" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="78"/>
+      <c r="H38" s="78"/>
+      <c r="I38" s="78"/>
+      <c r="J38" s="78"/>
+      <c r="K38" s="78"/>
+      <c r="L38" s="78"/>
+      <c r="M38" s="78"/>
+      <c r="N38" s="78"/>
+      <c r="O38" s="81"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="30"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="78"/>
+      <c r="H39" s="78"/>
+      <c r="I39" s="78"/>
+      <c r="J39" s="78"/>
+      <c r="K39" s="78"/>
+      <c r="L39" s="78"/>
+      <c r="M39" s="78"/>
+      <c r="N39" s="78"/>
+      <c r="O39" s="81"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="30"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="78"/>
+      <c r="F40" s="78"/>
+      <c r="G40" s="78"/>
+      <c r="H40" s="78"/>
+      <c r="I40" s="78"/>
+      <c r="J40" s="78"/>
+      <c r="K40" s="78"/>
+      <c r="L40" s="78"/>
+      <c r="M40" s="78"/>
+      <c r="N40" s="78"/>
+      <c r="O40" s="81"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="30"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="78"/>
+      <c r="E41" s="78"/>
+      <c r="F41" s="78"/>
+      <c r="G41" s="78"/>
+      <c r="H41" s="78"/>
+      <c r="I41" s="78"/>
+      <c r="J41" s="78"/>
+      <c r="K41" s="78"/>
+      <c r="L41" s="78"/>
+      <c r="M41" s="78"/>
+      <c r="N41" s="78"/>
+      <c r="O41" s="81"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="30"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="78"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="78"/>
+      <c r="H42" s="78"/>
+      <c r="I42" s="78"/>
+      <c r="J42" s="78"/>
+      <c r="K42" s="78"/>
+      <c r="L42" s="78"/>
+      <c r="M42" s="78"/>
+      <c r="N42" s="78"/>
+      <c r="O42" s="81"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="30"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="78"/>
+      <c r="F43" s="78"/>
+      <c r="G43" s="78"/>
+      <c r="H43" s="78"/>
+      <c r="I43" s="78"/>
+      <c r="J43" s="78"/>
+      <c r="K43" s="78"/>
+      <c r="L43" s="78"/>
+      <c r="M43" s="78"/>
+      <c r="N43" s="78"/>
+      <c r="O43" s="81"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="30"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="78"/>
+      <c r="E44" s="78"/>
+      <c r="F44" s="78"/>
+      <c r="G44" s="78"/>
+      <c r="H44" s="78"/>
+      <c r="I44" s="78"/>
+      <c r="J44" s="78"/>
+      <c r="K44" s="78"/>
+      <c r="L44" s="78"/>
+      <c r="M44" s="78"/>
+      <c r="N44" s="78"/>
+      <c r="O44" s="81"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="30"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="78"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="78"/>
+      <c r="H45" s="78"/>
+      <c r="I45" s="78"/>
+      <c r="J45" s="78"/>
+      <c r="K45" s="78"/>
+      <c r="L45" s="78"/>
+      <c r="M45" s="78"/>
+      <c r="N45" s="78"/>
+      <c r="O45" s="81"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A27:F27"/>
+  <mergeCells count="1">
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="61" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8081,8 +8800,8 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8096,14 +8815,14 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
@@ -8112,16 +8831,16 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="91" t="s">
         <v>214</v>
       </c>
-      <c r="E3" s="84"/>
+      <c r="E3" s="92"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="68" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="65" t="s">
@@ -8137,174 +8856,198 @@
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60"/>
       <c r="B5" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60"/>
       <c r="B6" s="59" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E6" s="75"/>
       <c r="F6" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>
       <c r="B7" s="59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E7" s="75"/>
       <c r="F7" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
       <c r="B8" s="59" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E8" s="75"/>
       <c r="F8" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60"/>
       <c r="B9" s="59" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C9" s="59"/>
       <c r="D9" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E9" s="75"/>
       <c r="F9" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="60"/>
       <c r="B10" s="59" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E10" s="75"/>
       <c r="F10" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="60"/>
       <c r="B11" s="59" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E11" s="75"/>
       <c r="F11" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60"/>
       <c r="B12" s="59" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E12" s="75"/>
       <c r="F12" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E13" s="75"/>
       <c r="F13" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E14" s="75"/>
       <c r="F14" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
-      <c r="B15" s="59"/>
+      <c r="B15" s="81" t="s">
+        <v>276</v>
+      </c>
       <c r="C15" s="59"/>
-      <c r="D15" s="74"/>
+      <c r="D15" s="74" t="s">
+        <v>226</v>
+      </c>
       <c r="E15" s="75"/>
-      <c r="F15" s="63"/>
+      <c r="F15" s="63" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
-      <c r="B16" s="59"/>
+      <c r="B16" s="81" t="s">
+        <v>277</v>
+      </c>
       <c r="C16" s="59"/>
-      <c r="D16" s="74"/>
+      <c r="D16" s="74" t="s">
+        <v>226</v>
+      </c>
       <c r="E16" s="75"/>
-      <c r="F16" s="63"/>
+      <c r="F16" s="63" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="60"/>
-      <c r="B17" s="59"/>
+      <c r="B17" s="59" t="s">
+        <v>279</v>
+      </c>
       <c r="C17" s="59"/>
-      <c r="D17" s="74"/>
+      <c r="D17" s="74" t="s">
+        <v>226</v>
+      </c>
       <c r="E17" s="75"/>
-      <c r="F17" s="63"/>
+      <c r="F17" s="63" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="60"/>
-      <c r="B18" s="59"/>
+      <c r="B18" s="59" t="s">
+        <v>285</v>
+      </c>
       <c r="C18" s="59"/>
-      <c r="D18" s="74"/>
+      <c r="D18" s="74" t="s">
+        <v>226</v>
+      </c>
       <c r="E18" s="75"/>
-      <c r="F18" s="63"/>
+      <c r="F18" s="63" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="60"/>
@@ -8351,32 +9094,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="81"/>
-      <c r="B24" s="81"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
+      <c r="A24" s="89"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="81"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
+      <c r="A25" s="89"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="81"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
+      <c r="A26" s="89"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="81"/>
-      <c r="B27" s="81"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
+      <c r="A27" s="89"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -8462,7 +9205,7 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -8488,17 +9231,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="86" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="87" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
+      <c r="A3" s="88"/>
       <c r="B3" s="39" t="s">
         <v>183</v>
       </c>
@@ -8524,7 +9267,7 @@
       </c>
       <c r="M3" s="39"/>
       <c r="N3" s="39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8558,92 +9301,92 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="90"/>
-      <c r="B5" s="91" t="s">
+      <c r="A5" s="84"/>
+      <c r="B5" s="85" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91" t="s">
+      <c r="C5" s="85"/>
+      <c r="D5" s="85" t="s">
         <v>202</v>
       </c>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91" t="s">
+      <c r="E5" s="85"/>
+      <c r="F5" s="85" t="s">
         <v>205</v>
       </c>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91" t="s">
+      <c r="G5" s="85"/>
+      <c r="H5" s="85" t="s">
         <v>209</v>
       </c>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91" t="s">
+      <c r="I5" s="85"/>
+      <c r="J5" s="85" t="s">
         <v>190</v>
       </c>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91" t="s">
+      <c r="K5" s="85"/>
+      <c r="L5" s="85" t="s">
         <v>193</v>
       </c>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91" t="s">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="90"/>
-      <c r="B6" s="91" t="s">
+      <c r="A6" s="84"/>
+      <c r="B6" s="85" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91" t="s">
+      <c r="C6" s="85"/>
+      <c r="D6" s="85" t="s">
         <v>203</v>
       </c>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91" t="s">
+      <c r="E6" s="85"/>
+      <c r="F6" s="85" t="s">
         <v>199</v>
       </c>
-      <c r="G6" s="91"/>
-      <c r="H6" s="91" t="s">
-        <v>255</v>
-      </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91" t="s">
+      <c r="G6" s="85"/>
+      <c r="H6" s="85" t="s">
+        <v>254</v>
+      </c>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85" t="s">
         <v>191</v>
       </c>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91" t="s">
+      <c r="K6" s="85"/>
+      <c r="L6" s="85" t="s">
         <v>194</v>
       </c>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91" t="s">
-        <v>257</v>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="90"/>
-      <c r="B7" s="91" t="s">
+      <c r="A7" s="84"/>
+      <c r="B7" s="85" t="s">
         <v>188</v>
       </c>
-      <c r="C7" s="91"/>
-      <c r="D7" s="91" t="s">
+      <c r="C7" s="85"/>
+      <c r="D7" s="85" t="s">
         <v>204</v>
       </c>
-      <c r="E7" s="91"/>
-      <c r="F7" s="91" t="s">
+      <c r="E7" s="85"/>
+      <c r="F7" s="85" t="s">
         <v>208</v>
       </c>
-      <c r="G7" s="91"/>
-      <c r="H7" s="91" t="s">
+      <c r="G7" s="85"/>
+      <c r="H7" s="85" t="s">
         <v>211</v>
       </c>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91" t="s">
+      <c r="I7" s="85"/>
+      <c r="J7" s="85" t="s">
         <v>198</v>
       </c>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91" t="s">
+      <c r="K7" s="85"/>
+      <c r="L7" s="85" t="s">
         <v>195</v>
       </c>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91" t="s">
+      <c r="M7" s="85"/>
+      <c r="N7" s="85" t="s">
         <v>219</v>
       </c>
     </row>
@@ -9168,27 +9911,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="81"/>
-      <c r="B17" s="81"/>
-      <c r="C17" s="81"/>
+      <c r="A17" s="89"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="81"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="81"/>
+      <c r="A18" s="89"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="81"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
+      <c r="A19" s="89"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="89"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -9627,30 +10370,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="88" t="s">
+      <c r="A42" s="93" t="s">
         <v>176</v>
       </c>
-      <c r="B42" s="88"/>
-      <c r="C42" s="88"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="93"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="89" t="s">
+      <c r="A43" s="94" t="s">
         <v>177</v>
       </c>
-      <c r="B43" s="89"/>
-      <c r="C43" s="89"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="94"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="88" t="s">
+      <c r="A44" s="93" t="s">
         <v>178</v>
       </c>
-      <c r="B44" s="88"/>
-      <c r="C44" s="88"/>
+      <c r="B44" s="93"/>
+      <c r="C44" s="93"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="81"/>
-      <c r="B45" s="81"/>
-      <c r="C45" s="81"/>
+      <c r="A45" s="89"/>
+      <c r="B45" s="89"/>
+      <c r="C45" s="89"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>

</xml_diff>

<commit_message>
Added studies to table on determinants
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="308">
   <si>
     <t>Total</t>
   </si>
@@ -842,9 +842,6 @@
     <t>Studies</t>
   </si>
   <si>
-    <t>Variable</t>
-  </si>
-  <si>
     <t>Bureacracy theory
 Administrative theory
 Scientific management</t>
@@ -941,12 +938,6 @@
     <t>Presence of university-affiliated incubator</t>
   </si>
   <si>
-    <t>High-autonomy of technology transfer operation</t>
-  </si>
-  <si>
-    <t>Low-autonomy of technology transfer operation</t>
-  </si>
-  <si>
     <t>Age of technology transfer operation</t>
   </si>
   <si>
@@ -1106,6 +1097,78 @@
   </si>
   <si>
     <t>Operationalizations of Technology Transfer</t>
+  </si>
+  <si>
+    <t>Process Perspective</t>
+  </si>
+  <si>
+    <t>Indogeneous</t>
+  </si>
+  <si>
+    <t>Exogenous</t>
+  </si>
+  <si>
+    <t>Development stage of technology</t>
+  </si>
+  <si>
+    <t>Munteanu (2012)</t>
+  </si>
+  <si>
+    <t>Age of technology</t>
+  </si>
+  <si>
+    <t>Analysis Level</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Society's perception of technology</t>
+  </si>
+  <si>
+    <t>Undefined</t>
+  </si>
+  <si>
+    <t>Society's perception of the technology transfer process</t>
+  </si>
+  <si>
+    <t>Perceived compatibility of goals between provider and acquirer</t>
+  </si>
+  <si>
+    <t>Society's attitude toward organizational learning</t>
+  </si>
+  <si>
+    <t>Compatibility between the cultures of the acquirer and the provider</t>
+  </si>
+  <si>
+    <t>Similarity of the development environment of acquirer to provider</t>
+  </si>
+  <si>
+    <t>Change management capabilities of acquirer</t>
+  </si>
+  <si>
+    <t>Level of preparation activity</t>
+  </si>
+  <si>
+    <t>Quality of technology transfer agreement</t>
+  </si>
+  <si>
+    <t>Use of alliances and collaborations</t>
+  </si>
+  <si>
+    <t>Degree of autonomy of technology transfer operation</t>
+  </si>
+  <si>
+    <t>Kundu, Bhar, &amp; Pandurangan (2015)</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1279,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1386,13 +1449,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1654,18 +1756,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1683,6 +1773,60 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7189,7 +7333,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7466,54 +7610,54 @@
       <c r="F20" s="29"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="89" t="s">
+      <c r="A21" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="89"/>
-      <c r="C21" s="89"/>
-      <c r="D21" s="89"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="89"/>
+      <c r="B21" s="97"/>
+      <c r="C21" s="97"/>
+      <c r="D21" s="97"/>
+      <c r="E21" s="97"/>
+      <c r="F21" s="97"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="90" t="s">
+      <c r="A22" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="B22" s="90"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="98"/>
+      <c r="D22" s="98"/>
+      <c r="E22" s="98"/>
+      <c r="F22" s="98"/>
     </row>
     <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="89" t="s">
+      <c r="A23" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="89"/>
-      <c r="C23" s="89"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="89"/>
+      <c r="B23" s="97"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
     </row>
     <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="89" t="s">
+      <c r="A24" s="97" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="89"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="89"/>
-      <c r="E24" s="89"/>
-      <c r="F24" s="89"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="97"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="89" t="s">
+      <c r="A25" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="89"/>
-      <c r="C25" s="89"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="89"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="97"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="97"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -7600,11 +7744,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7612,12 +7758,12 @@
     <col min="1" max="1" width="2.7109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="75.7109375" customWidth="1"/>
     <col min="3" max="3" width="2.7109375" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" style="79" customWidth="1"/>
-    <col min="6" max="14" width="5.7109375" style="79" customWidth="1"/>
-    <col min="15" max="15" width="40.7109375" style="96" customWidth="1"/>
+    <col min="4" max="11" width="12.7109375" style="79" customWidth="1"/>
+    <col min="12" max="20" width="5.7109375" style="79" customWidth="1"/>
+    <col min="21" max="21" width="40.7109375" style="92" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>184</v>
       </c>
@@ -7632,9 +7778,15 @@
       <c r="L1" s="61"/>
       <c r="M1" s="61"/>
       <c r="N1" s="61"/>
-      <c r="O1" s="81"/>
-    </row>
-    <row r="2" spans="1:15" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="81"/>
+    </row>
+    <row r="2" spans="1:21" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>65</v>
       </c>
@@ -7649,1149 +7801,1928 @@
       <c r="L2" s="61"/>
       <c r="M2" s="61"/>
       <c r="N2" s="61"/>
-      <c r="O2" s="81"/>
-    </row>
-    <row r="3" spans="1:15" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="81"/>
+    </row>
+    <row r="3" spans="1:21" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="99" t="s">
+        <v>290</v>
+      </c>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="99" t="s">
         <v>214</v>
       </c>
-      <c r="E3" s="92"/>
-      <c r="F3" s="100" t="s">
-        <v>286</v>
-      </c>
-      <c r="G3" s="83"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="95"/>
-    </row>
-    <row r="4" spans="1:15" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="100"/>
+      <c r="J3" s="99" t="s">
+        <v>284</v>
+      </c>
+      <c r="K3" s="100"/>
+      <c r="L3" s="96" t="s">
+        <v>283</v>
+      </c>
+      <c r="M3" s="83"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="94"/>
+      <c r="R3" s="94"/>
+      <c r="S3" s="94"/>
+      <c r="T3" s="95"/>
+      <c r="U3" s="91"/>
+    </row>
+    <row r="4" spans="1:21" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="68" t="s">
         <v>66</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="E4" s="111" t="s">
+        <v>291</v>
+      </c>
+      <c r="F4" s="104" t="s">
+        <v>292</v>
+      </c>
+      <c r="G4" s="66" t="s">
+        <v>293</v>
+      </c>
+      <c r="H4" s="65" t="s">
         <v>212</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="I4" s="66" t="s">
         <v>213</v>
       </c>
-      <c r="F4" s="62" t="s">
-        <v>263</v>
-      </c>
-      <c r="G4" s="62" t="s">
-        <v>264</v>
-      </c>
-      <c r="H4" s="62" t="s">
+      <c r="J4" s="65" t="s">
+        <v>285</v>
+      </c>
+      <c r="K4" s="66" t="s">
+        <v>286</v>
+      </c>
+      <c r="L4" s="62" t="s">
+        <v>260</v>
+      </c>
+      <c r="M4" s="62" t="s">
+        <v>261</v>
+      </c>
+      <c r="N4" s="62" t="s">
+        <v>226</v>
+      </c>
+      <c r="O4" s="62" t="s">
+        <v>255</v>
+      </c>
+      <c r="P4" s="62" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q4" s="62" t="s">
         <v>227</v>
       </c>
-      <c r="I4" s="62" t="s">
+      <c r="R4" s="62" t="s">
         <v>258</v>
       </c>
-      <c r="J4" s="62" t="s">
-        <v>265</v>
-      </c>
-      <c r="K4" s="62" t="s">
-        <v>228</v>
-      </c>
-      <c r="L4" s="62" t="s">
-        <v>261</v>
-      </c>
-      <c r="M4" s="62" t="s">
-        <v>262</v>
-      </c>
-      <c r="N4" s="62" t="s">
-        <v>216</v>
-      </c>
-      <c r="O4" s="72" t="s">
+      <c r="S4" s="62" t="s">
+        <v>259</v>
+      </c>
+      <c r="T4" s="62" t="s">
+        <v>296</v>
+      </c>
+      <c r="U4" s="72" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="30"/>
       <c r="B5" s="32" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C5" s="32"/>
-      <c r="D5" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E5" s="75"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" s="93"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I5" s="75"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L5" s="93"/>
+      <c r="M5" s="93"/>
       <c r="N5" s="78"/>
-      <c r="O5" s="63" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="O5" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R5" s="78"/>
+      <c r="S5" s="78"/>
+      <c r="T5" s="78"/>
+      <c r="U5" s="63" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
       <c r="B6" s="32" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C6" s="32"/>
-      <c r="D6" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E6" s="75"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97"/>
-      <c r="H6" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="63" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="74"/>
+      <c r="E6" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F6" s="93"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I6" s="75"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L6" s="93"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R6" s="78"/>
+      <c r="S6" s="78"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="63" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
       <c r="B7" s="32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C7" s="32"/>
-      <c r="D7" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E7" s="75"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="97"/>
-      <c r="H7" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="78"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="63" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="74"/>
+      <c r="E7" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F7" s="93"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I7" s="75"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L7" s="93"/>
+      <c r="M7" s="93"/>
+      <c r="N7" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O7" s="78"/>
+      <c r="P7" s="78"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="78"/>
+      <c r="S7" s="78"/>
+      <c r="T7" s="78"/>
+      <c r="U7" s="63" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
       <c r="B8" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C8" s="32"/>
-      <c r="D8" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E8" s="75"/>
-      <c r="F8" s="97"/>
-      <c r="G8" s="97"/>
-      <c r="H8" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="63" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="74"/>
+      <c r="E8" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F8" s="93"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I8" s="75"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L8" s="93"/>
+      <c r="M8" s="93"/>
+      <c r="N8" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O8" s="78"/>
+      <c r="P8" s="78"/>
+      <c r="Q8" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R8" s="78"/>
+      <c r="S8" s="78"/>
+      <c r="T8" s="78"/>
+      <c r="U8" s="63" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
       <c r="B9" s="32" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C9" s="32"/>
-      <c r="D9" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E9" s="75"/>
-      <c r="F9" s="97"/>
-      <c r="G9" s="97"/>
-      <c r="H9" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="63" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="74"/>
+      <c r="E9" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F9" s="93"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I9" s="75"/>
+      <c r="J9" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K9" s="75"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O9" s="78"/>
+      <c r="P9" s="78"/>
+      <c r="Q9" s="78"/>
+      <c r="R9" s="78"/>
+      <c r="S9" s="78"/>
+      <c r="T9" s="78"/>
+      <c r="U9" s="63" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
       <c r="B10" s="32" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C10" s="32"/>
-      <c r="D10" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E10" s="75"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="97"/>
-      <c r="H10" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I10" s="78"/>
-      <c r="J10" s="78"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="78"/>
-      <c r="M10" s="78"/>
-      <c r="N10" s="78"/>
-      <c r="O10" s="63" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="74"/>
+      <c r="E10" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F10" s="93"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I10" s="75"/>
+      <c r="J10" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K10" s="75"/>
+      <c r="L10" s="93"/>
+      <c r="M10" s="93"/>
+      <c r="N10" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O10" s="78"/>
+      <c r="P10" s="78"/>
+      <c r="Q10" s="78"/>
+      <c r="R10" s="78"/>
+      <c r="S10" s="78"/>
+      <c r="T10" s="78"/>
+      <c r="U10" s="63" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
       <c r="B11" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F11" s="93"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I11" s="75"/>
+      <c r="J11" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K11" s="75"/>
+      <c r="L11" s="93"/>
+      <c r="M11" s="93"/>
+      <c r="N11" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O11" s="78"/>
+      <c r="P11" s="78"/>
+      <c r="Q11" s="78"/>
+      <c r="R11" s="78"/>
+      <c r="S11" s="78"/>
+      <c r="T11" s="78"/>
+      <c r="U11" s="63" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="60"/>
+      <c r="B12" s="59" t="s">
         <v>233</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E11" s="75"/>
-      <c r="F11" s="97"/>
-      <c r="G11" s="97"/>
-      <c r="H11" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="78"/>
-      <c r="N11" s="78"/>
-      <c r="O11" s="63" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="32" t="s">
-        <v>232</v>
-      </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E12" s="75"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="97"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L12" s="78"/>
-      <c r="M12" s="78"/>
-      <c r="N12" s="78"/>
-      <c r="O12" s="63" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="59"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F12" s="93"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I12" s="75"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L12" s="93"/>
+      <c r="M12" s="93"/>
+      <c r="N12" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O12" s="78"/>
+      <c r="P12" s="78"/>
+      <c r="Q12" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R12" s="78"/>
+      <c r="S12" s="78"/>
+      <c r="T12" s="78"/>
+      <c r="U12" s="63" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="59" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C13" s="59"/>
-      <c r="D13" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E13" s="75"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L13" s="78"/>
-      <c r="M13" s="78"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="63" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="74"/>
+      <c r="E13" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F13" s="93"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I13" s="75"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L13" s="93"/>
+      <c r="M13" s="93"/>
+      <c r="N13" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O13" s="78"/>
+      <c r="P13" s="78"/>
+      <c r="Q13" s="78"/>
+      <c r="R13" s="78"/>
+      <c r="S13" s="78"/>
+      <c r="T13" s="78"/>
+      <c r="U13" s="63" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="59" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C14" s="59"/>
-      <c r="D14" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E14" s="75"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="97"/>
-      <c r="H14" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="78"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F14" s="93"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I14" s="75"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L14" s="93"/>
+      <c r="M14" s="93"/>
       <c r="N14" s="78"/>
-      <c r="O14" s="63" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="60"/>
-      <c r="B15" s="59" t="s">
-        <v>238</v>
-      </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E15" s="75"/>
-      <c r="F15" s="97"/>
-      <c r="G15" s="97"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L15" s="78"/>
-      <c r="M15" s="78"/>
+      <c r="O14" s="78"/>
+      <c r="P14" s="78"/>
+      <c r="Q14" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R14" s="78"/>
+      <c r="S14" s="78"/>
+      <c r="T14" s="78"/>
+      <c r="U14" s="63" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F15" s="93"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I15" s="75"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L15" s="93"/>
+      <c r="M15" s="93"/>
       <c r="N15" s="78"/>
-      <c r="O15" s="63" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O15" s="78"/>
+      <c r="P15" s="78"/>
+      <c r="Q15" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R15" s="78"/>
+      <c r="S15" s="78"/>
+      <c r="T15" s="78"/>
+      <c r="U15" s="63" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30"/>
       <c r="B16" s="32" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="C16" s="32"/>
-      <c r="D16" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E16" s="75"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L16" s="78"/>
-      <c r="M16" s="78"/>
-      <c r="N16" s="78"/>
-      <c r="O16" s="63" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="32" t="s">
-        <v>257</v>
-      </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E17" s="75"/>
-      <c r="F17" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="G17" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="H17" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I17" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J17" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="K17" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L17" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="M17" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="N17" s="78"/>
-      <c r="O17" s="63" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="74"/>
+      <c r="E16" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F16" s="93"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I16" s="75"/>
+      <c r="J16" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K16" s="75"/>
+      <c r="L16" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="M16" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="N16" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O16" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P16" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q16" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R16" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="S16" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="T16" s="78"/>
+      <c r="U16" s="63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="82"/>
+      <c r="B17" s="81" t="s">
+        <v>263</v>
+      </c>
+      <c r="C17" s="81"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F17" s="93"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I17" s="75"/>
+      <c r="J17" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K17" s="75"/>
+      <c r="L17" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="M17" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="N17" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O17" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P17" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q17" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R17" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="S17" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="T17" s="78"/>
+      <c r="U17" s="63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="82"/>
       <c r="B18" s="81" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C18" s="81"/>
-      <c r="D18" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E18" s="75"/>
-      <c r="F18" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="G18" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="H18" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I18" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J18" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="K18" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L18" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="M18" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="N18" s="78"/>
-      <c r="O18" s="63" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="74"/>
+      <c r="E18" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F18" s="93"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I18" s="75"/>
+      <c r="J18" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K18" s="75"/>
+      <c r="L18" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="M18" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="N18" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O18" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P18" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q18" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R18" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="S18" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="T18" s="78"/>
+      <c r="U18" s="63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="82"/>
       <c r="B19" s="81" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C19" s="81"/>
-      <c r="D19" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E19" s="75"/>
-      <c r="F19" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="G19" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="H19" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I19" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J19" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="K19" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L19" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="M19" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="N19" s="78"/>
-      <c r="O19" s="63" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="82"/>
-      <c r="B20" s="81" t="s">
-        <v>268</v>
-      </c>
-      <c r="C20" s="81"/>
-      <c r="D20" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E20" s="75"/>
-      <c r="F20" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="G20" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="H20" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I20" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J20" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="K20" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L20" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="M20" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="N20" s="78"/>
-      <c r="O20" s="63" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="74"/>
+      <c r="E19" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F19" s="93"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I19" s="75"/>
+      <c r="J19" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K19" s="75"/>
+      <c r="L19" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="M19" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="N19" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O19" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P19" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q19" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R19" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="S19" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="T19" s="78"/>
+      <c r="U19" s="63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
+      <c r="B20" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F20" s="93"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I20" s="75"/>
+      <c r="J20" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K20" s="75"/>
+      <c r="L20" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="M20" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="N20" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O20" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P20" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q20" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R20" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="S20" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="T20" s="78"/>
+      <c r="U20" s="63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
       <c r="B21" s="32" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C21" s="32"/>
-      <c r="D21" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E21" s="75"/>
-      <c r="F21" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="G21" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="H21" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I21" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J21" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="K21" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L21" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="M21" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="N21" s="78"/>
-      <c r="O21" s="63" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="32" t="s">
-        <v>270</v>
-      </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E22" s="75"/>
-      <c r="F22" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="G22" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="H22" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I22" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J22" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="K22" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L22" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="M22" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="N22" s="78"/>
-      <c r="O22" s="63" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="74"/>
+      <c r="E21" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F21" s="93"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I21" s="75"/>
+      <c r="J21" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K21" s="75"/>
+      <c r="L21" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="M21" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="N21" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O21" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P21" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q21" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R21" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="S21" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="T21" s="78"/>
+      <c r="U21" s="63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="82"/>
+      <c r="B22" s="81" t="s">
+        <v>268</v>
+      </c>
+      <c r="C22" s="81"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F22" s="93"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I22" s="75"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L22" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="M22" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="N22" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O22" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P22" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q22" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R22" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="S22" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="T22" s="78"/>
+      <c r="U22" s="63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="82"/>
       <c r="B23" s="81" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C23" s="81"/>
-      <c r="D23" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E23" s="75"/>
-      <c r="F23" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="G23" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="H23" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I23" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J23" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="K23" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L23" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="M23" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="N23" s="78"/>
-      <c r="O23" s="63" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="74"/>
+      <c r="E23" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F23" s="93"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I23" s="75"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L23" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="M23" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="N23" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O23" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P23" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q23" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R23" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="S23" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="T23" s="78"/>
+      <c r="U23" s="63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="82"/>
       <c r="B24" s="81" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C24" s="81"/>
-      <c r="D24" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E24" s="75"/>
-      <c r="F24" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="G24" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="H24" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I24" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J24" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="K24" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L24" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="M24" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="N24" s="78"/>
-      <c r="O24" s="63" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="74"/>
+      <c r="E24" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F24" s="93"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I24" s="75"/>
+      <c r="J24" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K24" s="75"/>
+      <c r="L24" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="M24" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="N24" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O24" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P24" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q24" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R24" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="S24" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="T24" s="78"/>
+      <c r="U24" s="63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="82"/>
       <c r="B25" s="81" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C25" s="81"/>
-      <c r="D25" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E25" s="75"/>
-      <c r="F25" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="G25" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="H25" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I25" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J25" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="K25" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L25" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="M25" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="N25" s="78"/>
-      <c r="O25" s="63" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="74"/>
+      <c r="E25" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F25" s="93"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I25" s="75"/>
+      <c r="J25" s="74"/>
+      <c r="K25" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L25" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="M25" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="N25" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O25" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P25" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q25" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="R25" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="S25" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="T25" s="78"/>
+      <c r="U25" s="63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="82"/>
       <c r="B26" s="81" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C26" s="81"/>
-      <c r="D26" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E26" s="75"/>
-      <c r="F26" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="G26" s="97" t="s">
-        <v>226</v>
-      </c>
-      <c r="H26" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="I26" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J26" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="K26" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="L26" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="M26" s="78" t="s">
-        <v>226</v>
-      </c>
+      <c r="D26" s="74"/>
+      <c r="E26" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F26" s="93"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I26" s="75"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L26" s="93"/>
+      <c r="M26" s="93"/>
       <c r="N26" s="78"/>
-      <c r="O26" s="63" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O26" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P26" s="78"/>
+      <c r="Q26" s="78"/>
+      <c r="R26" s="78"/>
+      <c r="S26" s="78"/>
+      <c r="T26" s="78"/>
+      <c r="U26" s="63" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="82"/>
       <c r="B27" s="81" t="s">
+        <v>278</v>
+      </c>
+      <c r="C27" s="81"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F27" s="93"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I27" s="75"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L27" s="93"/>
+      <c r="M27" s="93"/>
+      <c r="N27" s="78"/>
+      <c r="O27" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P27" s="78"/>
+      <c r="Q27" s="78"/>
+      <c r="R27" s="78"/>
+      <c r="S27" s="78"/>
+      <c r="T27" s="78"/>
+      <c r="U27" s="63" t="s">
         <v>275</v>
       </c>
-      <c r="C27" s="81"/>
-      <c r="D27" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E27" s="75"/>
-      <c r="F27" s="97"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J27" s="78"/>
-      <c r="K27" s="78"/>
-      <c r="L27" s="78"/>
-      <c r="M27" s="78"/>
-      <c r="N27" s="78"/>
-      <c r="O27" s="63" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="82"/>
       <c r="B28" s="81" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C28" s="81"/>
-      <c r="D28" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E28" s="75"/>
-      <c r="F28" s="97"/>
-      <c r="G28" s="97"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J28" s="78"/>
-      <c r="K28" s="78"/>
-      <c r="L28" s="78"/>
-      <c r="M28" s="78"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F28" s="93"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I28" s="75"/>
+      <c r="J28" s="74"/>
+      <c r="K28" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L28" s="93"/>
+      <c r="M28" s="93"/>
       <c r="N28" s="78"/>
-      <c r="O28" s="63" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O28" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P28" s="78"/>
+      <c r="Q28" s="78"/>
+      <c r="R28" s="78"/>
+      <c r="S28" s="78"/>
+      <c r="T28" s="78"/>
+      <c r="U28" s="63" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="82"/>
       <c r="B29" s="81" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C29" s="81"/>
-      <c r="D29" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E29" s="75"/>
-      <c r="F29" s="97"/>
-      <c r="G29" s="97"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="78"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F29" s="93"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I29" s="75"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L29" s="93"/>
+      <c r="M29" s="93"/>
       <c r="N29" s="78"/>
-      <c r="O29" s="63" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O29" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P29" s="78"/>
+      <c r="Q29" s="78"/>
+      <c r="R29" s="78"/>
+      <c r="S29" s="78"/>
+      <c r="T29" s="78"/>
+      <c r="U29" s="63" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="82"/>
       <c r="B30" s="81" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C30" s="81"/>
-      <c r="D30" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E30" s="75"/>
-      <c r="F30" s="97"/>
-      <c r="G30" s="97"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J30" s="78"/>
-      <c r="K30" s="78"/>
-      <c r="L30" s="78"/>
-      <c r="M30" s="78"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F30" s="93"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I30" s="75"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L30" s="93"/>
+      <c r="M30" s="93"/>
       <c r="N30" s="78"/>
-      <c r="O30" s="63" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O30" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P30" s="78"/>
+      <c r="Q30" s="78"/>
+      <c r="R30" s="78"/>
+      <c r="S30" s="78"/>
+      <c r="T30" s="78"/>
+      <c r="U30" s="63" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="82"/>
       <c r="B31" s="81" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="C31" s="81"/>
-      <c r="D31" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E31" s="75"/>
-      <c r="F31" s="97"/>
-      <c r="G31" s="97"/>
-      <c r="H31" s="78"/>
-      <c r="I31" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J31" s="78"/>
-      <c r="K31" s="78"/>
-      <c r="L31" s="78"/>
-      <c r="M31" s="78"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F31" s="93"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I31" s="75"/>
+      <c r="J31" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K31" s="75"/>
+      <c r="L31" s="93"/>
+      <c r="M31" s="93"/>
       <c r="N31" s="78"/>
-      <c r="O31" s="63" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O31" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P31" s="78"/>
+      <c r="Q31" s="78"/>
+      <c r="R31" s="78"/>
+      <c r="S31" s="78"/>
+      <c r="T31" s="78"/>
+      <c r="U31" s="63" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="82"/>
-      <c r="B32" s="81" t="s">
-        <v>280</v>
+      <c r="B32" s="103" t="s">
+        <v>287</v>
       </c>
       <c r="C32" s="81"/>
-      <c r="D32" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="E32" s="75"/>
-      <c r="F32" s="97"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="78"/>
-      <c r="I32" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="J32" s="78"/>
-      <c r="K32" s="78"/>
-      <c r="L32" s="78"/>
-      <c r="M32" s="78"/>
-      <c r="N32" s="78"/>
-      <c r="O32" s="63" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="105"/>
+      <c r="E32" s="113" t="s">
+        <v>225</v>
+      </c>
+      <c r="F32" s="107"/>
+      <c r="G32" s="106"/>
+      <c r="H32" s="105" t="s">
+        <v>225</v>
+      </c>
+      <c r="I32" s="106"/>
+      <c r="J32" s="105" t="s">
+        <v>225</v>
+      </c>
+      <c r="K32" s="106"/>
+      <c r="L32" s="107" t="s">
+        <v>225</v>
+      </c>
+      <c r="M32" s="107" t="s">
+        <v>225</v>
+      </c>
+      <c r="N32" s="108" t="s">
+        <v>225</v>
+      </c>
+      <c r="O32" s="108" t="s">
+        <v>225</v>
+      </c>
+      <c r="P32" s="108"/>
+      <c r="Q32" s="108"/>
+      <c r="R32" s="108"/>
+      <c r="S32" s="108"/>
+      <c r="T32" s="108"/>
+      <c r="U32" s="109" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="82"/>
-      <c r="B33" s="81"/>
+      <c r="B33" s="81" t="s">
+        <v>282</v>
+      </c>
       <c r="C33" s="81"/>
       <c r="D33" s="74"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="97"/>
-      <c r="G33" s="97"/>
-      <c r="H33" s="78"/>
-      <c r="I33" s="78"/>
-      <c r="J33" s="78"/>
-      <c r="K33" s="78"/>
-      <c r="L33" s="78"/>
-      <c r="M33" s="78"/>
-      <c r="N33" s="78"/>
-      <c r="O33" s="63"/>
-    </row>
-    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F33" s="93"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I33" s="75"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L33" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="M33" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="N33" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O33" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P33" s="78"/>
+      <c r="Q33" s="78"/>
+      <c r="R33" s="78"/>
+      <c r="S33" s="78"/>
+      <c r="T33" s="78"/>
+      <c r="U33" s="63" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="82"/>
-      <c r="B34" s="81"/>
+      <c r="B34" s="81" t="s">
+        <v>289</v>
+      </c>
       <c r="C34" s="81"/>
       <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="97"/>
-      <c r="G34" s="97"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="78"/>
-      <c r="K34" s="78"/>
-      <c r="L34" s="78"/>
-      <c r="M34" s="78"/>
-      <c r="N34" s="78"/>
-      <c r="O34" s="63"/>
-    </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="82"/>
-      <c r="B35" s="81"/>
-      <c r="C35" s="81"/>
+      <c r="E34" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="F34" s="93"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I34" s="75"/>
+      <c r="J34" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K34" s="75"/>
+      <c r="L34" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="M34" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="N34" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="O34" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="P34" s="78"/>
+      <c r="Q34" s="78"/>
+      <c r="R34" s="78"/>
+      <c r="S34" s="78"/>
+      <c r="T34" s="78"/>
+      <c r="U34" s="63" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="90"/>
+      <c r="B35" s="89" t="s">
+        <v>295</v>
+      </c>
+      <c r="C35" s="89"/>
       <c r="D35" s="74"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="97"/>
-      <c r="G35" s="97"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="78"/>
-      <c r="J35" s="78"/>
-      <c r="K35" s="78"/>
-      <c r="L35" s="78"/>
-      <c r="M35" s="78"/>
+      <c r="E35" s="112"/>
+      <c r="F35" s="93"/>
+      <c r="G35" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="H35" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I35" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="J35" s="74"/>
+      <c r="K35" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L35" s="93"/>
+      <c r="M35" s="93"/>
       <c r="N35" s="78"/>
-      <c r="O35" s="63"/>
-    </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="80"/>
-      <c r="G36" s="80"/>
-      <c r="H36" s="80"/>
-      <c r="I36" s="80"/>
-      <c r="J36" s="80"/>
-      <c r="K36" s="80"/>
-      <c r="L36" s="80"/>
-      <c r="M36" s="80"/>
-      <c r="N36" s="80"/>
-      <c r="O36" s="64"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="78"/>
-      <c r="J37" s="78"/>
-      <c r="K37" s="78"/>
-      <c r="L37" s="78"/>
-      <c r="M37" s="78"/>
+      <c r="O35" s="78"/>
+      <c r="P35" s="78"/>
+      <c r="Q35" s="78"/>
+      <c r="R35" s="78"/>
+      <c r="S35" s="78"/>
+      <c r="T35" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="U35" s="63" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="90"/>
+      <c r="B36" s="89" t="s">
+        <v>297</v>
+      </c>
+      <c r="C36" s="89"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="112"/>
+      <c r="F36" s="93"/>
+      <c r="G36" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="H36" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I36" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="J36" s="74"/>
+      <c r="K36" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L36" s="93"/>
+      <c r="M36" s="93"/>
+      <c r="N36" s="78"/>
+      <c r="O36" s="78"/>
+      <c r="P36" s="78"/>
+      <c r="Q36" s="78"/>
+      <c r="R36" s="78"/>
+      <c r="S36" s="78"/>
+      <c r="T36" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="U36" s="63" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="90"/>
+      <c r="B37" s="89" t="s">
+        <v>298</v>
+      </c>
+      <c r="C37" s="89"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="112"/>
+      <c r="F37" s="93"/>
+      <c r="G37" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="H37" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I37" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="J37" s="74"/>
+      <c r="K37" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L37" s="93"/>
+      <c r="M37" s="93"/>
       <c r="N37" s="78"/>
-      <c r="O37" s="81"/>
-    </row>
-    <row r="38" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
+      <c r="O37" s="78"/>
+      <c r="P37" s="78"/>
+      <c r="Q37" s="78"/>
+      <c r="R37" s="78"/>
+      <c r="S37" s="78"/>
+      <c r="T37" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="U37" s="63" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="90"/>
+      <c r="B38" s="89" t="s">
+        <v>299</v>
+      </c>
+      <c r="C38" s="89"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="112"/>
+      <c r="F38" s="93"/>
+      <c r="G38" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="H38" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I38" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="J38" s="74"/>
+      <c r="K38" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L38" s="93"/>
+      <c r="M38" s="93"/>
+      <c r="N38" s="78"/>
+      <c r="O38" s="78"/>
+      <c r="P38" s="78"/>
+      <c r="Q38" s="78"/>
+      <c r="R38" s="78"/>
+      <c r="S38" s="78"/>
+      <c r="T38" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="U38" s="63" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="90"/>
+      <c r="B39" s="89" t="s">
+        <v>301</v>
+      </c>
+      <c r="C39" s="89"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="112"/>
+      <c r="F39" s="93"/>
+      <c r="G39" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="H39" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I39" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="J39" s="74"/>
+      <c r="K39" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L39" s="93"/>
+      <c r="M39" s="93"/>
+      <c r="N39" s="78"/>
+      <c r="O39" s="78"/>
+      <c r="P39" s="78"/>
+      <c r="Q39" s="78"/>
+      <c r="R39" s="78"/>
+      <c r="S39" s="78"/>
+      <c r="T39" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="U39" s="63" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="90"/>
+      <c r="B40" s="89" t="s">
+        <v>300</v>
+      </c>
+      <c r="C40" s="89"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="112"/>
+      <c r="F40" s="93"/>
+      <c r="G40" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="H40" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I40" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="J40" s="74"/>
+      <c r="K40" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="L40" s="93"/>
+      <c r="M40" s="93"/>
+      <c r="N40" s="78"/>
+      <c r="O40" s="78"/>
+      <c r="P40" s="78"/>
+      <c r="Q40" s="78"/>
+      <c r="R40" s="78"/>
+      <c r="S40" s="78"/>
+      <c r="T40" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="U40" s="63" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="90"/>
+      <c r="B41" s="89" t="s">
+        <v>302</v>
+      </c>
+      <c r="C41" s="89"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="93"/>
+      <c r="G41" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="H41" s="74"/>
+      <c r="I41" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="J41" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K41" s="75"/>
+      <c r="L41" s="93"/>
+      <c r="M41" s="93"/>
+      <c r="N41" s="78"/>
+      <c r="O41" s="78"/>
+      <c r="P41" s="78"/>
+      <c r="Q41" s="78"/>
+      <c r="R41" s="78"/>
+      <c r="S41" s="78"/>
+      <c r="T41" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="U41" s="63" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="90"/>
+      <c r="B42" s="89" t="s">
+        <v>303</v>
+      </c>
+      <c r="C42" s="89"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="93"/>
+      <c r="G42" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="H42" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I42" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="J42" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K42" s="75"/>
+      <c r="L42" s="93"/>
+      <c r="M42" s="93"/>
+      <c r="N42" s="78"/>
+      <c r="O42" s="78"/>
+      <c r="P42" s="78"/>
+      <c r="Q42" s="78"/>
+      <c r="R42" s="78"/>
+      <c r="S42" s="78"/>
+      <c r="T42" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="U42" s="63" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="90"/>
+      <c r="B43" s="89" t="s">
+        <v>304</v>
+      </c>
+      <c r="C43" s="89"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="112"/>
+      <c r="F43" s="93"/>
+      <c r="G43" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="H43" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I43" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="J43" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K43" s="75"/>
+      <c r="L43" s="93"/>
+      <c r="M43" s="93"/>
+      <c r="N43" s="78"/>
+      <c r="O43" s="78"/>
+      <c r="P43" s="78"/>
+      <c r="Q43" s="78"/>
+      <c r="R43" s="78"/>
+      <c r="S43" s="78"/>
+      <c r="T43" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="U43" s="63" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="90"/>
+      <c r="B44" s="89" t="s">
+        <v>305</v>
+      </c>
+      <c r="C44" s="89"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="112"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="H44" s="74"/>
+      <c r="I44" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="J44" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K44" s="75"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="93"/>
+      <c r="N44" s="78"/>
+      <c r="O44" s="78"/>
+      <c r="P44" s="78"/>
+      <c r="Q44" s="78"/>
+      <c r="R44" s="78"/>
+      <c r="S44" s="78"/>
+      <c r="T44" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="U44" s="63" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="35"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="114"/>
+      <c r="F45" s="80"/>
+      <c r="G45" s="77"/>
+      <c r="H45" s="76"/>
+      <c r="I45" s="77"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="77"/>
+      <c r="L45" s="80"/>
+      <c r="M45" s="80"/>
+      <c r="N45" s="80"/>
+      <c r="O45" s="80"/>
+      <c r="P45" s="80"/>
+      <c r="Q45" s="80"/>
+      <c r="R45" s="80"/>
+      <c r="S45" s="80"/>
+      <c r="T45" s="80"/>
+      <c r="U45" s="64"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="30"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="78"/>
+      <c r="F46" s="78"/>
+      <c r="G46" s="78"/>
+      <c r="H46" s="78"/>
+      <c r="I46" s="78"/>
+      <c r="J46" s="78"/>
+      <c r="K46" s="78"/>
+      <c r="L46" s="78"/>
+      <c r="M46" s="78"/>
+      <c r="N46" s="78"/>
+      <c r="O46" s="78"/>
+      <c r="P46" s="78"/>
+      <c r="Q46" s="78"/>
+      <c r="R46" s="78"/>
+      <c r="S46" s="78"/>
+      <c r="T46" s="78"/>
+      <c r="U46" s="81"/>
+    </row>
+    <row r="47" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="78"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="78"/>
-      <c r="H38" s="78"/>
-      <c r="I38" s="78"/>
-      <c r="J38" s="78"/>
-      <c r="K38" s="78"/>
-      <c r="L38" s="78"/>
-      <c r="M38" s="78"/>
-      <c r="N38" s="78"/>
-      <c r="O38" s="81"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="78"/>
-      <c r="G39" s="78"/>
-      <c r="H39" s="78"/>
-      <c r="I39" s="78"/>
-      <c r="J39" s="78"/>
-      <c r="K39" s="78"/>
-      <c r="L39" s="78"/>
-      <c r="M39" s="78"/>
-      <c r="N39" s="78"/>
-      <c r="O39" s="81"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="78"/>
-      <c r="H40" s="78"/>
-      <c r="I40" s="78"/>
-      <c r="J40" s="78"/>
-      <c r="K40" s="78"/>
-      <c r="L40" s="78"/>
-      <c r="M40" s="78"/>
-      <c r="N40" s="78"/>
-      <c r="O40" s="81"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="78"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
-      <c r="H41" s="78"/>
-      <c r="I41" s="78"/>
-      <c r="J41" s="78"/>
-      <c r="K41" s="78"/>
-      <c r="L41" s="78"/>
-      <c r="M41" s="78"/>
-      <c r="N41" s="78"/>
-      <c r="O41" s="81"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78"/>
-      <c r="G42" s="78"/>
-      <c r="H42" s="78"/>
-      <c r="I42" s="78"/>
-      <c r="J42" s="78"/>
-      <c r="K42" s="78"/>
-      <c r="L42" s="78"/>
-      <c r="M42" s="78"/>
-      <c r="N42" s="78"/>
-      <c r="O42" s="81"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="78"/>
-      <c r="G43" s="78"/>
-      <c r="H43" s="78"/>
-      <c r="I43" s="78"/>
-      <c r="J43" s="78"/>
-      <c r="K43" s="78"/>
-      <c r="L43" s="78"/>
-      <c r="M43" s="78"/>
-      <c r="N43" s="78"/>
-      <c r="O43" s="81"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
-      <c r="G44" s="78"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="78"/>
-      <c r="J44" s="78"/>
-      <c r="K44" s="78"/>
-      <c r="L44" s="78"/>
-      <c r="M44" s="78"/>
-      <c r="N44" s="78"/>
-      <c r="O44" s="81"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="78"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="78"/>
-      <c r="G45" s="78"/>
-      <c r="H45" s="78"/>
-      <c r="I45" s="78"/>
-      <c r="J45" s="78"/>
-      <c r="K45" s="78"/>
-      <c r="L45" s="78"/>
-      <c r="M45" s="78"/>
-      <c r="N45" s="78"/>
-      <c r="O45" s="81"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="78"/>
+      <c r="F47" s="78"/>
+      <c r="G47" s="78"/>
+      <c r="H47" s="78"/>
+      <c r="I47" s="78"/>
+      <c r="J47" s="78"/>
+      <c r="K47" s="78"/>
+      <c r="L47" s="78"/>
+      <c r="M47" s="78"/>
+      <c r="N47" s="78"/>
+      <c r="O47" s="78"/>
+      <c r="P47" s="78"/>
+      <c r="Q47" s="78"/>
+      <c r="R47" s="78"/>
+      <c r="S47" s="78"/>
+      <c r="T47" s="78"/>
+      <c r="U47" s="81"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="30"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="78"/>
+      <c r="J48" s="78"/>
+      <c r="K48" s="78"/>
+      <c r="L48" s="78"/>
+      <c r="M48" s="78"/>
+      <c r="N48" s="78"/>
+      <c r="O48" s="78"/>
+      <c r="P48" s="78"/>
+      <c r="Q48" s="78"/>
+      <c r="R48" s="78"/>
+      <c r="S48" s="78"/>
+      <c r="T48" s="78"/>
+      <c r="U48" s="81"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="30"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="78"/>
+      <c r="E49" s="78"/>
+      <c r="F49" s="78"/>
+      <c r="G49" s="78"/>
+      <c r="H49" s="78"/>
+      <c r="I49" s="78"/>
+      <c r="J49" s="78"/>
+      <c r="K49" s="78"/>
+      <c r="L49" s="78"/>
+      <c r="M49" s="78"/>
+      <c r="N49" s="78"/>
+      <c r="O49" s="78"/>
+      <c r="P49" s="78"/>
+      <c r="Q49" s="78"/>
+      <c r="R49" s="78"/>
+      <c r="S49" s="78"/>
+      <c r="T49" s="78"/>
+      <c r="U49" s="81"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="30"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="78"/>
+      <c r="E50" s="78"/>
+      <c r="F50" s="78"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
+      <c r="L50" s="78"/>
+      <c r="M50" s="78"/>
+      <c r="N50" s="78"/>
+      <c r="O50" s="78"/>
+      <c r="P50" s="78"/>
+      <c r="Q50" s="78"/>
+      <c r="R50" s="78"/>
+      <c r="S50" s="78"/>
+      <c r="T50" s="78"/>
+      <c r="U50" s="81"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="30"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="78"/>
+      <c r="E51" s="78"/>
+      <c r="F51" s="78"/>
+      <c r="G51" s="78"/>
+      <c r="H51" s="78"/>
+      <c r="I51" s="78"/>
+      <c r="J51" s="78"/>
+      <c r="K51" s="78"/>
+      <c r="L51" s="78"/>
+      <c r="M51" s="78"/>
+      <c r="N51" s="78"/>
+      <c r="O51" s="78"/>
+      <c r="P51" s="78"/>
+      <c r="Q51" s="78"/>
+      <c r="R51" s="78"/>
+      <c r="S51" s="78"/>
+      <c r="T51" s="78"/>
+      <c r="U51" s="81"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="30"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="78"/>
+      <c r="E52" s="78"/>
+      <c r="F52" s="78"/>
+      <c r="G52" s="78"/>
+      <c r="H52" s="78"/>
+      <c r="I52" s="78"/>
+      <c r="J52" s="78"/>
+      <c r="K52" s="78"/>
+      <c r="L52" s="78"/>
+      <c r="M52" s="78"/>
+      <c r="N52" s="78"/>
+      <c r="O52" s="78"/>
+      <c r="P52" s="78"/>
+      <c r="Q52" s="78"/>
+      <c r="R52" s="78"/>
+      <c r="S52" s="78"/>
+      <c r="T52" s="78"/>
+      <c r="U52" s="81"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" s="30"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="78"/>
+      <c r="E53" s="78"/>
+      <c r="F53" s="78"/>
+      <c r="G53" s="78"/>
+      <c r="H53" s="78"/>
+      <c r="I53" s="78"/>
+      <c r="J53" s="78"/>
+      <c r="K53" s="78"/>
+      <c r="L53" s="78"/>
+      <c r="M53" s="78"/>
+      <c r="N53" s="78"/>
+      <c r="O53" s="78"/>
+      <c r="P53" s="78"/>
+      <c r="Q53" s="78"/>
+      <c r="R53" s="78"/>
+      <c r="S53" s="78"/>
+      <c r="T53" s="78"/>
+      <c r="U53" s="81"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A54" s="30"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="78"/>
+      <c r="E54" s="78"/>
+      <c r="F54" s="78"/>
+      <c r="G54" s="78"/>
+      <c r="H54" s="78"/>
+      <c r="I54" s="78"/>
+      <c r="J54" s="78"/>
+      <c r="K54" s="78"/>
+      <c r="L54" s="78"/>
+      <c r="M54" s="78"/>
+      <c r="N54" s="78"/>
+      <c r="O54" s="78"/>
+      <c r="P54" s="78"/>
+      <c r="Q54" s="78"/>
+      <c r="R54" s="78"/>
+      <c r="S54" s="78"/>
+      <c r="T54" s="78"/>
+      <c r="U54" s="81"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D3:E3"/>
+  <mergeCells count="3">
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="D3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="61" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8801,7 +9732,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8815,14 +9746,14 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
@@ -8831,16 +9762,16 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="99" t="s">
         <v>214</v>
       </c>
-      <c r="E3" s="92"/>
+      <c r="E3" s="100"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="68" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="65" t="s">
@@ -8856,197 +9787,197 @@
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60"/>
       <c r="B5" s="59" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60"/>
       <c r="B6" s="59" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E6" s="75"/>
       <c r="F6" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>
       <c r="B7" s="59" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E7" s="75"/>
       <c r="F7" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
       <c r="B8" s="59" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E8" s="75"/>
       <c r="F8" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60"/>
       <c r="B9" s="59" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C9" s="59"/>
       <c r="D9" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E9" s="75"/>
       <c r="F9" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="60"/>
       <c r="B10" s="59" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E10" s="75"/>
       <c r="F10" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="60"/>
       <c r="B11" s="59" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E11" s="75"/>
       <c r="F11" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60"/>
       <c r="B12" s="59" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E12" s="75"/>
       <c r="F12" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="59" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E13" s="75"/>
       <c r="F13" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="59" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E14" s="75"/>
       <c r="F14" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
       <c r="B15" s="81" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E15" s="75"/>
       <c r="F15" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
       <c r="B16" s="81" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C16" s="59"/>
       <c r="D16" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E16" s="75"/>
       <c r="F16" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="60"/>
       <c r="B17" s="59" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E17" s="75"/>
       <c r="F17" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="60"/>
       <c r="B18" s="59" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E18" s="75"/>
       <c r="F18" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9094,32 +10025,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="89"/>
-      <c r="B24" s="89"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="89"/>
-      <c r="E24" s="89"/>
+      <c r="A24" s="97"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="97"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="89"/>
-      <c r="B25" s="89"/>
-      <c r="C25" s="89"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="89"/>
+      <c r="A25" s="97"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="97"/>
+      <c r="E25" s="97"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="89"/>
-      <c r="B26" s="89"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="89"/>
+      <c r="A26" s="97"/>
+      <c r="B26" s="97"/>
+      <c r="C26" s="97"/>
+      <c r="D26" s="97"/>
+      <c r="E26" s="97"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="89"/>
-      <c r="B27" s="89"/>
-      <c r="C27" s="89"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
+      <c r="A27" s="97"/>
+      <c r="B27" s="97"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -9247,11 +10178,11 @@
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="39" t="s">
@@ -9259,7 +10190,7 @@
       </c>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K3" s="39"/>
       <c r="L3" s="39" t="s">
@@ -9267,7 +10198,7 @@
       </c>
       <c r="M3" s="39"/>
       <c r="N3" s="39" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9297,7 +10228,7 @@
       </c>
       <c r="M4" s="56"/>
       <c r="N4" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
@@ -9327,7 +10258,7 @@
       </c>
       <c r="M5" s="85"/>
       <c r="N5" s="85" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -9345,7 +10276,7 @@
       </c>
       <c r="G6" s="85"/>
       <c r="H6" s="85" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="I6" s="85"/>
       <c r="J6" s="85" t="s">
@@ -9357,7 +10288,7 @@
       </c>
       <c r="M6" s="85"/>
       <c r="N6" s="85" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -9387,7 +10318,7 @@
       </c>
       <c r="M7" s="85"/>
       <c r="N7" s="85" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -9454,7 +10385,7 @@
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -9464,7 +10395,7 @@
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B13" s="56"/>
       <c r="C13" s="56"/>
@@ -9911,27 +10842,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="89"/>
-      <c r="B17" s="89"/>
-      <c r="C17" s="89"/>
+      <c r="A17" s="97"/>
+      <c r="B17" s="97"/>
+      <c r="C17" s="97"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="89"/>
-      <c r="B18" s="89"/>
-      <c r="C18" s="89"/>
+      <c r="A18" s="97"/>
+      <c r="B18" s="97"/>
+      <c r="C18" s="97"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="89"/>
-      <c r="B19" s="89"/>
-      <c r="C19" s="89"/>
+      <c r="A19" s="97"/>
+      <c r="B19" s="97"/>
+      <c r="C19" s="97"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -10370,30 +11301,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="93" t="s">
+      <c r="A42" s="101" t="s">
         <v>176</v>
       </c>
-      <c r="B42" s="93"/>
-      <c r="C42" s="93"/>
+      <c r="B42" s="101"/>
+      <c r="C42" s="101"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="94" t="s">
+      <c r="A43" s="102" t="s">
         <v>177</v>
       </c>
-      <c r="B43" s="94"/>
-      <c r="C43" s="94"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="102"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="93" t="s">
+      <c r="A44" s="101" t="s">
         <v>178</v>
       </c>
-      <c r="B44" s="93"/>
-      <c r="C44" s="93"/>
+      <c r="B44" s="101"/>
+      <c r="C44" s="101"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="89"/>
-      <c r="B45" s="89"/>
-      <c r="C45" s="89"/>
+      <c r="A45" s="97"/>
+      <c r="B45" s="97"/>
+      <c r="C45" s="97"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>

</xml_diff>

<commit_message>
Corrected typos on table about org studies
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -798,9 +798,6 @@
     <t>How to maximize the rationality and efficiency organization activities.</t>
   </si>
   <si>
-    <t>How subjective perceptions affect the behavior of organizations.</t>
-  </si>
-  <si>
     <t>How theory and theorizing practices affect our understanding of organizations.</t>
   </si>
   <si>
@@ -986,13 +983,6 @@
     <t>Table</t>
   </si>
   <si>
-    <t>The organization is a pattern of meanings that created through human interaction that produces shared values, traditions, and customs (i.e., a culture).
-The organization is a political arena</t>
-  </si>
-  <si>
-    <t>Modeles, Theories, and Schools of Thought</t>
-  </si>
-  <si>
     <t>Human relations management
 Garbage can model</t>
   </si>
@@ -1237,6 +1227,16 @@
   </si>
   <si>
     <t>Emphasis on sponsored research</t>
+  </si>
+  <si>
+    <t>How subjective perceptions affect behavior in organizations.</t>
+  </si>
+  <si>
+    <t>The organization is a pattern of meanings created through human interaction that produces shared values, traditions, and customs (i.e., a culture).
+The organization is a political arena.</t>
+  </si>
+  <si>
+    <t>Models, Theories, and Schools of Thought</t>
   </si>
 </sst>
 </file>
@@ -1876,27 +1876,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1906,20 +1885,41 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7426,7 +7426,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7703,54 +7703,54 @@
       <c r="F20" s="29"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="104" t="s">
+      <c r="A21" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="104"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="104"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="108"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="105" t="s">
+      <c r="A22" s="109" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="105"/>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="105"/>
+      <c r="B22" s="109"/>
+      <c r="C22" s="109"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="109"/>
+      <c r="F22" s="109"/>
     </row>
     <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="104" t="s">
+      <c r="A23" s="108" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="104"/>
-      <c r="C23" s="104"/>
-      <c r="D23" s="104"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="104"/>
+      <c r="B23" s="108"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="108"/>
+      <c r="F23" s="108"/>
     </row>
     <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="104" t="s">
+      <c r="A24" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="104"/>
-      <c r="C24" s="104"/>
-      <c r="D24" s="104"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="104"/>
+      <c r="B24" s="108"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="108"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="104" t="s">
+      <c r="A25" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="104"/>
-      <c r="C25" s="104"/>
-      <c r="D25" s="104"/>
-      <c r="E25" s="104"/>
-      <c r="F25" s="104"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="108"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="108"/>
+      <c r="F25" s="108"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -7839,7 +7839,7 @@
   </sheetPr>
   <dimension ref="A1:AA78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -7887,7 +7887,7 @@
     </row>
     <row r="2" spans="1:27" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E2" s="61"/>
       <c r="F2" s="61"/>
@@ -7918,121 +7918,121 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="106" t="s">
-        <v>293</v>
-      </c>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="116" t="s">
-        <v>321</v>
-      </c>
-      <c r="J3" s="107"/>
-      <c r="K3" s="116" t="s">
-        <v>322</v>
-      </c>
-      <c r="L3" s="117"/>
-      <c r="M3" s="106" t="s">
-        <v>309</v>
-      </c>
-      <c r="N3" s="108"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="114" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108"/>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108"/>
-      <c r="W3" s="108"/>
-      <c r="X3" s="108"/>
-      <c r="Y3" s="108"/>
-      <c r="Z3" s="115"/>
+      <c r="E3" s="113" t="s">
+        <v>290</v>
+      </c>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="110" t="s">
+        <v>318</v>
+      </c>
+      <c r="J3" s="111"/>
+      <c r="K3" s="110" t="s">
+        <v>319</v>
+      </c>
+      <c r="L3" s="112"/>
+      <c r="M3" s="113" t="s">
+        <v>306</v>
+      </c>
+      <c r="N3" s="114"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="115" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q3" s="114"/>
+      <c r="R3" s="114"/>
+      <c r="S3" s="114"/>
+      <c r="T3" s="114"/>
+      <c r="U3" s="114"/>
+      <c r="V3" s="114"/>
+      <c r="W3" s="114"/>
+      <c r="X3" s="114"/>
+      <c r="Y3" s="114"/>
+      <c r="Z3" s="116"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
-      <c r="B4" s="111" t="s">
-        <v>307</v>
+      <c r="B4" s="104" t="s">
+        <v>304</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="68"/>
-      <c r="E4" s="112" t="s">
-        <v>326</v>
-      </c>
-      <c r="F4" s="118" t="s">
-        <v>325</v>
+      <c r="E4" s="105" t="s">
+        <v>323</v>
+      </c>
+      <c r="F4" s="107" t="s">
+        <v>322</v>
       </c>
       <c r="G4" s="62" t="s">
-        <v>324</v>
-      </c>
-      <c r="H4" s="113" t="s">
-        <v>323</v>
+        <v>321</v>
+      </c>
+      <c r="H4" s="106" t="s">
+        <v>320</v>
       </c>
       <c r="I4" s="65" t="s">
+        <v>209</v>
+      </c>
+      <c r="J4" s="66" t="s">
         <v>210</v>
       </c>
-      <c r="J4" s="66" t="s">
-        <v>211</v>
-      </c>
       <c r="K4" s="65" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="L4" s="66" t="s">
-        <v>276</v>
-      </c>
-      <c r="M4" s="112" t="s">
-        <v>311</v>
+        <v>273</v>
+      </c>
+      <c r="M4" s="105" t="s">
+        <v>308</v>
       </c>
       <c r="N4" s="62" t="s">
-        <v>312</v>
-      </c>
-      <c r="O4" s="113" t="s">
-        <v>310</v>
+        <v>309</v>
+      </c>
+      <c r="O4" s="106" t="s">
+        <v>307</v>
       </c>
       <c r="P4" s="62" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="Q4" s="62" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="R4" s="62" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S4" s="62" t="s">
+        <v>223</v>
+      </c>
+      <c r="T4" s="62" t="s">
+        <v>247</v>
+      </c>
+      <c r="U4" s="62" t="s">
+        <v>253</v>
+      </c>
+      <c r="V4" s="62" t="s">
         <v>224</v>
       </c>
-      <c r="T4" s="62" t="s">
+      <c r="W4" s="62" t="s">
+        <v>249</v>
+      </c>
+      <c r="X4" s="62" t="s">
         <v>250</v>
       </c>
-      <c r="U4" s="62" t="s">
-        <v>256</v>
-      </c>
-      <c r="V4" s="62" t="s">
-        <v>225</v>
-      </c>
-      <c r="W4" s="62" t="s">
-        <v>252</v>
-      </c>
-      <c r="X4" s="62" t="s">
-        <v>253</v>
-      </c>
       <c r="Y4" s="62" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="Z4" s="62" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="AA4" s="72" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="49" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C5" s="93"/>
       <c r="D5" s="93"/>
@@ -8064,25 +8064,25 @@
       <c r="A6" s="94"/>
       <c r="B6" s="82"/>
       <c r="C6" s="81" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D6" s="81"/>
       <c r="E6" s="74"/>
       <c r="F6" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G6" s="92"/>
       <c r="H6" s="75"/>
       <c r="I6" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J6" s="75"/>
       <c r="K6" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L6" s="75"/>
       <c r="M6" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N6" s="92"/>
       <c r="O6" s="75"/>
@@ -8091,7 +8091,7 @@
       <c r="R6" s="92"/>
       <c r="S6" s="78"/>
       <c r="T6" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U6" s="78"/>
       <c r="V6" s="78"/>
@@ -8100,32 +8100,32 @@
       <c r="Y6" s="78"/>
       <c r="Z6" s="78"/>
       <c r="AA6" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="94"/>
       <c r="B7" s="82"/>
       <c r="C7" s="93" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D7" s="81"/>
       <c r="E7" s="74"/>
       <c r="F7" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G7" s="92"/>
       <c r="H7" s="75"/>
       <c r="I7" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J7" s="75"/>
       <c r="K7" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L7" s="75"/>
       <c r="M7" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N7" s="92"/>
       <c r="O7" s="75"/>
@@ -8134,7 +8134,7 @@
       <c r="R7" s="92"/>
       <c r="S7" s="78"/>
       <c r="T7" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U7" s="78"/>
       <c r="V7" s="78"/>
@@ -8143,32 +8143,32 @@
       <c r="Y7" s="78"/>
       <c r="Z7" s="78"/>
       <c r="AA7" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="94"/>
       <c r="B8" s="82"/>
       <c r="C8" s="81" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D8" s="81"/>
       <c r="E8" s="74"/>
       <c r="F8" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G8" s="92"/>
       <c r="H8" s="75"/>
       <c r="I8" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J8" s="75"/>
       <c r="K8" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L8" s="75"/>
       <c r="M8" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N8" s="92"/>
       <c r="O8" s="75"/>
@@ -8177,7 +8177,7 @@
       <c r="R8" s="92"/>
       <c r="S8" s="78"/>
       <c r="T8" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U8" s="78"/>
       <c r="V8" s="78"/>
@@ -8186,47 +8186,47 @@
       <c r="Y8" s="78"/>
       <c r="Z8" s="78"/>
       <c r="AA8" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="94"/>
       <c r="B9" s="82"/>
       <c r="C9" s="93" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D9" s="81"/>
       <c r="E9" s="74"/>
       <c r="F9" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G9" s="92"/>
       <c r="H9" s="75"/>
       <c r="I9" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J9" s="75"/>
       <c r="K9" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L9" s="75"/>
       <c r="M9" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N9" s="92"/>
       <c r="O9" s="75"/>
       <c r="P9" s="92"/>
       <c r="Q9" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R9" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S9" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T9" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U9" s="78"/>
       <c r="V9" s="78"/>
@@ -8235,104 +8235,104 @@
       <c r="Y9" s="78"/>
       <c r="Z9" s="78"/>
       <c r="AA9" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
       <c r="B10" s="30"/>
       <c r="C10" s="32" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="74"/>
       <c r="F10" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G10" s="92"/>
       <c r="H10" s="75"/>
       <c r="I10" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J10" s="75"/>
       <c r="K10" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L10" s="75"/>
       <c r="M10" s="74"/>
       <c r="N10" s="92"/>
       <c r="O10" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P10" s="92"/>
       <c r="Q10" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R10" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S10" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T10" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U10" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V10" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W10" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X10" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y10" s="78"/>
       <c r="Z10" s="78"/>
       <c r="AA10" s="63" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="94"/>
       <c r="B11" s="82"/>
       <c r="C11" s="95" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D11" s="81"/>
       <c r="E11" s="96"/>
       <c r="F11" s="102" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G11" s="98"/>
       <c r="H11" s="97"/>
       <c r="I11" s="96" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J11" s="97"/>
       <c r="K11" s="96" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L11" s="97"/>
       <c r="M11" s="96" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N11" s="98"/>
       <c r="O11" s="97"/>
       <c r="P11" s="98"/>
       <c r="Q11" s="98" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R11" s="98" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S11" s="99" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T11" s="99" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U11" s="99"/>
       <c r="V11" s="99"/>
@@ -8341,7 +8341,7 @@
       <c r="Y11" s="99"/>
       <c r="Z11" s="99"/>
       <c r="AA11" s="100" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -8376,7 +8376,7 @@
     <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="49" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C13" s="93"/>
       <c r="D13" s="93"/>
@@ -8408,241 +8408,241 @@
       <c r="A14" s="94"/>
       <c r="B14" s="30"/>
       <c r="C14" s="32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="74"/>
       <c r="F14" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G14" s="92"/>
       <c r="H14" s="75"/>
       <c r="I14" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J14" s="75"/>
       <c r="K14" s="74"/>
       <c r="L14" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M14" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N14" s="92"/>
       <c r="O14" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P14" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q14" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R14" s="92"/>
       <c r="S14" s="78"/>
       <c r="T14" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U14" s="78"/>
       <c r="V14" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W14" s="78"/>
       <c r="X14" s="78"/>
       <c r="Y14" s="78"/>
       <c r="Z14" s="78"/>
       <c r="AA14" s="63" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="94"/>
       <c r="B15" s="30"/>
       <c r="C15" s="32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="74"/>
       <c r="F15" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G15" s="92"/>
       <c r="H15" s="75"/>
       <c r="I15" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J15" s="75"/>
       <c r="K15" s="74"/>
       <c r="L15" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M15" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N15" s="92"/>
       <c r="O15" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P15" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q15" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R15" s="92"/>
       <c r="S15" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T15" s="78"/>
       <c r="U15" s="78"/>
       <c r="V15" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W15" s="78"/>
       <c r="X15" s="78"/>
       <c r="Y15" s="78"/>
       <c r="Z15" s="78"/>
       <c r="AA15" s="63" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="94"/>
       <c r="B16" s="82"/>
       <c r="C16" s="81" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D16" s="81"/>
       <c r="E16" s="74"/>
       <c r="F16" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G16" s="92"/>
       <c r="H16" s="75"/>
       <c r="I16" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J16" s="75"/>
       <c r="K16" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L16" s="75"/>
       <c r="M16" s="74"/>
       <c r="N16" s="92"/>
       <c r="O16" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P16" s="92"/>
       <c r="Q16" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R16" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S16" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T16" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U16" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V16" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W16" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X16" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y16" s="78"/>
       <c r="Z16" s="78"/>
       <c r="AA16" s="63" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="94"/>
       <c r="B17" s="82"/>
       <c r="C17" s="81" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D17" s="81"/>
       <c r="E17" s="74"/>
       <c r="F17" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G17" s="92"/>
       <c r="H17" s="75"/>
       <c r="I17" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J17" s="75"/>
       <c r="K17" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L17" s="75"/>
       <c r="M17" s="74"/>
       <c r="N17" s="92"/>
       <c r="O17" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P17" s="92"/>
       <c r="Q17" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R17" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S17" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T17" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U17" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V17" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W17" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X17" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y17" s="78"/>
       <c r="Z17" s="78"/>
       <c r="AA17" s="63" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="94"/>
       <c r="B18" s="60"/>
       <c r="C18" s="59" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D18" s="59"/>
       <c r="E18" s="74"/>
       <c r="F18" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G18" s="92"/>
       <c r="H18" s="75"/>
       <c r="I18" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J18" s="75"/>
       <c r="K18" s="74"/>
       <c r="L18" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M18" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N18" s="92"/>
       <c r="O18" s="75"/>
@@ -8653,39 +8653,39 @@
       <c r="T18" s="78"/>
       <c r="U18" s="78"/>
       <c r="V18" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W18" s="78"/>
       <c r="X18" s="78"/>
       <c r="Y18" s="78"/>
       <c r="Z18" s="78"/>
       <c r="AA18" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="94"/>
       <c r="B19" s="30"/>
       <c r="C19" s="32" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="74"/>
       <c r="F19" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G19" s="92"/>
       <c r="H19" s="75"/>
       <c r="I19" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J19" s="75"/>
       <c r="K19" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L19" s="75"/>
       <c r="M19" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N19" s="92"/>
       <c r="O19" s="75"/>
@@ -8693,7 +8693,7 @@
       <c r="Q19" s="92"/>
       <c r="R19" s="92"/>
       <c r="S19" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T19" s="78"/>
       <c r="U19" s="78"/>
@@ -8703,32 +8703,32 @@
       <c r="Y19" s="78"/>
       <c r="Z19" s="78"/>
       <c r="AA19" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="94"/>
       <c r="B20" s="30"/>
       <c r="C20" s="32" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="74"/>
       <c r="F20" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G20" s="92"/>
       <c r="H20" s="75"/>
       <c r="I20" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J20" s="75"/>
       <c r="K20" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L20" s="75"/>
       <c r="M20" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N20" s="92"/>
       <c r="O20" s="75"/>
@@ -8736,7 +8736,7 @@
       <c r="Q20" s="92"/>
       <c r="R20" s="92"/>
       <c r="S20" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T20" s="78"/>
       <c r="U20" s="78"/>
@@ -8746,32 +8746,32 @@
       <c r="Y20" s="78"/>
       <c r="Z20" s="78"/>
       <c r="AA20" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="94"/>
       <c r="B21" s="30"/>
       <c r="C21" s="32" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="74"/>
       <c r="F21" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G21" s="92"/>
       <c r="H21" s="75"/>
       <c r="I21" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J21" s="75"/>
       <c r="K21" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L21" s="75"/>
       <c r="M21" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N21" s="92"/>
       <c r="O21" s="75"/>
@@ -8779,7 +8779,7 @@
       <c r="Q21" s="92"/>
       <c r="R21" s="92"/>
       <c r="S21" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T21" s="78"/>
       <c r="U21" s="78"/>
@@ -8789,349 +8789,349 @@
       <c r="Y21" s="78"/>
       <c r="Z21" s="78"/>
       <c r="AA21" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="94"/>
       <c r="B22" s="82"/>
       <c r="C22" s="81" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D22" s="81"/>
       <c r="E22" s="74"/>
       <c r="F22" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G22" s="92"/>
       <c r="H22" s="75"/>
       <c r="I22" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J22" s="75"/>
       <c r="K22" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L22" s="75"/>
       <c r="M22" s="74"/>
       <c r="N22" s="92"/>
       <c r="O22" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P22" s="92"/>
       <c r="Q22" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R22" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S22" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T22" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U22" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V22" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W22" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X22" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y22" s="78"/>
       <c r="Z22" s="78"/>
       <c r="AA22" s="63" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="94"/>
       <c r="B23" s="82"/>
       <c r="C23" s="81" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D23" s="81"/>
       <c r="E23" s="74"/>
       <c r="F23" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G23" s="92"/>
       <c r="H23" s="75"/>
       <c r="I23" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J23" s="75"/>
       <c r="K23" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L23" s="75"/>
       <c r="M23" s="74"/>
       <c r="N23" s="92"/>
       <c r="O23" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P23" s="92"/>
       <c r="Q23" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R23" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S23" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T23" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U23" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V23" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W23" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X23" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y23" s="78"/>
       <c r="Z23" s="78"/>
       <c r="AA23" s="63" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="94"/>
       <c r="B24" s="30"/>
       <c r="C24" s="32" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="74"/>
       <c r="F24" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G24" s="92"/>
       <c r="H24" s="75"/>
       <c r="I24" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J24" s="75"/>
       <c r="K24" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L24" s="75"/>
       <c r="M24" s="74"/>
       <c r="N24" s="92"/>
       <c r="O24" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P24" s="92"/>
       <c r="Q24" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R24" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S24" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T24" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U24" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V24" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W24" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X24" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y24" s="78"/>
       <c r="Z24" s="78"/>
       <c r="AA24" s="63" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="94"/>
       <c r="B25" s="30"/>
       <c r="C25" s="32" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="74"/>
       <c r="F25" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G25" s="92"/>
       <c r="H25" s="75"/>
       <c r="I25" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J25" s="75"/>
       <c r="K25" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L25" s="75"/>
       <c r="M25" s="74"/>
       <c r="N25" s="92"/>
       <c r="O25" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P25" s="92"/>
       <c r="Q25" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R25" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S25" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T25" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U25" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V25" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W25" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X25" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y25" s="78"/>
       <c r="Z25" s="78"/>
       <c r="AA25" s="63" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="94"/>
       <c r="B26" s="82"/>
       <c r="C26" s="81" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D26" s="81"/>
       <c r="E26" s="74"/>
       <c r="F26" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G26" s="92"/>
       <c r="H26" s="75"/>
       <c r="I26" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J26" s="75"/>
       <c r="K26" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L26" s="75"/>
       <c r="M26" s="74"/>
       <c r="N26" s="92"/>
       <c r="O26" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P26" s="92"/>
       <c r="Q26" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R26" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S26" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T26" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U26" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V26" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W26" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X26" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y26" s="78"/>
       <c r="Z26" s="78"/>
       <c r="AA26" s="63" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="94"/>
       <c r="B27" s="82"/>
       <c r="C27" s="81" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D27" s="81"/>
       <c r="E27" s="74"/>
       <c r="F27" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G27" s="92"/>
       <c r="H27" s="75"/>
       <c r="I27" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J27" s="75"/>
       <c r="K27" s="74"/>
       <c r="L27" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M27" s="74"/>
       <c r="N27" s="92"/>
       <c r="O27" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P27" s="92"/>
       <c r="Q27" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R27" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S27" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T27" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U27" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V27" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W27" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X27" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y27" s="78"/>
       <c r="Z27" s="78"/>
       <c r="AA27" s="63" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="28" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9166,7 +9166,7 @@
     <row r="29" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="94"/>
       <c r="B29" s="31" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C29" s="93"/>
       <c r="D29" s="93"/>
@@ -9198,40 +9198,40 @@
       <c r="A30" s="94"/>
       <c r="B30" s="82"/>
       <c r="C30" s="81" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D30" s="81"/>
       <c r="E30" s="74"/>
       <c r="F30" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G30" s="92"/>
       <c r="H30" s="75"/>
       <c r="I30" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J30" s="75"/>
       <c r="K30" s="74"/>
       <c r="L30" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M30" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N30" s="92"/>
       <c r="O30" s="75"/>
       <c r="P30" s="92"/>
       <c r="Q30" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R30" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S30" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T30" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U30" s="78"/>
       <c r="V30" s="78"/>
@@ -9240,32 +9240,32 @@
       <c r="Y30" s="78"/>
       <c r="Z30" s="78"/>
       <c r="AA30" s="63" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="31" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="94"/>
       <c r="B31" s="94"/>
       <c r="C31" s="93" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D31" s="93"/>
       <c r="E31" s="74"/>
       <c r="F31" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G31" s="92"/>
       <c r="H31" s="75"/>
       <c r="I31" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J31" s="75"/>
       <c r="K31" s="74"/>
       <c r="L31" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M31" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N31" s="92"/>
       <c r="O31" s="75"/>
@@ -9274,7 +9274,7 @@
       <c r="R31" s="92"/>
       <c r="S31" s="78"/>
       <c r="T31" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U31" s="78"/>
       <c r="V31" s="78"/>
@@ -9283,32 +9283,32 @@
       <c r="Y31" s="78"/>
       <c r="Z31" s="78"/>
       <c r="AA31" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="94"/>
       <c r="B32" s="94"/>
       <c r="C32" s="93" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D32" s="93"/>
       <c r="E32" s="74"/>
       <c r="F32" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G32" s="92"/>
       <c r="H32" s="75"/>
       <c r="I32" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J32" s="75"/>
       <c r="K32" s="74"/>
       <c r="L32" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M32" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N32" s="92"/>
       <c r="O32" s="75"/>
@@ -9317,7 +9317,7 @@
       <c r="R32" s="92"/>
       <c r="S32" s="78"/>
       <c r="T32" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U32" s="78"/>
       <c r="V32" s="78"/>
@@ -9326,38 +9326,38 @@
       <c r="Y32" s="78"/>
       <c r="Z32" s="78"/>
       <c r="AA32" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="94"/>
       <c r="B33" s="94"/>
       <c r="C33" s="93" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D33" s="93"/>
       <c r="E33" s="74"/>
       <c r="F33" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G33" s="92"/>
       <c r="H33" s="75"/>
       <c r="I33" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J33" s="75"/>
       <c r="K33" s="74"/>
       <c r="L33" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M33" s="74"/>
       <c r="N33" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O33" s="75"/>
       <c r="P33" s="92"/>
       <c r="Q33" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R33" s="92"/>
       <c r="S33" s="78"/>
@@ -9369,7 +9369,7 @@
       <c r="Y33" s="78"/>
       <c r="Z33" s="78"/>
       <c r="AA33" s="63" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="34" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9404,7 +9404,7 @@
     <row r="35" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
       <c r="B35" s="49" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C35" s="93"/>
       <c r="D35" s="93"/>
@@ -9436,25 +9436,25 @@
       <c r="A36" s="94"/>
       <c r="B36" s="30"/>
       <c r="C36" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D36" s="32"/>
       <c r="E36" s="74"/>
       <c r="F36" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G36" s="92"/>
       <c r="H36" s="75"/>
       <c r="I36" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J36" s="75"/>
       <c r="K36" s="74"/>
       <c r="L36" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M36" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N36" s="92"/>
       <c r="O36" s="75"/>
@@ -9462,7 +9462,7 @@
       <c r="Q36" s="92"/>
       <c r="R36" s="92"/>
       <c r="S36" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T36" s="78"/>
       <c r="U36" s="78"/>
@@ -9472,32 +9472,32 @@
       <c r="Y36" s="78"/>
       <c r="Z36" s="78"/>
       <c r="AA36" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="94"/>
       <c r="B37" s="30"/>
       <c r="C37" s="32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D37" s="32"/>
       <c r="E37" s="74"/>
       <c r="F37" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G37" s="92"/>
       <c r="H37" s="75"/>
       <c r="I37" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J37" s="75"/>
       <c r="K37" s="74"/>
       <c r="L37" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M37" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N37" s="92"/>
       <c r="O37" s="75"/>
@@ -9508,39 +9508,39 @@
       <c r="T37" s="78"/>
       <c r="U37" s="78"/>
       <c r="V37" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W37" s="78"/>
       <c r="X37" s="78"/>
       <c r="Y37" s="78"/>
       <c r="Z37" s="78"/>
       <c r="AA37" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="94"/>
       <c r="B38" s="94"/>
       <c r="C38" s="93" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D38" s="93"/>
       <c r="E38" s="74"/>
       <c r="F38" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G38" s="92"/>
       <c r="H38" s="75"/>
       <c r="I38" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J38" s="75"/>
       <c r="K38" s="74"/>
       <c r="L38" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M38" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N38" s="92"/>
       <c r="O38" s="75"/>
@@ -9548,7 +9548,7 @@
       <c r="Q38" s="92"/>
       <c r="R38" s="92"/>
       <c r="S38" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T38" s="78"/>
       <c r="U38" s="78"/>
@@ -9558,32 +9558,32 @@
       <c r="Y38" s="78"/>
       <c r="Z38" s="78"/>
       <c r="AA38" s="63" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="39" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="94"/>
       <c r="B39" s="94"/>
       <c r="C39" s="93" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D39" s="93"/>
       <c r="E39" s="74"/>
       <c r="F39" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G39" s="92"/>
       <c r="H39" s="75"/>
       <c r="I39" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J39" s="75"/>
       <c r="K39" s="74"/>
       <c r="L39" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M39" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N39" s="92"/>
       <c r="O39" s="75"/>
@@ -9591,44 +9591,44 @@
       <c r="Q39" s="92"/>
       <c r="R39" s="92"/>
       <c r="S39" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T39" s="78"/>
       <c r="U39" s="78"/>
       <c r="V39" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W39" s="78"/>
       <c r="X39" s="78"/>
       <c r="Y39" s="78"/>
       <c r="Z39" s="78"/>
       <c r="AA39" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="94"/>
       <c r="B40" s="94"/>
       <c r="C40" s="93" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D40" s="93"/>
       <c r="E40" s="74"/>
       <c r="F40" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G40" s="92"/>
       <c r="H40" s="75"/>
       <c r="I40" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J40" s="75"/>
       <c r="K40" s="74"/>
       <c r="L40" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M40" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N40" s="92"/>
       <c r="O40" s="75"/>
@@ -9636,93 +9636,93 @@
       <c r="Q40" s="92"/>
       <c r="R40" s="92"/>
       <c r="S40" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T40" s="78"/>
       <c r="U40" s="78"/>
       <c r="V40" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W40" s="78"/>
       <c r="X40" s="78"/>
       <c r="Y40" s="78"/>
       <c r="Z40" s="78"/>
       <c r="AA40" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="94"/>
       <c r="B41" s="94"/>
       <c r="C41" s="93" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D41" s="93"/>
       <c r="E41" s="74"/>
       <c r="F41" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G41" s="92"/>
       <c r="H41" s="75"/>
       <c r="I41" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J41" s="75"/>
       <c r="K41" s="74"/>
       <c r="L41" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M41" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N41" s="92"/>
       <c r="O41" s="75"/>
       <c r="P41" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q41" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R41" s="92"/>
       <c r="S41" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T41" s="78"/>
       <c r="U41" s="78"/>
       <c r="V41" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W41" s="78"/>
       <c r="X41" s="78"/>
       <c r="Y41" s="78"/>
       <c r="Z41" s="78"/>
       <c r="AA41" s="63" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="42" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="94"/>
       <c r="B42" s="94"/>
       <c r="C42" s="93" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D42" s="93"/>
       <c r="E42" s="74"/>
       <c r="F42" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G42" s="92"/>
       <c r="H42" s="75"/>
       <c r="I42" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J42" s="75"/>
       <c r="K42" s="74"/>
       <c r="L42" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M42" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N42" s="92"/>
       <c r="O42" s="75"/>
@@ -9731,7 +9731,7 @@
       <c r="R42" s="92"/>
       <c r="S42" s="78"/>
       <c r="T42" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U42" s="78"/>
       <c r="V42" s="78"/>
@@ -9740,32 +9740,32 @@
       <c r="Y42" s="78"/>
       <c r="Z42" s="78"/>
       <c r="AA42" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="94"/>
       <c r="B43" s="94"/>
       <c r="C43" s="93" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D43" s="93"/>
       <c r="E43" s="74"/>
       <c r="F43" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G43" s="92"/>
       <c r="H43" s="75"/>
       <c r="I43" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J43" s="75"/>
       <c r="K43" s="74"/>
       <c r="L43" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M43" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N43" s="92"/>
       <c r="O43" s="75"/>
@@ -9773,44 +9773,44 @@
       <c r="Q43" s="92"/>
       <c r="R43" s="92"/>
       <c r="S43" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T43" s="78"/>
       <c r="U43" s="78"/>
       <c r="V43" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W43" s="78"/>
       <c r="X43" s="78"/>
       <c r="Y43" s="78"/>
       <c r="Z43" s="78"/>
       <c r="AA43" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="44" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="94"/>
       <c r="B44" s="94"/>
       <c r="C44" s="93" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D44" s="93"/>
       <c r="E44" s="74"/>
       <c r="F44" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G44" s="92"/>
       <c r="H44" s="75"/>
       <c r="I44" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J44" s="75"/>
       <c r="K44" s="74"/>
       <c r="L44" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M44" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N44" s="92"/>
       <c r="O44" s="75"/>
@@ -9818,101 +9818,101 @@
       <c r="Q44" s="92"/>
       <c r="R44" s="92"/>
       <c r="S44" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T44" s="78"/>
       <c r="U44" s="78"/>
       <c r="V44" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W44" s="78"/>
       <c r="X44" s="78"/>
       <c r="Y44" s="78"/>
       <c r="Z44" s="78"/>
       <c r="AA44" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="94"/>
       <c r="B45" s="82"/>
       <c r="C45" s="81" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D45" s="81"/>
       <c r="E45" s="74"/>
       <c r="F45" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G45" s="92"/>
       <c r="H45" s="75"/>
       <c r="I45" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J45" s="75"/>
       <c r="K45" s="74"/>
       <c r="L45" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M45" s="74"/>
       <c r="N45" s="92"/>
       <c r="O45" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P45" s="92"/>
       <c r="Q45" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R45" s="92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S45" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T45" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U45" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V45" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W45" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X45" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y45" s="78"/>
       <c r="Z45" s="78"/>
       <c r="AA45" s="63" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="46" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="94"/>
       <c r="B46" s="60"/>
       <c r="C46" s="59" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D46" s="59"/>
       <c r="E46" s="74"/>
       <c r="F46" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G46" s="92"/>
       <c r="H46" s="75"/>
       <c r="I46" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J46" s="75"/>
       <c r="K46" s="74"/>
       <c r="L46" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M46" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N46" s="92"/>
       <c r="O46" s="75"/>
@@ -9920,44 +9920,44 @@
       <c r="Q46" s="92"/>
       <c r="R46" s="92"/>
       <c r="S46" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T46" s="78"/>
       <c r="U46" s="78"/>
       <c r="V46" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W46" s="78"/>
       <c r="X46" s="78"/>
       <c r="Y46" s="78"/>
       <c r="Z46" s="78"/>
       <c r="AA46" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="94"/>
       <c r="B47" s="60"/>
       <c r="C47" s="59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D47" s="59"/>
       <c r="E47" s="74"/>
       <c r="F47" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G47" s="92"/>
       <c r="H47" s="75"/>
       <c r="I47" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J47" s="75"/>
       <c r="K47" s="74"/>
       <c r="L47" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M47" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N47" s="92"/>
       <c r="O47" s="75"/>
@@ -9965,7 +9965,7 @@
       <c r="Q47" s="92"/>
       <c r="R47" s="92"/>
       <c r="S47" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T47" s="78"/>
       <c r="U47" s="78"/>
@@ -9975,32 +9975,32 @@
       <c r="Y47" s="78"/>
       <c r="Z47" s="78"/>
       <c r="AA47" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="48" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="94"/>
       <c r="B48" s="82"/>
       <c r="C48" s="81" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D48" s="81"/>
       <c r="E48" s="74"/>
       <c r="F48" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G48" s="92"/>
       <c r="H48" s="75"/>
       <c r="I48" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J48" s="75"/>
       <c r="K48" s="74"/>
       <c r="L48" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M48" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N48" s="92"/>
       <c r="O48" s="75"/>
@@ -10009,7 +10009,7 @@
       <c r="R48" s="92"/>
       <c r="S48" s="78"/>
       <c r="T48" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U48" s="78"/>
       <c r="V48" s="78"/>
@@ -10018,32 +10018,32 @@
       <c r="Y48" s="78"/>
       <c r="Z48" s="78"/>
       <c r="AA48" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="94"/>
       <c r="B49" s="94"/>
       <c r="C49" s="93" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D49" s="93"/>
       <c r="E49" s="74"/>
       <c r="F49" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G49" s="92"/>
       <c r="H49" s="75"/>
       <c r="I49" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J49" s="75"/>
       <c r="K49" s="74"/>
       <c r="L49" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M49" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N49" s="92"/>
       <c r="O49" s="75"/>
@@ -10052,7 +10052,7 @@
       <c r="R49" s="92"/>
       <c r="S49" s="78"/>
       <c r="T49" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U49" s="78"/>
       <c r="V49" s="78"/>
@@ -10061,32 +10061,32 @@
       <c r="Y49" s="78"/>
       <c r="Z49" s="78"/>
       <c r="AA49" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="94"/>
       <c r="B50" s="82"/>
       <c r="C50" s="81" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D50" s="81"/>
       <c r="E50" s="74"/>
       <c r="F50" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G50" s="92"/>
       <c r="H50" s="75"/>
       <c r="I50" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J50" s="75"/>
       <c r="K50" s="74"/>
       <c r="L50" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M50" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N50" s="92"/>
       <c r="O50" s="75"/>
@@ -10095,7 +10095,7 @@
       <c r="R50" s="92"/>
       <c r="S50" s="78"/>
       <c r="T50" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U50" s="78"/>
       <c r="V50" s="78"/>
@@ -10104,32 +10104,32 @@
       <c r="Y50" s="78"/>
       <c r="Z50" s="78"/>
       <c r="AA50" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="51" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="94"/>
       <c r="B51" s="82"/>
       <c r="C51" s="81" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D51" s="81"/>
       <c r="E51" s="74"/>
       <c r="F51" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G51" s="92"/>
       <c r="H51" s="75"/>
       <c r="I51" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J51" s="75"/>
       <c r="K51" s="74"/>
       <c r="L51" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M51" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N51" s="92"/>
       <c r="O51" s="75"/>
@@ -10138,7 +10138,7 @@
       <c r="R51" s="92"/>
       <c r="S51" s="78"/>
       <c r="T51" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U51" s="78"/>
       <c r="V51" s="78"/>
@@ -10147,32 +10147,32 @@
       <c r="Y51" s="78"/>
       <c r="Z51" s="78"/>
       <c r="AA51" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="52" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="94"/>
       <c r="B52" s="89"/>
       <c r="C52" s="88" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D52" s="88"/>
       <c r="E52" s="74"/>
       <c r="F52" s="101"/>
       <c r="G52" s="92"/>
       <c r="H52" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I52" s="74"/>
       <c r="J52" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K52" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L52" s="75"/>
       <c r="M52" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N52" s="92"/>
       <c r="O52" s="75"/>
@@ -10187,35 +10187,35 @@
       <c r="X52" s="78"/>
       <c r="Y52" s="78"/>
       <c r="Z52" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA52" s="63" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="53" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="94"/>
       <c r="B53" s="89"/>
       <c r="C53" s="88" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D53" s="88"/>
       <c r="E53" s="74"/>
       <c r="F53" s="101"/>
       <c r="G53" s="92"/>
       <c r="H53" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I53" s="74"/>
       <c r="J53" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K53" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L53" s="75"/>
       <c r="M53" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N53" s="92"/>
       <c r="O53" s="75"/>
@@ -10230,10 +10230,10 @@
       <c r="X53" s="78"/>
       <c r="Y53" s="78"/>
       <c r="Z53" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA53" s="63" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="54" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -10268,7 +10268,7 @@
     <row r="55" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49"/>
       <c r="B55" s="49" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C55" s="93"/>
       <c r="D55" s="93"/>
@@ -10300,29 +10300,29 @@
       <c r="A56" s="94"/>
       <c r="B56" s="89"/>
       <c r="C56" s="88" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D56" s="88"/>
       <c r="E56" s="74"/>
       <c r="F56" s="101"/>
       <c r="G56" s="92"/>
       <c r="H56" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I56" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J56" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K56" s="74"/>
       <c r="L56" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M56" s="74"/>
       <c r="N56" s="92"/>
       <c r="O56" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P56" s="92"/>
       <c r="Q56" s="92"/>
@@ -10335,39 +10335,39 @@
       <c r="X56" s="78"/>
       <c r="Y56" s="78"/>
       <c r="Z56" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA56" s="63" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="57" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="94"/>
       <c r="B57" s="89"/>
       <c r="C57" s="88" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D57" s="88"/>
       <c r="E57" s="74"/>
       <c r="F57" s="101"/>
       <c r="G57" s="92"/>
       <c r="H57" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I57" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J57" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K57" s="74"/>
       <c r="L57" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M57" s="74"/>
       <c r="N57" s="92"/>
       <c r="O57" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P57" s="92"/>
       <c r="Q57" s="92"/>
@@ -10380,39 +10380,39 @@
       <c r="X57" s="78"/>
       <c r="Y57" s="78"/>
       <c r="Z57" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA57" s="63" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="58" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="94"/>
       <c r="B58" s="89"/>
       <c r="C58" s="88" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D58" s="88"/>
       <c r="E58" s="74"/>
       <c r="F58" s="101"/>
       <c r="G58" s="92"/>
       <c r="H58" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I58" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J58" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K58" s="74"/>
       <c r="L58" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M58" s="74"/>
       <c r="N58" s="92"/>
       <c r="O58" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P58" s="92"/>
       <c r="Q58" s="92"/>
@@ -10425,39 +10425,39 @@
       <c r="X58" s="78"/>
       <c r="Y58" s="78"/>
       <c r="Z58" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA58" s="63" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="94"/>
       <c r="B59" s="89"/>
       <c r="C59" s="88" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D59" s="88"/>
       <c r="E59" s="74"/>
       <c r="F59" s="101"/>
       <c r="G59" s="92"/>
       <c r="H59" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I59" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J59" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K59" s="74"/>
       <c r="L59" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M59" s="74"/>
       <c r="N59" s="92"/>
       <c r="O59" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P59" s="92"/>
       <c r="Q59" s="92"/>
@@ -10470,39 +10470,39 @@
       <c r="X59" s="78"/>
       <c r="Y59" s="78"/>
       <c r="Z59" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA59" s="63" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="60" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="94"/>
       <c r="B60" s="89"/>
       <c r="C60" s="88" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D60" s="88"/>
       <c r="E60" s="74"/>
       <c r="F60" s="101"/>
       <c r="G60" s="92"/>
       <c r="H60" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I60" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J60" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K60" s="74"/>
       <c r="L60" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M60" s="74"/>
       <c r="N60" s="92"/>
       <c r="O60" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P60" s="92"/>
       <c r="Q60" s="92"/>
@@ -10515,39 +10515,39 @@
       <c r="X60" s="78"/>
       <c r="Y60" s="78"/>
       <c r="Z60" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA60" s="63" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="61" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="94"/>
       <c r="B61" s="89"/>
       <c r="C61" s="88" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D61" s="88"/>
       <c r="E61" s="74"/>
       <c r="F61" s="101"/>
       <c r="G61" s="92"/>
       <c r="H61" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I61" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J61" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K61" s="74"/>
       <c r="L61" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M61" s="74"/>
       <c r="N61" s="92"/>
       <c r="O61" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P61" s="92"/>
       <c r="Q61" s="92"/>
@@ -10560,39 +10560,39 @@
       <c r="X61" s="78"/>
       <c r="Y61" s="78"/>
       <c r="Z61" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA61" s="63" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="62" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="94"/>
       <c r="B62" s="89"/>
       <c r="C62" s="88" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D62" s="88"/>
       <c r="E62" s="74"/>
       <c r="F62" s="101"/>
       <c r="G62" s="92"/>
       <c r="H62" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I62" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J62" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K62" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L62" s="75"/>
       <c r="M62" s="74"/>
       <c r="N62" s="92"/>
       <c r="O62" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P62" s="92"/>
       <c r="Q62" s="92"/>
@@ -10605,39 +10605,39 @@
       <c r="X62" s="78"/>
       <c r="Y62" s="78"/>
       <c r="Z62" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA62" s="63" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="63" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="94"/>
       <c r="B63" s="89"/>
       <c r="C63" s="88" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D63" s="88"/>
       <c r="E63" s="74"/>
       <c r="F63" s="101"/>
       <c r="G63" s="92"/>
       <c r="H63" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I63" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J63" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K63" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L63" s="75"/>
       <c r="M63" s="74"/>
       <c r="N63" s="92"/>
       <c r="O63" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P63" s="92"/>
       <c r="Q63" s="92"/>
@@ -10650,35 +10650,35 @@
       <c r="X63" s="78"/>
       <c r="Y63" s="78"/>
       <c r="Z63" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA63" s="63" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="64" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="94"/>
       <c r="B64" s="94"/>
       <c r="C64" s="93" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D64" s="93"/>
       <c r="E64" s="74"/>
       <c r="F64" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G64" s="92"/>
       <c r="H64" s="75"/>
       <c r="I64" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J64" s="75"/>
       <c r="K64" s="74"/>
       <c r="L64" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M64" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N64" s="92"/>
       <c r="O64" s="75"/>
@@ -10686,44 +10686,44 @@
       <c r="Q64" s="92"/>
       <c r="R64" s="92"/>
       <c r="S64" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T64" s="78"/>
       <c r="U64" s="78"/>
       <c r="V64" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W64" s="78"/>
       <c r="X64" s="78"/>
       <c r="Y64" s="78"/>
       <c r="Z64" s="78"/>
       <c r="AA64" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="94"/>
       <c r="B65" s="94"/>
       <c r="C65" s="93" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D65" s="93"/>
       <c r="E65" s="74"/>
       <c r="F65" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G65" s="92"/>
       <c r="H65" s="75"/>
       <c r="I65" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J65" s="75"/>
       <c r="K65" s="74"/>
       <c r="L65" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M65" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N65" s="92"/>
       <c r="O65" s="75"/>
@@ -10731,44 +10731,44 @@
       <c r="Q65" s="92"/>
       <c r="R65" s="92"/>
       <c r="S65" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T65" s="78"/>
       <c r="U65" s="78"/>
       <c r="V65" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W65" s="78"/>
       <c r="X65" s="78"/>
       <c r="Y65" s="78"/>
       <c r="Z65" s="78"/>
       <c r="AA65" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="66" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="94"/>
       <c r="B66" s="94"/>
       <c r="C66" s="93" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D66" s="93"/>
       <c r="E66" s="74"/>
       <c r="F66" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G66" s="92"/>
       <c r="H66" s="75"/>
       <c r="I66" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J66" s="75"/>
       <c r="K66" s="74"/>
       <c r="L66" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M66" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N66" s="92"/>
       <c r="O66" s="75"/>
@@ -10776,44 +10776,44 @@
       <c r="Q66" s="92"/>
       <c r="R66" s="92"/>
       <c r="S66" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T66" s="78"/>
       <c r="U66" s="78"/>
       <c r="V66" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W66" s="78"/>
       <c r="X66" s="78"/>
       <c r="Y66" s="78"/>
       <c r="Z66" s="78"/>
       <c r="AA66" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="94"/>
       <c r="B67" s="94"/>
       <c r="C67" s="93" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D67" s="93"/>
       <c r="E67" s="74"/>
       <c r="F67" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G67" s="92"/>
       <c r="H67" s="75"/>
       <c r="I67" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J67" s="75"/>
       <c r="K67" s="74"/>
       <c r="L67" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M67" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N67" s="92"/>
       <c r="O67" s="75"/>
@@ -10821,44 +10821,44 @@
       <c r="Q67" s="92"/>
       <c r="R67" s="92"/>
       <c r="S67" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T67" s="78"/>
       <c r="U67" s="78"/>
       <c r="V67" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W67" s="78"/>
       <c r="X67" s="78"/>
       <c r="Y67" s="78"/>
       <c r="Z67" s="78"/>
       <c r="AA67" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="68" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="94"/>
       <c r="B68" s="94"/>
       <c r="C68" s="93" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D68" s="93"/>
       <c r="E68" s="74"/>
       <c r="F68" s="101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G68" s="92"/>
       <c r="H68" s="75"/>
       <c r="I68" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J68" s="75"/>
       <c r="K68" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L68" s="75"/>
       <c r="M68" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N68" s="92"/>
       <c r="O68" s="75"/>
@@ -10866,19 +10866,19 @@
       <c r="Q68" s="92"/>
       <c r="R68" s="92"/>
       <c r="S68" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T68" s="78"/>
       <c r="U68" s="78"/>
       <c r="V68" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W68" s="78"/>
       <c r="X68" s="78"/>
       <c r="Y68" s="78"/>
       <c r="Z68" s="78"/>
       <c r="AA68" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="69" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11209,14 +11209,14 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
@@ -11225,222 +11225,222 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="106" t="s">
-        <v>212</v>
-      </c>
-      <c r="E3" s="107"/>
+      <c r="D3" s="113" t="s">
+        <v>211</v>
+      </c>
+      <c r="E3" s="111"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="68" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="65" t="s">
+        <v>209</v>
+      </c>
+      <c r="E4" s="66" t="s">
         <v>210</v>
       </c>
-      <c r="E4" s="66" t="s">
-        <v>211</v>
-      </c>
       <c r="F4" s="72" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60"/>
       <c r="B5" s="59" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60"/>
       <c r="B6" s="59" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E6" s="75"/>
       <c r="F6" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>
       <c r="B7" s="59" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E7" s="75"/>
       <c r="F7" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
       <c r="B8" s="59" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E8" s="75"/>
       <c r="F8" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60"/>
       <c r="B9" s="59" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C9" s="59"/>
       <c r="D9" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E9" s="75"/>
       <c r="F9" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="60"/>
       <c r="B10" s="59" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E10" s="75"/>
       <c r="F10" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="60"/>
       <c r="B11" s="59" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E11" s="75"/>
       <c r="F11" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60"/>
       <c r="B12" s="59" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E12" s="75"/>
       <c r="F12" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="59" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E13" s="75"/>
       <c r="F13" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E14" s="75"/>
       <c r="F14" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
       <c r="B15" s="81" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E15" s="75"/>
       <c r="F15" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
       <c r="B16" s="81" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C16" s="59"/>
       <c r="D16" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E16" s="75"/>
       <c r="F16" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="60"/>
       <c r="B17" s="59" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E17" s="75"/>
       <c r="F17" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="60"/>
       <c r="B18" s="59" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E18" s="75"/>
       <c r="F18" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11488,32 +11488,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="104"/>
-      <c r="B24" s="104"/>
-      <c r="C24" s="104"/>
-      <c r="D24" s="104"/>
-      <c r="E24" s="104"/>
+      <c r="A24" s="108"/>
+      <c r="B24" s="108"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="108"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="104"/>
-      <c r="B25" s="104"/>
-      <c r="C25" s="104"/>
-      <c r="D25" s="104"/>
-      <c r="E25" s="104"/>
+      <c r="A25" s="108"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="108"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="108"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="104"/>
-      <c r="B26" s="104"/>
-      <c r="C26" s="104"/>
-      <c r="D26" s="104"/>
-      <c r="E26" s="104"/>
+      <c r="A26" s="108"/>
+      <c r="B26" s="108"/>
+      <c r="C26" s="108"/>
+      <c r="D26" s="108"/>
+      <c r="E26" s="108"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="104"/>
-      <c r="B27" s="104"/>
-      <c r="C27" s="104"/>
-      <c r="D27" s="104"/>
-      <c r="E27" s="104"/>
+      <c r="A27" s="108"/>
+      <c r="B27" s="108"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="108"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -11599,11 +11599,11 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11641,19 +11641,19 @@
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K3" s="39"/>
       <c r="L3" s="39" t="s">
@@ -11661,7 +11661,7 @@
       </c>
       <c r="M3" s="39"/>
       <c r="N3" s="39" t="s">
-        <v>247</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11675,11 +11675,11 @@
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="58" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I4" s="58"/>
       <c r="J4" s="56" t="s">
@@ -11691,7 +11691,7 @@
       </c>
       <c r="M4" s="56"/>
       <c r="N4" s="56" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
@@ -11705,11 +11705,11 @@
       </c>
       <c r="E5" s="84"/>
       <c r="F5" s="84" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G5" s="84"/>
       <c r="H5" s="84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I5" s="84"/>
       <c r="J5" s="84" t="s">
@@ -11721,7 +11721,7 @@
       </c>
       <c r="M5" s="84"/>
       <c r="N5" s="84" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -11731,7 +11731,7 @@
       </c>
       <c r="C6" s="84"/>
       <c r="D6" s="84" t="s">
-        <v>201</v>
+        <v>326</v>
       </c>
       <c r="E6" s="84"/>
       <c r="F6" s="84" t="s">
@@ -11739,7 +11739,7 @@
       </c>
       <c r="G6" s="84"/>
       <c r="H6" s="84" t="s">
-        <v>246</v>
+        <v>327</v>
       </c>
       <c r="I6" s="84"/>
       <c r="J6" s="84" t="s">
@@ -11751,25 +11751,25 @@
       </c>
       <c r="M6" s="84"/>
       <c r="N6" s="84" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="83"/>
       <c r="B7" s="84" t="s">
         <v>186</v>
       </c>
       <c r="C7" s="84"/>
       <c r="D7" s="84" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E7" s="84"/>
       <c r="F7" s="84" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G7" s="84"/>
       <c r="H7" s="84" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I7" s="84"/>
       <c r="J7" s="84" t="s">
@@ -11781,7 +11781,7 @@
       </c>
       <c r="M7" s="84"/>
       <c r="N7" s="84" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -11848,7 +11848,7 @@
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -11858,7 +11858,7 @@
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B13" s="56"/>
       <c r="C13" s="56"/>
@@ -12305,27 +12305,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="104"/>
-      <c r="B17" s="104"/>
-      <c r="C17" s="104"/>
+      <c r="A17" s="108"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="108"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="104"/>
-      <c r="B18" s="104"/>
-      <c r="C18" s="104"/>
+      <c r="A18" s="108"/>
+      <c r="B18" s="108"/>
+      <c r="C18" s="108"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="104"/>
-      <c r="B19" s="104"/>
-      <c r="C19" s="104"/>
+      <c r="A19" s="108"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="108"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -12764,30 +12764,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="109" t="s">
+      <c r="A42" s="117" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="109"/>
-      <c r="C42" s="109"/>
+      <c r="B42" s="117"/>
+      <c r="C42" s="117"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="110" t="s">
+      <c r="A43" s="118" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="110"/>
-      <c r="C43" s="110"/>
+      <c r="B43" s="118"/>
+      <c r="C43" s="118"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="109" t="s">
+      <c r="A44" s="117" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="109"/>
-      <c r="C44" s="109"/>
+      <c r="B44" s="117"/>
+      <c r="C44" s="117"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="104"/>
-      <c r="B45" s="104"/>
-      <c r="C45" s="104"/>
+      <c r="A45" s="108"/>
+      <c r="B45" s="108"/>
+      <c r="C45" s="108"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>

</xml_diff>

<commit_message>
Minor modifications to table on org studies
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -810,9 +810,6 @@
     <t>Key Metaphors</t>
   </si>
   <si>
-    <t>Since all knowledge is filtered by the experience of the observer, all distinctions used to describe reality are arbitrary and semantic in origin.  The organization is an abstraction that is best understood by revealing and comprehending the underlying assumptions used to construct it.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The organization is a machine that management designs, constructs, and maintains to achieve specific goals and objectives.
 The organization is a living organism comprised of systems that perform the functions necessary for its survival. </t>
   </si>
@@ -834,16 +831,6 @@
   </si>
   <si>
     <t>Studies</t>
-  </si>
-  <si>
-    <t>Bureacracy theory
-Administrative theory
-Scientific management</t>
-  </si>
-  <si>
-    <t>Scientific management
-Econometric
-Open systems theory</t>
   </si>
   <si>
     <t>Autopoietic systems theory
@@ -983,10 +970,6 @@
     <t>Table</t>
   </si>
   <si>
-    <t>Human relations management
-Garbage can model</t>
-  </si>
-  <si>
     <t>Patent effectiveness</t>
   </si>
   <si>
@@ -1237,6 +1220,24 @@
   </si>
   <si>
     <t>Models, Theories, and Schools of Thought</t>
+  </si>
+  <si>
+    <t>Scientific management
+Administrative theory
+Econometric
+Open systems theory</t>
+  </si>
+  <si>
+    <t>Bureacracy theory
+Scientific management</t>
+  </si>
+  <si>
+    <t>Administrative theory
+Human relations management
+Garbage can model</t>
+  </si>
+  <si>
+    <t>Since all knowledge is filtered by the experience of the observer, all distinctions used to describe reality are arbitrary and semantic in origin.  The organization is an abstraction that is best understood by revealing the underlying assumptions used to construct it and considering their implications.</t>
   </si>
 </sst>
 </file>
@@ -7426,7 +7427,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7887,7 +7888,7 @@
     </row>
     <row r="2" spans="1:27" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E2" s="61"/>
       <c r="F2" s="61"/>
@@ -7919,26 +7920,26 @@
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
       <c r="E3" s="113" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F3" s="114"/>
       <c r="G3" s="114"/>
       <c r="H3" s="111"/>
       <c r="I3" s="110" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="J3" s="111"/>
       <c r="K3" s="110" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="L3" s="112"/>
       <c r="M3" s="113" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="N3" s="114"/>
       <c r="O3" s="111"/>
       <c r="P3" s="115" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="Q3" s="114"/>
       <c r="R3" s="114"/>
@@ -7955,84 +7956,84 @@
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="104" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="68"/>
       <c r="E4" s="105" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F4" s="107" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="G4" s="62" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="H4" s="106" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="I4" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="J4" s="66" t="s">
         <v>209</v>
       </c>
-      <c r="J4" s="66" t="s">
-        <v>210</v>
-      </c>
       <c r="K4" s="65" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="L4" s="66" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="M4" s="105" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="N4" s="62" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="O4" s="106" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="P4" s="62" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="Q4" s="62" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="R4" s="62" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="S4" s="62" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="T4" s="62" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="U4" s="62" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="V4" s="62" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="W4" s="62" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="X4" s="62" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="Y4" s="62" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="Z4" s="62" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="AA4" s="72" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="49" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C5" s="93"/>
       <c r="D5" s="93"/>
@@ -8064,25 +8065,25 @@
       <c r="A6" s="94"/>
       <c r="B6" s="82"/>
       <c r="C6" s="81" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D6" s="81"/>
       <c r="E6" s="74"/>
       <c r="F6" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G6" s="92"/>
       <c r="H6" s="75"/>
       <c r="I6" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J6" s="75"/>
       <c r="K6" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L6" s="75"/>
       <c r="M6" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N6" s="92"/>
       <c r="O6" s="75"/>
@@ -8091,7 +8092,7 @@
       <c r="R6" s="92"/>
       <c r="S6" s="78"/>
       <c r="T6" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U6" s="78"/>
       <c r="V6" s="78"/>
@@ -8100,32 +8101,32 @@
       <c r="Y6" s="78"/>
       <c r="Z6" s="78"/>
       <c r="AA6" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="94"/>
       <c r="B7" s="82"/>
       <c r="C7" s="93" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D7" s="81"/>
       <c r="E7" s="74"/>
       <c r="F7" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G7" s="92"/>
       <c r="H7" s="75"/>
       <c r="I7" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J7" s="75"/>
       <c r="K7" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L7" s="75"/>
       <c r="M7" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N7" s="92"/>
       <c r="O7" s="75"/>
@@ -8134,7 +8135,7 @@
       <c r="R7" s="92"/>
       <c r="S7" s="78"/>
       <c r="T7" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U7" s="78"/>
       <c r="V7" s="78"/>
@@ -8143,32 +8144,32 @@
       <c r="Y7" s="78"/>
       <c r="Z7" s="78"/>
       <c r="AA7" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="94"/>
       <c r="B8" s="82"/>
       <c r="C8" s="81" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D8" s="81"/>
       <c r="E8" s="74"/>
       <c r="F8" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G8" s="92"/>
       <c r="H8" s="75"/>
       <c r="I8" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J8" s="75"/>
       <c r="K8" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L8" s="75"/>
       <c r="M8" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N8" s="92"/>
       <c r="O8" s="75"/>
@@ -8177,7 +8178,7 @@
       <c r="R8" s="92"/>
       <c r="S8" s="78"/>
       <c r="T8" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U8" s="78"/>
       <c r="V8" s="78"/>
@@ -8186,47 +8187,47 @@
       <c r="Y8" s="78"/>
       <c r="Z8" s="78"/>
       <c r="AA8" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="94"/>
       <c r="B9" s="82"/>
       <c r="C9" s="93" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D9" s="81"/>
       <c r="E9" s="74"/>
       <c r="F9" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G9" s="92"/>
       <c r="H9" s="75"/>
       <c r="I9" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J9" s="75"/>
       <c r="K9" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L9" s="75"/>
       <c r="M9" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N9" s="92"/>
       <c r="O9" s="75"/>
       <c r="P9" s="92"/>
       <c r="Q9" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R9" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S9" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T9" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U9" s="78"/>
       <c r="V9" s="78"/>
@@ -8235,104 +8236,104 @@
       <c r="Y9" s="78"/>
       <c r="Z9" s="78"/>
       <c r="AA9" s="63" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
       <c r="B10" s="30"/>
       <c r="C10" s="32" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="74"/>
       <c r="F10" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G10" s="92"/>
       <c r="H10" s="75"/>
       <c r="I10" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J10" s="75"/>
       <c r="K10" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L10" s="75"/>
       <c r="M10" s="74"/>
       <c r="N10" s="92"/>
       <c r="O10" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P10" s="92"/>
       <c r="Q10" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R10" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S10" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T10" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U10" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="V10" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W10" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="X10" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Y10" s="78"/>
       <c r="Z10" s="78"/>
       <c r="AA10" s="63" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="94"/>
       <c r="B11" s="82"/>
       <c r="C11" s="95" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D11" s="81"/>
       <c r="E11" s="96"/>
       <c r="F11" s="102" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G11" s="98"/>
       <c r="H11" s="97"/>
       <c r="I11" s="96" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J11" s="97"/>
       <c r="K11" s="96" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L11" s="97"/>
       <c r="M11" s="96" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N11" s="98"/>
       <c r="O11" s="97"/>
       <c r="P11" s="98"/>
       <c r="Q11" s="98" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R11" s="98" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S11" s="99" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T11" s="99" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U11" s="99"/>
       <c r="V11" s="99"/>
@@ -8341,7 +8342,7 @@
       <c r="Y11" s="99"/>
       <c r="Z11" s="99"/>
       <c r="AA11" s="100" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -8376,7 +8377,7 @@
     <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="49" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C13" s="93"/>
       <c r="D13" s="93"/>
@@ -8408,241 +8409,241 @@
       <c r="A14" s="94"/>
       <c r="B14" s="30"/>
       <c r="C14" s="32" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="74"/>
       <c r="F14" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G14" s="92"/>
       <c r="H14" s="75"/>
       <c r="I14" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J14" s="75"/>
       <c r="K14" s="74"/>
       <c r="L14" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M14" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N14" s="92"/>
       <c r="O14" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P14" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Q14" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R14" s="92"/>
       <c r="S14" s="78"/>
       <c r="T14" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U14" s="78"/>
       <c r="V14" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W14" s="78"/>
       <c r="X14" s="78"/>
       <c r="Y14" s="78"/>
       <c r="Z14" s="78"/>
       <c r="AA14" s="63" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="94"/>
       <c r="B15" s="30"/>
       <c r="C15" s="32" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="74"/>
       <c r="F15" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G15" s="92"/>
       <c r="H15" s="75"/>
       <c r="I15" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J15" s="75"/>
       <c r="K15" s="74"/>
       <c r="L15" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M15" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N15" s="92"/>
       <c r="O15" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P15" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Q15" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R15" s="92"/>
       <c r="S15" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T15" s="78"/>
       <c r="U15" s="78"/>
       <c r="V15" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W15" s="78"/>
       <c r="X15" s="78"/>
       <c r="Y15" s="78"/>
       <c r="Z15" s="78"/>
       <c r="AA15" s="63" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="94"/>
       <c r="B16" s="82"/>
       <c r="C16" s="81" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D16" s="81"/>
       <c r="E16" s="74"/>
       <c r="F16" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G16" s="92"/>
       <c r="H16" s="75"/>
       <c r="I16" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J16" s="75"/>
       <c r="K16" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L16" s="75"/>
       <c r="M16" s="74"/>
       <c r="N16" s="92"/>
       <c r="O16" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P16" s="92"/>
       <c r="Q16" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R16" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S16" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T16" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U16" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="V16" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W16" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="X16" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Y16" s="78"/>
       <c r="Z16" s="78"/>
       <c r="AA16" s="63" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="94"/>
       <c r="B17" s="82"/>
       <c r="C17" s="81" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D17" s="81"/>
       <c r="E17" s="74"/>
       <c r="F17" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G17" s="92"/>
       <c r="H17" s="75"/>
       <c r="I17" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J17" s="75"/>
       <c r="K17" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L17" s="75"/>
       <c r="M17" s="74"/>
       <c r="N17" s="92"/>
       <c r="O17" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P17" s="92"/>
       <c r="Q17" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R17" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S17" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T17" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U17" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="V17" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W17" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="X17" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Y17" s="78"/>
       <c r="Z17" s="78"/>
       <c r="AA17" s="63" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="94"/>
       <c r="B18" s="60"/>
       <c r="C18" s="59" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D18" s="59"/>
       <c r="E18" s="74"/>
       <c r="F18" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G18" s="92"/>
       <c r="H18" s="75"/>
       <c r="I18" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J18" s="75"/>
       <c r="K18" s="74"/>
       <c r="L18" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M18" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N18" s="92"/>
       <c r="O18" s="75"/>
@@ -8653,39 +8654,39 @@
       <c r="T18" s="78"/>
       <c r="U18" s="78"/>
       <c r="V18" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W18" s="78"/>
       <c r="X18" s="78"/>
       <c r="Y18" s="78"/>
       <c r="Z18" s="78"/>
       <c r="AA18" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="94"/>
       <c r="B19" s="30"/>
       <c r="C19" s="32" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="74"/>
       <c r="F19" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G19" s="92"/>
       <c r="H19" s="75"/>
       <c r="I19" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J19" s="75"/>
       <c r="K19" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L19" s="75"/>
       <c r="M19" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N19" s="92"/>
       <c r="O19" s="75"/>
@@ -8693,7 +8694,7 @@
       <c r="Q19" s="92"/>
       <c r="R19" s="92"/>
       <c r="S19" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T19" s="78"/>
       <c r="U19" s="78"/>
@@ -8703,32 +8704,32 @@
       <c r="Y19" s="78"/>
       <c r="Z19" s="78"/>
       <c r="AA19" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="94"/>
       <c r="B20" s="30"/>
       <c r="C20" s="32" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="74"/>
       <c r="F20" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G20" s="92"/>
       <c r="H20" s="75"/>
       <c r="I20" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J20" s="75"/>
       <c r="K20" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L20" s="75"/>
       <c r="M20" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N20" s="92"/>
       <c r="O20" s="75"/>
@@ -8736,7 +8737,7 @@
       <c r="Q20" s="92"/>
       <c r="R20" s="92"/>
       <c r="S20" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T20" s="78"/>
       <c r="U20" s="78"/>
@@ -8746,32 +8747,32 @@
       <c r="Y20" s="78"/>
       <c r="Z20" s="78"/>
       <c r="AA20" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="94"/>
       <c r="B21" s="30"/>
       <c r="C21" s="32" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="74"/>
       <c r="F21" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G21" s="92"/>
       <c r="H21" s="75"/>
       <c r="I21" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J21" s="75"/>
       <c r="K21" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L21" s="75"/>
       <c r="M21" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N21" s="92"/>
       <c r="O21" s="75"/>
@@ -8779,7 +8780,7 @@
       <c r="Q21" s="92"/>
       <c r="R21" s="92"/>
       <c r="S21" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T21" s="78"/>
       <c r="U21" s="78"/>
@@ -8789,349 +8790,349 @@
       <c r="Y21" s="78"/>
       <c r="Z21" s="78"/>
       <c r="AA21" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="94"/>
       <c r="B22" s="82"/>
       <c r="C22" s="81" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D22" s="81"/>
       <c r="E22" s="74"/>
       <c r="F22" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G22" s="92"/>
       <c r="H22" s="75"/>
       <c r="I22" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J22" s="75"/>
       <c r="K22" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L22" s="75"/>
       <c r="M22" s="74"/>
       <c r="N22" s="92"/>
       <c r="O22" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P22" s="92"/>
       <c r="Q22" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R22" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S22" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T22" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U22" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="V22" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W22" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="X22" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Y22" s="78"/>
       <c r="Z22" s="78"/>
       <c r="AA22" s="63" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="94"/>
       <c r="B23" s="82"/>
       <c r="C23" s="81" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D23" s="81"/>
       <c r="E23" s="74"/>
       <c r="F23" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G23" s="92"/>
       <c r="H23" s="75"/>
       <c r="I23" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J23" s="75"/>
       <c r="K23" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L23" s="75"/>
       <c r="M23" s="74"/>
       <c r="N23" s="92"/>
       <c r="O23" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P23" s="92"/>
       <c r="Q23" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R23" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S23" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T23" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U23" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="V23" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W23" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="X23" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Y23" s="78"/>
       <c r="Z23" s="78"/>
       <c r="AA23" s="63" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="94"/>
       <c r="B24" s="30"/>
       <c r="C24" s="32" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="74"/>
       <c r="F24" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G24" s="92"/>
       <c r="H24" s="75"/>
       <c r="I24" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J24" s="75"/>
       <c r="K24" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L24" s="75"/>
       <c r="M24" s="74"/>
       <c r="N24" s="92"/>
       <c r="O24" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P24" s="92"/>
       <c r="Q24" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R24" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S24" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T24" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U24" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="V24" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W24" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="X24" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Y24" s="78"/>
       <c r="Z24" s="78"/>
       <c r="AA24" s="63" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="94"/>
       <c r="B25" s="30"/>
       <c r="C25" s="32" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="74"/>
       <c r="F25" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G25" s="92"/>
       <c r="H25" s="75"/>
       <c r="I25" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J25" s="75"/>
       <c r="K25" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L25" s="75"/>
       <c r="M25" s="74"/>
       <c r="N25" s="92"/>
       <c r="O25" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P25" s="92"/>
       <c r="Q25" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R25" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S25" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T25" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U25" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="V25" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W25" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="X25" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Y25" s="78"/>
       <c r="Z25" s="78"/>
       <c r="AA25" s="63" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="94"/>
       <c r="B26" s="82"/>
       <c r="C26" s="81" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D26" s="81"/>
       <c r="E26" s="74"/>
       <c r="F26" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G26" s="92"/>
       <c r="H26" s="75"/>
       <c r="I26" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J26" s="75"/>
       <c r="K26" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L26" s="75"/>
       <c r="M26" s="74"/>
       <c r="N26" s="92"/>
       <c r="O26" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P26" s="92"/>
       <c r="Q26" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R26" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S26" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T26" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U26" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="V26" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W26" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="X26" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Y26" s="78"/>
       <c r="Z26" s="78"/>
       <c r="AA26" s="63" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="94"/>
       <c r="B27" s="82"/>
       <c r="C27" s="81" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D27" s="81"/>
       <c r="E27" s="74"/>
       <c r="F27" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G27" s="92"/>
       <c r="H27" s="75"/>
       <c r="I27" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J27" s="75"/>
       <c r="K27" s="74"/>
       <c r="L27" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M27" s="74"/>
       <c r="N27" s="92"/>
       <c r="O27" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P27" s="92"/>
       <c r="Q27" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R27" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S27" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T27" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U27" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="V27" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W27" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="X27" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Y27" s="78"/>
       <c r="Z27" s="78"/>
       <c r="AA27" s="63" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9166,7 +9167,7 @@
     <row r="29" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="94"/>
       <c r="B29" s="31" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C29" s="93"/>
       <c r="D29" s="93"/>
@@ -9198,40 +9199,40 @@
       <c r="A30" s="94"/>
       <c r="B30" s="82"/>
       <c r="C30" s="81" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D30" s="81"/>
       <c r="E30" s="74"/>
       <c r="F30" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G30" s="92"/>
       <c r="H30" s="75"/>
       <c r="I30" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J30" s="75"/>
       <c r="K30" s="74"/>
       <c r="L30" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M30" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N30" s="92"/>
       <c r="O30" s="75"/>
       <c r="P30" s="92"/>
       <c r="Q30" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R30" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S30" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T30" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U30" s="78"/>
       <c r="V30" s="78"/>
@@ -9240,32 +9241,32 @@
       <c r="Y30" s="78"/>
       <c r="Z30" s="78"/>
       <c r="AA30" s="63" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="94"/>
       <c r="B31" s="94"/>
       <c r="C31" s="93" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D31" s="93"/>
       <c r="E31" s="74"/>
       <c r="F31" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G31" s="92"/>
       <c r="H31" s="75"/>
       <c r="I31" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J31" s="75"/>
       <c r="K31" s="74"/>
       <c r="L31" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M31" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N31" s="92"/>
       <c r="O31" s="75"/>
@@ -9274,7 +9275,7 @@
       <c r="R31" s="92"/>
       <c r="S31" s="78"/>
       <c r="T31" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U31" s="78"/>
       <c r="V31" s="78"/>
@@ -9283,32 +9284,32 @@
       <c r="Y31" s="78"/>
       <c r="Z31" s="78"/>
       <c r="AA31" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="94"/>
       <c r="B32" s="94"/>
       <c r="C32" s="93" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D32" s="93"/>
       <c r="E32" s="74"/>
       <c r="F32" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G32" s="92"/>
       <c r="H32" s="75"/>
       <c r="I32" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J32" s="75"/>
       <c r="K32" s="74"/>
       <c r="L32" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M32" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N32" s="92"/>
       <c r="O32" s="75"/>
@@ -9317,7 +9318,7 @@
       <c r="R32" s="92"/>
       <c r="S32" s="78"/>
       <c r="T32" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U32" s="78"/>
       <c r="V32" s="78"/>
@@ -9326,38 +9327,38 @@
       <c r="Y32" s="78"/>
       <c r="Z32" s="78"/>
       <c r="AA32" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="94"/>
       <c r="B33" s="94"/>
       <c r="C33" s="93" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D33" s="93"/>
       <c r="E33" s="74"/>
       <c r="F33" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G33" s="92"/>
       <c r="H33" s="75"/>
       <c r="I33" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J33" s="75"/>
       <c r="K33" s="74"/>
       <c r="L33" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M33" s="74"/>
       <c r="N33" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="O33" s="75"/>
       <c r="P33" s="92"/>
       <c r="Q33" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R33" s="92"/>
       <c r="S33" s="78"/>
@@ -9369,7 +9370,7 @@
       <c r="Y33" s="78"/>
       <c r="Z33" s="78"/>
       <c r="AA33" s="63" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="34" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9404,7 +9405,7 @@
     <row r="35" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
       <c r="B35" s="49" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C35" s="93"/>
       <c r="D35" s="93"/>
@@ -9436,25 +9437,25 @@
       <c r="A36" s="94"/>
       <c r="B36" s="30"/>
       <c r="C36" s="32" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D36" s="32"/>
       <c r="E36" s="74"/>
       <c r="F36" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G36" s="92"/>
       <c r="H36" s="75"/>
       <c r="I36" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J36" s="75"/>
       <c r="K36" s="74"/>
       <c r="L36" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M36" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N36" s="92"/>
       <c r="O36" s="75"/>
@@ -9462,7 +9463,7 @@
       <c r="Q36" s="92"/>
       <c r="R36" s="92"/>
       <c r="S36" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T36" s="78"/>
       <c r="U36" s="78"/>
@@ -9472,32 +9473,32 @@
       <c r="Y36" s="78"/>
       <c r="Z36" s="78"/>
       <c r="AA36" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="94"/>
       <c r="B37" s="30"/>
       <c r="C37" s="32" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D37" s="32"/>
       <c r="E37" s="74"/>
       <c r="F37" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G37" s="92"/>
       <c r="H37" s="75"/>
       <c r="I37" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J37" s="75"/>
       <c r="K37" s="74"/>
       <c r="L37" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M37" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N37" s="92"/>
       <c r="O37" s="75"/>
@@ -9508,39 +9509,39 @@
       <c r="T37" s="78"/>
       <c r="U37" s="78"/>
       <c r="V37" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W37" s="78"/>
       <c r="X37" s="78"/>
       <c r="Y37" s="78"/>
       <c r="Z37" s="78"/>
       <c r="AA37" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="94"/>
       <c r="B38" s="94"/>
       <c r="C38" s="93" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D38" s="93"/>
       <c r="E38" s="74"/>
       <c r="F38" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G38" s="92"/>
       <c r="H38" s="75"/>
       <c r="I38" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J38" s="75"/>
       <c r="K38" s="74"/>
       <c r="L38" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M38" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N38" s="92"/>
       <c r="O38" s="75"/>
@@ -9548,7 +9549,7 @@
       <c r="Q38" s="92"/>
       <c r="R38" s="92"/>
       <c r="S38" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T38" s="78"/>
       <c r="U38" s="78"/>
@@ -9558,32 +9559,32 @@
       <c r="Y38" s="78"/>
       <c r="Z38" s="78"/>
       <c r="AA38" s="63" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="39" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="94"/>
       <c r="B39" s="94"/>
       <c r="C39" s="93" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D39" s="93"/>
       <c r="E39" s="74"/>
       <c r="F39" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G39" s="92"/>
       <c r="H39" s="75"/>
       <c r="I39" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J39" s="75"/>
       <c r="K39" s="74"/>
       <c r="L39" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M39" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N39" s="92"/>
       <c r="O39" s="75"/>
@@ -9591,44 +9592,44 @@
       <c r="Q39" s="92"/>
       <c r="R39" s="92"/>
       <c r="S39" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T39" s="78"/>
       <c r="U39" s="78"/>
       <c r="V39" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W39" s="78"/>
       <c r="X39" s="78"/>
       <c r="Y39" s="78"/>
       <c r="Z39" s="78"/>
       <c r="AA39" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="94"/>
       <c r="B40" s="94"/>
       <c r="C40" s="93" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D40" s="93"/>
       <c r="E40" s="74"/>
       <c r="F40" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G40" s="92"/>
       <c r="H40" s="75"/>
       <c r="I40" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J40" s="75"/>
       <c r="K40" s="74"/>
       <c r="L40" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M40" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N40" s="92"/>
       <c r="O40" s="75"/>
@@ -9636,93 +9637,93 @@
       <c r="Q40" s="92"/>
       <c r="R40" s="92"/>
       <c r="S40" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T40" s="78"/>
       <c r="U40" s="78"/>
       <c r="V40" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W40" s="78"/>
       <c r="X40" s="78"/>
       <c r="Y40" s="78"/>
       <c r="Z40" s="78"/>
       <c r="AA40" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="94"/>
       <c r="B41" s="94"/>
       <c r="C41" s="93" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D41" s="93"/>
       <c r="E41" s="74"/>
       <c r="F41" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G41" s="92"/>
       <c r="H41" s="75"/>
       <c r="I41" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J41" s="75"/>
       <c r="K41" s="74"/>
       <c r="L41" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M41" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N41" s="92"/>
       <c r="O41" s="75"/>
       <c r="P41" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Q41" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R41" s="92"/>
       <c r="S41" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T41" s="78"/>
       <c r="U41" s="78"/>
       <c r="V41" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W41" s="78"/>
       <c r="X41" s="78"/>
       <c r="Y41" s="78"/>
       <c r="Z41" s="78"/>
       <c r="AA41" s="63" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="42" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="94"/>
       <c r="B42" s="94"/>
       <c r="C42" s="93" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D42" s="93"/>
       <c r="E42" s="74"/>
       <c r="F42" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G42" s="92"/>
       <c r="H42" s="75"/>
       <c r="I42" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J42" s="75"/>
       <c r="K42" s="74"/>
       <c r="L42" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M42" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N42" s="92"/>
       <c r="O42" s="75"/>
@@ -9731,7 +9732,7 @@
       <c r="R42" s="92"/>
       <c r="S42" s="78"/>
       <c r="T42" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U42" s="78"/>
       <c r="V42" s="78"/>
@@ -9740,32 +9741,32 @@
       <c r="Y42" s="78"/>
       <c r="Z42" s="78"/>
       <c r="AA42" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="43" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="94"/>
       <c r="B43" s="94"/>
       <c r="C43" s="93" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D43" s="93"/>
       <c r="E43" s="74"/>
       <c r="F43" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G43" s="92"/>
       <c r="H43" s="75"/>
       <c r="I43" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J43" s="75"/>
       <c r="K43" s="74"/>
       <c r="L43" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M43" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N43" s="92"/>
       <c r="O43" s="75"/>
@@ -9773,44 +9774,44 @@
       <c r="Q43" s="92"/>
       <c r="R43" s="92"/>
       <c r="S43" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T43" s="78"/>
       <c r="U43" s="78"/>
       <c r="V43" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W43" s="78"/>
       <c r="X43" s="78"/>
       <c r="Y43" s="78"/>
       <c r="Z43" s="78"/>
       <c r="AA43" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="94"/>
       <c r="B44" s="94"/>
       <c r="C44" s="93" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D44" s="93"/>
       <c r="E44" s="74"/>
       <c r="F44" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G44" s="92"/>
       <c r="H44" s="75"/>
       <c r="I44" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J44" s="75"/>
       <c r="K44" s="74"/>
       <c r="L44" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M44" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N44" s="92"/>
       <c r="O44" s="75"/>
@@ -9818,101 +9819,101 @@
       <c r="Q44" s="92"/>
       <c r="R44" s="92"/>
       <c r="S44" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T44" s="78"/>
       <c r="U44" s="78"/>
       <c r="V44" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W44" s="78"/>
       <c r="X44" s="78"/>
       <c r="Y44" s="78"/>
       <c r="Z44" s="78"/>
       <c r="AA44" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="45" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="94"/>
       <c r="B45" s="82"/>
       <c r="C45" s="81" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D45" s="81"/>
       <c r="E45" s="74"/>
       <c r="F45" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G45" s="92"/>
       <c r="H45" s="75"/>
       <c r="I45" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J45" s="75"/>
       <c r="K45" s="74"/>
       <c r="L45" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M45" s="74"/>
       <c r="N45" s="92"/>
       <c r="O45" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P45" s="92"/>
       <c r="Q45" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R45" s="92" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S45" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T45" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U45" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="V45" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W45" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="X45" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Y45" s="78"/>
       <c r="Z45" s="78"/>
       <c r="AA45" s="63" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="94"/>
       <c r="B46" s="60"/>
       <c r="C46" s="59" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D46" s="59"/>
       <c r="E46" s="74"/>
       <c r="F46" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G46" s="92"/>
       <c r="H46" s="75"/>
       <c r="I46" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J46" s="75"/>
       <c r="K46" s="74"/>
       <c r="L46" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M46" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N46" s="92"/>
       <c r="O46" s="75"/>
@@ -9920,44 +9921,44 @@
       <c r="Q46" s="92"/>
       <c r="R46" s="92"/>
       <c r="S46" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T46" s="78"/>
       <c r="U46" s="78"/>
       <c r="V46" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W46" s="78"/>
       <c r="X46" s="78"/>
       <c r="Y46" s="78"/>
       <c r="Z46" s="78"/>
       <c r="AA46" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="94"/>
       <c r="B47" s="60"/>
       <c r="C47" s="59" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D47" s="59"/>
       <c r="E47" s="74"/>
       <c r="F47" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G47" s="92"/>
       <c r="H47" s="75"/>
       <c r="I47" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J47" s="75"/>
       <c r="K47" s="74"/>
       <c r="L47" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M47" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N47" s="92"/>
       <c r="O47" s="75"/>
@@ -9965,7 +9966,7 @@
       <c r="Q47" s="92"/>
       <c r="R47" s="92"/>
       <c r="S47" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T47" s="78"/>
       <c r="U47" s="78"/>
@@ -9975,32 +9976,32 @@
       <c r="Y47" s="78"/>
       <c r="Z47" s="78"/>
       <c r="AA47" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="94"/>
       <c r="B48" s="82"/>
       <c r="C48" s="81" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D48" s="81"/>
       <c r="E48" s="74"/>
       <c r="F48" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G48" s="92"/>
       <c r="H48" s="75"/>
       <c r="I48" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J48" s="75"/>
       <c r="K48" s="74"/>
       <c r="L48" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M48" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N48" s="92"/>
       <c r="O48" s="75"/>
@@ -10009,7 +10010,7 @@
       <c r="R48" s="92"/>
       <c r="S48" s="78"/>
       <c r="T48" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U48" s="78"/>
       <c r="V48" s="78"/>
@@ -10018,32 +10019,32 @@
       <c r="Y48" s="78"/>
       <c r="Z48" s="78"/>
       <c r="AA48" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="49" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="94"/>
       <c r="B49" s="94"/>
       <c r="C49" s="93" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D49" s="93"/>
       <c r="E49" s="74"/>
       <c r="F49" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G49" s="92"/>
       <c r="H49" s="75"/>
       <c r="I49" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J49" s="75"/>
       <c r="K49" s="74"/>
       <c r="L49" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M49" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N49" s="92"/>
       <c r="O49" s="75"/>
@@ -10052,7 +10053,7 @@
       <c r="R49" s="92"/>
       <c r="S49" s="78"/>
       <c r="T49" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U49" s="78"/>
       <c r="V49" s="78"/>
@@ -10061,32 +10062,32 @@
       <c r="Y49" s="78"/>
       <c r="Z49" s="78"/>
       <c r="AA49" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="50" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="94"/>
       <c r="B50" s="82"/>
       <c r="C50" s="81" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D50" s="81"/>
       <c r="E50" s="74"/>
       <c r="F50" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G50" s="92"/>
       <c r="H50" s="75"/>
       <c r="I50" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J50" s="75"/>
       <c r="K50" s="74"/>
       <c r="L50" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M50" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N50" s="92"/>
       <c r="O50" s="75"/>
@@ -10095,7 +10096,7 @@
       <c r="R50" s="92"/>
       <c r="S50" s="78"/>
       <c r="T50" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U50" s="78"/>
       <c r="V50" s="78"/>
@@ -10104,32 +10105,32 @@
       <c r="Y50" s="78"/>
       <c r="Z50" s="78"/>
       <c r="AA50" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="51" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="94"/>
       <c r="B51" s="82"/>
       <c r="C51" s="81" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D51" s="81"/>
       <c r="E51" s="74"/>
       <c r="F51" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G51" s="92"/>
       <c r="H51" s="75"/>
       <c r="I51" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J51" s="75"/>
       <c r="K51" s="74"/>
       <c r="L51" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M51" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N51" s="92"/>
       <c r="O51" s="75"/>
@@ -10138,7 +10139,7 @@
       <c r="R51" s="92"/>
       <c r="S51" s="78"/>
       <c r="T51" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="U51" s="78"/>
       <c r="V51" s="78"/>
@@ -10147,32 +10148,32 @@
       <c r="Y51" s="78"/>
       <c r="Z51" s="78"/>
       <c r="AA51" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="52" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="94"/>
       <c r="B52" s="89"/>
       <c r="C52" s="88" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D52" s="88"/>
       <c r="E52" s="74"/>
       <c r="F52" s="101"/>
       <c r="G52" s="92"/>
       <c r="H52" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I52" s="74"/>
       <c r="J52" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K52" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L52" s="75"/>
       <c r="M52" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N52" s="92"/>
       <c r="O52" s="75"/>
@@ -10187,35 +10188,35 @@
       <c r="X52" s="78"/>
       <c r="Y52" s="78"/>
       <c r="Z52" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AA52" s="63" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="53" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="94"/>
       <c r="B53" s="89"/>
       <c r="C53" s="88" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D53" s="88"/>
       <c r="E53" s="74"/>
       <c r="F53" s="101"/>
       <c r="G53" s="92"/>
       <c r="H53" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I53" s="74"/>
       <c r="J53" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K53" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L53" s="75"/>
       <c r="M53" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N53" s="92"/>
       <c r="O53" s="75"/>
@@ -10230,10 +10231,10 @@
       <c r="X53" s="78"/>
       <c r="Y53" s="78"/>
       <c r="Z53" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AA53" s="63" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -10268,7 +10269,7 @@
     <row r="55" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49"/>
       <c r="B55" s="49" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C55" s="93"/>
       <c r="D55" s="93"/>
@@ -10300,29 +10301,29 @@
       <c r="A56" s="94"/>
       <c r="B56" s="89"/>
       <c r="C56" s="88" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D56" s="88"/>
       <c r="E56" s="74"/>
       <c r="F56" s="101"/>
       <c r="G56" s="92"/>
       <c r="H56" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I56" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J56" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K56" s="74"/>
       <c r="L56" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M56" s="74"/>
       <c r="N56" s="92"/>
       <c r="O56" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P56" s="92"/>
       <c r="Q56" s="92"/>
@@ -10335,39 +10336,39 @@
       <c r="X56" s="78"/>
       <c r="Y56" s="78"/>
       <c r="Z56" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AA56" s="63" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="57" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="94"/>
       <c r="B57" s="89"/>
       <c r="C57" s="88" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D57" s="88"/>
       <c r="E57" s="74"/>
       <c r="F57" s="101"/>
       <c r="G57" s="92"/>
       <c r="H57" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I57" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J57" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K57" s="74"/>
       <c r="L57" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M57" s="74"/>
       <c r="N57" s="92"/>
       <c r="O57" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P57" s="92"/>
       <c r="Q57" s="92"/>
@@ -10380,39 +10381,39 @@
       <c r="X57" s="78"/>
       <c r="Y57" s="78"/>
       <c r="Z57" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AA57" s="63" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="58" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="94"/>
       <c r="B58" s="89"/>
       <c r="C58" s="88" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D58" s="88"/>
       <c r="E58" s="74"/>
       <c r="F58" s="101"/>
       <c r="G58" s="92"/>
       <c r="H58" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I58" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J58" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K58" s="74"/>
       <c r="L58" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M58" s="74"/>
       <c r="N58" s="92"/>
       <c r="O58" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P58" s="92"/>
       <c r="Q58" s="92"/>
@@ -10425,39 +10426,39 @@
       <c r="X58" s="78"/>
       <c r="Y58" s="78"/>
       <c r="Z58" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AA58" s="63" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="59" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="94"/>
       <c r="B59" s="89"/>
       <c r="C59" s="88" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D59" s="88"/>
       <c r="E59" s="74"/>
       <c r="F59" s="101"/>
       <c r="G59" s="92"/>
       <c r="H59" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I59" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J59" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K59" s="74"/>
       <c r="L59" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M59" s="74"/>
       <c r="N59" s="92"/>
       <c r="O59" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P59" s="92"/>
       <c r="Q59" s="92"/>
@@ -10470,39 +10471,39 @@
       <c r="X59" s="78"/>
       <c r="Y59" s="78"/>
       <c r="Z59" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AA59" s="63" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="60" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="94"/>
       <c r="B60" s="89"/>
       <c r="C60" s="88" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D60" s="88"/>
       <c r="E60" s="74"/>
       <c r="F60" s="101"/>
       <c r="G60" s="92"/>
       <c r="H60" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I60" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J60" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K60" s="74"/>
       <c r="L60" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M60" s="74"/>
       <c r="N60" s="92"/>
       <c r="O60" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P60" s="92"/>
       <c r="Q60" s="92"/>
@@ -10515,39 +10516,39 @@
       <c r="X60" s="78"/>
       <c r="Y60" s="78"/>
       <c r="Z60" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AA60" s="63" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="61" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="94"/>
       <c r="B61" s="89"/>
       <c r="C61" s="88" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D61" s="88"/>
       <c r="E61" s="74"/>
       <c r="F61" s="101"/>
       <c r="G61" s="92"/>
       <c r="H61" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I61" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J61" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K61" s="74"/>
       <c r="L61" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M61" s="74"/>
       <c r="N61" s="92"/>
       <c r="O61" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P61" s="92"/>
       <c r="Q61" s="92"/>
@@ -10560,39 +10561,39 @@
       <c r="X61" s="78"/>
       <c r="Y61" s="78"/>
       <c r="Z61" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AA61" s="63" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="62" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="94"/>
       <c r="B62" s="89"/>
       <c r="C62" s="88" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D62" s="88"/>
       <c r="E62" s="74"/>
       <c r="F62" s="101"/>
       <c r="G62" s="92"/>
       <c r="H62" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I62" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J62" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K62" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L62" s="75"/>
       <c r="M62" s="74"/>
       <c r="N62" s="92"/>
       <c r="O62" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P62" s="92"/>
       <c r="Q62" s="92"/>
@@ -10605,39 +10606,39 @@
       <c r="X62" s="78"/>
       <c r="Y62" s="78"/>
       <c r="Z62" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AA62" s="63" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="63" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="94"/>
       <c r="B63" s="89"/>
       <c r="C63" s="88" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D63" s="88"/>
       <c r="E63" s="74"/>
       <c r="F63" s="101"/>
       <c r="G63" s="92"/>
       <c r="H63" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I63" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J63" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K63" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L63" s="75"/>
       <c r="M63" s="74"/>
       <c r="N63" s="92"/>
       <c r="O63" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P63" s="92"/>
       <c r="Q63" s="92"/>
@@ -10650,35 +10651,35 @@
       <c r="X63" s="78"/>
       <c r="Y63" s="78"/>
       <c r="Z63" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AA63" s="63" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="64" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="94"/>
       <c r="B64" s="94"/>
       <c r="C64" s="93" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D64" s="93"/>
       <c r="E64" s="74"/>
       <c r="F64" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G64" s="92"/>
       <c r="H64" s="75"/>
       <c r="I64" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J64" s="75"/>
       <c r="K64" s="74"/>
       <c r="L64" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M64" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N64" s="92"/>
       <c r="O64" s="75"/>
@@ -10686,44 +10687,44 @@
       <c r="Q64" s="92"/>
       <c r="R64" s="92"/>
       <c r="S64" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T64" s="78"/>
       <c r="U64" s="78"/>
       <c r="V64" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W64" s="78"/>
       <c r="X64" s="78"/>
       <c r="Y64" s="78"/>
       <c r="Z64" s="78"/>
       <c r="AA64" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="65" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="94"/>
       <c r="B65" s="94"/>
       <c r="C65" s="93" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D65" s="93"/>
       <c r="E65" s="74"/>
       <c r="F65" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G65" s="92"/>
       <c r="H65" s="75"/>
       <c r="I65" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J65" s="75"/>
       <c r="K65" s="74"/>
       <c r="L65" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M65" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N65" s="92"/>
       <c r="O65" s="75"/>
@@ -10731,44 +10732,44 @@
       <c r="Q65" s="92"/>
       <c r="R65" s="92"/>
       <c r="S65" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T65" s="78"/>
       <c r="U65" s="78"/>
       <c r="V65" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W65" s="78"/>
       <c r="X65" s="78"/>
       <c r="Y65" s="78"/>
       <c r="Z65" s="78"/>
       <c r="AA65" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="94"/>
       <c r="B66" s="94"/>
       <c r="C66" s="93" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D66" s="93"/>
       <c r="E66" s="74"/>
       <c r="F66" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G66" s="92"/>
       <c r="H66" s="75"/>
       <c r="I66" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J66" s="75"/>
       <c r="K66" s="74"/>
       <c r="L66" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M66" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N66" s="92"/>
       <c r="O66" s="75"/>
@@ -10776,44 +10777,44 @@
       <c r="Q66" s="92"/>
       <c r="R66" s="92"/>
       <c r="S66" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T66" s="78"/>
       <c r="U66" s="78"/>
       <c r="V66" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W66" s="78"/>
       <c r="X66" s="78"/>
       <c r="Y66" s="78"/>
       <c r="Z66" s="78"/>
       <c r="AA66" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="67" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="94"/>
       <c r="B67" s="94"/>
       <c r="C67" s="93" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D67" s="93"/>
       <c r="E67" s="74"/>
       <c r="F67" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G67" s="92"/>
       <c r="H67" s="75"/>
       <c r="I67" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J67" s="75"/>
       <c r="K67" s="74"/>
       <c r="L67" s="75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M67" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N67" s="92"/>
       <c r="O67" s="75"/>
@@ -10821,44 +10822,44 @@
       <c r="Q67" s="92"/>
       <c r="R67" s="92"/>
       <c r="S67" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T67" s="78"/>
       <c r="U67" s="78"/>
       <c r="V67" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W67" s="78"/>
       <c r="X67" s="78"/>
       <c r="Y67" s="78"/>
       <c r="Z67" s="78"/>
       <c r="AA67" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="68" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="94"/>
       <c r="B68" s="94"/>
       <c r="C68" s="93" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D68" s="93"/>
       <c r="E68" s="74"/>
       <c r="F68" s="101" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G68" s="92"/>
       <c r="H68" s="75"/>
       <c r="I68" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J68" s="75"/>
       <c r="K68" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L68" s="75"/>
       <c r="M68" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N68" s="92"/>
       <c r="O68" s="75"/>
@@ -10866,19 +10867,19 @@
       <c r="Q68" s="92"/>
       <c r="R68" s="92"/>
       <c r="S68" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T68" s="78"/>
       <c r="U68" s="78"/>
       <c r="V68" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="W68" s="78"/>
       <c r="X68" s="78"/>
       <c r="Y68" s="78"/>
       <c r="Z68" s="78"/>
       <c r="AA68" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="69" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11209,14 +11210,14 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
@@ -11226,7 +11227,7 @@
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
       <c r="D3" s="113" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E3" s="111"/>
       <c r="F3" s="73"/>
@@ -11234,213 +11235,213 @@
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="68" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="66" t="s">
         <v>209</v>
       </c>
-      <c r="E4" s="66" t="s">
-        <v>210</v>
-      </c>
       <c r="F4" s="72" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60"/>
       <c r="B5" s="59" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60"/>
       <c r="B6" s="59" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E6" s="75"/>
       <c r="F6" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>
       <c r="B7" s="59" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E7" s="75"/>
       <c r="F7" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
       <c r="B8" s="59" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E8" s="75"/>
       <c r="F8" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60"/>
       <c r="B9" s="59" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C9" s="59"/>
       <c r="D9" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E9" s="75"/>
       <c r="F9" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="60"/>
       <c r="B10" s="59" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E10" s="75"/>
       <c r="F10" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="60"/>
       <c r="B11" s="59" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E11" s="75"/>
       <c r="F11" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60"/>
       <c r="B12" s="59" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E12" s="75"/>
       <c r="F12" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="59" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E13" s="75"/>
       <c r="F13" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="59" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E14" s="75"/>
       <c r="F14" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
       <c r="B15" s="81" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E15" s="75"/>
       <c r="F15" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
       <c r="B16" s="81" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C16" s="59"/>
       <c r="D16" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E16" s="75"/>
       <c r="F16" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="60"/>
       <c r="B17" s="59" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E17" s="75"/>
       <c r="F17" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="60"/>
       <c r="B18" s="59" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E18" s="75"/>
       <c r="F18" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11600,10 +11601,10 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11641,11 +11642,11 @@
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="39" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="39" t="s">
@@ -11653,7 +11654,7 @@
       </c>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="K3" s="39"/>
       <c r="L3" s="39" t="s">
@@ -11661,7 +11662,7 @@
       </c>
       <c r="M3" s="39"/>
       <c r="N3" s="39" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11679,7 +11680,7 @@
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="58" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I4" s="58"/>
       <c r="J4" s="56" t="s">
@@ -11691,7 +11692,7 @@
       </c>
       <c r="M4" s="56"/>
       <c r="N4" s="56" t="s">
-        <v>213</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
@@ -11709,7 +11710,7 @@
       </c>
       <c r="G5" s="84"/>
       <c r="H5" s="84" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I5" s="84"/>
       <c r="J5" s="84" t="s">
@@ -11721,7 +11722,7 @@
       </c>
       <c r="M5" s="84"/>
       <c r="N5" s="84" t="s">
-        <v>214</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -11731,7 +11732,7 @@
       </c>
       <c r="C6" s="84"/>
       <c r="D6" s="84" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E6" s="84"/>
       <c r="F6" s="84" t="s">
@@ -11739,7 +11740,7 @@
       </c>
       <c r="G6" s="84"/>
       <c r="H6" s="84" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="I6" s="84"/>
       <c r="J6" s="84" t="s">
@@ -11751,10 +11752,10 @@
       </c>
       <c r="M6" s="84"/>
       <c r="N6" s="84" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="83"/>
       <c r="B7" s="84" t="s">
         <v>186</v>
@@ -11765,11 +11766,11 @@
       </c>
       <c r="E7" s="84"/>
       <c r="F7" s="84" t="s">
-        <v>205</v>
+        <v>328</v>
       </c>
       <c r="G7" s="84"/>
       <c r="H7" s="84" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I7" s="84"/>
       <c r="J7" s="84" t="s">
@@ -11781,7 +11782,7 @@
       </c>
       <c r="M7" s="84"/>
       <c r="N7" s="84" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -11848,7 +11849,7 @@
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -11858,7 +11859,7 @@
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B13" s="56"/>
       <c r="C13" s="56"/>

</xml_diff>

<commit_message>
Added annotation for Hatch (1997)
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -810,10 +810,6 @@
     <t>Key Metaphors</t>
   </si>
   <si>
-    <t xml:space="preserve">The organization is a machine that management designs, constructs, and maintains to achieve specific goals and objectives.
-The organization is a living organism comprised of systems that perform the functions necessary for its survival. </t>
-  </si>
-  <si>
     <t>The organization is a machine that management designs, constructs, and maintains to achieve specific goals and objectives.</t>
   </si>
   <si>
@@ -1232,12 +1228,18 @@
 Scientific management</t>
   </si>
   <si>
+    <t>Since all knowledge is filtered by the experience of the observer, all distinctions used to describe reality are arbitrary and semantic in origin.  The organization is an abstraction that is best understood by revealing the underlying assumptions used to construct it and considering their implications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The organization is a living organism comprised of systems that perform the functions necessary for its survival. </t>
+  </si>
+  <si>
     <t>Administrative theory
 Human relations management
-Garbage can model</t>
-  </si>
-  <si>
-    <t>Since all knowledge is filtered by the experience of the observer, all distinctions used to describe reality are arbitrary and semantic in origin.  The organization is an abstraction that is best understood by revealing the underlying assumptions used to construct it and considering their implications.</t>
+Coalition model of decision-making
+Garbage can model of decision-making
+Incremental model of decision-making
+Rational model of decision-making</t>
   </si>
 </sst>
 </file>
@@ -7427,7 +7429,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7888,7 +7890,7 @@
     </row>
     <row r="2" spans="1:27" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E2" s="61"/>
       <c r="F2" s="61"/>
@@ -7920,26 +7922,26 @@
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
       <c r="E3" s="113" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F3" s="114"/>
       <c r="G3" s="114"/>
       <c r="H3" s="111"/>
       <c r="I3" s="110" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J3" s="111"/>
       <c r="K3" s="110" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L3" s="112"/>
       <c r="M3" s="113" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N3" s="114"/>
       <c r="O3" s="111"/>
       <c r="P3" s="115" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q3" s="114"/>
       <c r="R3" s="114"/>
@@ -7956,84 +7958,84 @@
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="104" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="68"/>
       <c r="E4" s="105" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F4" s="107" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G4" s="62" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H4" s="106" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I4" s="65" t="s">
+        <v>207</v>
+      </c>
+      <c r="J4" s="66" t="s">
         <v>208</v>
       </c>
-      <c r="J4" s="66" t="s">
-        <v>209</v>
-      </c>
       <c r="K4" s="65" t="s">
+        <v>267</v>
+      </c>
+      <c r="L4" s="66" t="s">
         <v>268</v>
       </c>
-      <c r="L4" s="66" t="s">
-        <v>269</v>
-      </c>
       <c r="M4" s="105" t="s">
+        <v>303</v>
+      </c>
+      <c r="N4" s="62" t="s">
         <v>304</v>
       </c>
-      <c r="N4" s="62" t="s">
-        <v>305</v>
-      </c>
       <c r="O4" s="106" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P4" s="62" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q4" s="62" t="s">
+        <v>246</v>
+      </c>
+      <c r="R4" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="R4" s="62" t="s">
+      <c r="S4" s="62" t="s">
+        <v>219</v>
+      </c>
+      <c r="T4" s="62" t="s">
+        <v>242</v>
+      </c>
+      <c r="U4" s="62" t="s">
         <v>248</v>
       </c>
-      <c r="S4" s="62" t="s">
+      <c r="V4" s="62" t="s">
         <v>220</v>
       </c>
-      <c r="T4" s="62" t="s">
-        <v>243</v>
-      </c>
-      <c r="U4" s="62" t="s">
-        <v>249</v>
-      </c>
-      <c r="V4" s="62" t="s">
-        <v>221</v>
-      </c>
       <c r="W4" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="X4" s="62" t="s">
         <v>245</v>
       </c>
-      <c r="X4" s="62" t="s">
-        <v>246</v>
-      </c>
       <c r="Y4" s="62" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Z4" s="62" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AA4" s="72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="49" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C5" s="93"/>
       <c r="D5" s="93"/>
@@ -8065,25 +8067,25 @@
       <c r="A6" s="94"/>
       <c r="B6" s="82"/>
       <c r="C6" s="81" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="81"/>
       <c r="E6" s="74"/>
       <c r="F6" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G6" s="92"/>
       <c r="H6" s="75"/>
       <c r="I6" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J6" s="75"/>
       <c r="K6" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L6" s="75"/>
       <c r="M6" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N6" s="92"/>
       <c r="O6" s="75"/>
@@ -8092,7 +8094,7 @@
       <c r="R6" s="92"/>
       <c r="S6" s="78"/>
       <c r="T6" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U6" s="78"/>
       <c r="V6" s="78"/>
@@ -8101,32 +8103,32 @@
       <c r="Y6" s="78"/>
       <c r="Z6" s="78"/>
       <c r="AA6" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="94"/>
       <c r="B7" s="82"/>
       <c r="C7" s="93" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D7" s="81"/>
       <c r="E7" s="74"/>
       <c r="F7" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G7" s="92"/>
       <c r="H7" s="75"/>
       <c r="I7" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J7" s="75"/>
       <c r="K7" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L7" s="75"/>
       <c r="M7" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N7" s="92"/>
       <c r="O7" s="75"/>
@@ -8135,7 +8137,7 @@
       <c r="R7" s="92"/>
       <c r="S7" s="78"/>
       <c r="T7" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U7" s="78"/>
       <c r="V7" s="78"/>
@@ -8144,32 +8146,32 @@
       <c r="Y7" s="78"/>
       <c r="Z7" s="78"/>
       <c r="AA7" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="94"/>
       <c r="B8" s="82"/>
       <c r="C8" s="81" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D8" s="81"/>
       <c r="E8" s="74"/>
       <c r="F8" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G8" s="92"/>
       <c r="H8" s="75"/>
       <c r="I8" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J8" s="75"/>
       <c r="K8" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L8" s="75"/>
       <c r="M8" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N8" s="92"/>
       <c r="O8" s="75"/>
@@ -8178,7 +8180,7 @@
       <c r="R8" s="92"/>
       <c r="S8" s="78"/>
       <c r="T8" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U8" s="78"/>
       <c r="V8" s="78"/>
@@ -8187,47 +8189,47 @@
       <c r="Y8" s="78"/>
       <c r="Z8" s="78"/>
       <c r="AA8" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="94"/>
       <c r="B9" s="82"/>
       <c r="C9" s="93" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D9" s="81"/>
       <c r="E9" s="74"/>
       <c r="F9" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G9" s="92"/>
       <c r="H9" s="75"/>
       <c r="I9" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J9" s="75"/>
       <c r="K9" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L9" s="75"/>
       <c r="M9" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N9" s="92"/>
       <c r="O9" s="75"/>
       <c r="P9" s="92"/>
       <c r="Q9" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R9" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S9" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T9" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U9" s="78"/>
       <c r="V9" s="78"/>
@@ -8236,104 +8238,104 @@
       <c r="Y9" s="78"/>
       <c r="Z9" s="78"/>
       <c r="AA9" s="63" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
       <c r="B10" s="30"/>
       <c r="C10" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="74"/>
       <c r="F10" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G10" s="92"/>
       <c r="H10" s="75"/>
       <c r="I10" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J10" s="75"/>
       <c r="K10" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L10" s="75"/>
       <c r="M10" s="74"/>
       <c r="N10" s="92"/>
       <c r="O10" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P10" s="92"/>
       <c r="Q10" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R10" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S10" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T10" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U10" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V10" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W10" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X10" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y10" s="78"/>
       <c r="Z10" s="78"/>
       <c r="AA10" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="94"/>
       <c r="B11" s="82"/>
       <c r="C11" s="95" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D11" s="81"/>
       <c r="E11" s="96"/>
       <c r="F11" s="102" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G11" s="98"/>
       <c r="H11" s="97"/>
       <c r="I11" s="96" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J11" s="97"/>
       <c r="K11" s="96" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L11" s="97"/>
       <c r="M11" s="96" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N11" s="98"/>
       <c r="O11" s="97"/>
       <c r="P11" s="98"/>
       <c r="Q11" s="98" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R11" s="98" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S11" s="99" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T11" s="99" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U11" s="99"/>
       <c r="V11" s="99"/>
@@ -8342,7 +8344,7 @@
       <c r="Y11" s="99"/>
       <c r="Z11" s="99"/>
       <c r="AA11" s="100" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -8377,7 +8379,7 @@
     <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="49" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C13" s="93"/>
       <c r="D13" s="93"/>
@@ -8409,241 +8411,241 @@
       <c r="A14" s="94"/>
       <c r="B14" s="30"/>
       <c r="C14" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="74"/>
       <c r="F14" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G14" s="92"/>
       <c r="H14" s="75"/>
       <c r="I14" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J14" s="75"/>
       <c r="K14" s="74"/>
       <c r="L14" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M14" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N14" s="92"/>
       <c r="O14" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P14" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q14" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R14" s="92"/>
       <c r="S14" s="78"/>
       <c r="T14" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U14" s="78"/>
       <c r="V14" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W14" s="78"/>
       <c r="X14" s="78"/>
       <c r="Y14" s="78"/>
       <c r="Z14" s="78"/>
       <c r="AA14" s="63" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="94"/>
       <c r="B15" s="30"/>
       <c r="C15" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="74"/>
       <c r="F15" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G15" s="92"/>
       <c r="H15" s="75"/>
       <c r="I15" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J15" s="75"/>
       <c r="K15" s="74"/>
       <c r="L15" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M15" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N15" s="92"/>
       <c r="O15" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P15" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q15" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R15" s="92"/>
       <c r="S15" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T15" s="78"/>
       <c r="U15" s="78"/>
       <c r="V15" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W15" s="78"/>
       <c r="X15" s="78"/>
       <c r="Y15" s="78"/>
       <c r="Z15" s="78"/>
       <c r="AA15" s="63" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="94"/>
       <c r="B16" s="82"/>
       <c r="C16" s="81" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D16" s="81"/>
       <c r="E16" s="74"/>
       <c r="F16" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G16" s="92"/>
       <c r="H16" s="75"/>
       <c r="I16" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J16" s="75"/>
       <c r="K16" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L16" s="75"/>
       <c r="M16" s="74"/>
       <c r="N16" s="92"/>
       <c r="O16" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P16" s="92"/>
       <c r="Q16" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R16" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S16" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T16" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U16" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V16" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W16" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X16" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y16" s="78"/>
       <c r="Z16" s="78"/>
       <c r="AA16" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="94"/>
       <c r="B17" s="82"/>
       <c r="C17" s="81" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D17" s="81"/>
       <c r="E17" s="74"/>
       <c r="F17" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G17" s="92"/>
       <c r="H17" s="75"/>
       <c r="I17" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J17" s="75"/>
       <c r="K17" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L17" s="75"/>
       <c r="M17" s="74"/>
       <c r="N17" s="92"/>
       <c r="O17" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P17" s="92"/>
       <c r="Q17" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R17" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S17" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T17" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U17" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V17" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W17" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X17" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y17" s="78"/>
       <c r="Z17" s="78"/>
       <c r="AA17" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="94"/>
       <c r="B18" s="60"/>
       <c r="C18" s="59" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D18" s="59"/>
       <c r="E18" s="74"/>
       <c r="F18" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G18" s="92"/>
       <c r="H18" s="75"/>
       <c r="I18" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J18" s="75"/>
       <c r="K18" s="74"/>
       <c r="L18" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M18" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N18" s="92"/>
       <c r="O18" s="75"/>
@@ -8654,39 +8656,39 @@
       <c r="T18" s="78"/>
       <c r="U18" s="78"/>
       <c r="V18" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W18" s="78"/>
       <c r="X18" s="78"/>
       <c r="Y18" s="78"/>
       <c r="Z18" s="78"/>
       <c r="AA18" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="94"/>
       <c r="B19" s="30"/>
       <c r="C19" s="32" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="74"/>
       <c r="F19" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G19" s="92"/>
       <c r="H19" s="75"/>
       <c r="I19" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J19" s="75"/>
       <c r="K19" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L19" s="75"/>
       <c r="M19" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N19" s="92"/>
       <c r="O19" s="75"/>
@@ -8694,7 +8696,7 @@
       <c r="Q19" s="92"/>
       <c r="R19" s="92"/>
       <c r="S19" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T19" s="78"/>
       <c r="U19" s="78"/>
@@ -8704,32 +8706,32 @@
       <c r="Y19" s="78"/>
       <c r="Z19" s="78"/>
       <c r="AA19" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="94"/>
       <c r="B20" s="30"/>
       <c r="C20" s="32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="74"/>
       <c r="F20" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G20" s="92"/>
       <c r="H20" s="75"/>
       <c r="I20" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J20" s="75"/>
       <c r="K20" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L20" s="75"/>
       <c r="M20" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N20" s="92"/>
       <c r="O20" s="75"/>
@@ -8737,7 +8739,7 @@
       <c r="Q20" s="92"/>
       <c r="R20" s="92"/>
       <c r="S20" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T20" s="78"/>
       <c r="U20" s="78"/>
@@ -8747,32 +8749,32 @@
       <c r="Y20" s="78"/>
       <c r="Z20" s="78"/>
       <c r="AA20" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="94"/>
       <c r="B21" s="30"/>
       <c r="C21" s="32" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="74"/>
       <c r="F21" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G21" s="92"/>
       <c r="H21" s="75"/>
       <c r="I21" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J21" s="75"/>
       <c r="K21" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L21" s="75"/>
       <c r="M21" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N21" s="92"/>
       <c r="O21" s="75"/>
@@ -8780,7 +8782,7 @@
       <c r="Q21" s="92"/>
       <c r="R21" s="92"/>
       <c r="S21" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T21" s="78"/>
       <c r="U21" s="78"/>
@@ -8790,349 +8792,349 @@
       <c r="Y21" s="78"/>
       <c r="Z21" s="78"/>
       <c r="AA21" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="94"/>
       <c r="B22" s="82"/>
       <c r="C22" s="81" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D22" s="81"/>
       <c r="E22" s="74"/>
       <c r="F22" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G22" s="92"/>
       <c r="H22" s="75"/>
       <c r="I22" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J22" s="75"/>
       <c r="K22" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L22" s="75"/>
       <c r="M22" s="74"/>
       <c r="N22" s="92"/>
       <c r="O22" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P22" s="92"/>
       <c r="Q22" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R22" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S22" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T22" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U22" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V22" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W22" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X22" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y22" s="78"/>
       <c r="Z22" s="78"/>
       <c r="AA22" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="94"/>
       <c r="B23" s="82"/>
       <c r="C23" s="81" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D23" s="81"/>
       <c r="E23" s="74"/>
       <c r="F23" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G23" s="92"/>
       <c r="H23" s="75"/>
       <c r="I23" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J23" s="75"/>
       <c r="K23" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L23" s="75"/>
       <c r="M23" s="74"/>
       <c r="N23" s="92"/>
       <c r="O23" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P23" s="92"/>
       <c r="Q23" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R23" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S23" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T23" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U23" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V23" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W23" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X23" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y23" s="78"/>
       <c r="Z23" s="78"/>
       <c r="AA23" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="94"/>
       <c r="B24" s="30"/>
       <c r="C24" s="32" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="74"/>
       <c r="F24" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G24" s="92"/>
       <c r="H24" s="75"/>
       <c r="I24" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J24" s="75"/>
       <c r="K24" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L24" s="75"/>
       <c r="M24" s="74"/>
       <c r="N24" s="92"/>
       <c r="O24" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P24" s="92"/>
       <c r="Q24" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R24" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S24" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T24" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U24" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V24" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W24" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X24" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y24" s="78"/>
       <c r="Z24" s="78"/>
       <c r="AA24" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="94"/>
       <c r="B25" s="30"/>
       <c r="C25" s="32" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="74"/>
       <c r="F25" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G25" s="92"/>
       <c r="H25" s="75"/>
       <c r="I25" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J25" s="75"/>
       <c r="K25" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L25" s="75"/>
       <c r="M25" s="74"/>
       <c r="N25" s="92"/>
       <c r="O25" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P25" s="92"/>
       <c r="Q25" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R25" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S25" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T25" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U25" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V25" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W25" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X25" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y25" s="78"/>
       <c r="Z25" s="78"/>
       <c r="AA25" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="94"/>
       <c r="B26" s="82"/>
       <c r="C26" s="81" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D26" s="81"/>
       <c r="E26" s="74"/>
       <c r="F26" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G26" s="92"/>
       <c r="H26" s="75"/>
       <c r="I26" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J26" s="75"/>
       <c r="K26" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L26" s="75"/>
       <c r="M26" s="74"/>
       <c r="N26" s="92"/>
       <c r="O26" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P26" s="92"/>
       <c r="Q26" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R26" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S26" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T26" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U26" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V26" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W26" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X26" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y26" s="78"/>
       <c r="Z26" s="78"/>
       <c r="AA26" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="94"/>
       <c r="B27" s="82"/>
       <c r="C27" s="81" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D27" s="81"/>
       <c r="E27" s="74"/>
       <c r="F27" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G27" s="92"/>
       <c r="H27" s="75"/>
       <c r="I27" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J27" s="75"/>
       <c r="K27" s="74"/>
       <c r="L27" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M27" s="74"/>
       <c r="N27" s="92"/>
       <c r="O27" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P27" s="92"/>
       <c r="Q27" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R27" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S27" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T27" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U27" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V27" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W27" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X27" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y27" s="78"/>
       <c r="Z27" s="78"/>
       <c r="AA27" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9167,7 +9169,7 @@
     <row r="29" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="94"/>
       <c r="B29" s="31" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C29" s="93"/>
       <c r="D29" s="93"/>
@@ -9199,40 +9201,40 @@
       <c r="A30" s="94"/>
       <c r="B30" s="82"/>
       <c r="C30" s="81" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D30" s="81"/>
       <c r="E30" s="74"/>
       <c r="F30" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G30" s="92"/>
       <c r="H30" s="75"/>
       <c r="I30" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J30" s="75"/>
       <c r="K30" s="74"/>
       <c r="L30" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M30" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N30" s="92"/>
       <c r="O30" s="75"/>
       <c r="P30" s="92"/>
       <c r="Q30" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R30" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S30" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T30" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U30" s="78"/>
       <c r="V30" s="78"/>
@@ -9241,32 +9243,32 @@
       <c r="Y30" s="78"/>
       <c r="Z30" s="78"/>
       <c r="AA30" s="63" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="94"/>
       <c r="B31" s="94"/>
       <c r="C31" s="93" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D31" s="93"/>
       <c r="E31" s="74"/>
       <c r="F31" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G31" s="92"/>
       <c r="H31" s="75"/>
       <c r="I31" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J31" s="75"/>
       <c r="K31" s="74"/>
       <c r="L31" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M31" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N31" s="92"/>
       <c r="O31" s="75"/>
@@ -9275,7 +9277,7 @@
       <c r="R31" s="92"/>
       <c r="S31" s="78"/>
       <c r="T31" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U31" s="78"/>
       <c r="V31" s="78"/>
@@ -9284,32 +9286,32 @@
       <c r="Y31" s="78"/>
       <c r="Z31" s="78"/>
       <c r="AA31" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="94"/>
       <c r="B32" s="94"/>
       <c r="C32" s="93" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D32" s="93"/>
       <c r="E32" s="74"/>
       <c r="F32" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G32" s="92"/>
       <c r="H32" s="75"/>
       <c r="I32" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J32" s="75"/>
       <c r="K32" s="74"/>
       <c r="L32" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M32" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N32" s="92"/>
       <c r="O32" s="75"/>
@@ -9318,7 +9320,7 @@
       <c r="R32" s="92"/>
       <c r="S32" s="78"/>
       <c r="T32" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U32" s="78"/>
       <c r="V32" s="78"/>
@@ -9327,38 +9329,38 @@
       <c r="Y32" s="78"/>
       <c r="Z32" s="78"/>
       <c r="AA32" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="94"/>
       <c r="B33" s="94"/>
       <c r="C33" s="93" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D33" s="93"/>
       <c r="E33" s="74"/>
       <c r="F33" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G33" s="92"/>
       <c r="H33" s="75"/>
       <c r="I33" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J33" s="75"/>
       <c r="K33" s="74"/>
       <c r="L33" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M33" s="74"/>
       <c r="N33" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="O33" s="75"/>
       <c r="P33" s="92"/>
       <c r="Q33" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R33" s="92"/>
       <c r="S33" s="78"/>
@@ -9370,7 +9372,7 @@
       <c r="Y33" s="78"/>
       <c r="Z33" s="78"/>
       <c r="AA33" s="63" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9405,7 +9407,7 @@
     <row r="35" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
       <c r="B35" s="49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C35" s="93"/>
       <c r="D35" s="93"/>
@@ -9437,25 +9439,25 @@
       <c r="A36" s="94"/>
       <c r="B36" s="30"/>
       <c r="C36" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D36" s="32"/>
       <c r="E36" s="74"/>
       <c r="F36" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G36" s="92"/>
       <c r="H36" s="75"/>
       <c r="I36" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J36" s="75"/>
       <c r="K36" s="74"/>
       <c r="L36" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M36" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N36" s="92"/>
       <c r="O36" s="75"/>
@@ -9463,7 +9465,7 @@
       <c r="Q36" s="92"/>
       <c r="R36" s="92"/>
       <c r="S36" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T36" s="78"/>
       <c r="U36" s="78"/>
@@ -9473,32 +9475,32 @@
       <c r="Y36" s="78"/>
       <c r="Z36" s="78"/>
       <c r="AA36" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="94"/>
       <c r="B37" s="30"/>
       <c r="C37" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D37" s="32"/>
       <c r="E37" s="74"/>
       <c r="F37" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G37" s="92"/>
       <c r="H37" s="75"/>
       <c r="I37" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J37" s="75"/>
       <c r="K37" s="74"/>
       <c r="L37" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M37" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N37" s="92"/>
       <c r="O37" s="75"/>
@@ -9509,39 +9511,39 @@
       <c r="T37" s="78"/>
       <c r="U37" s="78"/>
       <c r="V37" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W37" s="78"/>
       <c r="X37" s="78"/>
       <c r="Y37" s="78"/>
       <c r="Z37" s="78"/>
       <c r="AA37" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="94"/>
       <c r="B38" s="94"/>
       <c r="C38" s="93" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D38" s="93"/>
       <c r="E38" s="74"/>
       <c r="F38" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G38" s="92"/>
       <c r="H38" s="75"/>
       <c r="I38" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J38" s="75"/>
       <c r="K38" s="74"/>
       <c r="L38" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M38" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N38" s="92"/>
       <c r="O38" s="75"/>
@@ -9549,7 +9551,7 @@
       <c r="Q38" s="92"/>
       <c r="R38" s="92"/>
       <c r="S38" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T38" s="78"/>
       <c r="U38" s="78"/>
@@ -9559,32 +9561,32 @@
       <c r="Y38" s="78"/>
       <c r="Z38" s="78"/>
       <c r="AA38" s="63" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="39" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="94"/>
       <c r="B39" s="94"/>
       <c r="C39" s="93" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D39" s="93"/>
       <c r="E39" s="74"/>
       <c r="F39" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G39" s="92"/>
       <c r="H39" s="75"/>
       <c r="I39" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J39" s="75"/>
       <c r="K39" s="74"/>
       <c r="L39" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M39" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N39" s="92"/>
       <c r="O39" s="75"/>
@@ -9592,44 +9594,44 @@
       <c r="Q39" s="92"/>
       <c r="R39" s="92"/>
       <c r="S39" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T39" s="78"/>
       <c r="U39" s="78"/>
       <c r="V39" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W39" s="78"/>
       <c r="X39" s="78"/>
       <c r="Y39" s="78"/>
       <c r="Z39" s="78"/>
       <c r="AA39" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="94"/>
       <c r="B40" s="94"/>
       <c r="C40" s="93" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D40" s="93"/>
       <c r="E40" s="74"/>
       <c r="F40" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G40" s="92"/>
       <c r="H40" s="75"/>
       <c r="I40" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J40" s="75"/>
       <c r="K40" s="74"/>
       <c r="L40" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M40" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N40" s="92"/>
       <c r="O40" s="75"/>
@@ -9637,93 +9639,93 @@
       <c r="Q40" s="92"/>
       <c r="R40" s="92"/>
       <c r="S40" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T40" s="78"/>
       <c r="U40" s="78"/>
       <c r="V40" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W40" s="78"/>
       <c r="X40" s="78"/>
       <c r="Y40" s="78"/>
       <c r="Z40" s="78"/>
       <c r="AA40" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="94"/>
       <c r="B41" s="94"/>
       <c r="C41" s="93" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D41" s="93"/>
       <c r="E41" s="74"/>
       <c r="F41" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G41" s="92"/>
       <c r="H41" s="75"/>
       <c r="I41" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J41" s="75"/>
       <c r="K41" s="74"/>
       <c r="L41" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M41" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N41" s="92"/>
       <c r="O41" s="75"/>
       <c r="P41" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q41" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R41" s="92"/>
       <c r="S41" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T41" s="78"/>
       <c r="U41" s="78"/>
       <c r="V41" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W41" s="78"/>
       <c r="X41" s="78"/>
       <c r="Y41" s="78"/>
       <c r="Z41" s="78"/>
       <c r="AA41" s="63" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="94"/>
       <c r="B42" s="94"/>
       <c r="C42" s="93" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D42" s="93"/>
       <c r="E42" s="74"/>
       <c r="F42" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G42" s="92"/>
       <c r="H42" s="75"/>
       <c r="I42" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J42" s="75"/>
       <c r="K42" s="74"/>
       <c r="L42" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M42" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N42" s="92"/>
       <c r="O42" s="75"/>
@@ -9732,7 +9734,7 @@
       <c r="R42" s="92"/>
       <c r="S42" s="78"/>
       <c r="T42" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U42" s="78"/>
       <c r="V42" s="78"/>
@@ -9741,32 +9743,32 @@
       <c r="Y42" s="78"/>
       <c r="Z42" s="78"/>
       <c r="AA42" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="94"/>
       <c r="B43" s="94"/>
       <c r="C43" s="93" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D43" s="93"/>
       <c r="E43" s="74"/>
       <c r="F43" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G43" s="92"/>
       <c r="H43" s="75"/>
       <c r="I43" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J43" s="75"/>
       <c r="K43" s="74"/>
       <c r="L43" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M43" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N43" s="92"/>
       <c r="O43" s="75"/>
@@ -9774,44 +9776,44 @@
       <c r="Q43" s="92"/>
       <c r="R43" s="92"/>
       <c r="S43" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T43" s="78"/>
       <c r="U43" s="78"/>
       <c r="V43" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W43" s="78"/>
       <c r="X43" s="78"/>
       <c r="Y43" s="78"/>
       <c r="Z43" s="78"/>
       <c r="AA43" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="94"/>
       <c r="B44" s="94"/>
       <c r="C44" s="93" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D44" s="93"/>
       <c r="E44" s="74"/>
       <c r="F44" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G44" s="92"/>
       <c r="H44" s="75"/>
       <c r="I44" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J44" s="75"/>
       <c r="K44" s="74"/>
       <c r="L44" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M44" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N44" s="92"/>
       <c r="O44" s="75"/>
@@ -9819,101 +9821,101 @@
       <c r="Q44" s="92"/>
       <c r="R44" s="92"/>
       <c r="S44" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T44" s="78"/>
       <c r="U44" s="78"/>
       <c r="V44" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W44" s="78"/>
       <c r="X44" s="78"/>
       <c r="Y44" s="78"/>
       <c r="Z44" s="78"/>
       <c r="AA44" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="94"/>
       <c r="B45" s="82"/>
       <c r="C45" s="81" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D45" s="81"/>
       <c r="E45" s="74"/>
       <c r="F45" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G45" s="92"/>
       <c r="H45" s="75"/>
       <c r="I45" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J45" s="75"/>
       <c r="K45" s="74"/>
       <c r="L45" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M45" s="74"/>
       <c r="N45" s="92"/>
       <c r="O45" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P45" s="92"/>
       <c r="Q45" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R45" s="92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S45" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T45" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U45" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V45" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W45" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X45" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y45" s="78"/>
       <c r="Z45" s="78"/>
       <c r="AA45" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="94"/>
       <c r="B46" s="60"/>
       <c r="C46" s="59" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D46" s="59"/>
       <c r="E46" s="74"/>
       <c r="F46" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G46" s="92"/>
       <c r="H46" s="75"/>
       <c r="I46" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J46" s="75"/>
       <c r="K46" s="74"/>
       <c r="L46" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M46" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N46" s="92"/>
       <c r="O46" s="75"/>
@@ -9921,44 +9923,44 @@
       <c r="Q46" s="92"/>
       <c r="R46" s="92"/>
       <c r="S46" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T46" s="78"/>
       <c r="U46" s="78"/>
       <c r="V46" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W46" s="78"/>
       <c r="X46" s="78"/>
       <c r="Y46" s="78"/>
       <c r="Z46" s="78"/>
       <c r="AA46" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="94"/>
       <c r="B47" s="60"/>
       <c r="C47" s="59" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D47" s="59"/>
       <c r="E47" s="74"/>
       <c r="F47" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G47" s="92"/>
       <c r="H47" s="75"/>
       <c r="I47" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J47" s="75"/>
       <c r="K47" s="74"/>
       <c r="L47" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M47" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N47" s="92"/>
       <c r="O47" s="75"/>
@@ -9966,7 +9968,7 @@
       <c r="Q47" s="92"/>
       <c r="R47" s="92"/>
       <c r="S47" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T47" s="78"/>
       <c r="U47" s="78"/>
@@ -9976,32 +9978,32 @@
       <c r="Y47" s="78"/>
       <c r="Z47" s="78"/>
       <c r="AA47" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="94"/>
       <c r="B48" s="82"/>
       <c r="C48" s="81" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D48" s="81"/>
       <c r="E48" s="74"/>
       <c r="F48" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G48" s="92"/>
       <c r="H48" s="75"/>
       <c r="I48" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J48" s="75"/>
       <c r="K48" s="74"/>
       <c r="L48" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M48" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N48" s="92"/>
       <c r="O48" s="75"/>
@@ -10010,7 +10012,7 @@
       <c r="R48" s="92"/>
       <c r="S48" s="78"/>
       <c r="T48" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U48" s="78"/>
       <c r="V48" s="78"/>
@@ -10019,32 +10021,32 @@
       <c r="Y48" s="78"/>
       <c r="Z48" s="78"/>
       <c r="AA48" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="94"/>
       <c r="B49" s="94"/>
       <c r="C49" s="93" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D49" s="93"/>
       <c r="E49" s="74"/>
       <c r="F49" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G49" s="92"/>
       <c r="H49" s="75"/>
       <c r="I49" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J49" s="75"/>
       <c r="K49" s="74"/>
       <c r="L49" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M49" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N49" s="92"/>
       <c r="O49" s="75"/>
@@ -10053,7 +10055,7 @@
       <c r="R49" s="92"/>
       <c r="S49" s="78"/>
       <c r="T49" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U49" s="78"/>
       <c r="V49" s="78"/>
@@ -10062,32 +10064,32 @@
       <c r="Y49" s="78"/>
       <c r="Z49" s="78"/>
       <c r="AA49" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="50" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="94"/>
       <c r="B50" s="82"/>
       <c r="C50" s="81" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D50" s="81"/>
       <c r="E50" s="74"/>
       <c r="F50" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G50" s="92"/>
       <c r="H50" s="75"/>
       <c r="I50" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J50" s="75"/>
       <c r="K50" s="74"/>
       <c r="L50" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M50" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N50" s="92"/>
       <c r="O50" s="75"/>
@@ -10096,7 +10098,7 @@
       <c r="R50" s="92"/>
       <c r="S50" s="78"/>
       <c r="T50" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U50" s="78"/>
       <c r="V50" s="78"/>
@@ -10105,32 +10107,32 @@
       <c r="Y50" s="78"/>
       <c r="Z50" s="78"/>
       <c r="AA50" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="94"/>
       <c r="B51" s="82"/>
       <c r="C51" s="81" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D51" s="81"/>
       <c r="E51" s="74"/>
       <c r="F51" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G51" s="92"/>
       <c r="H51" s="75"/>
       <c r="I51" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J51" s="75"/>
       <c r="K51" s="74"/>
       <c r="L51" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M51" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N51" s="92"/>
       <c r="O51" s="75"/>
@@ -10139,7 +10141,7 @@
       <c r="R51" s="92"/>
       <c r="S51" s="78"/>
       <c r="T51" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U51" s="78"/>
       <c r="V51" s="78"/>
@@ -10148,32 +10150,32 @@
       <c r="Y51" s="78"/>
       <c r="Z51" s="78"/>
       <c r="AA51" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="94"/>
       <c r="B52" s="89"/>
       <c r="C52" s="88" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D52" s="88"/>
       <c r="E52" s="74"/>
       <c r="F52" s="101"/>
       <c r="G52" s="92"/>
       <c r="H52" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I52" s="74"/>
       <c r="J52" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K52" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L52" s="75"/>
       <c r="M52" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N52" s="92"/>
       <c r="O52" s="75"/>
@@ -10188,35 +10190,35 @@
       <c r="X52" s="78"/>
       <c r="Y52" s="78"/>
       <c r="Z52" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AA52" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="94"/>
       <c r="B53" s="89"/>
       <c r="C53" s="88" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D53" s="88"/>
       <c r="E53" s="74"/>
       <c r="F53" s="101"/>
       <c r="G53" s="92"/>
       <c r="H53" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I53" s="74"/>
       <c r="J53" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K53" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L53" s="75"/>
       <c r="M53" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N53" s="92"/>
       <c r="O53" s="75"/>
@@ -10231,10 +10233,10 @@
       <c r="X53" s="78"/>
       <c r="Y53" s="78"/>
       <c r="Z53" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AA53" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="54" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -10269,7 +10271,7 @@
     <row r="55" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49"/>
       <c r="B55" s="49" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C55" s="93"/>
       <c r="D55" s="93"/>
@@ -10301,29 +10303,29 @@
       <c r="A56" s="94"/>
       <c r="B56" s="89"/>
       <c r="C56" s="88" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D56" s="88"/>
       <c r="E56" s="74"/>
       <c r="F56" s="101"/>
       <c r="G56" s="92"/>
       <c r="H56" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I56" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J56" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K56" s="74"/>
       <c r="L56" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M56" s="74"/>
       <c r="N56" s="92"/>
       <c r="O56" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P56" s="92"/>
       <c r="Q56" s="92"/>
@@ -10336,39 +10338,39 @@
       <c r="X56" s="78"/>
       <c r="Y56" s="78"/>
       <c r="Z56" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AA56" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="57" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="94"/>
       <c r="B57" s="89"/>
       <c r="C57" s="88" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D57" s="88"/>
       <c r="E57" s="74"/>
       <c r="F57" s="101"/>
       <c r="G57" s="92"/>
       <c r="H57" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I57" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J57" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K57" s="74"/>
       <c r="L57" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M57" s="74"/>
       <c r="N57" s="92"/>
       <c r="O57" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P57" s="92"/>
       <c r="Q57" s="92"/>
@@ -10381,39 +10383,39 @@
       <c r="X57" s="78"/>
       <c r="Y57" s="78"/>
       <c r="Z57" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AA57" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="58" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="94"/>
       <c r="B58" s="89"/>
       <c r="C58" s="88" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D58" s="88"/>
       <c r="E58" s="74"/>
       <c r="F58" s="101"/>
       <c r="G58" s="92"/>
       <c r="H58" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I58" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J58" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K58" s="74"/>
       <c r="L58" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M58" s="74"/>
       <c r="N58" s="92"/>
       <c r="O58" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P58" s="92"/>
       <c r="Q58" s="92"/>
@@ -10426,39 +10428,39 @@
       <c r="X58" s="78"/>
       <c r="Y58" s="78"/>
       <c r="Z58" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AA58" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="59" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="94"/>
       <c r="B59" s="89"/>
       <c r="C59" s="88" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D59" s="88"/>
       <c r="E59" s="74"/>
       <c r="F59" s="101"/>
       <c r="G59" s="92"/>
       <c r="H59" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I59" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J59" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K59" s="74"/>
       <c r="L59" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M59" s="74"/>
       <c r="N59" s="92"/>
       <c r="O59" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P59" s="92"/>
       <c r="Q59" s="92"/>
@@ -10471,39 +10473,39 @@
       <c r="X59" s="78"/>
       <c r="Y59" s="78"/>
       <c r="Z59" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AA59" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="60" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="94"/>
       <c r="B60" s="89"/>
       <c r="C60" s="88" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D60" s="88"/>
       <c r="E60" s="74"/>
       <c r="F60" s="101"/>
       <c r="G60" s="92"/>
       <c r="H60" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I60" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J60" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K60" s="74"/>
       <c r="L60" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M60" s="74"/>
       <c r="N60" s="92"/>
       <c r="O60" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P60" s="92"/>
       <c r="Q60" s="92"/>
@@ -10516,39 +10518,39 @@
       <c r="X60" s="78"/>
       <c r="Y60" s="78"/>
       <c r="Z60" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AA60" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="61" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="94"/>
       <c r="B61" s="89"/>
       <c r="C61" s="88" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D61" s="88"/>
       <c r="E61" s="74"/>
       <c r="F61" s="101"/>
       <c r="G61" s="92"/>
       <c r="H61" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I61" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J61" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K61" s="74"/>
       <c r="L61" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M61" s="74"/>
       <c r="N61" s="92"/>
       <c r="O61" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P61" s="92"/>
       <c r="Q61" s="92"/>
@@ -10561,39 +10563,39 @@
       <c r="X61" s="78"/>
       <c r="Y61" s="78"/>
       <c r="Z61" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AA61" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="62" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="94"/>
       <c r="B62" s="89"/>
       <c r="C62" s="88" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D62" s="88"/>
       <c r="E62" s="74"/>
       <c r="F62" s="101"/>
       <c r="G62" s="92"/>
       <c r="H62" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I62" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J62" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K62" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L62" s="75"/>
       <c r="M62" s="74"/>
       <c r="N62" s="92"/>
       <c r="O62" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P62" s="92"/>
       <c r="Q62" s="92"/>
@@ -10606,39 +10608,39 @@
       <c r="X62" s="78"/>
       <c r="Y62" s="78"/>
       <c r="Z62" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AA62" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="63" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="94"/>
       <c r="B63" s="89"/>
       <c r="C63" s="88" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D63" s="88"/>
       <c r="E63" s="74"/>
       <c r="F63" s="101"/>
       <c r="G63" s="92"/>
       <c r="H63" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I63" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J63" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K63" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L63" s="75"/>
       <c r="M63" s="74"/>
       <c r="N63" s="92"/>
       <c r="O63" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P63" s="92"/>
       <c r="Q63" s="92"/>
@@ -10651,35 +10653,35 @@
       <c r="X63" s="78"/>
       <c r="Y63" s="78"/>
       <c r="Z63" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AA63" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="64" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="94"/>
       <c r="B64" s="94"/>
       <c r="C64" s="93" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D64" s="93"/>
       <c r="E64" s="74"/>
       <c r="F64" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G64" s="92"/>
       <c r="H64" s="75"/>
       <c r="I64" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J64" s="75"/>
       <c r="K64" s="74"/>
       <c r="L64" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M64" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N64" s="92"/>
       <c r="O64" s="75"/>
@@ -10687,44 +10689,44 @@
       <c r="Q64" s="92"/>
       <c r="R64" s="92"/>
       <c r="S64" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T64" s="78"/>
       <c r="U64" s="78"/>
       <c r="V64" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W64" s="78"/>
       <c r="X64" s="78"/>
       <c r="Y64" s="78"/>
       <c r="Z64" s="78"/>
       <c r="AA64" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="94"/>
       <c r="B65" s="94"/>
       <c r="C65" s="93" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D65" s="93"/>
       <c r="E65" s="74"/>
       <c r="F65" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G65" s="92"/>
       <c r="H65" s="75"/>
       <c r="I65" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J65" s="75"/>
       <c r="K65" s="74"/>
       <c r="L65" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M65" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N65" s="92"/>
       <c r="O65" s="75"/>
@@ -10732,44 +10734,44 @@
       <c r="Q65" s="92"/>
       <c r="R65" s="92"/>
       <c r="S65" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T65" s="78"/>
       <c r="U65" s="78"/>
       <c r="V65" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W65" s="78"/>
       <c r="X65" s="78"/>
       <c r="Y65" s="78"/>
       <c r="Z65" s="78"/>
       <c r="AA65" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="94"/>
       <c r="B66" s="94"/>
       <c r="C66" s="93" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D66" s="93"/>
       <c r="E66" s="74"/>
       <c r="F66" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G66" s="92"/>
       <c r="H66" s="75"/>
       <c r="I66" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J66" s="75"/>
       <c r="K66" s="74"/>
       <c r="L66" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M66" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N66" s="92"/>
       <c r="O66" s="75"/>
@@ -10777,44 +10779,44 @@
       <c r="Q66" s="92"/>
       <c r="R66" s="92"/>
       <c r="S66" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T66" s="78"/>
       <c r="U66" s="78"/>
       <c r="V66" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W66" s="78"/>
       <c r="X66" s="78"/>
       <c r="Y66" s="78"/>
       <c r="Z66" s="78"/>
       <c r="AA66" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="94"/>
       <c r="B67" s="94"/>
       <c r="C67" s="93" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D67" s="93"/>
       <c r="E67" s="74"/>
       <c r="F67" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G67" s="92"/>
       <c r="H67" s="75"/>
       <c r="I67" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J67" s="75"/>
       <c r="K67" s="74"/>
       <c r="L67" s="75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M67" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N67" s="92"/>
       <c r="O67" s="75"/>
@@ -10822,44 +10824,44 @@
       <c r="Q67" s="92"/>
       <c r="R67" s="92"/>
       <c r="S67" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T67" s="78"/>
       <c r="U67" s="78"/>
       <c r="V67" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W67" s="78"/>
       <c r="X67" s="78"/>
       <c r="Y67" s="78"/>
       <c r="Z67" s="78"/>
       <c r="AA67" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="68" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="94"/>
       <c r="B68" s="94"/>
       <c r="C68" s="93" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D68" s="93"/>
       <c r="E68" s="74"/>
       <c r="F68" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G68" s="92"/>
       <c r="H68" s="75"/>
       <c r="I68" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J68" s="75"/>
       <c r="K68" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L68" s="75"/>
       <c r="M68" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N68" s="92"/>
       <c r="O68" s="75"/>
@@ -10867,19 +10869,19 @@
       <c r="Q68" s="92"/>
       <c r="R68" s="92"/>
       <c r="S68" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T68" s="78"/>
       <c r="U68" s="78"/>
       <c r="V68" s="78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W68" s="78"/>
       <c r="X68" s="78"/>
       <c r="Y68" s="78"/>
       <c r="Z68" s="78"/>
       <c r="AA68" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="69" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11210,14 +11212,14 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
@@ -11227,7 +11229,7 @@
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
       <c r="D3" s="113" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E3" s="111"/>
       <c r="F3" s="73"/>
@@ -11235,213 +11237,213 @@
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="68" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="65" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" s="66" t="s">
         <v>208</v>
       </c>
-      <c r="E4" s="66" t="s">
-        <v>209</v>
-      </c>
       <c r="F4" s="72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60"/>
       <c r="B5" s="59" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60"/>
       <c r="B6" s="59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E6" s="75"/>
       <c r="F6" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>
       <c r="B7" s="59" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E7" s="75"/>
       <c r="F7" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
       <c r="B8" s="59" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E8" s="75"/>
       <c r="F8" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60"/>
       <c r="B9" s="59" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C9" s="59"/>
       <c r="D9" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E9" s="75"/>
       <c r="F9" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="60"/>
       <c r="B10" s="59" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E10" s="75"/>
       <c r="F10" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="60"/>
       <c r="B11" s="59" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E11" s="75"/>
       <c r="F11" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60"/>
       <c r="B12" s="59" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E12" s="75"/>
       <c r="F12" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="59" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E13" s="75"/>
       <c r="F13" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="59" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E14" s="75"/>
       <c r="F14" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
       <c r="B15" s="81" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E15" s="75"/>
       <c r="F15" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
       <c r="B16" s="81" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C16" s="59"/>
       <c r="D16" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E16" s="75"/>
       <c r="F16" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="60"/>
       <c r="B17" s="59" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E17" s="75"/>
       <c r="F17" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="60"/>
       <c r="B18" s="59" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E18" s="75"/>
       <c r="F18" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11642,11 +11644,11 @@
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="39" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="39" t="s">
@@ -11654,7 +11656,7 @@
       </c>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K3" s="39"/>
       <c r="L3" s="39" t="s">
@@ -11662,7 +11664,7 @@
       </c>
       <c r="M3" s="39"/>
       <c r="N3" s="39" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11680,7 +11682,7 @@
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="58" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I4" s="58"/>
       <c r="J4" s="56" t="s">
@@ -11692,10 +11694,10 @@
       </c>
       <c r="M4" s="56"/>
       <c r="N4" s="56" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="83"/>
       <c r="B5" s="84" t="s">
         <v>184</v>
@@ -11710,7 +11712,7 @@
       </c>
       <c r="G5" s="84"/>
       <c r="H5" s="84" t="s">
-        <v>205</v>
+        <v>327</v>
       </c>
       <c r="I5" s="84"/>
       <c r="J5" s="84" t="s">
@@ -11722,7 +11724,7 @@
       </c>
       <c r="M5" s="84"/>
       <c r="N5" s="84" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -11732,7 +11734,7 @@
       </c>
       <c r="C6" s="84"/>
       <c r="D6" s="84" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E6" s="84"/>
       <c r="F6" s="84" t="s">
@@ -11740,7 +11742,7 @@
       </c>
       <c r="G6" s="84"/>
       <c r="H6" s="84" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I6" s="84"/>
       <c r="J6" s="84" t="s">
@@ -11752,7 +11754,7 @@
       </c>
       <c r="M6" s="84"/>
       <c r="N6" s="84" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
@@ -11766,11 +11768,11 @@
       </c>
       <c r="E7" s="84"/>
       <c r="F7" s="84" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G7" s="84"/>
       <c r="H7" s="84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I7" s="84"/>
       <c r="J7" s="84" t="s">
@@ -11782,7 +11784,7 @@
       </c>
       <c r="M7" s="84"/>
       <c r="N7" s="84" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -11849,7 +11851,7 @@
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -11859,7 +11861,7 @@
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B13" s="56"/>
       <c r="C13" s="56"/>

</xml_diff>

<commit_message>
Added content to table on org studies
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="330">
   <si>
     <t>Total</t>
   </si>
@@ -731,10 +731,6 @@
 Correlation among measures</t>
   </si>
   <si>
-    <t>Participant observation
-Ethnography</t>
-  </si>
-  <si>
     <t>Typologies
 Theoretical frameworks
 Prescriptions for management practice</t>
@@ -754,32 +750,6 @@
     <t>Typical Types of Research Output</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Hatch, M. J. (1997). </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Organization theory: Modern, symbolic interpretivism, and postmodern perspectives </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(p. 49). New York, NY: Oxford University Press.</t>
-    </r>
-  </si>
-  <si>
     <t>Deconstruction of theories and practices
 Negation of assumptions
 Reflexivity</t>
@@ -788,9 +758,6 @@
     <t>Even if there is an objective reality, all knowledge is filtered by the experience of the observer.  The organization is a subject whose meaning is to be understood and appreciated.</t>
   </si>
   <si>
-    <t>Comparison of Perspectives and Schools of Thought in Organization Studies</t>
-  </si>
-  <si>
     <t>How organizations affect society.
 How organization activities are coordinated.</t>
   </si>
@@ -798,9 +765,6 @@
     <t>How to maximize the rationality and efficiency organization activities.</t>
   </si>
   <si>
-    <t>How theory and theorizing practices affect our understanding of organizations.</t>
-  </si>
-  <si>
     <t>There is an objective reality independent of the observer that can only be known through reasoned and logical analysis of data and information gathered from sensory experience. The organization is an object that can be measured and analyzed.</t>
   </si>
   <si>
@@ -813,10 +777,6 @@
     <t>The organization is a machine that management designs, constructs, and maintains to achieve specific goals and objectives.</t>
   </si>
   <si>
-    <t>The abstraction we call the organization is a collage composed of bits of knowledge and understanding that form a new perspective when rearranged.
-The organization is a text, a narrative, and a discourse.</t>
-  </si>
-  <si>
     <t>Supply-Side</t>
   </si>
   <si>
@@ -827,10 +787,6 @@
   </si>
   <si>
     <t>Studies</t>
-  </si>
-  <si>
-    <t>Autopoietic systems theory
-Discourse theory</t>
   </si>
   <si>
     <r>
@@ -1218,28 +1174,107 @@
     <t>Models, Theories, and Schools of Thought</t>
   </si>
   <si>
+    <t>Bureacracy theory
+Scientific management</t>
+  </si>
+  <si>
+    <t>Since all knowledge is filtered by the experience of the observer, all distinctions used to describe reality are arbitrary and semantic in origin.  The organization is an abstraction that is best understood by revealing the underlying assumptions used to construct it and considering their implications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The organization is a living organism comprised of systems that perform the functions necessary for its survival. </t>
+  </si>
+  <si>
+    <t>How theory and theorizing practices affect our understanding of the concept of the organization.</t>
+  </si>
+  <si>
+    <t>The abstraction we call the organization is a collage composed of bits of meaning that form a new perspective when rearranged.
+The organization is a text, a narrative, and a discourse.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hatch, M. J. (1997). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Organization theory: Modern, symbolic, and postmodern perspectives</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. New York, NY: Oxford University Press.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hatch, M. J. (2018). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Organization theory: Modern, symbolic, and postmodern perspectives </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Fourth Ed.). New York, NY: Oxford University Press.</t>
+    </r>
+  </si>
+  <si>
     <t>Scientific management
 Administrative theory
+Contingency theory
 Econometric
-Open systems theory</t>
-  </si>
-  <si>
-    <t>Bureacracy theory
-Scientific management</t>
-  </si>
-  <si>
-    <t>Since all knowledge is filtered by the experience of the observer, all distinctions used to describe reality are arbitrary and semantic in origin.  The organization is an abstraction that is best understood by revealing the underlying assumptions used to construct it and considering their implications.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The organization is a living organism comprised of systems that perform the functions necessary for its survival. </t>
-  </si>
-  <si>
-    <t>Administrative theory
+Rational model of decision making
+Open systems theory
+Resource dependence theory
+Population ecology
+Socio-technical systems theory</t>
+  </si>
+  <si>
+    <t>Enactment theory
 Human relations management
+Neo-Institutional theory
 Coalition model of decision-making
 Garbage can model of decision-making
-Incremental model of decision-making
-Rational model of decision-making</t>
+Incremental model of decision-making</t>
+  </si>
+  <si>
+    <t>Participant observation
+Ethnography
+Grounded theory</t>
+  </si>
+  <si>
+    <t>Antenarrative theory
+Autopoietic systems theory
+Discourse theory
+Hegemonic resistance
+Intertextuality theory</t>
+  </si>
+  <si>
+    <t>Comparison of Perspectives Applied in Organization Studies</t>
   </si>
 </sst>
 </file>
@@ -7429,7 +7464,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7890,7 +7925,7 @@
     </row>
     <row r="2" spans="1:27" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="E2" s="61"/>
       <c r="F2" s="61"/>
@@ -7922,26 +7957,26 @@
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
       <c r="E3" s="113" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F3" s="114"/>
       <c r="G3" s="114"/>
       <c r="H3" s="111"/>
       <c r="I3" s="110" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="J3" s="111"/>
       <c r="K3" s="110" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="L3" s="112"/>
       <c r="M3" s="113" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="N3" s="114"/>
       <c r="O3" s="111"/>
       <c r="P3" s="115" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="Q3" s="114"/>
       <c r="R3" s="114"/>
@@ -7958,84 +7993,84 @@
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="104" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="68"/>
       <c r="E4" s="105" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="F4" s="107" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="G4" s="62" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="H4" s="106" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="I4" s="65" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="J4" s="66" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="K4" s="65" t="s">
+        <v>261</v>
+      </c>
+      <c r="L4" s="66" t="s">
+        <v>262</v>
+      </c>
+      <c r="M4" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="N4" s="62" t="s">
+        <v>298</v>
+      </c>
+      <c r="O4" s="106" t="s">
+        <v>296</v>
+      </c>
+      <c r="P4" s="62" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q4" s="62" t="s">
+        <v>240</v>
+      </c>
+      <c r="R4" s="62" t="s">
+        <v>241</v>
+      </c>
+      <c r="S4" s="62" t="s">
+        <v>213</v>
+      </c>
+      <c r="T4" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="U4" s="62" t="s">
+        <v>242</v>
+      </c>
+      <c r="V4" s="62" t="s">
+        <v>214</v>
+      </c>
+      <c r="W4" s="62" t="s">
+        <v>238</v>
+      </c>
+      <c r="X4" s="62" t="s">
+        <v>239</v>
+      </c>
+      <c r="Y4" s="62" t="s">
+        <v>281</v>
+      </c>
+      <c r="Z4" s="62" t="s">
         <v>267</v>
       </c>
-      <c r="L4" s="66" t="s">
-        <v>268</v>
-      </c>
-      <c r="M4" s="105" t="s">
-        <v>303</v>
-      </c>
-      <c r="N4" s="62" t="s">
-        <v>304</v>
-      </c>
-      <c r="O4" s="106" t="s">
-        <v>302</v>
-      </c>
-      <c r="P4" s="62" t="s">
-        <v>293</v>
-      </c>
-      <c r="Q4" s="62" t="s">
-        <v>246</v>
-      </c>
-      <c r="R4" s="62" t="s">
-        <v>247</v>
-      </c>
-      <c r="S4" s="62" t="s">
-        <v>219</v>
-      </c>
-      <c r="T4" s="62" t="s">
-        <v>242</v>
-      </c>
-      <c r="U4" s="62" t="s">
-        <v>248</v>
-      </c>
-      <c r="V4" s="62" t="s">
-        <v>220</v>
-      </c>
-      <c r="W4" s="62" t="s">
-        <v>244</v>
-      </c>
-      <c r="X4" s="62" t="s">
-        <v>245</v>
-      </c>
-      <c r="Y4" s="62" t="s">
-        <v>287</v>
-      </c>
-      <c r="Z4" s="62" t="s">
-        <v>273</v>
-      </c>
       <c r="AA4" s="72" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="49" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C5" s="93"/>
       <c r="D5" s="93"/>
@@ -8067,25 +8102,25 @@
       <c r="A6" s="94"/>
       <c r="B6" s="82"/>
       <c r="C6" s="81" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D6" s="81"/>
       <c r="E6" s="74"/>
       <c r="F6" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G6" s="92"/>
       <c r="H6" s="75"/>
       <c r="I6" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J6" s="75"/>
       <c r="K6" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L6" s="75"/>
       <c r="M6" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N6" s="92"/>
       <c r="O6" s="75"/>
@@ -8094,7 +8129,7 @@
       <c r="R6" s="92"/>
       <c r="S6" s="78"/>
       <c r="T6" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U6" s="78"/>
       <c r="V6" s="78"/>
@@ -8103,32 +8138,32 @@
       <c r="Y6" s="78"/>
       <c r="Z6" s="78"/>
       <c r="AA6" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="94"/>
       <c r="B7" s="82"/>
       <c r="C7" s="93" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D7" s="81"/>
       <c r="E7" s="74"/>
       <c r="F7" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G7" s="92"/>
       <c r="H7" s="75"/>
       <c r="I7" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J7" s="75"/>
       <c r="K7" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L7" s="75"/>
       <c r="M7" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N7" s="92"/>
       <c r="O7" s="75"/>
@@ -8137,7 +8172,7 @@
       <c r="R7" s="92"/>
       <c r="S7" s="78"/>
       <c r="T7" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U7" s="78"/>
       <c r="V7" s="78"/>
@@ -8146,32 +8181,32 @@
       <c r="Y7" s="78"/>
       <c r="Z7" s="78"/>
       <c r="AA7" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="94"/>
       <c r="B8" s="82"/>
       <c r="C8" s="81" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D8" s="81"/>
       <c r="E8" s="74"/>
       <c r="F8" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G8" s="92"/>
       <c r="H8" s="75"/>
       <c r="I8" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J8" s="75"/>
       <c r="K8" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L8" s="75"/>
       <c r="M8" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N8" s="92"/>
       <c r="O8" s="75"/>
@@ -8180,7 +8215,7 @@
       <c r="R8" s="92"/>
       <c r="S8" s="78"/>
       <c r="T8" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U8" s="78"/>
       <c r="V8" s="78"/>
@@ -8189,47 +8224,47 @@
       <c r="Y8" s="78"/>
       <c r="Z8" s="78"/>
       <c r="AA8" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="94"/>
       <c r="B9" s="82"/>
       <c r="C9" s="93" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D9" s="81"/>
       <c r="E9" s="74"/>
       <c r="F9" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G9" s="92"/>
       <c r="H9" s="75"/>
       <c r="I9" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J9" s="75"/>
       <c r="K9" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L9" s="75"/>
       <c r="M9" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N9" s="92"/>
       <c r="O9" s="75"/>
       <c r="P9" s="92"/>
       <c r="Q9" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R9" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S9" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T9" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U9" s="78"/>
       <c r="V9" s="78"/>
@@ -8238,104 +8273,104 @@
       <c r="Y9" s="78"/>
       <c r="Z9" s="78"/>
       <c r="AA9" s="63" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
       <c r="B10" s="30"/>
       <c r="C10" s="32" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="74"/>
       <c r="F10" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G10" s="92"/>
       <c r="H10" s="75"/>
       <c r="I10" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J10" s="75"/>
       <c r="K10" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L10" s="75"/>
       <c r="M10" s="74"/>
       <c r="N10" s="92"/>
       <c r="O10" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P10" s="92"/>
       <c r="Q10" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R10" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S10" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T10" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U10" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="V10" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W10" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="X10" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Y10" s="78"/>
       <c r="Z10" s="78"/>
       <c r="AA10" s="63" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="94"/>
       <c r="B11" s="82"/>
       <c r="C11" s="95" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D11" s="81"/>
       <c r="E11" s="96"/>
       <c r="F11" s="102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G11" s="98"/>
       <c r="H11" s="97"/>
       <c r="I11" s="96" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J11" s="97"/>
       <c r="K11" s="96" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L11" s="97"/>
       <c r="M11" s="96" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N11" s="98"/>
       <c r="O11" s="97"/>
       <c r="P11" s="98"/>
       <c r="Q11" s="98" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R11" s="98" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S11" s="99" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T11" s="99" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U11" s="99"/>
       <c r="V11" s="99"/>
@@ -8344,7 +8379,7 @@
       <c r="Y11" s="99"/>
       <c r="Z11" s="99"/>
       <c r="AA11" s="100" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -8379,7 +8414,7 @@
     <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="49" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C13" s="93"/>
       <c r="D13" s="93"/>
@@ -8411,241 +8446,241 @@
       <c r="A14" s="94"/>
       <c r="B14" s="30"/>
       <c r="C14" s="32" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="74"/>
       <c r="F14" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G14" s="92"/>
       <c r="H14" s="75"/>
       <c r="I14" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J14" s="75"/>
       <c r="K14" s="74"/>
       <c r="L14" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M14" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N14" s="92"/>
       <c r="O14" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P14" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Q14" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R14" s="92"/>
       <c r="S14" s="78"/>
       <c r="T14" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U14" s="78"/>
       <c r="V14" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W14" s="78"/>
       <c r="X14" s="78"/>
       <c r="Y14" s="78"/>
       <c r="Z14" s="78"/>
       <c r="AA14" s="63" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="94"/>
       <c r="B15" s="30"/>
       <c r="C15" s="32" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="74"/>
       <c r="F15" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G15" s="92"/>
       <c r="H15" s="75"/>
       <c r="I15" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J15" s="75"/>
       <c r="K15" s="74"/>
       <c r="L15" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M15" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N15" s="92"/>
       <c r="O15" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P15" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Q15" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R15" s="92"/>
       <c r="S15" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T15" s="78"/>
       <c r="U15" s="78"/>
       <c r="V15" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W15" s="78"/>
       <c r="X15" s="78"/>
       <c r="Y15" s="78"/>
       <c r="Z15" s="78"/>
       <c r="AA15" s="63" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="94"/>
       <c r="B16" s="82"/>
       <c r="C16" s="81" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D16" s="81"/>
       <c r="E16" s="74"/>
       <c r="F16" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G16" s="92"/>
       <c r="H16" s="75"/>
       <c r="I16" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J16" s="75"/>
       <c r="K16" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L16" s="75"/>
       <c r="M16" s="74"/>
       <c r="N16" s="92"/>
       <c r="O16" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P16" s="92"/>
       <c r="Q16" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R16" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S16" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T16" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U16" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="V16" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W16" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="X16" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Y16" s="78"/>
       <c r="Z16" s="78"/>
       <c r="AA16" s="63" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="94"/>
       <c r="B17" s="82"/>
       <c r="C17" s="81" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D17" s="81"/>
       <c r="E17" s="74"/>
       <c r="F17" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G17" s="92"/>
       <c r="H17" s="75"/>
       <c r="I17" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J17" s="75"/>
       <c r="K17" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L17" s="75"/>
       <c r="M17" s="74"/>
       <c r="N17" s="92"/>
       <c r="O17" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P17" s="92"/>
       <c r="Q17" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R17" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S17" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T17" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U17" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="V17" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W17" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="X17" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Y17" s="78"/>
       <c r="Z17" s="78"/>
       <c r="AA17" s="63" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="94"/>
       <c r="B18" s="60"/>
       <c r="C18" s="59" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D18" s="59"/>
       <c r="E18" s="74"/>
       <c r="F18" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G18" s="92"/>
       <c r="H18" s="75"/>
       <c r="I18" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J18" s="75"/>
       <c r="K18" s="74"/>
       <c r="L18" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M18" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N18" s="92"/>
       <c r="O18" s="75"/>
@@ -8656,39 +8691,39 @@
       <c r="T18" s="78"/>
       <c r="U18" s="78"/>
       <c r="V18" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W18" s="78"/>
       <c r="X18" s="78"/>
       <c r="Y18" s="78"/>
       <c r="Z18" s="78"/>
       <c r="AA18" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="94"/>
       <c r="B19" s="30"/>
       <c r="C19" s="32" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="74"/>
       <c r="F19" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G19" s="92"/>
       <c r="H19" s="75"/>
       <c r="I19" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J19" s="75"/>
       <c r="K19" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L19" s="75"/>
       <c r="M19" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N19" s="92"/>
       <c r="O19" s="75"/>
@@ -8696,7 +8731,7 @@
       <c r="Q19" s="92"/>
       <c r="R19" s="92"/>
       <c r="S19" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T19" s="78"/>
       <c r="U19" s="78"/>
@@ -8706,32 +8741,32 @@
       <c r="Y19" s="78"/>
       <c r="Z19" s="78"/>
       <c r="AA19" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="94"/>
       <c r="B20" s="30"/>
       <c r="C20" s="32" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="74"/>
       <c r="F20" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G20" s="92"/>
       <c r="H20" s="75"/>
       <c r="I20" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J20" s="75"/>
       <c r="K20" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L20" s="75"/>
       <c r="M20" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N20" s="92"/>
       <c r="O20" s="75"/>
@@ -8739,7 +8774,7 @@
       <c r="Q20" s="92"/>
       <c r="R20" s="92"/>
       <c r="S20" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T20" s="78"/>
       <c r="U20" s="78"/>
@@ -8749,32 +8784,32 @@
       <c r="Y20" s="78"/>
       <c r="Z20" s="78"/>
       <c r="AA20" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="94"/>
       <c r="B21" s="30"/>
       <c r="C21" s="32" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="74"/>
       <c r="F21" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G21" s="92"/>
       <c r="H21" s="75"/>
       <c r="I21" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J21" s="75"/>
       <c r="K21" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L21" s="75"/>
       <c r="M21" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N21" s="92"/>
       <c r="O21" s="75"/>
@@ -8782,7 +8817,7 @@
       <c r="Q21" s="92"/>
       <c r="R21" s="92"/>
       <c r="S21" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T21" s="78"/>
       <c r="U21" s="78"/>
@@ -8792,349 +8827,349 @@
       <c r="Y21" s="78"/>
       <c r="Z21" s="78"/>
       <c r="AA21" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="94"/>
       <c r="B22" s="82"/>
       <c r="C22" s="81" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D22" s="81"/>
       <c r="E22" s="74"/>
       <c r="F22" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G22" s="92"/>
       <c r="H22" s="75"/>
       <c r="I22" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J22" s="75"/>
       <c r="K22" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L22" s="75"/>
       <c r="M22" s="74"/>
       <c r="N22" s="92"/>
       <c r="O22" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P22" s="92"/>
       <c r="Q22" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R22" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S22" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T22" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U22" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="V22" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W22" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="X22" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Y22" s="78"/>
       <c r="Z22" s="78"/>
       <c r="AA22" s="63" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="94"/>
       <c r="B23" s="82"/>
       <c r="C23" s="81" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="D23" s="81"/>
       <c r="E23" s="74"/>
       <c r="F23" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G23" s="92"/>
       <c r="H23" s="75"/>
       <c r="I23" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J23" s="75"/>
       <c r="K23" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L23" s="75"/>
       <c r="M23" s="74"/>
       <c r="N23" s="92"/>
       <c r="O23" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P23" s="92"/>
       <c r="Q23" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R23" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S23" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T23" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U23" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="V23" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W23" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="X23" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Y23" s="78"/>
       <c r="Z23" s="78"/>
       <c r="AA23" s="63" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="94"/>
       <c r="B24" s="30"/>
       <c r="C24" s="32" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="74"/>
       <c r="F24" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G24" s="92"/>
       <c r="H24" s="75"/>
       <c r="I24" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J24" s="75"/>
       <c r="K24" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L24" s="75"/>
       <c r="M24" s="74"/>
       <c r="N24" s="92"/>
       <c r="O24" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P24" s="92"/>
       <c r="Q24" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R24" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S24" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T24" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U24" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="V24" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W24" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="X24" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Y24" s="78"/>
       <c r="Z24" s="78"/>
       <c r="AA24" s="63" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="94"/>
       <c r="B25" s="30"/>
       <c r="C25" s="32" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="74"/>
       <c r="F25" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G25" s="92"/>
       <c r="H25" s="75"/>
       <c r="I25" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J25" s="75"/>
       <c r="K25" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L25" s="75"/>
       <c r="M25" s="74"/>
       <c r="N25" s="92"/>
       <c r="O25" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P25" s="92"/>
       <c r="Q25" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R25" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S25" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T25" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U25" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="V25" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W25" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="X25" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Y25" s="78"/>
       <c r="Z25" s="78"/>
       <c r="AA25" s="63" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="94"/>
       <c r="B26" s="82"/>
       <c r="C26" s="81" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D26" s="81"/>
       <c r="E26" s="74"/>
       <c r="F26" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G26" s="92"/>
       <c r="H26" s="75"/>
       <c r="I26" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J26" s="75"/>
       <c r="K26" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L26" s="75"/>
       <c r="M26" s="74"/>
       <c r="N26" s="92"/>
       <c r="O26" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P26" s="92"/>
       <c r="Q26" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R26" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S26" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T26" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U26" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="V26" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W26" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="X26" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Y26" s="78"/>
       <c r="Z26" s="78"/>
       <c r="AA26" s="63" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="94"/>
       <c r="B27" s="82"/>
       <c r="C27" s="81" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D27" s="81"/>
       <c r="E27" s="74"/>
       <c r="F27" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G27" s="92"/>
       <c r="H27" s="75"/>
       <c r="I27" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J27" s="75"/>
       <c r="K27" s="74"/>
       <c r="L27" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M27" s="74"/>
       <c r="N27" s="92"/>
       <c r="O27" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P27" s="92"/>
       <c r="Q27" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R27" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S27" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T27" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U27" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="V27" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W27" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="X27" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Y27" s="78"/>
       <c r="Z27" s="78"/>
       <c r="AA27" s="63" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9169,7 +9204,7 @@
     <row r="29" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="94"/>
       <c r="B29" s="31" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C29" s="93"/>
       <c r="D29" s="93"/>
@@ -9201,40 +9236,40 @@
       <c r="A30" s="94"/>
       <c r="B30" s="82"/>
       <c r="C30" s="81" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D30" s="81"/>
       <c r="E30" s="74"/>
       <c r="F30" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G30" s="92"/>
       <c r="H30" s="75"/>
       <c r="I30" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J30" s="75"/>
       <c r="K30" s="74"/>
       <c r="L30" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M30" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N30" s="92"/>
       <c r="O30" s="75"/>
       <c r="P30" s="92"/>
       <c r="Q30" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R30" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S30" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T30" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U30" s="78"/>
       <c r="V30" s="78"/>
@@ -9243,32 +9278,32 @@
       <c r="Y30" s="78"/>
       <c r="Z30" s="78"/>
       <c r="AA30" s="63" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="31" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="94"/>
       <c r="B31" s="94"/>
       <c r="C31" s="93" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D31" s="93"/>
       <c r="E31" s="74"/>
       <c r="F31" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G31" s="92"/>
       <c r="H31" s="75"/>
       <c r="I31" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J31" s="75"/>
       <c r="K31" s="74"/>
       <c r="L31" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M31" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N31" s="92"/>
       <c r="O31" s="75"/>
@@ -9277,7 +9312,7 @@
       <c r="R31" s="92"/>
       <c r="S31" s="78"/>
       <c r="T31" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U31" s="78"/>
       <c r="V31" s="78"/>
@@ -9286,32 +9321,32 @@
       <c r="Y31" s="78"/>
       <c r="Z31" s="78"/>
       <c r="AA31" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="94"/>
       <c r="B32" s="94"/>
       <c r="C32" s="93" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D32" s="93"/>
       <c r="E32" s="74"/>
       <c r="F32" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G32" s="92"/>
       <c r="H32" s="75"/>
       <c r="I32" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J32" s="75"/>
       <c r="K32" s="74"/>
       <c r="L32" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M32" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N32" s="92"/>
       <c r="O32" s="75"/>
@@ -9320,7 +9355,7 @@
       <c r="R32" s="92"/>
       <c r="S32" s="78"/>
       <c r="T32" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U32" s="78"/>
       <c r="V32" s="78"/>
@@ -9329,38 +9364,38 @@
       <c r="Y32" s="78"/>
       <c r="Z32" s="78"/>
       <c r="AA32" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="94"/>
       <c r="B33" s="94"/>
       <c r="C33" s="93" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D33" s="93"/>
       <c r="E33" s="74"/>
       <c r="F33" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G33" s="92"/>
       <c r="H33" s="75"/>
       <c r="I33" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J33" s="75"/>
       <c r="K33" s="74"/>
       <c r="L33" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M33" s="74"/>
       <c r="N33" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="O33" s="75"/>
       <c r="P33" s="92"/>
       <c r="Q33" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R33" s="92"/>
       <c r="S33" s="78"/>
@@ -9372,7 +9407,7 @@
       <c r="Y33" s="78"/>
       <c r="Z33" s="78"/>
       <c r="AA33" s="63" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="34" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9407,7 +9442,7 @@
     <row r="35" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
       <c r="B35" s="49" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C35" s="93"/>
       <c r="D35" s="93"/>
@@ -9439,25 +9474,25 @@
       <c r="A36" s="94"/>
       <c r="B36" s="30"/>
       <c r="C36" s="32" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D36" s="32"/>
       <c r="E36" s="74"/>
       <c r="F36" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G36" s="92"/>
       <c r="H36" s="75"/>
       <c r="I36" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J36" s="75"/>
       <c r="K36" s="74"/>
       <c r="L36" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M36" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N36" s="92"/>
       <c r="O36" s="75"/>
@@ -9465,7 +9500,7 @@
       <c r="Q36" s="92"/>
       <c r="R36" s="92"/>
       <c r="S36" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T36" s="78"/>
       <c r="U36" s="78"/>
@@ -9475,32 +9510,32 @@
       <c r="Y36" s="78"/>
       <c r="Z36" s="78"/>
       <c r="AA36" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="94"/>
       <c r="B37" s="30"/>
       <c r="C37" s="32" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D37" s="32"/>
       <c r="E37" s="74"/>
       <c r="F37" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G37" s="92"/>
       <c r="H37" s="75"/>
       <c r="I37" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J37" s="75"/>
       <c r="K37" s="74"/>
       <c r="L37" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M37" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N37" s="92"/>
       <c r="O37" s="75"/>
@@ -9511,39 +9546,39 @@
       <c r="T37" s="78"/>
       <c r="U37" s="78"/>
       <c r="V37" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W37" s="78"/>
       <c r="X37" s="78"/>
       <c r="Y37" s="78"/>
       <c r="Z37" s="78"/>
       <c r="AA37" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="94"/>
       <c r="B38" s="94"/>
       <c r="C38" s="93" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D38" s="93"/>
       <c r="E38" s="74"/>
       <c r="F38" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G38" s="92"/>
       <c r="H38" s="75"/>
       <c r="I38" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J38" s="75"/>
       <c r="K38" s="74"/>
       <c r="L38" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M38" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N38" s="92"/>
       <c r="O38" s="75"/>
@@ -9551,7 +9586,7 @@
       <c r="Q38" s="92"/>
       <c r="R38" s="92"/>
       <c r="S38" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T38" s="78"/>
       <c r="U38" s="78"/>
@@ -9561,32 +9596,32 @@
       <c r="Y38" s="78"/>
       <c r="Z38" s="78"/>
       <c r="AA38" s="63" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="94"/>
       <c r="B39" s="94"/>
       <c r="C39" s="93" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D39" s="93"/>
       <c r="E39" s="74"/>
       <c r="F39" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G39" s="92"/>
       <c r="H39" s="75"/>
       <c r="I39" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J39" s="75"/>
       <c r="K39" s="74"/>
       <c r="L39" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M39" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N39" s="92"/>
       <c r="O39" s="75"/>
@@ -9594,44 +9629,44 @@
       <c r="Q39" s="92"/>
       <c r="R39" s="92"/>
       <c r="S39" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T39" s="78"/>
       <c r="U39" s="78"/>
       <c r="V39" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W39" s="78"/>
       <c r="X39" s="78"/>
       <c r="Y39" s="78"/>
       <c r="Z39" s="78"/>
       <c r="AA39" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="94"/>
       <c r="B40" s="94"/>
       <c r="C40" s="93" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D40" s="93"/>
       <c r="E40" s="74"/>
       <c r="F40" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G40" s="92"/>
       <c r="H40" s="75"/>
       <c r="I40" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J40" s="75"/>
       <c r="K40" s="74"/>
       <c r="L40" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M40" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N40" s="92"/>
       <c r="O40" s="75"/>
@@ -9639,93 +9674,93 @@
       <c r="Q40" s="92"/>
       <c r="R40" s="92"/>
       <c r="S40" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T40" s="78"/>
       <c r="U40" s="78"/>
       <c r="V40" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W40" s="78"/>
       <c r="X40" s="78"/>
       <c r="Y40" s="78"/>
       <c r="Z40" s="78"/>
       <c r="AA40" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="94"/>
       <c r="B41" s="94"/>
       <c r="C41" s="93" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D41" s="93"/>
       <c r="E41" s="74"/>
       <c r="F41" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G41" s="92"/>
       <c r="H41" s="75"/>
       <c r="I41" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J41" s="75"/>
       <c r="K41" s="74"/>
       <c r="L41" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M41" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N41" s="92"/>
       <c r="O41" s="75"/>
       <c r="P41" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Q41" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R41" s="92"/>
       <c r="S41" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T41" s="78"/>
       <c r="U41" s="78"/>
       <c r="V41" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W41" s="78"/>
       <c r="X41" s="78"/>
       <c r="Y41" s="78"/>
       <c r="Z41" s="78"/>
       <c r="AA41" s="63" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="42" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="94"/>
       <c r="B42" s="94"/>
       <c r="C42" s="93" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D42" s="93"/>
       <c r="E42" s="74"/>
       <c r="F42" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G42" s="92"/>
       <c r="H42" s="75"/>
       <c r="I42" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J42" s="75"/>
       <c r="K42" s="74"/>
       <c r="L42" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M42" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N42" s="92"/>
       <c r="O42" s="75"/>
@@ -9734,7 +9769,7 @@
       <c r="R42" s="92"/>
       <c r="S42" s="78"/>
       <c r="T42" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U42" s="78"/>
       <c r="V42" s="78"/>
@@ -9743,32 +9778,32 @@
       <c r="Y42" s="78"/>
       <c r="Z42" s="78"/>
       <c r="AA42" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="43" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="94"/>
       <c r="B43" s="94"/>
       <c r="C43" s="93" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D43" s="93"/>
       <c r="E43" s="74"/>
       <c r="F43" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G43" s="92"/>
       <c r="H43" s="75"/>
       <c r="I43" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J43" s="75"/>
       <c r="K43" s="74"/>
       <c r="L43" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M43" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N43" s="92"/>
       <c r="O43" s="75"/>
@@ -9776,44 +9811,44 @@
       <c r="Q43" s="92"/>
       <c r="R43" s="92"/>
       <c r="S43" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T43" s="78"/>
       <c r="U43" s="78"/>
       <c r="V43" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W43" s="78"/>
       <c r="X43" s="78"/>
       <c r="Y43" s="78"/>
       <c r="Z43" s="78"/>
       <c r="AA43" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="44" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="94"/>
       <c r="B44" s="94"/>
       <c r="C44" s="93" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D44" s="93"/>
       <c r="E44" s="74"/>
       <c r="F44" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G44" s="92"/>
       <c r="H44" s="75"/>
       <c r="I44" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J44" s="75"/>
       <c r="K44" s="74"/>
       <c r="L44" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M44" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N44" s="92"/>
       <c r="O44" s="75"/>
@@ -9821,101 +9856,101 @@
       <c r="Q44" s="92"/>
       <c r="R44" s="92"/>
       <c r="S44" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T44" s="78"/>
       <c r="U44" s="78"/>
       <c r="V44" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W44" s="78"/>
       <c r="X44" s="78"/>
       <c r="Y44" s="78"/>
       <c r="Z44" s="78"/>
       <c r="AA44" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="94"/>
       <c r="B45" s="82"/>
       <c r="C45" s="81" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D45" s="81"/>
       <c r="E45" s="74"/>
       <c r="F45" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G45" s="92"/>
       <c r="H45" s="75"/>
       <c r="I45" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J45" s="75"/>
       <c r="K45" s="74"/>
       <c r="L45" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M45" s="74"/>
       <c r="N45" s="92"/>
       <c r="O45" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P45" s="92"/>
       <c r="Q45" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R45" s="92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S45" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T45" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U45" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="V45" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W45" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="X45" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Y45" s="78"/>
       <c r="Z45" s="78"/>
       <c r="AA45" s="63" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="94"/>
       <c r="B46" s="60"/>
       <c r="C46" s="59" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D46" s="59"/>
       <c r="E46" s="74"/>
       <c r="F46" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G46" s="92"/>
       <c r="H46" s="75"/>
       <c r="I46" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J46" s="75"/>
       <c r="K46" s="74"/>
       <c r="L46" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M46" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N46" s="92"/>
       <c r="O46" s="75"/>
@@ -9923,44 +9958,44 @@
       <c r="Q46" s="92"/>
       <c r="R46" s="92"/>
       <c r="S46" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T46" s="78"/>
       <c r="U46" s="78"/>
       <c r="V46" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W46" s="78"/>
       <c r="X46" s="78"/>
       <c r="Y46" s="78"/>
       <c r="Z46" s="78"/>
       <c r="AA46" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="94"/>
       <c r="B47" s="60"/>
       <c r="C47" s="59" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D47" s="59"/>
       <c r="E47" s="74"/>
       <c r="F47" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G47" s="92"/>
       <c r="H47" s="75"/>
       <c r="I47" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J47" s="75"/>
       <c r="K47" s="74"/>
       <c r="L47" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M47" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N47" s="92"/>
       <c r="O47" s="75"/>
@@ -9968,7 +10003,7 @@
       <c r="Q47" s="92"/>
       <c r="R47" s="92"/>
       <c r="S47" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T47" s="78"/>
       <c r="U47" s="78"/>
@@ -9978,32 +10013,32 @@
       <c r="Y47" s="78"/>
       <c r="Z47" s="78"/>
       <c r="AA47" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="48" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="94"/>
       <c r="B48" s="82"/>
       <c r="C48" s="81" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="D48" s="81"/>
       <c r="E48" s="74"/>
       <c r="F48" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G48" s="92"/>
       <c r="H48" s="75"/>
       <c r="I48" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J48" s="75"/>
       <c r="K48" s="74"/>
       <c r="L48" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M48" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N48" s="92"/>
       <c r="O48" s="75"/>
@@ -10012,7 +10047,7 @@
       <c r="R48" s="92"/>
       <c r="S48" s="78"/>
       <c r="T48" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U48" s="78"/>
       <c r="V48" s="78"/>
@@ -10021,32 +10056,32 @@
       <c r="Y48" s="78"/>
       <c r="Z48" s="78"/>
       <c r="AA48" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="49" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="94"/>
       <c r="B49" s="94"/>
       <c r="C49" s="93" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D49" s="93"/>
       <c r="E49" s="74"/>
       <c r="F49" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G49" s="92"/>
       <c r="H49" s="75"/>
       <c r="I49" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J49" s="75"/>
       <c r="K49" s="74"/>
       <c r="L49" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M49" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N49" s="92"/>
       <c r="O49" s="75"/>
@@ -10055,7 +10090,7 @@
       <c r="R49" s="92"/>
       <c r="S49" s="78"/>
       <c r="T49" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U49" s="78"/>
       <c r="V49" s="78"/>
@@ -10064,32 +10099,32 @@
       <c r="Y49" s="78"/>
       <c r="Z49" s="78"/>
       <c r="AA49" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="50" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="94"/>
       <c r="B50" s="82"/>
       <c r="C50" s="81" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="D50" s="81"/>
       <c r="E50" s="74"/>
       <c r="F50" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G50" s="92"/>
       <c r="H50" s="75"/>
       <c r="I50" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J50" s="75"/>
       <c r="K50" s="74"/>
       <c r="L50" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M50" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N50" s="92"/>
       <c r="O50" s="75"/>
@@ -10098,7 +10133,7 @@
       <c r="R50" s="92"/>
       <c r="S50" s="78"/>
       <c r="T50" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U50" s="78"/>
       <c r="V50" s="78"/>
@@ -10107,32 +10142,32 @@
       <c r="Y50" s="78"/>
       <c r="Z50" s="78"/>
       <c r="AA50" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="51" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="94"/>
       <c r="B51" s="82"/>
       <c r="C51" s="81" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D51" s="81"/>
       <c r="E51" s="74"/>
       <c r="F51" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G51" s="92"/>
       <c r="H51" s="75"/>
       <c r="I51" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J51" s="75"/>
       <c r="K51" s="74"/>
       <c r="L51" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M51" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N51" s="92"/>
       <c r="O51" s="75"/>
@@ -10141,7 +10176,7 @@
       <c r="R51" s="92"/>
       <c r="S51" s="78"/>
       <c r="T51" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U51" s="78"/>
       <c r="V51" s="78"/>
@@ -10150,32 +10185,32 @@
       <c r="Y51" s="78"/>
       <c r="Z51" s="78"/>
       <c r="AA51" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="52" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="94"/>
       <c r="B52" s="89"/>
       <c r="C52" s="88" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D52" s="88"/>
       <c r="E52" s="74"/>
       <c r="F52" s="101"/>
       <c r="G52" s="92"/>
       <c r="H52" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="I52" s="74"/>
       <c r="J52" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K52" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L52" s="75"/>
       <c r="M52" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N52" s="92"/>
       <c r="O52" s="75"/>
@@ -10190,35 +10225,35 @@
       <c r="X52" s="78"/>
       <c r="Y52" s="78"/>
       <c r="Z52" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AA52" s="63" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="53" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="94"/>
       <c r="B53" s="89"/>
       <c r="C53" s="88" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D53" s="88"/>
       <c r="E53" s="74"/>
       <c r="F53" s="101"/>
       <c r="G53" s="92"/>
       <c r="H53" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="I53" s="74"/>
       <c r="J53" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K53" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L53" s="75"/>
       <c r="M53" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N53" s="92"/>
       <c r="O53" s="75"/>
@@ -10233,10 +10268,10 @@
       <c r="X53" s="78"/>
       <c r="Y53" s="78"/>
       <c r="Z53" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AA53" s="63" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -10271,7 +10306,7 @@
     <row r="55" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49"/>
       <c r="B55" s="49" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C55" s="93"/>
       <c r="D55" s="93"/>
@@ -10303,29 +10338,29 @@
       <c r="A56" s="94"/>
       <c r="B56" s="89"/>
       <c r="C56" s="88" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D56" s="88"/>
       <c r="E56" s="74"/>
       <c r="F56" s="101"/>
       <c r="G56" s="92"/>
       <c r="H56" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="I56" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J56" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K56" s="74"/>
       <c r="L56" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M56" s="74"/>
       <c r="N56" s="92"/>
       <c r="O56" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P56" s="92"/>
       <c r="Q56" s="92"/>
@@ -10338,39 +10373,39 @@
       <c r="X56" s="78"/>
       <c r="Y56" s="78"/>
       <c r="Z56" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AA56" s="63" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="57" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="94"/>
       <c r="B57" s="89"/>
       <c r="C57" s="88" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D57" s="88"/>
       <c r="E57" s="74"/>
       <c r="F57" s="101"/>
       <c r="G57" s="92"/>
       <c r="H57" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="I57" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J57" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K57" s="74"/>
       <c r="L57" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M57" s="74"/>
       <c r="N57" s="92"/>
       <c r="O57" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P57" s="92"/>
       <c r="Q57" s="92"/>
@@ -10383,39 +10418,39 @@
       <c r="X57" s="78"/>
       <c r="Y57" s="78"/>
       <c r="Z57" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AA57" s="63" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="58" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="94"/>
       <c r="B58" s="89"/>
       <c r="C58" s="88" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D58" s="88"/>
       <c r="E58" s="74"/>
       <c r="F58" s="101"/>
       <c r="G58" s="92"/>
       <c r="H58" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="I58" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J58" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K58" s="74"/>
       <c r="L58" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M58" s="74"/>
       <c r="N58" s="92"/>
       <c r="O58" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P58" s="92"/>
       <c r="Q58" s="92"/>
@@ -10428,39 +10463,39 @@
       <c r="X58" s="78"/>
       <c r="Y58" s="78"/>
       <c r="Z58" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AA58" s="63" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="59" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="94"/>
       <c r="B59" s="89"/>
       <c r="C59" s="88" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D59" s="88"/>
       <c r="E59" s="74"/>
       <c r="F59" s="101"/>
       <c r="G59" s="92"/>
       <c r="H59" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="I59" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J59" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K59" s="74"/>
       <c r="L59" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M59" s="74"/>
       <c r="N59" s="92"/>
       <c r="O59" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P59" s="92"/>
       <c r="Q59" s="92"/>
@@ -10473,39 +10508,39 @@
       <c r="X59" s="78"/>
       <c r="Y59" s="78"/>
       <c r="Z59" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AA59" s="63" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="60" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="94"/>
       <c r="B60" s="89"/>
       <c r="C60" s="88" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D60" s="88"/>
       <c r="E60" s="74"/>
       <c r="F60" s="101"/>
       <c r="G60" s="92"/>
       <c r="H60" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="I60" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J60" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K60" s="74"/>
       <c r="L60" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M60" s="74"/>
       <c r="N60" s="92"/>
       <c r="O60" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P60" s="92"/>
       <c r="Q60" s="92"/>
@@ -10518,39 +10553,39 @@
       <c r="X60" s="78"/>
       <c r="Y60" s="78"/>
       <c r="Z60" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AA60" s="63" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="61" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="94"/>
       <c r="B61" s="89"/>
       <c r="C61" s="88" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D61" s="88"/>
       <c r="E61" s="74"/>
       <c r="F61" s="101"/>
       <c r="G61" s="92"/>
       <c r="H61" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="I61" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J61" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K61" s="74"/>
       <c r="L61" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M61" s="74"/>
       <c r="N61" s="92"/>
       <c r="O61" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P61" s="92"/>
       <c r="Q61" s="92"/>
@@ -10563,39 +10598,39 @@
       <c r="X61" s="78"/>
       <c r="Y61" s="78"/>
       <c r="Z61" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AA61" s="63" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="62" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="94"/>
       <c r="B62" s="89"/>
       <c r="C62" s="88" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D62" s="88"/>
       <c r="E62" s="74"/>
       <c r="F62" s="101"/>
       <c r="G62" s="92"/>
       <c r="H62" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="I62" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J62" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K62" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L62" s="75"/>
       <c r="M62" s="74"/>
       <c r="N62" s="92"/>
       <c r="O62" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P62" s="92"/>
       <c r="Q62" s="92"/>
@@ -10608,39 +10643,39 @@
       <c r="X62" s="78"/>
       <c r="Y62" s="78"/>
       <c r="Z62" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AA62" s="63" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="94"/>
       <c r="B63" s="89"/>
       <c r="C63" s="88" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D63" s="88"/>
       <c r="E63" s="74"/>
       <c r="F63" s="101"/>
       <c r="G63" s="92"/>
       <c r="H63" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="I63" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J63" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K63" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L63" s="75"/>
       <c r="M63" s="74"/>
       <c r="N63" s="92"/>
       <c r="O63" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P63" s="92"/>
       <c r="Q63" s="92"/>
@@ -10653,35 +10688,35 @@
       <c r="X63" s="78"/>
       <c r="Y63" s="78"/>
       <c r="Z63" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AA63" s="63" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="64" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="94"/>
       <c r="B64" s="94"/>
       <c r="C64" s="93" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D64" s="93"/>
       <c r="E64" s="74"/>
       <c r="F64" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G64" s="92"/>
       <c r="H64" s="75"/>
       <c r="I64" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J64" s="75"/>
       <c r="K64" s="74"/>
       <c r="L64" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M64" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N64" s="92"/>
       <c r="O64" s="75"/>
@@ -10689,44 +10724,44 @@
       <c r="Q64" s="92"/>
       <c r="R64" s="92"/>
       <c r="S64" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T64" s="78"/>
       <c r="U64" s="78"/>
       <c r="V64" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W64" s="78"/>
       <c r="X64" s="78"/>
       <c r="Y64" s="78"/>
       <c r="Z64" s="78"/>
       <c r="AA64" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="94"/>
       <c r="B65" s="94"/>
       <c r="C65" s="93" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D65" s="93"/>
       <c r="E65" s="74"/>
       <c r="F65" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G65" s="92"/>
       <c r="H65" s="75"/>
       <c r="I65" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J65" s="75"/>
       <c r="K65" s="74"/>
       <c r="L65" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M65" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N65" s="92"/>
       <c r="O65" s="75"/>
@@ -10734,44 +10769,44 @@
       <c r="Q65" s="92"/>
       <c r="R65" s="92"/>
       <c r="S65" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T65" s="78"/>
       <c r="U65" s="78"/>
       <c r="V65" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W65" s="78"/>
       <c r="X65" s="78"/>
       <c r="Y65" s="78"/>
       <c r="Z65" s="78"/>
       <c r="AA65" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="94"/>
       <c r="B66" s="94"/>
       <c r="C66" s="93" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D66" s="93"/>
       <c r="E66" s="74"/>
       <c r="F66" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G66" s="92"/>
       <c r="H66" s="75"/>
       <c r="I66" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J66" s="75"/>
       <c r="K66" s="74"/>
       <c r="L66" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M66" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N66" s="92"/>
       <c r="O66" s="75"/>
@@ -10779,44 +10814,44 @@
       <c r="Q66" s="92"/>
       <c r="R66" s="92"/>
       <c r="S66" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T66" s="78"/>
       <c r="U66" s="78"/>
       <c r="V66" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W66" s="78"/>
       <c r="X66" s="78"/>
       <c r="Y66" s="78"/>
       <c r="Z66" s="78"/>
       <c r="AA66" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="94"/>
       <c r="B67" s="94"/>
       <c r="C67" s="93" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D67" s="93"/>
       <c r="E67" s="74"/>
       <c r="F67" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G67" s="92"/>
       <c r="H67" s="75"/>
       <c r="I67" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J67" s="75"/>
       <c r="K67" s="74"/>
       <c r="L67" s="75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M67" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N67" s="92"/>
       <c r="O67" s="75"/>
@@ -10824,44 +10859,44 @@
       <c r="Q67" s="92"/>
       <c r="R67" s="92"/>
       <c r="S67" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T67" s="78"/>
       <c r="U67" s="78"/>
       <c r="V67" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W67" s="78"/>
       <c r="X67" s="78"/>
       <c r="Y67" s="78"/>
       <c r="Z67" s="78"/>
       <c r="AA67" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="94"/>
       <c r="B68" s="94"/>
       <c r="C68" s="93" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D68" s="93"/>
       <c r="E68" s="74"/>
       <c r="F68" s="101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G68" s="92"/>
       <c r="H68" s="75"/>
       <c r="I68" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J68" s="75"/>
       <c r="K68" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L68" s="75"/>
       <c r="M68" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N68" s="92"/>
       <c r="O68" s="75"/>
@@ -10869,19 +10904,19 @@
       <c r="Q68" s="92"/>
       <c r="R68" s="92"/>
       <c r="S68" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T68" s="78"/>
       <c r="U68" s="78"/>
       <c r="V68" s="78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W68" s="78"/>
       <c r="X68" s="78"/>
       <c r="Y68" s="78"/>
       <c r="Z68" s="78"/>
       <c r="AA68" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="69" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11212,14 +11247,14 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
@@ -11229,7 +11264,7 @@
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
       <c r="D3" s="113" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E3" s="111"/>
       <c r="F3" s="73"/>
@@ -11237,213 +11272,213 @@
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="68" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="65" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E4" s="66" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F4" s="72" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60"/>
       <c r="B5" s="59" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60"/>
       <c r="B6" s="59" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E6" s="75"/>
       <c r="F6" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>
       <c r="B7" s="59" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E7" s="75"/>
       <c r="F7" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
       <c r="B8" s="59" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E8" s="75"/>
       <c r="F8" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60"/>
       <c r="B9" s="59" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C9" s="59"/>
       <c r="D9" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E9" s="75"/>
       <c r="F9" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="60"/>
       <c r="B10" s="59" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E10" s="75"/>
       <c r="F10" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="60"/>
       <c r="B11" s="59" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E11" s="75"/>
       <c r="F11" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60"/>
       <c r="B12" s="59" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E12" s="75"/>
       <c r="F12" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="59" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E13" s="75"/>
       <c r="F13" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="59" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E14" s="75"/>
       <c r="F14" s="63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
       <c r="B15" s="81" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E15" s="75"/>
       <c r="F15" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
       <c r="B16" s="81" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C16" s="59"/>
       <c r="D16" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E16" s="75"/>
       <c r="F16" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="60"/>
       <c r="B17" s="59" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E17" s="75"/>
       <c r="F17" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="60"/>
       <c r="B18" s="59" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E18" s="75"/>
       <c r="F18" s="63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11600,7 +11635,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
@@ -11634,7 +11669,7 @@
     </row>
     <row r="2" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="86" t="s">
-        <v>198</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -11644,27 +11679,27 @@
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="39" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="39" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="K3" s="39"/>
       <c r="L3" s="39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M3" s="39"/>
       <c r="N3" s="39" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11674,15 +11709,15 @@
       </c>
       <c r="C4" s="56"/>
       <c r="D4" s="56" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="58" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="58" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I4" s="58"/>
       <c r="J4" s="56" t="s">
@@ -11690,29 +11725,29 @@
       </c>
       <c r="K4" s="56"/>
       <c r="L4" s="56" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M4" s="56"/>
       <c r="N4" s="56" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="83"/>
       <c r="B5" s="84" t="s">
         <v>184</v>
       </c>
       <c r="C5" s="84"/>
       <c r="D5" s="84" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E5" s="84"/>
       <c r="F5" s="84" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G5" s="84"/>
       <c r="H5" s="84" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="I5" s="84"/>
       <c r="J5" s="84" t="s">
@@ -11720,11 +11755,11 @@
       </c>
       <c r="K5" s="84"/>
       <c r="L5" s="84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M5" s="84"/>
       <c r="N5" s="84" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -11734,27 +11769,27 @@
       </c>
       <c r="C6" s="84"/>
       <c r="D6" s="84" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E6" s="84"/>
       <c r="F6" s="84" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G6" s="84"/>
       <c r="H6" s="84" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I6" s="84"/>
       <c r="J6" s="84" t="s">
-        <v>189</v>
+        <v>327</v>
       </c>
       <c r="K6" s="84"/>
       <c r="L6" s="84" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M6" s="84"/>
       <c r="N6" s="84" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
@@ -11764,27 +11799,27 @@
       </c>
       <c r="C7" s="84"/>
       <c r="D7" s="84" t="s">
-        <v>201</v>
+        <v>321</v>
       </c>
       <c r="E7" s="84"/>
       <c r="F7" s="84" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="G7" s="84"/>
       <c r="H7" s="84" t="s">
-        <v>206</v>
+        <v>322</v>
       </c>
       <c r="I7" s="84"/>
       <c r="J7" s="84" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K7" s="84"/>
       <c r="L7" s="84" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M7" s="84"/>
       <c r="N7" s="84" t="s">
-        <v>211</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -11841,7 +11876,7 @@
     </row>
     <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>195</v>
+        <v>323</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -11851,7 +11886,7 @@
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>213</v>
+        <v>324</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -11861,16 +11896,18 @@
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
+        <v>207</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>206</v>
+      </c>
       <c r="B14" s="56"/>
       <c r="C14" s="56"/>
       <c r="D14" s="56"/>
@@ -11886,18 +11923,10 @@
       <c r="N15" s="56"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="56"/>
       <c r="C16" s="56"/>
       <c r="D16" s="56"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
       <c r="M16" s="56"/>
       <c r="N16" s="56"/>
     </row>
@@ -12012,6 +12041,22 @@
       <c r="L23" s="56"/>
       <c r="M23" s="56"/>
       <c r="N23" s="56"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="57"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Annotation for Hatch (2018)
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -1243,17 +1243,6 @@
     </r>
   </si>
   <si>
-    <t>Scientific management
-Administrative theory
-Contingency theory
-Econometric
-Rational model of decision making
-Open systems theory
-Resource dependence theory
-Population ecology
-Socio-technical systems theory</t>
-  </si>
-  <si>
     <t>Enactment theory
 Human relations management
 Neo-Institutional theory
@@ -1275,6 +1264,20 @@
   </si>
   <si>
     <t>Comparison of Perspectives Applied in Organization Studies</t>
+  </si>
+  <si>
+    <t>Scientific management
+Administrative theory
+Agency theory
+Contingency theory
+Cybernetic theory
+Econometric
+Rational model of decision making
+Open systems theory
+Resource dependence theory
+Population ecology
+Socio-technical systems theory
+Transaction cost theory</t>
   </si>
 </sst>
 </file>
@@ -11669,7 +11672,7 @@
     </row>
     <row r="2" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="86" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -11732,7 +11735,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="83"/>
       <c r="B5" s="84" t="s">
         <v>184</v>
@@ -11759,7 +11762,7 @@
       </c>
       <c r="M5" s="84"/>
       <c r="N5" s="84" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -11781,7 +11784,7 @@
       </c>
       <c r="I6" s="84"/>
       <c r="J6" s="84" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K6" s="84"/>
       <c r="L6" s="84" t="s">
@@ -11789,7 +11792,7 @@
       </c>
       <c r="M6" s="84"/>
       <c r="N6" s="84" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
@@ -11819,7 +11822,7 @@
       </c>
       <c r="M7" s="84"/>
       <c r="N7" s="84" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modified figure for causal diagram
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -5608,14 +5608,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5630,7 +5630,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3048000" y="4333875"/>
+          <a:off x="3048000" y="4733925"/>
           <a:ext cx="1828800" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5678,7 +5678,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>3</a:t>
+            <a:t>n</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5866,13 +5866,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>533401</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>109535</xdr:rowOff>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5889,8 +5889,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="516731" y="2259805"/>
-          <a:ext cx="3157539" cy="1905000"/>
+          <a:off x="319088" y="2462212"/>
+          <a:ext cx="3552825" cy="1905000"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -6041,13 +6041,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -6064,8 +6064,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4876800" y="1647825"/>
-          <a:ext cx="1847850" cy="3143250"/>
+          <a:off x="4876800" y="1638300"/>
+          <a:ext cx="1847850" cy="3552825"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -6092,6 +6092,73 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>109538</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>166689</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>461963</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>52389</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B7D077-5FD9-4402-9CB4-F8AAA2C8A7B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3714751" y="4219576"/>
+          <a:ext cx="457200" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>. . .</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -7438,7 +7505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -11640,7 +11707,7 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>

</xml_diff>

<commit_message>
Added Munteanu (2012) and modified table on org studies
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -755,9 +755,6 @@
 Reflexivity</t>
   </si>
   <si>
-    <t>Even if there is an objective reality, all knowledge is filtered by the experience of the observer.  The organization is a subject whose meaning is to be understood and appreciated.</t>
-  </si>
-  <si>
     <t>How organizations affect society.
 How organization activities are coordinated.</t>
   </si>
@@ -766,9 +763,6 @@
   </si>
   <si>
     <t>There is an objective reality independent of the observer that can only be known through reasoned and logical analysis of data and information gathered from sensory experience. The organization is an object that can be measured and analyzed.</t>
-  </si>
-  <si>
-    <t>There is an objective reality independent of the observer.  The organization is a kind of  sociological process that both affects and is affected by society.</t>
   </si>
   <si>
     <t>Key Metaphors</t>
@@ -847,9 +841,6 @@
     <t>Typical Methods of Study</t>
   </si>
   <si>
-    <t>General Epistemological Approach</t>
-  </si>
-  <si>
     <t>Markman, Gianiodis, &amp; Phan (2009)</t>
   </si>
   <si>
@@ -1278,6 +1269,15 @@
 Population ecology
 Socio-technical systems theory
 Transaction cost theory</t>
+  </si>
+  <si>
+    <t>Ontological and Epistemological Approach</t>
+  </si>
+  <si>
+    <t>Even if there is an objective reality, all knowledge is filtered by the experience of the observer.  The organization is a situation whose meaning is to be understood.</t>
+  </si>
+  <si>
+    <t>There is an objective reality independent of the observer.  The organization is a  sociological process that both affects and is affected by society.</t>
   </si>
 </sst>
 </file>
@@ -7505,7 +7505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -7534,7 +7534,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7995,7 +7995,7 @@
     </row>
     <row r="2" spans="1:27" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E2" s="61"/>
       <c r="F2" s="61"/>
@@ -8027,26 +8027,26 @@
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
       <c r="E3" s="113" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F3" s="114"/>
       <c r="G3" s="114"/>
       <c r="H3" s="111"/>
       <c r="I3" s="110" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="J3" s="111"/>
       <c r="K3" s="110" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="L3" s="112"/>
       <c r="M3" s="113" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N3" s="114"/>
       <c r="O3" s="111"/>
       <c r="P3" s="115" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="Q3" s="114"/>
       <c r="R3" s="114"/>
@@ -8063,84 +8063,84 @@
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="104" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="68"/>
       <c r="E4" s="105" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F4" s="107" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G4" s="62" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="H4" s="106" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="I4" s="65" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J4" s="66" t="s">
+        <v>201</v>
+      </c>
+      <c r="K4" s="65" t="s">
+        <v>258</v>
+      </c>
+      <c r="L4" s="66" t="s">
+        <v>259</v>
+      </c>
+      <c r="M4" s="105" t="s">
+        <v>294</v>
+      </c>
+      <c r="N4" s="62" t="s">
+        <v>295</v>
+      </c>
+      <c r="O4" s="106" t="s">
+        <v>293</v>
+      </c>
+      <c r="P4" s="62" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q4" s="62" t="s">
+        <v>237</v>
+      </c>
+      <c r="R4" s="62" t="s">
+        <v>238</v>
+      </c>
+      <c r="S4" s="62" t="s">
+        <v>210</v>
+      </c>
+      <c r="T4" s="62" t="s">
+        <v>233</v>
+      </c>
+      <c r="U4" s="62" t="s">
+        <v>239</v>
+      </c>
+      <c r="V4" s="62" t="s">
+        <v>211</v>
+      </c>
+      <c r="W4" s="62" t="s">
+        <v>235</v>
+      </c>
+      <c r="X4" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="Y4" s="62" t="s">
+        <v>278</v>
+      </c>
+      <c r="Z4" s="62" t="s">
+        <v>264</v>
+      </c>
+      <c r="AA4" s="72" t="s">
         <v>203</v>
-      </c>
-      <c r="K4" s="65" t="s">
-        <v>261</v>
-      </c>
-      <c r="L4" s="66" t="s">
-        <v>262</v>
-      </c>
-      <c r="M4" s="105" t="s">
-        <v>297</v>
-      </c>
-      <c r="N4" s="62" t="s">
-        <v>298</v>
-      </c>
-      <c r="O4" s="106" t="s">
-        <v>296</v>
-      </c>
-      <c r="P4" s="62" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q4" s="62" t="s">
-        <v>240</v>
-      </c>
-      <c r="R4" s="62" t="s">
-        <v>241</v>
-      </c>
-      <c r="S4" s="62" t="s">
-        <v>213</v>
-      </c>
-      <c r="T4" s="62" t="s">
-        <v>236</v>
-      </c>
-      <c r="U4" s="62" t="s">
-        <v>242</v>
-      </c>
-      <c r="V4" s="62" t="s">
-        <v>214</v>
-      </c>
-      <c r="W4" s="62" t="s">
-        <v>238</v>
-      </c>
-      <c r="X4" s="62" t="s">
-        <v>239</v>
-      </c>
-      <c r="Y4" s="62" t="s">
-        <v>281</v>
-      </c>
-      <c r="Z4" s="62" t="s">
-        <v>267</v>
-      </c>
-      <c r="AA4" s="72" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="49" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C5" s="93"/>
       <c r="D5" s="93"/>
@@ -8172,25 +8172,25 @@
       <c r="A6" s="94"/>
       <c r="B6" s="82"/>
       <c r="C6" s="81" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D6" s="81"/>
       <c r="E6" s="74"/>
       <c r="F6" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G6" s="92"/>
       <c r="H6" s="75"/>
       <c r="I6" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J6" s="75"/>
       <c r="K6" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L6" s="75"/>
       <c r="M6" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N6" s="92"/>
       <c r="O6" s="75"/>
@@ -8199,7 +8199,7 @@
       <c r="R6" s="92"/>
       <c r="S6" s="78"/>
       <c r="T6" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U6" s="78"/>
       <c r="V6" s="78"/>
@@ -8208,32 +8208,32 @@
       <c r="Y6" s="78"/>
       <c r="Z6" s="78"/>
       <c r="AA6" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="94"/>
       <c r="B7" s="82"/>
       <c r="C7" s="93" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D7" s="81"/>
       <c r="E7" s="74"/>
       <c r="F7" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G7" s="92"/>
       <c r="H7" s="75"/>
       <c r="I7" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J7" s="75"/>
       <c r="K7" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L7" s="75"/>
       <c r="M7" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N7" s="92"/>
       <c r="O7" s="75"/>
@@ -8242,7 +8242,7 @@
       <c r="R7" s="92"/>
       <c r="S7" s="78"/>
       <c r="T7" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U7" s="78"/>
       <c r="V7" s="78"/>
@@ -8251,32 +8251,32 @@
       <c r="Y7" s="78"/>
       <c r="Z7" s="78"/>
       <c r="AA7" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="94"/>
       <c r="B8" s="82"/>
       <c r="C8" s="81" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D8" s="81"/>
       <c r="E8" s="74"/>
       <c r="F8" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G8" s="92"/>
       <c r="H8" s="75"/>
       <c r="I8" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J8" s="75"/>
       <c r="K8" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L8" s="75"/>
       <c r="M8" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N8" s="92"/>
       <c r="O8" s="75"/>
@@ -8285,7 +8285,7 @@
       <c r="R8" s="92"/>
       <c r="S8" s="78"/>
       <c r="T8" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U8" s="78"/>
       <c r="V8" s="78"/>
@@ -8294,47 +8294,47 @@
       <c r="Y8" s="78"/>
       <c r="Z8" s="78"/>
       <c r="AA8" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="94"/>
       <c r="B9" s="82"/>
       <c r="C9" s="93" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D9" s="81"/>
       <c r="E9" s="74"/>
       <c r="F9" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G9" s="92"/>
       <c r="H9" s="75"/>
       <c r="I9" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J9" s="75"/>
       <c r="K9" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L9" s="75"/>
       <c r="M9" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N9" s="92"/>
       <c r="O9" s="75"/>
       <c r="P9" s="92"/>
       <c r="Q9" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R9" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S9" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T9" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U9" s="78"/>
       <c r="V9" s="78"/>
@@ -8343,104 +8343,104 @@
       <c r="Y9" s="78"/>
       <c r="Z9" s="78"/>
       <c r="AA9" s="63" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
       <c r="B10" s="30"/>
       <c r="C10" s="32" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="74"/>
       <c r="F10" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G10" s="92"/>
       <c r="H10" s="75"/>
       <c r="I10" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J10" s="75"/>
       <c r="K10" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L10" s="75"/>
       <c r="M10" s="74"/>
       <c r="N10" s="92"/>
       <c r="O10" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P10" s="92"/>
       <c r="Q10" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R10" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S10" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T10" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U10" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="V10" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W10" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="X10" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Y10" s="78"/>
       <c r="Z10" s="78"/>
       <c r="AA10" s="63" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="94"/>
       <c r="B11" s="82"/>
       <c r="C11" s="95" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D11" s="81"/>
       <c r="E11" s="96"/>
       <c r="F11" s="102" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G11" s="98"/>
       <c r="H11" s="97"/>
       <c r="I11" s="96" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J11" s="97"/>
       <c r="K11" s="96" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L11" s="97"/>
       <c r="M11" s="96" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N11" s="98"/>
       <c r="O11" s="97"/>
       <c r="P11" s="98"/>
       <c r="Q11" s="98" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R11" s="98" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S11" s="99" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T11" s="99" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U11" s="99"/>
       <c r="V11" s="99"/>
@@ -8449,7 +8449,7 @@
       <c r="Y11" s="99"/>
       <c r="Z11" s="99"/>
       <c r="AA11" s="100" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -8484,7 +8484,7 @@
     <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="49" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C13" s="93"/>
       <c r="D13" s="93"/>
@@ -8516,241 +8516,241 @@
       <c r="A14" s="94"/>
       <c r="B14" s="30"/>
       <c r="C14" s="32" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="74"/>
       <c r="F14" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G14" s="92"/>
       <c r="H14" s="75"/>
       <c r="I14" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J14" s="75"/>
       <c r="K14" s="74"/>
       <c r="L14" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M14" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N14" s="92"/>
       <c r="O14" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P14" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Q14" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R14" s="92"/>
       <c r="S14" s="78"/>
       <c r="T14" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U14" s="78"/>
       <c r="V14" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W14" s="78"/>
       <c r="X14" s="78"/>
       <c r="Y14" s="78"/>
       <c r="Z14" s="78"/>
       <c r="AA14" s="63" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="94"/>
       <c r="B15" s="30"/>
       <c r="C15" s="32" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="74"/>
       <c r="F15" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G15" s="92"/>
       <c r="H15" s="75"/>
       <c r="I15" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J15" s="75"/>
       <c r="K15" s="74"/>
       <c r="L15" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M15" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N15" s="92"/>
       <c r="O15" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P15" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Q15" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R15" s="92"/>
       <c r="S15" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T15" s="78"/>
       <c r="U15" s="78"/>
       <c r="V15" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W15" s="78"/>
       <c r="X15" s="78"/>
       <c r="Y15" s="78"/>
       <c r="Z15" s="78"/>
       <c r="AA15" s="63" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="94"/>
       <c r="B16" s="82"/>
       <c r="C16" s="81" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D16" s="81"/>
       <c r="E16" s="74"/>
       <c r="F16" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G16" s="92"/>
       <c r="H16" s="75"/>
       <c r="I16" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J16" s="75"/>
       <c r="K16" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L16" s="75"/>
       <c r="M16" s="74"/>
       <c r="N16" s="92"/>
       <c r="O16" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P16" s="92"/>
       <c r="Q16" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R16" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S16" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T16" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U16" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="V16" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W16" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="X16" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Y16" s="78"/>
       <c r="Z16" s="78"/>
       <c r="AA16" s="63" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="94"/>
       <c r="B17" s="82"/>
       <c r="C17" s="81" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D17" s="81"/>
       <c r="E17" s="74"/>
       <c r="F17" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G17" s="92"/>
       <c r="H17" s="75"/>
       <c r="I17" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J17" s="75"/>
       <c r="K17" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L17" s="75"/>
       <c r="M17" s="74"/>
       <c r="N17" s="92"/>
       <c r="O17" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P17" s="92"/>
       <c r="Q17" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R17" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S17" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T17" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U17" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="V17" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W17" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="X17" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Y17" s="78"/>
       <c r="Z17" s="78"/>
       <c r="AA17" s="63" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="94"/>
       <c r="B18" s="60"/>
       <c r="C18" s="59" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D18" s="59"/>
       <c r="E18" s="74"/>
       <c r="F18" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G18" s="92"/>
       <c r="H18" s="75"/>
       <c r="I18" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J18" s="75"/>
       <c r="K18" s="74"/>
       <c r="L18" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M18" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N18" s="92"/>
       <c r="O18" s="75"/>
@@ -8761,39 +8761,39 @@
       <c r="T18" s="78"/>
       <c r="U18" s="78"/>
       <c r="V18" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W18" s="78"/>
       <c r="X18" s="78"/>
       <c r="Y18" s="78"/>
       <c r="Z18" s="78"/>
       <c r="AA18" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="94"/>
       <c r="B19" s="30"/>
       <c r="C19" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="74"/>
       <c r="F19" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G19" s="92"/>
       <c r="H19" s="75"/>
       <c r="I19" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J19" s="75"/>
       <c r="K19" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L19" s="75"/>
       <c r="M19" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N19" s="92"/>
       <c r="O19" s="75"/>
@@ -8801,7 +8801,7 @@
       <c r="Q19" s="92"/>
       <c r="R19" s="92"/>
       <c r="S19" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T19" s="78"/>
       <c r="U19" s="78"/>
@@ -8811,32 +8811,32 @@
       <c r="Y19" s="78"/>
       <c r="Z19" s="78"/>
       <c r="AA19" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="94"/>
       <c r="B20" s="30"/>
       <c r="C20" s="32" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="74"/>
       <c r="F20" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G20" s="92"/>
       <c r="H20" s="75"/>
       <c r="I20" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J20" s="75"/>
       <c r="K20" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L20" s="75"/>
       <c r="M20" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N20" s="92"/>
       <c r="O20" s="75"/>
@@ -8844,7 +8844,7 @@
       <c r="Q20" s="92"/>
       <c r="R20" s="92"/>
       <c r="S20" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T20" s="78"/>
       <c r="U20" s="78"/>
@@ -8854,32 +8854,32 @@
       <c r="Y20" s="78"/>
       <c r="Z20" s="78"/>
       <c r="AA20" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="94"/>
       <c r="B21" s="30"/>
       <c r="C21" s="32" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="74"/>
       <c r="F21" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G21" s="92"/>
       <c r="H21" s="75"/>
       <c r="I21" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J21" s="75"/>
       <c r="K21" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L21" s="75"/>
       <c r="M21" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N21" s="92"/>
       <c r="O21" s="75"/>
@@ -8887,7 +8887,7 @@
       <c r="Q21" s="92"/>
       <c r="R21" s="92"/>
       <c r="S21" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T21" s="78"/>
       <c r="U21" s="78"/>
@@ -8897,349 +8897,349 @@
       <c r="Y21" s="78"/>
       <c r="Z21" s="78"/>
       <c r="AA21" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="94"/>
       <c r="B22" s="82"/>
       <c r="C22" s="81" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D22" s="81"/>
       <c r="E22" s="74"/>
       <c r="F22" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G22" s="92"/>
       <c r="H22" s="75"/>
       <c r="I22" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J22" s="75"/>
       <c r="K22" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L22" s="75"/>
       <c r="M22" s="74"/>
       <c r="N22" s="92"/>
       <c r="O22" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P22" s="92"/>
       <c r="Q22" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R22" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S22" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T22" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U22" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="V22" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W22" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="X22" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Y22" s="78"/>
       <c r="Z22" s="78"/>
       <c r="AA22" s="63" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="94"/>
       <c r="B23" s="82"/>
       <c r="C23" s="81" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D23" s="81"/>
       <c r="E23" s="74"/>
       <c r="F23" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G23" s="92"/>
       <c r="H23" s="75"/>
       <c r="I23" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J23" s="75"/>
       <c r="K23" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L23" s="75"/>
       <c r="M23" s="74"/>
       <c r="N23" s="92"/>
       <c r="O23" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P23" s="92"/>
       <c r="Q23" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R23" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S23" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T23" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U23" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="V23" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W23" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="X23" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Y23" s="78"/>
       <c r="Z23" s="78"/>
       <c r="AA23" s="63" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="94"/>
       <c r="B24" s="30"/>
       <c r="C24" s="32" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="74"/>
       <c r="F24" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G24" s="92"/>
       <c r="H24" s="75"/>
       <c r="I24" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J24" s="75"/>
       <c r="K24" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L24" s="75"/>
       <c r="M24" s="74"/>
       <c r="N24" s="92"/>
       <c r="O24" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P24" s="92"/>
       <c r="Q24" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R24" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S24" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T24" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U24" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="V24" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W24" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="X24" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Y24" s="78"/>
       <c r="Z24" s="78"/>
       <c r="AA24" s="63" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="94"/>
       <c r="B25" s="30"/>
       <c r="C25" s="32" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="74"/>
       <c r="F25" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G25" s="92"/>
       <c r="H25" s="75"/>
       <c r="I25" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J25" s="75"/>
       <c r="K25" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L25" s="75"/>
       <c r="M25" s="74"/>
       <c r="N25" s="92"/>
       <c r="O25" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P25" s="92"/>
       <c r="Q25" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R25" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S25" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T25" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U25" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="V25" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W25" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="X25" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Y25" s="78"/>
       <c r="Z25" s="78"/>
       <c r="AA25" s="63" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="94"/>
       <c r="B26" s="82"/>
       <c r="C26" s="81" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D26" s="81"/>
       <c r="E26" s="74"/>
       <c r="F26" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G26" s="92"/>
       <c r="H26" s="75"/>
       <c r="I26" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J26" s="75"/>
       <c r="K26" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L26" s="75"/>
       <c r="M26" s="74"/>
       <c r="N26" s="92"/>
       <c r="O26" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P26" s="92"/>
       <c r="Q26" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R26" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S26" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T26" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U26" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="V26" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W26" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="X26" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Y26" s="78"/>
       <c r="Z26" s="78"/>
       <c r="AA26" s="63" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="94"/>
       <c r="B27" s="82"/>
       <c r="C27" s="81" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D27" s="81"/>
       <c r="E27" s="74"/>
       <c r="F27" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G27" s="92"/>
       <c r="H27" s="75"/>
       <c r="I27" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J27" s="75"/>
       <c r="K27" s="74"/>
       <c r="L27" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M27" s="74"/>
       <c r="N27" s="92"/>
       <c r="O27" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P27" s="92"/>
       <c r="Q27" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R27" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S27" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T27" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U27" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="V27" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W27" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="X27" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Y27" s="78"/>
       <c r="Z27" s="78"/>
       <c r="AA27" s="63" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9274,7 +9274,7 @@
     <row r="29" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="94"/>
       <c r="B29" s="31" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C29" s="93"/>
       <c r="D29" s="93"/>
@@ -9306,40 +9306,40 @@
       <c r="A30" s="94"/>
       <c r="B30" s="82"/>
       <c r="C30" s="81" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D30" s="81"/>
       <c r="E30" s="74"/>
       <c r="F30" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G30" s="92"/>
       <c r="H30" s="75"/>
       <c r="I30" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J30" s="75"/>
       <c r="K30" s="74"/>
       <c r="L30" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M30" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N30" s="92"/>
       <c r="O30" s="75"/>
       <c r="P30" s="92"/>
       <c r="Q30" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R30" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S30" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T30" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U30" s="78"/>
       <c r="V30" s="78"/>
@@ -9348,32 +9348,32 @@
       <c r="Y30" s="78"/>
       <c r="Z30" s="78"/>
       <c r="AA30" s="63" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="31" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="94"/>
       <c r="B31" s="94"/>
       <c r="C31" s="93" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D31" s="93"/>
       <c r="E31" s="74"/>
       <c r="F31" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G31" s="92"/>
       <c r="H31" s="75"/>
       <c r="I31" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J31" s="75"/>
       <c r="K31" s="74"/>
       <c r="L31" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M31" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N31" s="92"/>
       <c r="O31" s="75"/>
@@ -9382,7 +9382,7 @@
       <c r="R31" s="92"/>
       <c r="S31" s="78"/>
       <c r="T31" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U31" s="78"/>
       <c r="V31" s="78"/>
@@ -9391,32 +9391,32 @@
       <c r="Y31" s="78"/>
       <c r="Z31" s="78"/>
       <c r="AA31" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="94"/>
       <c r="B32" s="94"/>
       <c r="C32" s="93" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D32" s="93"/>
       <c r="E32" s="74"/>
       <c r="F32" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G32" s="92"/>
       <c r="H32" s="75"/>
       <c r="I32" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J32" s="75"/>
       <c r="K32" s="74"/>
       <c r="L32" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M32" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N32" s="92"/>
       <c r="O32" s="75"/>
@@ -9425,7 +9425,7 @@
       <c r="R32" s="92"/>
       <c r="S32" s="78"/>
       <c r="T32" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U32" s="78"/>
       <c r="V32" s="78"/>
@@ -9434,38 +9434,38 @@
       <c r="Y32" s="78"/>
       <c r="Z32" s="78"/>
       <c r="AA32" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="33" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="94"/>
       <c r="B33" s="94"/>
       <c r="C33" s="93" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D33" s="93"/>
       <c r="E33" s="74"/>
       <c r="F33" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G33" s="92"/>
       <c r="H33" s="75"/>
       <c r="I33" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J33" s="75"/>
       <c r="K33" s="74"/>
       <c r="L33" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M33" s="74"/>
       <c r="N33" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="O33" s="75"/>
       <c r="P33" s="92"/>
       <c r="Q33" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R33" s="92"/>
       <c r="S33" s="78"/>
@@ -9477,7 +9477,7 @@
       <c r="Y33" s="78"/>
       <c r="Z33" s="78"/>
       <c r="AA33" s="63" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="34" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9512,7 +9512,7 @@
     <row r="35" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
       <c r="B35" s="49" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C35" s="93"/>
       <c r="D35" s="93"/>
@@ -9544,25 +9544,25 @@
       <c r="A36" s="94"/>
       <c r="B36" s="30"/>
       <c r="C36" s="32" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D36" s="32"/>
       <c r="E36" s="74"/>
       <c r="F36" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G36" s="92"/>
       <c r="H36" s="75"/>
       <c r="I36" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J36" s="75"/>
       <c r="K36" s="74"/>
       <c r="L36" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M36" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N36" s="92"/>
       <c r="O36" s="75"/>
@@ -9570,7 +9570,7 @@
       <c r="Q36" s="92"/>
       <c r="R36" s="92"/>
       <c r="S36" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T36" s="78"/>
       <c r="U36" s="78"/>
@@ -9580,32 +9580,32 @@
       <c r="Y36" s="78"/>
       <c r="Z36" s="78"/>
       <c r="AA36" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="94"/>
       <c r="B37" s="30"/>
       <c r="C37" s="32" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D37" s="32"/>
       <c r="E37" s="74"/>
       <c r="F37" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G37" s="92"/>
       <c r="H37" s="75"/>
       <c r="I37" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J37" s="75"/>
       <c r="K37" s="74"/>
       <c r="L37" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M37" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N37" s="92"/>
       <c r="O37" s="75"/>
@@ -9616,39 +9616,39 @@
       <c r="T37" s="78"/>
       <c r="U37" s="78"/>
       <c r="V37" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W37" s="78"/>
       <c r="X37" s="78"/>
       <c r="Y37" s="78"/>
       <c r="Z37" s="78"/>
       <c r="AA37" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="94"/>
       <c r="B38" s="94"/>
       <c r="C38" s="93" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D38" s="93"/>
       <c r="E38" s="74"/>
       <c r="F38" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G38" s="92"/>
       <c r="H38" s="75"/>
       <c r="I38" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J38" s="75"/>
       <c r="K38" s="74"/>
       <c r="L38" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M38" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N38" s="92"/>
       <c r="O38" s="75"/>
@@ -9656,7 +9656,7 @@
       <c r="Q38" s="92"/>
       <c r="R38" s="92"/>
       <c r="S38" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T38" s="78"/>
       <c r="U38" s="78"/>
@@ -9666,32 +9666,32 @@
       <c r="Y38" s="78"/>
       <c r="Z38" s="78"/>
       <c r="AA38" s="63" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="94"/>
       <c r="B39" s="94"/>
       <c r="C39" s="93" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D39" s="93"/>
       <c r="E39" s="74"/>
       <c r="F39" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G39" s="92"/>
       <c r="H39" s="75"/>
       <c r="I39" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J39" s="75"/>
       <c r="K39" s="74"/>
       <c r="L39" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M39" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N39" s="92"/>
       <c r="O39" s="75"/>
@@ -9699,44 +9699,44 @@
       <c r="Q39" s="92"/>
       <c r="R39" s="92"/>
       <c r="S39" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T39" s="78"/>
       <c r="U39" s="78"/>
       <c r="V39" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W39" s="78"/>
       <c r="X39" s="78"/>
       <c r="Y39" s="78"/>
       <c r="Z39" s="78"/>
       <c r="AA39" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="94"/>
       <c r="B40" s="94"/>
       <c r="C40" s="93" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D40" s="93"/>
       <c r="E40" s="74"/>
       <c r="F40" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G40" s="92"/>
       <c r="H40" s="75"/>
       <c r="I40" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J40" s="75"/>
       <c r="K40" s="74"/>
       <c r="L40" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M40" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N40" s="92"/>
       <c r="O40" s="75"/>
@@ -9744,93 +9744,93 @@
       <c r="Q40" s="92"/>
       <c r="R40" s="92"/>
       <c r="S40" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T40" s="78"/>
       <c r="U40" s="78"/>
       <c r="V40" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W40" s="78"/>
       <c r="X40" s="78"/>
       <c r="Y40" s="78"/>
       <c r="Z40" s="78"/>
       <c r="AA40" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="94"/>
       <c r="B41" s="94"/>
       <c r="C41" s="93" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D41" s="93"/>
       <c r="E41" s="74"/>
       <c r="F41" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G41" s="92"/>
       <c r="H41" s="75"/>
       <c r="I41" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J41" s="75"/>
       <c r="K41" s="74"/>
       <c r="L41" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M41" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N41" s="92"/>
       <c r="O41" s="75"/>
       <c r="P41" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Q41" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R41" s="92"/>
       <c r="S41" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T41" s="78"/>
       <c r="U41" s="78"/>
       <c r="V41" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W41" s="78"/>
       <c r="X41" s="78"/>
       <c r="Y41" s="78"/>
       <c r="Z41" s="78"/>
       <c r="AA41" s="63" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="94"/>
       <c r="B42" s="94"/>
       <c r="C42" s="93" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D42" s="93"/>
       <c r="E42" s="74"/>
       <c r="F42" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G42" s="92"/>
       <c r="H42" s="75"/>
       <c r="I42" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J42" s="75"/>
       <c r="K42" s="74"/>
       <c r="L42" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M42" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N42" s="92"/>
       <c r="O42" s="75"/>
@@ -9839,7 +9839,7 @@
       <c r="R42" s="92"/>
       <c r="S42" s="78"/>
       <c r="T42" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U42" s="78"/>
       <c r="V42" s="78"/>
@@ -9848,32 +9848,32 @@
       <c r="Y42" s="78"/>
       <c r="Z42" s="78"/>
       <c r="AA42" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="94"/>
       <c r="B43" s="94"/>
       <c r="C43" s="93" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D43" s="93"/>
       <c r="E43" s="74"/>
       <c r="F43" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G43" s="92"/>
       <c r="H43" s="75"/>
       <c r="I43" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J43" s="75"/>
       <c r="K43" s="74"/>
       <c r="L43" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M43" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N43" s="92"/>
       <c r="O43" s="75"/>
@@ -9881,44 +9881,44 @@
       <c r="Q43" s="92"/>
       <c r="R43" s="92"/>
       <c r="S43" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T43" s="78"/>
       <c r="U43" s="78"/>
       <c r="V43" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W43" s="78"/>
       <c r="X43" s="78"/>
       <c r="Y43" s="78"/>
       <c r="Z43" s="78"/>
       <c r="AA43" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="94"/>
       <c r="B44" s="94"/>
       <c r="C44" s="93" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D44" s="93"/>
       <c r="E44" s="74"/>
       <c r="F44" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G44" s="92"/>
       <c r="H44" s="75"/>
       <c r="I44" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J44" s="75"/>
       <c r="K44" s="74"/>
       <c r="L44" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M44" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N44" s="92"/>
       <c r="O44" s="75"/>
@@ -9926,101 +9926,101 @@
       <c r="Q44" s="92"/>
       <c r="R44" s="92"/>
       <c r="S44" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T44" s="78"/>
       <c r="U44" s="78"/>
       <c r="V44" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W44" s="78"/>
       <c r="X44" s="78"/>
       <c r="Y44" s="78"/>
       <c r="Z44" s="78"/>
       <c r="AA44" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="94"/>
       <c r="B45" s="82"/>
       <c r="C45" s="81" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D45" s="81"/>
       <c r="E45" s="74"/>
       <c r="F45" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G45" s="92"/>
       <c r="H45" s="75"/>
       <c r="I45" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J45" s="75"/>
       <c r="K45" s="74"/>
       <c r="L45" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M45" s="74"/>
       <c r="N45" s="92"/>
       <c r="O45" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P45" s="92"/>
       <c r="Q45" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="R45" s="92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S45" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T45" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U45" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="V45" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W45" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="X45" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Y45" s="78"/>
       <c r="Z45" s="78"/>
       <c r="AA45" s="63" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="94"/>
       <c r="B46" s="60"/>
       <c r="C46" s="59" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D46" s="59"/>
       <c r="E46" s="74"/>
       <c r="F46" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G46" s="92"/>
       <c r="H46" s="75"/>
       <c r="I46" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J46" s="75"/>
       <c r="K46" s="74"/>
       <c r="L46" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M46" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N46" s="92"/>
       <c r="O46" s="75"/>
@@ -10028,44 +10028,44 @@
       <c r="Q46" s="92"/>
       <c r="R46" s="92"/>
       <c r="S46" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T46" s="78"/>
       <c r="U46" s="78"/>
       <c r="V46" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W46" s="78"/>
       <c r="X46" s="78"/>
       <c r="Y46" s="78"/>
       <c r="Z46" s="78"/>
       <c r="AA46" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="94"/>
       <c r="B47" s="60"/>
       <c r="C47" s="59" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D47" s="59"/>
       <c r="E47" s="74"/>
       <c r="F47" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G47" s="92"/>
       <c r="H47" s="75"/>
       <c r="I47" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J47" s="75"/>
       <c r="K47" s="74"/>
       <c r="L47" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M47" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N47" s="92"/>
       <c r="O47" s="75"/>
@@ -10073,7 +10073,7 @@
       <c r="Q47" s="92"/>
       <c r="R47" s="92"/>
       <c r="S47" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T47" s="78"/>
       <c r="U47" s="78"/>
@@ -10083,32 +10083,32 @@
       <c r="Y47" s="78"/>
       <c r="Z47" s="78"/>
       <c r="AA47" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="48" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="94"/>
       <c r="B48" s="82"/>
       <c r="C48" s="81" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D48" s="81"/>
       <c r="E48" s="74"/>
       <c r="F48" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G48" s="92"/>
       <c r="H48" s="75"/>
       <c r="I48" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J48" s="75"/>
       <c r="K48" s="74"/>
       <c r="L48" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M48" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N48" s="92"/>
       <c r="O48" s="75"/>
@@ -10117,7 +10117,7 @@
       <c r="R48" s="92"/>
       <c r="S48" s="78"/>
       <c r="T48" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U48" s="78"/>
       <c r="V48" s="78"/>
@@ -10126,32 +10126,32 @@
       <c r="Y48" s="78"/>
       <c r="Z48" s="78"/>
       <c r="AA48" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="49" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="94"/>
       <c r="B49" s="94"/>
       <c r="C49" s="93" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D49" s="93"/>
       <c r="E49" s="74"/>
       <c r="F49" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G49" s="92"/>
       <c r="H49" s="75"/>
       <c r="I49" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J49" s="75"/>
       <c r="K49" s="74"/>
       <c r="L49" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M49" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N49" s="92"/>
       <c r="O49" s="75"/>
@@ -10160,7 +10160,7 @@
       <c r="R49" s="92"/>
       <c r="S49" s="78"/>
       <c r="T49" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U49" s="78"/>
       <c r="V49" s="78"/>
@@ -10169,32 +10169,32 @@
       <c r="Y49" s="78"/>
       <c r="Z49" s="78"/>
       <c r="AA49" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="94"/>
       <c r="B50" s="82"/>
       <c r="C50" s="81" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D50" s="81"/>
       <c r="E50" s="74"/>
       <c r="F50" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G50" s="92"/>
       <c r="H50" s="75"/>
       <c r="I50" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J50" s="75"/>
       <c r="K50" s="74"/>
       <c r="L50" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M50" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N50" s="92"/>
       <c r="O50" s="75"/>
@@ -10203,7 +10203,7 @@
       <c r="R50" s="92"/>
       <c r="S50" s="78"/>
       <c r="T50" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U50" s="78"/>
       <c r="V50" s="78"/>
@@ -10212,32 +10212,32 @@
       <c r="Y50" s="78"/>
       <c r="Z50" s="78"/>
       <c r="AA50" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="94"/>
       <c r="B51" s="82"/>
       <c r="C51" s="81" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D51" s="81"/>
       <c r="E51" s="74"/>
       <c r="F51" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G51" s="92"/>
       <c r="H51" s="75"/>
       <c r="I51" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J51" s="75"/>
       <c r="K51" s="74"/>
       <c r="L51" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M51" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N51" s="92"/>
       <c r="O51" s="75"/>
@@ -10246,7 +10246,7 @@
       <c r="R51" s="92"/>
       <c r="S51" s="78"/>
       <c r="T51" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="U51" s="78"/>
       <c r="V51" s="78"/>
@@ -10255,32 +10255,32 @@
       <c r="Y51" s="78"/>
       <c r="Z51" s="78"/>
       <c r="AA51" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="52" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="94"/>
       <c r="B52" s="89"/>
       <c r="C52" s="88" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D52" s="88"/>
       <c r="E52" s="74"/>
       <c r="F52" s="101"/>
       <c r="G52" s="92"/>
       <c r="H52" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I52" s="74"/>
       <c r="J52" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K52" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L52" s="75"/>
       <c r="M52" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N52" s="92"/>
       <c r="O52" s="75"/>
@@ -10295,35 +10295,35 @@
       <c r="X52" s="78"/>
       <c r="Y52" s="78"/>
       <c r="Z52" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AA52" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="53" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="94"/>
       <c r="B53" s="89"/>
       <c r="C53" s="88" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D53" s="88"/>
       <c r="E53" s="74"/>
       <c r="F53" s="101"/>
       <c r="G53" s="92"/>
       <c r="H53" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I53" s="74"/>
       <c r="J53" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K53" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L53" s="75"/>
       <c r="M53" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N53" s="92"/>
       <c r="O53" s="75"/>
@@ -10338,10 +10338,10 @@
       <c r="X53" s="78"/>
       <c r="Y53" s="78"/>
       <c r="Z53" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AA53" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="54" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -10376,7 +10376,7 @@
     <row r="55" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49"/>
       <c r="B55" s="49" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C55" s="93"/>
       <c r="D55" s="93"/>
@@ -10408,29 +10408,29 @@
       <c r="A56" s="94"/>
       <c r="B56" s="89"/>
       <c r="C56" s="88" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D56" s="88"/>
       <c r="E56" s="74"/>
       <c r="F56" s="101"/>
       <c r="G56" s="92"/>
       <c r="H56" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I56" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J56" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K56" s="74"/>
       <c r="L56" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M56" s="74"/>
       <c r="N56" s="92"/>
       <c r="O56" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P56" s="92"/>
       <c r="Q56" s="92"/>
@@ -10443,39 +10443,39 @@
       <c r="X56" s="78"/>
       <c r="Y56" s="78"/>
       <c r="Z56" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AA56" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="57" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="94"/>
       <c r="B57" s="89"/>
       <c r="C57" s="88" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D57" s="88"/>
       <c r="E57" s="74"/>
       <c r="F57" s="101"/>
       <c r="G57" s="92"/>
       <c r="H57" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I57" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J57" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K57" s="74"/>
       <c r="L57" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M57" s="74"/>
       <c r="N57" s="92"/>
       <c r="O57" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P57" s="92"/>
       <c r="Q57" s="92"/>
@@ -10488,39 +10488,39 @@
       <c r="X57" s="78"/>
       <c r="Y57" s="78"/>
       <c r="Z57" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AA57" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="58" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="94"/>
       <c r="B58" s="89"/>
       <c r="C58" s="88" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D58" s="88"/>
       <c r="E58" s="74"/>
       <c r="F58" s="101"/>
       <c r="G58" s="92"/>
       <c r="H58" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I58" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J58" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K58" s="74"/>
       <c r="L58" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M58" s="74"/>
       <c r="N58" s="92"/>
       <c r="O58" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P58" s="92"/>
       <c r="Q58" s="92"/>
@@ -10533,39 +10533,39 @@
       <c r="X58" s="78"/>
       <c r="Y58" s="78"/>
       <c r="Z58" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AA58" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="59" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="94"/>
       <c r="B59" s="89"/>
       <c r="C59" s="88" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D59" s="88"/>
       <c r="E59" s="74"/>
       <c r="F59" s="101"/>
       <c r="G59" s="92"/>
       <c r="H59" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I59" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J59" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K59" s="74"/>
       <c r="L59" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M59" s="74"/>
       <c r="N59" s="92"/>
       <c r="O59" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P59" s="92"/>
       <c r="Q59" s="92"/>
@@ -10578,39 +10578,39 @@
       <c r="X59" s="78"/>
       <c r="Y59" s="78"/>
       <c r="Z59" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AA59" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="60" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="94"/>
       <c r="B60" s="89"/>
       <c r="C60" s="88" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D60" s="88"/>
       <c r="E60" s="74"/>
       <c r="F60" s="101"/>
       <c r="G60" s="92"/>
       <c r="H60" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I60" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J60" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K60" s="74"/>
       <c r="L60" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M60" s="74"/>
       <c r="N60" s="92"/>
       <c r="O60" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P60" s="92"/>
       <c r="Q60" s="92"/>
@@ -10623,39 +10623,39 @@
       <c r="X60" s="78"/>
       <c r="Y60" s="78"/>
       <c r="Z60" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AA60" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="61" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="94"/>
       <c r="B61" s="89"/>
       <c r="C61" s="88" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D61" s="88"/>
       <c r="E61" s="74"/>
       <c r="F61" s="101"/>
       <c r="G61" s="92"/>
       <c r="H61" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I61" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J61" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K61" s="74"/>
       <c r="L61" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M61" s="74"/>
       <c r="N61" s="92"/>
       <c r="O61" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P61" s="92"/>
       <c r="Q61" s="92"/>
@@ -10668,39 +10668,39 @@
       <c r="X61" s="78"/>
       <c r="Y61" s="78"/>
       <c r="Z61" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AA61" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="62" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="94"/>
       <c r="B62" s="89"/>
       <c r="C62" s="88" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D62" s="88"/>
       <c r="E62" s="74"/>
       <c r="F62" s="101"/>
       <c r="G62" s="92"/>
       <c r="H62" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I62" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J62" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K62" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L62" s="75"/>
       <c r="M62" s="74"/>
       <c r="N62" s="92"/>
       <c r="O62" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P62" s="92"/>
       <c r="Q62" s="92"/>
@@ -10713,39 +10713,39 @@
       <c r="X62" s="78"/>
       <c r="Y62" s="78"/>
       <c r="Z62" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AA62" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="63" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="94"/>
       <c r="B63" s="89"/>
       <c r="C63" s="88" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D63" s="88"/>
       <c r="E63" s="74"/>
       <c r="F63" s="101"/>
       <c r="G63" s="92"/>
       <c r="H63" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I63" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J63" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K63" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L63" s="75"/>
       <c r="M63" s="74"/>
       <c r="N63" s="92"/>
       <c r="O63" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P63" s="92"/>
       <c r="Q63" s="92"/>
@@ -10758,35 +10758,35 @@
       <c r="X63" s="78"/>
       <c r="Y63" s="78"/>
       <c r="Z63" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AA63" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="64" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="94"/>
       <c r="B64" s="94"/>
       <c r="C64" s="93" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D64" s="93"/>
       <c r="E64" s="74"/>
       <c r="F64" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G64" s="92"/>
       <c r="H64" s="75"/>
       <c r="I64" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J64" s="75"/>
       <c r="K64" s="74"/>
       <c r="L64" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M64" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N64" s="92"/>
       <c r="O64" s="75"/>
@@ -10794,44 +10794,44 @@
       <c r="Q64" s="92"/>
       <c r="R64" s="92"/>
       <c r="S64" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T64" s="78"/>
       <c r="U64" s="78"/>
       <c r="V64" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W64" s="78"/>
       <c r="X64" s="78"/>
       <c r="Y64" s="78"/>
       <c r="Z64" s="78"/>
       <c r="AA64" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="65" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="94"/>
       <c r="B65" s="94"/>
       <c r="C65" s="93" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D65" s="93"/>
       <c r="E65" s="74"/>
       <c r="F65" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G65" s="92"/>
       <c r="H65" s="75"/>
       <c r="I65" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J65" s="75"/>
       <c r="K65" s="74"/>
       <c r="L65" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M65" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N65" s="92"/>
       <c r="O65" s="75"/>
@@ -10839,44 +10839,44 @@
       <c r="Q65" s="92"/>
       <c r="R65" s="92"/>
       <c r="S65" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T65" s="78"/>
       <c r="U65" s="78"/>
       <c r="V65" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W65" s="78"/>
       <c r="X65" s="78"/>
       <c r="Y65" s="78"/>
       <c r="Z65" s="78"/>
       <c r="AA65" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="66" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="94"/>
       <c r="B66" s="94"/>
       <c r="C66" s="93" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D66" s="93"/>
       <c r="E66" s="74"/>
       <c r="F66" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G66" s="92"/>
       <c r="H66" s="75"/>
       <c r="I66" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J66" s="75"/>
       <c r="K66" s="74"/>
       <c r="L66" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M66" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N66" s="92"/>
       <c r="O66" s="75"/>
@@ -10884,44 +10884,44 @@
       <c r="Q66" s="92"/>
       <c r="R66" s="92"/>
       <c r="S66" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T66" s="78"/>
       <c r="U66" s="78"/>
       <c r="V66" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W66" s="78"/>
       <c r="X66" s="78"/>
       <c r="Y66" s="78"/>
       <c r="Z66" s="78"/>
       <c r="AA66" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="67" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="94"/>
       <c r="B67" s="94"/>
       <c r="C67" s="93" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D67" s="93"/>
       <c r="E67" s="74"/>
       <c r="F67" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G67" s="92"/>
       <c r="H67" s="75"/>
       <c r="I67" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J67" s="75"/>
       <c r="K67" s="74"/>
       <c r="L67" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M67" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N67" s="92"/>
       <c r="O67" s="75"/>
@@ -10929,44 +10929,44 @@
       <c r="Q67" s="92"/>
       <c r="R67" s="92"/>
       <c r="S67" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T67" s="78"/>
       <c r="U67" s="78"/>
       <c r="V67" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W67" s="78"/>
       <c r="X67" s="78"/>
       <c r="Y67" s="78"/>
       <c r="Z67" s="78"/>
       <c r="AA67" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="94"/>
       <c r="B68" s="94"/>
       <c r="C68" s="93" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D68" s="93"/>
       <c r="E68" s="74"/>
       <c r="F68" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G68" s="92"/>
       <c r="H68" s="75"/>
       <c r="I68" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J68" s="75"/>
       <c r="K68" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L68" s="75"/>
       <c r="M68" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N68" s="92"/>
       <c r="O68" s="75"/>
@@ -10974,19 +10974,19 @@
       <c r="Q68" s="92"/>
       <c r="R68" s="92"/>
       <c r="S68" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T68" s="78"/>
       <c r="U68" s="78"/>
       <c r="V68" s="78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="W68" s="78"/>
       <c r="X68" s="78"/>
       <c r="Y68" s="78"/>
       <c r="Z68" s="78"/>
       <c r="AA68" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11317,14 +11317,14 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
@@ -11334,7 +11334,7 @@
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
       <c r="D3" s="113" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E3" s="111"/>
       <c r="F3" s="73"/>
@@ -11342,213 +11342,213 @@
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="68" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="65" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E4" s="66" t="s">
+        <v>201</v>
+      </c>
+      <c r="F4" s="72" t="s">
         <v>203</v>
-      </c>
-      <c r="F4" s="72" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60"/>
       <c r="B5" s="59" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60"/>
       <c r="B6" s="59" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E6" s="75"/>
       <c r="F6" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>
       <c r="B7" s="59" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E7" s="75"/>
       <c r="F7" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
       <c r="B8" s="59" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E8" s="75"/>
       <c r="F8" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60"/>
       <c r="B9" s="59" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C9" s="59"/>
       <c r="D9" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E9" s="75"/>
       <c r="F9" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="60"/>
       <c r="B10" s="59" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E10" s="75"/>
       <c r="F10" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="60"/>
       <c r="B11" s="59" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E11" s="75"/>
       <c r="F11" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60"/>
       <c r="B12" s="59" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E12" s="75"/>
       <c r="F12" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="59" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E13" s="75"/>
       <c r="F13" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="59" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E14" s="75"/>
       <c r="F14" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
       <c r="B15" s="81" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E15" s="75"/>
       <c r="F15" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
       <c r="B16" s="81" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C16" s="59"/>
       <c r="D16" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E16" s="75"/>
       <c r="F16" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="60"/>
       <c r="B17" s="59" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E17" s="75"/>
       <c r="F17" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="60"/>
       <c r="B18" s="59" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="74" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E18" s="75"/>
       <c r="F18" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11707,11 +11707,11 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11739,7 +11739,7 @@
     </row>
     <row r="2" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="86" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -11749,19 +11749,19 @@
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="39" t="s">
-        <v>210</v>
+        <v>327</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="39" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K3" s="39"/>
       <c r="L3" s="39" t="s">
@@ -11769,7 +11769,7 @@
       </c>
       <c r="M3" s="39"/>
       <c r="N3" s="39" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11779,15 +11779,15 @@
       </c>
       <c r="C4" s="56"/>
       <c r="D4" s="56" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="58" t="s">
-        <v>199</v>
+        <v>329</v>
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="58" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I4" s="58"/>
       <c r="J4" s="56" t="s">
@@ -11799,7 +11799,7 @@
       </c>
       <c r="M4" s="56"/>
       <c r="N4" s="56" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="195" customHeight="1" x14ac:dyDescent="0.25">
@@ -11809,15 +11809,15 @@
       </c>
       <c r="C5" s="84"/>
       <c r="D5" s="84" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E5" s="84"/>
       <c r="F5" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G5" s="84"/>
       <c r="H5" s="84" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="I5" s="84"/>
       <c r="J5" s="84" t="s">
@@ -11829,7 +11829,7 @@
       </c>
       <c r="M5" s="84"/>
       <c r="N5" s="84" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -11839,19 +11839,19 @@
       </c>
       <c r="C6" s="84"/>
       <c r="D6" s="84" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E6" s="84"/>
       <c r="F6" s="84" t="s">
-        <v>195</v>
+        <v>328</v>
       </c>
       <c r="G6" s="84"/>
       <c r="H6" s="84" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="I6" s="84"/>
       <c r="J6" s="84" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="K6" s="84"/>
       <c r="L6" s="84" t="s">
@@ -11859,7 +11859,7 @@
       </c>
       <c r="M6" s="84"/>
       <c r="N6" s="84" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
@@ -11869,15 +11869,15 @@
       </c>
       <c r="C7" s="84"/>
       <c r="D7" s="84" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E7" s="84"/>
       <c r="F7" s="84" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G7" s="84"/>
       <c r="H7" s="84" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="I7" s="84"/>
       <c r="J7" s="84" t="s">
@@ -11889,7 +11889,7 @@
       </c>
       <c r="M7" s="84"/>
       <c r="N7" s="84" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -11946,7 +11946,7 @@
     </row>
     <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -11956,7 +11956,7 @@
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -11966,7 +11966,7 @@
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -11976,7 +11976,7 @@
     </row>
     <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B14" s="56"/>
       <c r="C14" s="56"/>

</xml_diff>

<commit_message>
Added figures on narrowing of technology and dynamic model of research
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -19,10 +19,12 @@
     <sheet name="Table - Org Studies" sheetId="10" r:id="rId5"/>
     <sheet name="Table - NASA TRL Scale" sheetId="7" r:id="rId6"/>
     <sheet name="Table - Alt Readiness Scales" sheetId="8" r:id="rId7"/>
-    <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId8"/>
-    <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId9"/>
-    <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId10"/>
-    <sheet name="Figure - Causal Diagram" sheetId="9" r:id="rId11"/>
+    <sheet name="Figure - Defining Technology" sheetId="12" r:id="rId8"/>
+    <sheet name="Figure - Dynamic Research Model" sheetId="13" r:id="rId9"/>
+    <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId10"/>
+    <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId11"/>
+    <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId12"/>
+    <sheet name="Figure - Causal Diagram" sheetId="9" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Table - Determinants Examined'!$3:$4</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="333">
   <si>
     <t>Total</t>
   </si>
@@ -1278,6 +1280,15 @@
   </si>
   <si>
     <t>There is an objective reality independent of the observer.  The organization is a  sociological process that both affects and is affected by society.</t>
+  </si>
+  <si>
+    <t>Figure</t>
+  </si>
+  <si>
+    <t>The Narrowing Definition of Technology</t>
+  </si>
+  <si>
+    <t>Dynamic Model of Research</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1627,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1962,6 +1973,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -5151,6 +5163,1662 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>481012</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>608647</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="44" name="Group 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{222B9149-065C-46EA-B831-ACFBF237DFA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1090612" y="838200"/>
+          <a:ext cx="9271635" cy="11534774"/>
+          <a:chOff x="1090612" y="838200"/>
+          <a:chExt cx="9271635" cy="11534774"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Trapezoid 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F153538E-5E30-44AA-BBD8-82A83A4729C9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="4038600" y="2297112"/>
+            <a:ext cx="3200400" cy="1828800"/>
+          </a:xfrm>
+          <a:prstGeom prst="trapezoid">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent3">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent3"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent3"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Rectangle 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D17FC8BE-1DD1-4112-B125-C87BE036924D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4038600" y="838200"/>
+            <a:ext cx="3200400" cy="1371600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Knowledge</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> about the natural sciences </a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t>and useful arts</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Rectangle 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13F12FDB-88A4-4431-9EC5-CB05A2D91BBF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4495800" y="4213224"/>
+            <a:ext cx="2286000" cy="1371600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Distinction between science, technology, and engineering</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Trapezoid 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76B2CF10-0C72-41FB-91AC-6A009FF7D191}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="4500563" y="5700711"/>
+            <a:ext cx="2286000" cy="1828800"/>
+          </a:xfrm>
+          <a:prstGeom prst="trapezoid">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 12500"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent3">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent3"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent3"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="Rectangle 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D376913-460C-43FD-BCAB-E2B3F5CCEB25}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4724400" y="7626348"/>
+            <a:ext cx="1828800" cy="1371600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent4">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent4"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent4"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Instrumental</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> devices that apply scientific knowledge</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Rectangle 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F581AC27-7147-476E-AB26-FFDAF71ADA74}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4953000" y="11001374"/>
+            <a:ext cx="1371600" cy="1371600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent2"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Patentable</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> inventions and trade secrets</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Trapezoid 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B54E527-B87B-4F58-9532-02296D39E650}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="4724400" y="9085260"/>
+            <a:ext cx="1828800" cy="1828800"/>
+          </a:xfrm>
+          <a:prstGeom prst="trapezoid">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 13021"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent3">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent3"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent3"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="TextBox 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94D12191-147C-4429-918E-1D7213D34EC9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1228725" y="8020050"/>
+            <a:ext cx="2009775" cy="581025"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Lay notion of technology</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DBB0A20-EAE5-4446-95E1-0F36E33620FE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="9" idx="3"/>
+            <a:endCxn id="6" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3238500" y="8310563"/>
+            <a:ext cx="1485900" cy="1585"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="TextBox 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3CE918-4457-4F95-A940-828D175F526C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1090612" y="4438649"/>
+            <a:ext cx="2286000" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Academic and occupational</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> conceptualizaitons of </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>technology</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55C6E8C5-2422-4D23-AC3A-AFEF57791C01}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="12" idx="3"/>
+            <a:endCxn id="4" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3376612" y="4895849"/>
+            <a:ext cx="1119188" cy="3175"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="TextBox 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6AC24CB-F17C-4B82-88D3-70E815E0CC8E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1228725" y="1066800"/>
+            <a:ext cx="2009775" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Ancient cognates</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> of </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>technology</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97B451F4-9540-4824-A333-50C2C56F4A54}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="15" idx="3"/>
+            <a:endCxn id="3" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3238500" y="1524000"/>
+            <a:ext cx="800100" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="TextBox 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C6751BB-93E0-47C7-8F18-5C1AC3CA7B4E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1228725" y="11229974"/>
+            <a:ext cx="2009775" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Concepualization</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> of technology in </a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t>U.S. public policy</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD9CC42D-A73B-472C-9DB4-FAB873CE50CF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="18" idx="3"/>
+            <a:endCxn id="7" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3238500" y="11687174"/>
+            <a:ext cx="1714500" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="21" name="TextBox 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F8E5997-DAB4-465A-9FCC-3F269A78B800}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7710487" y="2752725"/>
+            <a:ext cx="2651760" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Mistranslations,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> p</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>olitical</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> ambitions, social status concerns, and professional objectives</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B391ADC-353B-41EC-8DC4-B70C74AB200D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="21" idx="1"/>
+            <a:endCxn id="2" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="7010400" y="3209925"/>
+            <a:ext cx="700087" cy="1587"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="36" name="TextBox 35">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21F38797-18E6-421B-BD0D-429037175DD2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8031480" y="6153150"/>
+            <a:ext cx="2009775" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Limited scientific</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> literacy and historical awareness of the public</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="37" name="Straight Arrow Connector 36">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAB6E4EE-FC27-4B40-8176-B9902B8930BE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="36" idx="1"/>
+            <a:endCxn id="5" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="6672263" y="6610350"/>
+            <a:ext cx="1359217" cy="4761"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="40" name="TextBox 39">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE5EC53E-3DF2-4FA7-8A2A-AEBCACB954B2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7893367" y="9544050"/>
+            <a:ext cx="2286000" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Measurement</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> limitations and political expediency</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="41" name="Straight Arrow Connector 40">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E77E87D6-554F-4DB4-A8A0-DD00645554CF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="40" idx="1"/>
+            <a:endCxn id="8" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="6434136" y="9999660"/>
+            <a:ext cx="1459231" cy="1590"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12ACAC29-579E-4DE1-8156-F22D5829FFB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1590675" y="3162300"/>
+          <a:ext cx="923925" cy="895350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="34" name="Group 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD7B8D4D-A2F8-457B-BC7B-E9CF350C0283}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="219075" y="990600"/>
+          <a:ext cx="8924925" cy="3571875"/>
+          <a:chOff x="219075" y="990600"/>
+          <a:chExt cx="8924925" cy="3571875"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Oval 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E10819E4-450E-49A4-91C4-82AF281BA697}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="219075" y="3190875"/>
+            <a:ext cx="2743200" cy="1371600"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>What are the</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> gaps in society's</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t> fundamental understanding</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> of the natural and social world?</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Oval 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{930E372F-5F04-4DE8-A25C-B16E7B2C883F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3309938" y="990600"/>
+            <a:ext cx="2743200" cy="1371600"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t>How can society apply current knowledge about the natural and social world to achieve specific ends?</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Oval 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDAE0998-753E-4345-9310-EC249E6CCC00}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6400800" y="3190875"/>
+            <a:ext cx="2743200" cy="1371600"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="9144" rIns="9144" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>What limitations prevent society from successfully applying current knowledge</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> about the natural and social world to achieve specific ends?</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50B02649-67D0-4B2F-97A3-2E8CC6A38276}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="7"/>
+            <a:endCxn id="3" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="2560543" y="2161334"/>
+            <a:ext cx="1151127" cy="1230407"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1794563F-DB42-4648-A1E2-F3FD2700A092}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="3" idx="5"/>
+            <a:endCxn id="4" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5651406" y="2161334"/>
+            <a:ext cx="1151126" cy="1230407"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4BC694B-4A8B-4F15-9C1A-6322870BC39E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="4" idx="2"/>
+            <a:endCxn id="2" idx="6"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="2962275" y="3876675"/>
+            <a:ext cx="3438525" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="med"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="29" name="TextBox 28">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AB3B73C-A23F-481D-AC44-54596C488527}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="18817857">
+            <a:off x="2038350" y="2581276"/>
+            <a:ext cx="1828800" cy="276225"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Basic research</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="30" name="TextBox 29">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8F54F25-E6AF-46B4-8656-23BB78E03F1E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="2811508">
+            <a:off x="5443537" y="2528887"/>
+            <a:ext cx="1828800" cy="276225"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Applied research</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="31" name="TextBox 30">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97CA5EE9-4332-42E6-9E6F-044D7BADDCF1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3738563" y="3948112"/>
+            <a:ext cx="2011680" cy="276225"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Research problem identification</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>14286</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -5188,7 +6856,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5229,7 +6897,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5270,7 +6938,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6918,6 +8586,722 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1967</v>
+      </c>
+      <c r="B2" s="19">
+        <v>1454.3</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1968</v>
+      </c>
+      <c r="B3" s="19">
+        <v>1487.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>1969</v>
+      </c>
+      <c r="B4" s="19">
+        <v>1529.2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>1970</v>
+      </c>
+      <c r="B5" s="19">
+        <v>1475.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>1971</v>
+      </c>
+      <c r="B6" s="19">
+        <v>1644.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>1972</v>
+      </c>
+      <c r="B7" s="19">
+        <v>1903.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>1973</v>
+      </c>
+      <c r="B8" s="19">
+        <v>1916.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>1974</v>
+      </c>
+      <c r="B9" s="19">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>1975</v>
+      </c>
+      <c r="B10" s="19">
+        <v>2411.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>1976</v>
+      </c>
+      <c r="B11" s="19">
+        <v>2551.8000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>1977</v>
+      </c>
+      <c r="B12" s="19">
+        <v>2905.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>1978</v>
+      </c>
+      <c r="B13" s="19">
+        <v>3374.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>1979</v>
+      </c>
+      <c r="B14" s="19">
+        <v>3888.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>1980</v>
+      </c>
+      <c r="B15" s="19">
+        <v>4263.3999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>1981</v>
+      </c>
+      <c r="B16" s="19">
+        <v>4465.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>1982</v>
+      </c>
+      <c r="B17" s="19">
+        <v>4605.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>1983</v>
+      </c>
+      <c r="B18" s="19">
+        <v>4966.3999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>1984</v>
+      </c>
+      <c r="B19" s="19">
+        <v>5546.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>1985</v>
+      </c>
+      <c r="B20" s="19">
+        <v>6339.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>1986</v>
+      </c>
+      <c r="B21" s="19">
+        <v>6558.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>1987</v>
+      </c>
+      <c r="B22" s="19">
+        <v>7337.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>1988</v>
+      </c>
+      <c r="B23" s="19">
+        <v>7827.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>1989</v>
+      </c>
+      <c r="B24" s="19">
+        <v>8672</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>1990</v>
+      </c>
+      <c r="B25" s="19">
+        <v>9137.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>1991</v>
+      </c>
+      <c r="B26" s="19">
+        <v>10168.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>1992</v>
+      </c>
+      <c r="B27" s="19">
+        <v>10271.200000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>1993</v>
+      </c>
+      <c r="B28" s="19">
+        <v>11208.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>1994</v>
+      </c>
+      <c r="B29" s="19">
+        <v>11796.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>1995</v>
+      </c>
+      <c r="B30" s="19">
+        <v>11927.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>1996</v>
+      </c>
+      <c r="B31" s="19">
+        <v>11977.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>1997</v>
+      </c>
+      <c r="B32" s="19">
+        <v>12559</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>1998</v>
+      </c>
+      <c r="B33" s="19">
+        <v>13380.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>1999</v>
+      </c>
+      <c r="B34" s="19">
+        <v>14959.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>2000</v>
+      </c>
+      <c r="B35" s="19">
+        <v>16890.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>2001</v>
+      </c>
+      <c r="B36" s="19">
+        <v>20065.099999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>2002</v>
+      </c>
+      <c r="B37" s="19">
+        <v>21620</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>2003</v>
+      </c>
+      <c r="B38" s="19">
+        <v>23005.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>2004</v>
+      </c>
+      <c r="B39" s="19">
+        <v>24947</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>2005</v>
+      </c>
+      <c r="B40" s="19">
+        <v>25687.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>2006</v>
+      </c>
+      <c r="B41" s="19">
+        <v>24669.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
+        <v>2007</v>
+      </c>
+      <c r="B42" s="19">
+        <v>25547.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="10">
+        <v>2008</v>
+      </c>
+      <c r="B43" s="19">
+        <v>26026.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>2009</v>
+      </c>
+      <c r="B44" s="19">
+        <v>31557.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
+        <v>2010</v>
+      </c>
+      <c r="B45" s="19">
+        <v>31192.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>2011</v>
+      </c>
+      <c r="B46" s="19">
+        <v>27680.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
+        <v>2012</v>
+      </c>
+      <c r="B47" s="19">
+        <v>27509.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
+        <v>2013</v>
+      </c>
+      <c r="B48" s="19">
+        <v>25772</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>2014</v>
+      </c>
+      <c r="B49" s="19">
+        <v>27429.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
+        <v>2015</v>
+      </c>
+      <c r="B50" s="19">
+        <v>27414.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="10">
+        <v>2016</v>
+      </c>
+      <c r="B51" s="19">
+        <v>28199.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="10">
+        <v>2017</v>
+      </c>
+      <c r="B52" s="19">
+        <v>28963.200000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="10">
+        <v>2018</v>
+      </c>
+      <c r="B53" s="19">
+        <v>31534.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="19">
+        <v>33359.199999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B2" s="8">
+        <v>15479.372747849708</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B3" s="8">
+        <v>16749.889769746431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B4" s="8">
+        <v>17697.708904694166</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B5" s="8">
+        <v>17450.413505627348</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B6" s="8">
+        <v>18440.740712537394</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B7" s="8">
+        <v>18476.421251664444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B8" s="8">
+        <v>18379.698666666663</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B9" s="8">
+        <v>19064.807244701347</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B10" s="8">
+        <v>20072.725999238672</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B11" s="8">
+        <v>22102.142939481269</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B12" s="8">
+        <v>24070.008444826311</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B13" s="8">
+        <v>26352.22656437305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B14" s="8">
+        <v>28355.276914002588</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B15" s="8">
+        <v>29911.36182428521</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B16" s="8">
+        <v>30386.137851575735</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B17" s="8">
+        <v>30522.589420654913</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B18" s="8">
+        <v>29928.347475604583</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B19" s="8">
+        <v>29286.985873605947</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B20" s="8">
+        <v>29255.380151745067</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B21" s="8">
+        <v>36183.475799999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>2010</v>
+      </c>
+      <c r="B22" s="8">
+        <v>34556.874385408402</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B23" s="8">
+        <v>30821.780472165548</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B24" s="8">
+        <v>29685.470852017937</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B25" s="8">
+        <v>27717.298705197973</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B26" s="8">
+        <v>28767.64301114899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B27" s="8">
+        <v>27865.534067935514</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7501,7 +9885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -11707,7 +14091,7 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -12964,716 +15348,59 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="19" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>1967</v>
-      </c>
-      <c r="B2" s="19">
-        <v>1454.3</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1968</v>
-      </c>
-      <c r="B3" s="19">
-        <v>1487.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>1969</v>
-      </c>
-      <c r="B4" s="19">
-        <v>1529.2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>1970</v>
-      </c>
-      <c r="B5" s="19">
-        <v>1475.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>1971</v>
-      </c>
-      <c r="B6" s="19">
-        <v>1644.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>1972</v>
-      </c>
-      <c r="B7" s="19">
-        <v>1903.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>1973</v>
-      </c>
-      <c r="B8" s="19">
-        <v>1916.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>1974</v>
-      </c>
-      <c r="B9" s="19">
-        <v>2214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>1975</v>
-      </c>
-      <c r="B10" s="19">
-        <v>2411.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>1976</v>
-      </c>
-      <c r="B11" s="19">
-        <v>2551.8000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>1977</v>
-      </c>
-      <c r="B12" s="19">
-        <v>2905.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>1978</v>
-      </c>
-      <c r="B13" s="19">
-        <v>3374.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>1979</v>
-      </c>
-      <c r="B14" s="19">
-        <v>3888.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>1980</v>
-      </c>
-      <c r="B15" s="19">
-        <v>4263.3999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>1981</v>
-      </c>
-      <c r="B16" s="19">
-        <v>4465.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>1982</v>
-      </c>
-      <c r="B17" s="19">
-        <v>4605.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>1983</v>
-      </c>
-      <c r="B18" s="19">
-        <v>4966.3999999999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>1984</v>
-      </c>
-      <c r="B19" s="19">
-        <v>5546.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>1985</v>
-      </c>
-      <c r="B20" s="19">
-        <v>6339.7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
-        <v>1986</v>
-      </c>
-      <c r="B21" s="19">
-        <v>6558.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>1987</v>
-      </c>
-      <c r="B22" s="19">
-        <v>7337.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
-        <v>1988</v>
-      </c>
-      <c r="B23" s="19">
-        <v>7827.7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
-        <v>1989</v>
-      </c>
-      <c r="B24" s="19">
-        <v>8672</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
-        <v>1990</v>
-      </c>
-      <c r="B25" s="19">
-        <v>9137.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
-        <v>1991</v>
-      </c>
-      <c r="B26" s="19">
-        <v>10168.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>1992</v>
-      </c>
-      <c r="B27" s="19">
-        <v>10271.200000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
-        <v>1993</v>
-      </c>
-      <c r="B28" s="19">
-        <v>11208.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
-        <v>1994</v>
-      </c>
-      <c r="B29" s="19">
-        <v>11796.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
-        <v>1995</v>
-      </c>
-      <c r="B30" s="19">
-        <v>11927.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
-        <v>1996</v>
-      </c>
-      <c r="B31" s="19">
-        <v>11977.8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
-        <v>1997</v>
-      </c>
-      <c r="B32" s="19">
-        <v>12559</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
-        <v>1998</v>
-      </c>
-      <c r="B33" s="19">
-        <v>13380.7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
-        <v>1999</v>
-      </c>
-      <c r="B34" s="19">
-        <v>14959.1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
-        <v>2000</v>
-      </c>
-      <c r="B35" s="19">
-        <v>16890.7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
-        <v>2001</v>
-      </c>
-      <c r="B36" s="19">
-        <v>20065.099999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
-        <v>2002</v>
-      </c>
-      <c r="B37" s="19">
-        <v>21620</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="10">
-        <v>2003</v>
-      </c>
-      <c r="B38" s="19">
-        <v>23005.8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="10">
-        <v>2004</v>
-      </c>
-      <c r="B39" s="19">
-        <v>24947</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="10">
-        <v>2005</v>
-      </c>
-      <c r="B40" s="19">
-        <v>25687.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="10">
-        <v>2006</v>
-      </c>
-      <c r="B41" s="19">
-        <v>24669.7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="10">
-        <v>2007</v>
-      </c>
-      <c r="B42" s="19">
-        <v>25547.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="10">
-        <v>2008</v>
-      </c>
-      <c r="B43" s="19">
-        <v>26026.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="10">
-        <v>2009</v>
-      </c>
-      <c r="B44" s="19">
-        <v>31557.8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="10">
-        <v>2010</v>
-      </c>
-      <c r="B45" s="19">
-        <v>31192.3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="10">
-        <v>2011</v>
-      </c>
-      <c r="B46" s="19">
-        <v>27680.3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="10">
-        <v>2012</v>
-      </c>
-      <c r="B47" s="19">
-        <v>27509.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="10">
-        <v>2013</v>
-      </c>
-      <c r="B48" s="19">
-        <v>25772</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="10">
-        <v>2014</v>
-      </c>
-      <c r="B49" s="19">
-        <v>27429.3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="10">
-        <v>2015</v>
-      </c>
-      <c r="B50" s="19">
-        <v>27414.7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="10">
-        <v>2016</v>
-      </c>
-      <c r="B51" s="19">
-        <v>28199.3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="10">
-        <v>2017</v>
-      </c>
-      <c r="B52" s="19">
-        <v>28963.200000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="10">
-        <v>2018</v>
-      </c>
-      <c r="B53" s="19">
-        <v>31534.1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B54" s="19">
-        <v>33359.199999999997</v>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="119" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="119" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup scale="58" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1990</v>
-      </c>
-      <c r="B2" s="8">
-        <v>15479.372747849708</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1991</v>
-      </c>
-      <c r="B3" s="8">
-        <v>16749.889769746431</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1992</v>
-      </c>
-      <c r="B4" s="8">
-        <v>17697.708904694166</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1993</v>
-      </c>
-      <c r="B5" s="8">
-        <v>17450.413505627348</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1994</v>
-      </c>
-      <c r="B6" s="8">
-        <v>18440.740712537394</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1995</v>
-      </c>
-      <c r="B7" s="8">
-        <v>18476.421251664444</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1996</v>
-      </c>
-      <c r="B8" s="8">
-        <v>18379.698666666663</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1997</v>
-      </c>
-      <c r="B9" s="8">
-        <v>19064.807244701347</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1998</v>
-      </c>
-      <c r="B10" s="8">
-        <v>20072.725999238672</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1999</v>
-      </c>
-      <c r="B11" s="8">
-        <v>22102.142939481269</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>2000</v>
-      </c>
-      <c r="B12" s="8">
-        <v>24070.008444826311</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>2001</v>
-      </c>
-      <c r="B13" s="8">
-        <v>26352.22656437305</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>2002</v>
-      </c>
-      <c r="B14" s="8">
-        <v>28355.276914002588</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>2003</v>
-      </c>
-      <c r="B15" s="8">
-        <v>29911.36182428521</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>2004</v>
-      </c>
-      <c r="B16" s="8">
-        <v>30386.137851575735</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>2005</v>
-      </c>
-      <c r="B17" s="8">
-        <v>30522.589420654913</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>2006</v>
-      </c>
-      <c r="B18" s="8">
-        <v>29928.347475604583</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>2007</v>
-      </c>
-      <c r="B19" s="8">
-        <v>29286.985873605947</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>2008</v>
-      </c>
-      <c r="B20" s="8">
-        <v>29255.380151745067</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>2009</v>
-      </c>
-      <c r="B21" s="8">
-        <v>36183.475799999993</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>2010</v>
-      </c>
-      <c r="B22" s="8">
-        <v>34556.874385408402</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B23" s="8">
-        <v>30821.780472165548</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>2012</v>
-      </c>
-      <c r="B24" s="8">
-        <v>29685.470852017937</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>2013</v>
-      </c>
-      <c r="B25" s="8">
-        <v>27717.298705197973</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>2014</v>
-      </c>
-      <c r="B26" s="8">
-        <v>28767.64301114899</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>2015</v>
-      </c>
-      <c r="B27" s="8">
-        <v>27865.534067935514</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="8"/>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="119" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="119"/>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="119" t="s">
+        <v>332</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="61" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Annotation for Shapira (2008)
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId11"/>
     <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId12"/>
     <sheet name="Figure - Causal Diagram" sheetId="9" r:id="rId13"/>
+    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Table - Determinants Examined'!$3:$4</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="334">
   <si>
     <t>Total</t>
   </si>
@@ -1289,6 +1290,9 @@
   </si>
   <si>
     <t>Dynamic Model of Research</t>
+  </si>
+  <si>
+    <t>Landscape of the Technology Transfer Literature</t>
   </si>
 </sst>
 </file>
@@ -1940,6 +1944,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1973,7 +1978,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -5176,10 +5180,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="44" name="Group 43">
+        <xdr:cNvPr id="14" name="Group 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{222B9149-065C-46EA-B831-ACFBF237DFA9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFA75878-1F3E-4CA0-9AFE-CEFDB7D7253A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5206,11 +5210,13 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm flipV="1">
-            <a:off x="4038600" y="2297112"/>
-            <a:ext cx="3200400" cy="1828800"/>
+            <a:off x="3810000" y="2297112"/>
+            <a:ext cx="3657600" cy="1828800"/>
           </a:xfrm>
           <a:prstGeom prst="trapezoid">
-            <a:avLst/>
+            <a:avLst>
+              <a:gd name="adj" fmla="val 37500"/>
+            </a:avLst>
           </a:prstGeom>
         </xdr:spPr>
         <xdr:style>
@@ -5251,8 +5257,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4038600" y="838200"/>
-            <a:ext cx="3200400" cy="1371600"/>
+            <a:off x="3810000" y="838200"/>
+            <a:ext cx="3657600" cy="1371600"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -5823,7 +5829,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="3238500" y="1524000"/>
-            <a:ext cx="800100" cy="0"/>
+            <a:ext cx="571500" cy="0"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
             <a:avLst/>
@@ -6039,8 +6045,8 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipH="1">
-            <a:off x="7010400" y="3209925"/>
-            <a:ext cx="700087" cy="1587"/>
+            <a:off x="7124700" y="3209925"/>
+            <a:ext cx="585787" cy="1587"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
             <a:avLst/>
@@ -6281,14 +6287,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -6305,8 +6311,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1590675" y="3162300"/>
-          <a:ext cx="923925" cy="895350"/>
+          <a:off x="1590675" y="981075"/>
+          <a:ext cx="923925" cy="885825"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -6334,23 +6340,200 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>490538</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50B02649-67D0-4B2F-97A3-2E8CC6A38276}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="6"/>
+          <a:endCxn id="3" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2962275" y="1666875"/>
+          <a:ext cx="2405063" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257874</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>33338</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>134191</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1794563F-DB42-4648-A1E2-F3FD2700A092}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="4"/>
+          <a:endCxn id="4" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5134674" y="2352675"/>
+          <a:ext cx="1604264" cy="1429591"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>146938</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>134191</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4BC694B-4A8B-4F15-9C1A-6322870BC39E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="1"/>
+          <a:endCxn id="2" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1590675" y="2352675"/>
+          <a:ext cx="1604263" cy="1429591"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>185738</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="34" name="Group 33">
+        <xdr:cNvPr id="19" name="Group 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD7B8D4D-A2F8-457B-BC7B-E9CF350C0283}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95875C9D-F54D-4871-BAFA-BA27BD4273AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6358,10 +6541,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="219075" y="990600"/>
-          <a:ext cx="8924925" cy="3571875"/>
-          <a:chOff x="219075" y="990600"/>
-          <a:chExt cx="8924925" cy="3571875"/>
+          <a:off x="219075" y="981075"/>
+          <a:ext cx="7891463" cy="3971925"/>
+          <a:chOff x="219075" y="981075"/>
+          <a:chExt cx="7891463" cy="3971925"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -6377,7 +6560,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="219075" y="3190875"/>
+            <a:off x="219075" y="981075"/>
             <a:ext cx="2743200" cy="1371600"/>
           </a:xfrm>
           <a:prstGeom prst="ellipse">
@@ -6438,7 +6621,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="3309938" y="990600"/>
+            <a:off x="5367338" y="981075"/>
             <a:ext cx="2743200" cy="1371600"/>
           </a:xfrm>
           <a:prstGeom prst="ellipse">
@@ -6487,7 +6670,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="6400800" y="3190875"/>
+            <a:off x="2793206" y="3581400"/>
             <a:ext cx="2743200" cy="1371600"/>
           </a:xfrm>
           <a:prstGeom prst="ellipse">
@@ -6527,138 +6710,6 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50B02649-67D0-4B2F-97A3-2E8CC6A38276}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="2" idx="7"/>
-            <a:endCxn id="3" idx="3"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="2560543" y="2161334"/>
-            <a:ext cx="1151127" cy="1230407"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:tailEnd type="triangle" w="lg" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1794563F-DB42-4648-A1E2-F3FD2700A092}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="3" idx="5"/>
-            <a:endCxn id="4" idx="1"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5651406" y="2161334"/>
-            <a:ext cx="1151126" cy="1230407"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:tailEnd type="triangle" w="lg" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4BC694B-4A8B-4F15-9C1A-6322870BC39E}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="4" idx="2"/>
-            <a:endCxn id="2" idx="6"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="2962275" y="3876675"/>
-            <a:ext cx="3438525" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:tailEnd type="triangle" w="lg" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
           <xdr:cNvPr id="29" name="TextBox 28">
@@ -6671,8 +6722,8 @@
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
-          <a:xfrm rot="18817857">
-            <a:off x="2038350" y="2581276"/>
+          <a:xfrm>
+            <a:off x="3143250" y="1390651"/>
             <a:ext cx="1828800" cy="276225"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -6721,8 +6772,8 @@
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
-          <a:xfrm rot="2811508">
-            <a:off x="5443537" y="2528887"/>
+          <a:xfrm rot="19068039">
+            <a:off x="5186361" y="3014662"/>
             <a:ext cx="1828800" cy="276225"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -6771,8 +6822,8 @@
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3738563" y="3948112"/>
+          <a:xfrm rot="2515645">
+            <a:off x="1290636" y="3062288"/>
             <a:ext cx="2011680" cy="276225"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7832,6 +7883,533 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>138112</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="16" name="Group 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ABA0FA4-84FC-4CC8-93D9-F9995137D79D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="138112" y="1447799"/>
+          <a:ext cx="6577013" cy="5305426"/>
+          <a:chOff x="585787" y="1447799"/>
+          <a:chExt cx="6577013" cy="5305426"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="3" name="Straight Connector 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D052D879-FECA-4ED7-8CEE-F3EAA04FB3AD}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4876800" y="1447799"/>
+            <a:ext cx="0" cy="4572000"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="4" name="Straight Connector 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4150CF5C-937B-4CE7-9150-CE8938AF1378}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="4876800" y="1447800"/>
+            <a:ext cx="0" cy="4572000"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="6" name="Straight Connector 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88A46163-3817-4B4C-9B32-F707056A5B8D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2562225" y="1476375"/>
+            <a:ext cx="0" cy="4572000"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="7" name="Straight Connector 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{735397BA-0237-4A09-8C10-6BB614A2404C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="4876800" y="3771900"/>
+            <a:ext cx="0" cy="4572000"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="TextBox 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22E619F1-71AD-4CC5-9132-621D821EE49E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2771775" y="6229350"/>
+            <a:ext cx="1838325" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Supply-Side</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="TextBox 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17F6B6C1-9C8C-4C36-8602-B1402047338C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5162550" y="6200775"/>
+            <a:ext cx="1838325" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Demand-Side</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="TextBox 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FD3130E-F110-467E-827C-B7BBA17952B1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="633413" y="4610100"/>
+            <a:ext cx="1838325" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Economic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> approach</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="TextBox 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1276320-DCDF-453E-8D71-B1F49995CD3F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="633413" y="2276475"/>
+            <a:ext cx="1838325" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Sociological</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> approach</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="TextBox 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17CB8D6C-AA5E-4022-9F24-C42E3BAD2D8F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3971925" y="6486525"/>
+            <a:ext cx="1838325" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1"/>
+              <a:t>Study</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+              <a:t> Perspective</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="TextBox 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D91C2FB0-30B3-47C7-B9E3-B25BB2E8E3F8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="-423863" y="3624263"/>
+            <a:ext cx="2286000" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1"/>
+              <a:t>Theorectical Framework</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9898,6 +10476,34 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="108" t="s">
+        <v>333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="82" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
@@ -10195,54 +10801,54 @@
       <c r="F20" s="29"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="108" t="s">
+      <c r="A21" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="108"/>
-      <c r="C21" s="108"/>
-      <c r="D21" s="108"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="108"/>
+      <c r="B21" s="109"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="109" t="s">
+      <c r="A22" s="110" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="109"/>
-      <c r="C22" s="109"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="109"/>
-      <c r="F22" s="109"/>
+      <c r="B22" s="110"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="110"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="110"/>
     </row>
     <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="108" t="s">
+      <c r="A23" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="108"/>
-      <c r="C23" s="108"/>
-      <c r="D23" s="108"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="108"/>
+      <c r="B23" s="109"/>
+      <c r="C23" s="109"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="109"/>
     </row>
     <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="108" t="s">
+      <c r="A24" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="108"/>
-      <c r="C24" s="108"/>
-      <c r="D24" s="108"/>
-      <c r="E24" s="108"/>
-      <c r="F24" s="108"/>
+      <c r="B24" s="109"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="109"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="108" t="s">
+      <c r="A25" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="108"/>
-      <c r="C25" s="108"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="108"/>
-      <c r="F25" s="108"/>
+      <c r="B25" s="109"/>
+      <c r="C25" s="109"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="109"/>
+      <c r="F25" s="109"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -10410,38 +11016,38 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="113" t="s">
+      <c r="E3" s="114" t="s">
         <v>276</v>
       </c>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="110" t="s">
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="111" t="s">
         <v>304</v>
       </c>
-      <c r="J3" s="111"/>
-      <c r="K3" s="110" t="s">
+      <c r="J3" s="112"/>
+      <c r="K3" s="111" t="s">
         <v>305</v>
       </c>
-      <c r="L3" s="112"/>
-      <c r="M3" s="113" t="s">
+      <c r="L3" s="113"/>
+      <c r="M3" s="114" t="s">
         <v>292</v>
       </c>
-      <c r="N3" s="114"/>
-      <c r="O3" s="111"/>
-      <c r="P3" s="115" t="s">
+      <c r="N3" s="115"/>
+      <c r="O3" s="112"/>
+      <c r="P3" s="116" t="s">
         <v>257</v>
       </c>
-      <c r="Q3" s="114"/>
-      <c r="R3" s="114"/>
-      <c r="S3" s="114"/>
-      <c r="T3" s="114"/>
-      <c r="U3" s="114"/>
-      <c r="V3" s="114"/>
-      <c r="W3" s="114"/>
-      <c r="X3" s="114"/>
-      <c r="Y3" s="114"/>
-      <c r="Z3" s="116"/>
+      <c r="Q3" s="115"/>
+      <c r="R3" s="115"/>
+      <c r="S3" s="115"/>
+      <c r="T3" s="115"/>
+      <c r="U3" s="115"/>
+      <c r="V3" s="115"/>
+      <c r="W3" s="115"/>
+      <c r="X3" s="115"/>
+      <c r="Y3" s="115"/>
+      <c r="Z3" s="117"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -13717,10 +14323,10 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="113" t="s">
+      <c r="D3" s="114" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="111"/>
+      <c r="E3" s="112"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -13980,32 +14586,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="108"/>
-      <c r="B24" s="108"/>
-      <c r="C24" s="108"/>
-      <c r="D24" s="108"/>
-      <c r="E24" s="108"/>
+      <c r="A24" s="109"/>
+      <c r="B24" s="109"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="109"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="108"/>
-      <c r="B25" s="108"/>
-      <c r="C25" s="108"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="108"/>
+      <c r="A25" s="109"/>
+      <c r="B25" s="109"/>
+      <c r="C25" s="109"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="109"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="108"/>
-      <c r="B26" s="108"/>
-      <c r="C26" s="108"/>
-      <c r="D26" s="108"/>
-      <c r="E26" s="108"/>
+      <c r="A26" s="109"/>
+      <c r="B26" s="109"/>
+      <c r="C26" s="109"/>
+      <c r="D26" s="109"/>
+      <c r="E26" s="109"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="108"/>
-      <c r="B27" s="108"/>
-      <c r="C27" s="108"/>
-      <c r="D27" s="108"/>
-      <c r="E27" s="108"/>
+      <c r="A27" s="109"/>
+      <c r="B27" s="109"/>
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -14807,27 +15413,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="108"/>
-      <c r="B17" s="108"/>
-      <c r="C17" s="108"/>
+      <c r="A17" s="109"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="109"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="108"/>
-      <c r="B18" s="108"/>
-      <c r="C18" s="108"/>
+      <c r="A18" s="109"/>
+      <c r="B18" s="109"/>
+      <c r="C18" s="109"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="108"/>
-      <c r="B19" s="108"/>
-      <c r="C19" s="108"/>
+      <c r="A19" s="109"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="109"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -15266,30 +15872,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="117" t="s">
+      <c r="A42" s="118" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="117"/>
-      <c r="C42" s="117"/>
+      <c r="B42" s="118"/>
+      <c r="C42" s="118"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="118" t="s">
+      <c r="A43" s="119" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="118"/>
-      <c r="C43" s="118"/>
+      <c r="B43" s="119"/>
+      <c r="C43" s="119"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="117" t="s">
+      <c r="A44" s="118" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="117"/>
-      <c r="C44" s="117"/>
+      <c r="B44" s="118"/>
+      <c r="C44" s="118"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="108"/>
-      <c r="B45" s="108"/>
-      <c r="C45" s="108"/>
+      <c r="A45" s="109"/>
+      <c r="B45" s="109"/>
+      <c r="C45" s="109"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>
@@ -15353,23 +15959,23 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="108" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="119" t="s">
+      <c r="A3" s="108" t="s">
         <v>331</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="58" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="54" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -15381,26 +15987,28 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="108" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="119"/>
+      <c r="A2" s="108"/>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="119" t="s">
+      <c r="A3" s="108" t="s">
         <v>332</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="61" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="70" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modifed figure on experimental situation
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="339">
   <si>
     <t>Total</t>
   </si>
@@ -1293,6 +1293,22 @@
   </si>
   <si>
     <t>Landscape of the Technology Transfer Literature</t>
+  </si>
+  <si>
+    <t>Policy Target</t>
+  </si>
+  <si>
+    <t>Supply-side</t>
+  </si>
+  <si>
+    <t>Demand-side</t>
+  </si>
+  <si>
+    <t>Demand-side
+Supply-side</t>
+  </si>
+  <si>
+    <t>Conceptual Model of Experimental Situation</t>
   </si>
 </sst>
 </file>
@@ -1631,7 +1647,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1949,6 +1965,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1978,6 +1997,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -6285,14 +6305,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>221457</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
@@ -6311,8 +6331,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1590675" y="981075"/>
-          <a:ext cx="923925" cy="885825"/>
+          <a:off x="2050257" y="981075"/>
+          <a:ext cx="540543" cy="885825"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -6340,14 +6360,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>373857</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>490538</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>519113</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -6367,8 +6387,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2962275" y="1666875"/>
-          <a:ext cx="2405063" cy="0"/>
+          <a:off x="3421857" y="1666875"/>
+          <a:ext cx="4412456" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -6399,16 +6419,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>257874</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>501953</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>27734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>33338</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>311245</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>134191</xdr:rowOff>
+      <xdr:rowOff>153241</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -6420,14 +6440,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="3" idx="4"/>
+          <a:stCxn id="3" idx="3"/>
           <a:endCxn id="4" idx="7"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5134674" y="2352675"/>
-          <a:ext cx="1604264" cy="1429591"/>
+          <a:off x="6597953" y="2151809"/>
+          <a:ext cx="1638092" cy="1649507"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -6458,16 +6478,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581725</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>27734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>146938</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>391017</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>134191</xdr:rowOff>
+      <xdr:rowOff>153241</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -6480,13 +6500,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="4" idx="1"/>
-          <a:endCxn id="2" idx="4"/>
+          <a:endCxn id="2" idx="5"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="1590675" y="2352675"/>
-          <a:ext cx="1604263" cy="1429591"/>
+          <a:off x="3020125" y="2151809"/>
+          <a:ext cx="1638092" cy="1649507"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -6517,350 +6537,413 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>69057</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>185738</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>373857</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="19" name="Group 18">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95875C9D-F54D-4871-BAFA-BA27BD4273AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E10819E4-450E-49A4-91C4-82AF281BA697}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="219075" y="981075"/>
-          <a:ext cx="7891463" cy="3971925"/>
-          <a:chOff x="219075" y="981075"/>
-          <a:chExt cx="7891463" cy="3971925"/>
+          <a:off x="678657" y="981075"/>
+          <a:ext cx="2743200" cy="1371600"/>
         </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="2" name="Oval 1">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E10819E4-450E-49A4-91C4-82AF281BA697}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="219075" y="981075"/>
-            <a:ext cx="2743200" cy="1371600"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>What are the</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" baseline="0"/>
-              <a:t> gaps in society's</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t> fundamental understanding</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" baseline="0"/>
-              <a:t> of the natural and social world?</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Oval 2">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{930E372F-5F04-4DE8-A25C-B16E7B2C883F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5367338" y="981075"/>
-            <a:ext cx="2743200" cy="1371600"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" baseline="0"/>
-              <a:t>How can society apply current knowledge about the natural and social world to achieve specific ends?</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Oval 3">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDAE0998-753E-4345-9310-EC249E6CCC00}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2793206" y="3581400"/>
-            <a:ext cx="2743200" cy="1371600"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="9144" rIns="9144" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>What limitations prevent society from successfully applying current knowledge</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" baseline="0"/>
-              <a:t> about the natural and social world to achieve specific ends?</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="29" name="TextBox 28">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AB3B73C-A23F-481D-AC44-54596C488527}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3143250" y="1390651"/>
-            <a:ext cx="1828800" cy="276225"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>What are the</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> gaps in society's</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> fundamental understanding</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> of the natural and social world?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>519113</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>214313</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{930E372F-5F04-4DE8-A25C-B16E7B2C883F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7834313" y="981075"/>
+          <a:ext cx="2743200" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>How can society apply current knowledge about the natural and social world to achieve specific ends?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>598885</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>294085</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Oval 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDAE0998-753E-4345-9310-EC249E6CCC00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4256485" y="3600450"/>
+          <a:ext cx="2743200" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="9144" rIns="9144" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>What limitations prevent society from successfully applying current knowledge</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> about the natural and social world to achieve specific ends?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>468630</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="TextBox 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AB3B73C-A23F-481D-AC44-54596C488527}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4552950" y="1390651"/>
+          <a:ext cx="2011680" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
           <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>Basic research</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="30" name="TextBox 29">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8F54F25-E6AF-46B4-8656-23BB78E03F1E}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="19068039">
-            <a:off x="5186361" y="3014662"/>
-            <a:ext cx="1828800" cy="276225"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="9144" rIns="9144" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Curiosity-inspried</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>basic research</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123822</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>400047</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="TextBox 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8F54F25-E6AF-46B4-8656-23BB78E03F1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18880966">
+          <a:off x="6662735" y="2909887"/>
+          <a:ext cx="1828800" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
           <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>Applied research</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="31" name="TextBox 30">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97CA5EE9-4332-42E6-9E6F-044D7BADDCF1}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="2515645">
-            <a:off x="1290636" y="3062288"/>
-            <a:ext cx="2011680" cy="276225"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Applied research</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>529590</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>146687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>196215</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>62867</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="TextBox 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97CA5EE9-4332-42E6-9E6F-044D7BADDCF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2712934">
+          <a:off x="2709863" y="2947989"/>
+          <a:ext cx="2011680" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
           <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>Research problem identification</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Use-inspried basic research</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6993,15 +7076,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7017,7 +7100,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="752475" y="728662"/>
+          <a:off x="485775" y="3224212"/>
           <a:ext cx="1828800" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7077,15 +7160,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7101,7 +7184,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5334000" y="728662"/>
+          <a:off x="5562600" y="3224212"/>
           <a:ext cx="1828800" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7165,13 +7248,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7227,7 +7310,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>KP</a:t>
+            <a:t>DP</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="-25000">
@@ -7246,13 +7329,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7308,7 +7391,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>KP</a:t>
+            <a:t>DP</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="-25000">
@@ -7327,13 +7410,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7389,7 +7472,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>KP</a:t>
+            <a:t>DP</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="-25000">
@@ -7406,15 +7489,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7433,8 +7516,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2581275" y="1185862"/>
-          <a:ext cx="2752725" cy="0"/>
+          <a:off x="2314575" y="3681412"/>
+          <a:ext cx="3248025" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -7466,14 +7549,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7486,17 +7569,18 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="2" idx="2"/>
           <a:endCxn id="9" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="1902618" y="1407318"/>
-          <a:ext cx="909638" cy="1381125"/>
+        <a:xfrm>
+          <a:off x="1657350" y="4138612"/>
+          <a:ext cx="1390650" cy="909638"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln w="25400">
           <a:solidFill>
@@ -7526,13 +7610,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>180976</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>104777</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>52386</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7545,13 +7629,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
           <a:endCxn id="10" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="1197771" y="1831182"/>
-          <a:ext cx="2043109" cy="1638300"/>
+          <a:off x="1204913" y="4333874"/>
+          <a:ext cx="2028825" cy="1638300"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -7584,13 +7669,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>533401</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7640,16 +7725,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -7660,15 +7745,12 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="9" idx="3"/>
-          <a:endCxn id="8" idx="2"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4876800" y="1643062"/>
-          <a:ext cx="1371600" cy="909638"/>
+          <a:off x="4867275" y="4148137"/>
+          <a:ext cx="1390650" cy="909638"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -7701,13 +7783,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7721,12 +7803,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="10" idx="3"/>
+          <a:endCxn id="8" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4867275" y="1647825"/>
-          <a:ext cx="1609725" cy="2024062"/>
+          <a:off x="4867275" y="4138612"/>
+          <a:ext cx="1609725" cy="2028825"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -7759,13 +7842,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7817,13 +7900,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>109538</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>166689</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>461963</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>52389</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7878,6 +7961,268 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rectangle 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{607722A7-0A06-44C0-835D-2088A6A4A6C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="2409825" y="1171575"/>
+          <a:ext cx="1828800" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Asborptive capacity</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rectangle 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC4F0E75-89CB-4D8A-8F57-C110832D2580}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="3514725" y="1171575"/>
+          <a:ext cx="1828800" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Organizational slack</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8CC71DE-30FA-4561-98F8-E7B24F9EBA13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="16" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3324225" y="2543175"/>
+          <a:ext cx="0" cy="1133475"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>166688</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{927C467B-1531-4473-9834-ECF608E77259}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="18" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4429125" y="2543175"/>
+          <a:ext cx="4763" cy="1119187"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -10465,14 +10810,26 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="121" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10483,7 +10840,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -10493,7 +10850,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="121" t="s">
         <v>333</v>
       </c>
     </row>
@@ -10506,33 +10863,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="2.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" customWidth="1"/>
     <col min="5" max="5" width="2.7109375" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
@@ -10547,8 +10904,12 @@
       <c r="F3" s="34" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="34"/>
+      <c r="H3" s="34" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>1980</v>
       </c>
@@ -10563,8 +10924,12 @@
       <c r="F4" s="29" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="109"/>
+      <c r="H4" s="109" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>1980</v>
       </c>
@@ -10579,8 +10944,12 @@
       <c r="F5" s="29" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="109"/>
+      <c r="H5" s="109" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>1982</v>
       </c>
@@ -10595,8 +10964,12 @@
       <c r="F6" s="29" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="109"/>
+      <c r="H6" s="109" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30">
         <v>1984</v>
       </c>
@@ -10611,8 +10984,12 @@
       <c r="F7" s="29" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="109"/>
+      <c r="H7" s="109" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
         <v>1986</v>
       </c>
@@ -10627,8 +11004,12 @@
       <c r="F8" s="29" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="109"/>
+      <c r="H8" s="109" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30">
         <v>1987</v>
       </c>
@@ -10643,8 +11024,12 @@
       <c r="F9" s="29" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="109"/>
+      <c r="H9" s="109" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30">
         <v>1987</v>
       </c>
@@ -10659,8 +11044,12 @@
       <c r="F10" s="29" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="109"/>
+      <c r="H10" s="109" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30">
         <v>1988</v>
       </c>
@@ -10675,8 +11064,12 @@
       <c r="F11" s="29" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="109"/>
+      <c r="H11" s="109" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30">
         <v>1989</v>
       </c>
@@ -10691,8 +11084,12 @@
       <c r="F12" s="29" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="109"/>
+      <c r="H12" s="109" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30">
         <v>1991</v>
       </c>
@@ -10707,8 +11104,12 @@
       <c r="F13" s="29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="109"/>
+      <c r="H13" s="109" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
         <v>1993</v>
       </c>
@@ -10723,8 +11124,12 @@
       <c r="F14" s="29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="109"/>
+      <c r="H14" s="109" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30">
         <v>1995</v>
       </c>
@@ -10739,8 +11144,12 @@
       <c r="F15" s="29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="109"/>
+      <c r="H15" s="109" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="54">
         <v>2000</v>
       </c>
@@ -10755,8 +11164,12 @@
       <c r="F16" s="38" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="38"/>
+      <c r="H16" s="38" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="54">
         <v>2011</v>
       </c>
@@ -10771,16 +11184,22 @@
       <c r="F17" s="38" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="38"/>
+      <c r="H17" s="38" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="55"/>
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
       <c r="D18" s="41"/>
       <c r="E18" s="41"/>
       <c r="F18" s="41"/>
-    </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+    </row>
+    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>22</v>
       </c>
@@ -10789,8 +11208,10 @@
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="109"/>
+      <c r="H19" s="109"/>
+    </row>
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>55</v>
       </c>
@@ -10799,120 +11220,138 @@
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
-    </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="109" t="s">
+      <c r="G20" s="109"/>
+      <c r="H20" s="109"/>
+    </row>
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="110" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="109"/>
-      <c r="C21" s="109"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="109"/>
-      <c r="F21" s="109"/>
-    </row>
-    <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="110" t="s">
+      <c r="B21" s="110"/>
+      <c r="C21" s="110"/>
+      <c r="D21" s="110"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="110"/>
+    </row>
+    <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="111" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="110"/>
-      <c r="C22" s="110"/>
-      <c r="D22" s="110"/>
-      <c r="E22" s="110"/>
-      <c r="F22" s="110"/>
-    </row>
-    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="109" t="s">
+      <c r="B22" s="111"/>
+      <c r="C22" s="111"/>
+      <c r="D22" s="111"/>
+      <c r="E22" s="111"/>
+      <c r="F22" s="111"/>
+    </row>
+    <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="110" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="109"/>
-      <c r="C23" s="109"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="109"/>
-      <c r="F23" s="109"/>
-    </row>
-    <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="109" t="s">
+      <c r="B23" s="110"/>
+      <c r="C23" s="110"/>
+      <c r="D23" s="110"/>
+      <c r="E23" s="110"/>
+      <c r="F23" s="110"/>
+    </row>
+    <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="110" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="109"/>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="109"/>
-    </row>
-    <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="109" t="s">
+      <c r="B24" s="110"/>
+      <c r="C24" s="110"/>
+      <c r="D24" s="110"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="110"/>
+    </row>
+    <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="110" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="109"/>
-      <c r="C25" s="109"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="109"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="110"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="110"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="110"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
       <c r="F26" s="29"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="109"/>
+      <c r="H26" s="109"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="30"/>
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="109"/>
+      <c r="H27" s="109"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="30"/>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
       <c r="F28" s="29"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="109"/>
+      <c r="H28" s="109"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="30"/>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
       <c r="E29" s="29"/>
       <c r="F29" s="29"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="109"/>
+      <c r="H29" s="109"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="30"/>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
       <c r="D30" s="29"/>
       <c r="E30" s="29"/>
       <c r="F30" s="29"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="109"/>
+      <c r="H30" s="109"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="30"/>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
       <c r="D31" s="29"/>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="109"/>
+      <c r="H31" s="109"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
       <c r="F32" s="29"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="109"/>
+      <c r="H32" s="109"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
       <c r="D33" s="29"/>
       <c r="E33" s="29"/>
       <c r="F33" s="29"/>
+      <c r="G33" s="109"/>
+      <c r="H33" s="109"/>
     </row>
   </sheetData>
   <sortState ref="A2:D28">
@@ -11016,38 +11455,38 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="114" t="s">
+      <c r="E3" s="115" t="s">
         <v>276</v>
       </c>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="111" t="s">
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="112" t="s">
         <v>304</v>
       </c>
-      <c r="J3" s="112"/>
-      <c r="K3" s="111" t="s">
+      <c r="J3" s="113"/>
+      <c r="K3" s="112" t="s">
         <v>305</v>
       </c>
-      <c r="L3" s="113"/>
-      <c r="M3" s="114" t="s">
+      <c r="L3" s="114"/>
+      <c r="M3" s="115" t="s">
         <v>292</v>
       </c>
-      <c r="N3" s="115"/>
-      <c r="O3" s="112"/>
-      <c r="P3" s="116" t="s">
+      <c r="N3" s="116"/>
+      <c r="O3" s="113"/>
+      <c r="P3" s="117" t="s">
         <v>257</v>
       </c>
-      <c r="Q3" s="115"/>
-      <c r="R3" s="115"/>
-      <c r="S3" s="115"/>
-      <c r="T3" s="115"/>
-      <c r="U3" s="115"/>
-      <c r="V3" s="115"/>
-      <c r="W3" s="115"/>
-      <c r="X3" s="115"/>
-      <c r="Y3" s="115"/>
-      <c r="Z3" s="117"/>
+      <c r="Q3" s="116"/>
+      <c r="R3" s="116"/>
+      <c r="S3" s="116"/>
+      <c r="T3" s="116"/>
+      <c r="U3" s="116"/>
+      <c r="V3" s="116"/>
+      <c r="W3" s="116"/>
+      <c r="X3" s="116"/>
+      <c r="Y3" s="116"/>
+      <c r="Z3" s="118"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14323,10 +14762,10 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="114" t="s">
+      <c r="D3" s="115" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="112"/>
+      <c r="E3" s="113"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14586,32 +15025,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="109"/>
-      <c r="B24" s="109"/>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
+      <c r="A24" s="110"/>
+      <c r="B24" s="110"/>
+      <c r="C24" s="110"/>
+      <c r="D24" s="110"/>
+      <c r="E24" s="110"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="109"/>
-      <c r="B25" s="109"/>
-      <c r="C25" s="109"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="109"/>
+      <c r="A25" s="110"/>
+      <c r="B25" s="110"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="110"/>
+      <c r="E25" s="110"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="109"/>
-      <c r="B26" s="109"/>
-      <c r="C26" s="109"/>
-      <c r="D26" s="109"/>
-      <c r="E26" s="109"/>
+      <c r="A26" s="110"/>
+      <c r="B26" s="110"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="110"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="109"/>
-      <c r="B27" s="109"/>
-      <c r="C27" s="109"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="109"/>
+      <c r="A27" s="110"/>
+      <c r="B27" s="110"/>
+      <c r="C27" s="110"/>
+      <c r="D27" s="110"/>
+      <c r="E27" s="110"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -15413,27 +15852,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="109"/>
-      <c r="B17" s="109"/>
-      <c r="C17" s="109"/>
+      <c r="A17" s="110"/>
+      <c r="B17" s="110"/>
+      <c r="C17" s="110"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="109"/>
-      <c r="B18" s="109"/>
-      <c r="C18" s="109"/>
+      <c r="A18" s="110"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="110"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="109"/>
-      <c r="B19" s="109"/>
-      <c r="C19" s="109"/>
+      <c r="A19" s="110"/>
+      <c r="B19" s="110"/>
+      <c r="C19" s="110"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -15872,30 +16311,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="118" t="s">
+      <c r="A42" s="119" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="118"/>
-      <c r="C42" s="118"/>
+      <c r="B42" s="119"/>
+      <c r="C42" s="119"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="119" t="s">
+      <c r="A43" s="120" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="119"/>
-      <c r="C43" s="119"/>
+      <c r="B43" s="120"/>
+      <c r="C43" s="120"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="118" t="s">
+      <c r="A44" s="119" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="118"/>
-      <c r="C44" s="118"/>
+      <c r="B44" s="119"/>
+      <c r="C44" s="119"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="109"/>
-      <c r="B45" s="109"/>
-      <c r="C45" s="109"/>
+      <c r="A45" s="110"/>
+      <c r="B45" s="110"/>
+      <c r="C45" s="110"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>
@@ -15959,7 +16398,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -15969,7 +16410,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="121" t="s">
         <v>331</v>
       </c>
     </row>
@@ -15987,9 +16428,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -16002,7 +16441,7 @@
       <c r="A2" s="108"/>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="121" t="s">
         <v>332</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Figure on theory of human behavior in organizational contexts
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -24,8 +24,9 @@
     <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId10"/>
     <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId11"/>
     <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId12"/>
-    <sheet name="Figure - Causal Diagram" sheetId="9" r:id="rId13"/>
-    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId14"/>
+    <sheet name="Figure - Experimental Situation" sheetId="9" r:id="rId13"/>
+    <sheet name="Figure - Theory" sheetId="15" r:id="rId14"/>
+    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Table - Determinants Examined'!$3:$4</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="340">
   <si>
     <t>Total</t>
   </si>
@@ -1309,6 +1310,9 @@
   </si>
   <si>
     <t>Conceptual Model of Experimental Situation</t>
+  </si>
+  <si>
+    <t>Conceptual Theory of Human Behavior in Organizational Contexts</t>
   </si>
 </sst>
 </file>
@@ -1964,6 +1968,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1997,7 +2002,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -8233,6 +8237,2271 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{112D4868-B282-4C3E-93A6-7029C3F8EE2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66675" y="3224212"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Motivation</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369094</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>521494</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6169B0DD-68CB-4FC2-A52E-A411FB8FEE39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2807494" y="3224212"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Goal</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Decisions</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ADC73F4-8064-4E0C-97CD-607A2E0330F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1533525" y="4276725"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Decision Premises</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C87B261B-F5D3-4ADC-AFC1-767297EAED04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6915150" y="4276725"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Decision Premises</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369094</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9D4ED10-AF00-495B-84E6-7262040648DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1438275" y="3452812"/>
+          <a:ext cx="1369219" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>257177</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76203</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Connector: Elbow 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{579D0DC2-B176-4FD9-9CA7-6B30E73F024B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="804865" y="3776665"/>
+          <a:ext cx="790572" cy="666747"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Connector: Elbow 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F35639BC-17AA-4A20-B1FE-C31691DD264E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="47" idx="1"/>
+          <a:endCxn id="2" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="752476" y="3681412"/>
+          <a:ext cx="6181725" cy="1843088"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>130969</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Connector: Elbow 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA365311-2A9E-4E91-ADB9-0466D14C0B1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="50" idx="2"/>
+          <a:endCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="6156722" y="3746896"/>
+          <a:ext cx="828675" cy="688181"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>445294</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Connector: Elbow 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEBC04C0-C200-4103-B345-288E135D6C8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="3" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2905125" y="3681412"/>
+          <a:ext cx="588169" cy="823913"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Connector: Elbow 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{178BF1B2-5124-4AFF-9876-37D1AA50280C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="40" idx="2"/>
+          <a:endCxn id="47" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="10472738" y="1509713"/>
+          <a:ext cx="1847850" cy="6181725"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>471488</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Connector: Elbow 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7662CE94-3FF8-4F3A-9ECC-299F86A9B0B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="3"/>
+          <a:endCxn id="19" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8286750" y="3676650"/>
+          <a:ext cx="719138" cy="828675"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>109538</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>166689</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>461963</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>52389</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC8E44C7-8653-4DAF-A98D-6C82D9F6276A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3714751" y="6715126"/>
+          <a:ext cx="457200" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>. . .</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>395288</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>547688</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Rectangle 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{222E1D97-B053-4F72-B79C-FCF721309183}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8320088" y="3219450"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Action Decisions</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>207169</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>395288</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB33D517-9176-4DD8-A158-4702B345613E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="50" idx="3"/>
+          <a:endCxn id="19" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6912769" y="3448050"/>
+          <a:ext cx="1407319" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>88107</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>240507</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Rectangle 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DDF71EE-3507-4CB2-A353-4275753CD67B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11060907" y="3219450"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Actions</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>547688</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>88107</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A21EB507-804E-4AA9-A1D9-BA7B9F1C771C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="19" idx="3"/>
+          <a:endCxn id="22" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9691688" y="3448050"/>
+          <a:ext cx="1369219" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Rectangle 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34280298-5C2E-4C59-B30A-2BD06D9D6EDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13801725" y="3219450"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Outcomes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>240507</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Arrow Connector 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01841C2A-75FF-4B6F-834F-3736959FE6B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="22" idx="3"/>
+          <a:endCxn id="40" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12432507" y="3448050"/>
+          <a:ext cx="1369218" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="Rectangle 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7732693-81E6-4C04-921A-9F7D33823AAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6934200" y="5295900"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Assessment</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>54769</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>207169</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Rectangle 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBB14082-7FD4-4E35-9392-EEC6D5D32D82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5541169" y="3219450"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Perceived Options</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>521494</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>54769</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Straight Arrow Connector 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49FCC327-0912-42FE-925A-FCAE31B5B98A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="50" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4179094" y="3448050"/>
+          <a:ext cx="1362075" cy="4762"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="157" name="Group 156">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0728202-5D9E-4DFF-9D8D-1A6E81A5045B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2009776" y="1009649"/>
+          <a:ext cx="11115674" cy="2447926"/>
+          <a:chOff x="2002632" y="1014412"/>
+          <a:chExt cx="11072812" cy="2447926"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="45" name="Group 44">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{818FB88D-4680-48AD-8A12-7201248072B4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="6624638" y="1014412"/>
+            <a:ext cx="1821656" cy="1828800"/>
+            <a:chOff x="5353050" y="1009649"/>
+            <a:chExt cx="1828800" cy="1828800"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="43" name="Group 42">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78DF7D60-F0A3-4C1C-B4B2-BEE4C1B91C67}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="5444490" y="1128712"/>
+              <a:ext cx="1645920" cy="1590675"/>
+              <a:chOff x="5396865" y="1084421"/>
+              <a:chExt cx="1645920" cy="1590675"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="84" name="Rectangle 83">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D1C0CA5-37D6-4047-8AE5-BC1F0AC3FB9E}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="5396865" y="2217896"/>
+                <a:ext cx="1645920" cy="457200"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Environmental Factors</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="85" name="Rectangle 84">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA3A926B-81E6-4DBA-9BCD-82E23E39637A}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="5396865" y="1651159"/>
+                <a:ext cx="1645920" cy="457200"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Organizational Factors</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="88" name="Rectangle 87">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEDF6A07-79AD-4608-8341-C909208EB683}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="5396865" y="1084421"/>
+                <a:ext cx="1645920" cy="457200"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Individual Factors</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="44" name="Rectangle 43">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F65BFDC2-7932-4B76-B187-D70D5CDA7D65}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5353050" y="1009649"/>
+              <a:ext cx="1828800" cy="1828800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="111" name="Connector: Elbow 110">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7AE589E-F38F-4650-8A0D-FC78B8CF6865}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="44" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="10800000" flipV="1">
+            <a:off x="2002632" y="1928812"/>
+            <a:ext cx="4622007" cy="1533526"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 99897"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="116" name="Connector: Elbow 115">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BB9F9BF-953C-422B-AB92-216F0C93D0FA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="44" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="10800000" flipV="1">
+            <a:off x="4745831" y="1928812"/>
+            <a:ext cx="1878807" cy="1514476"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 100000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="121" name="Connector: Elbow 120">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDC9698B-739E-4491-9CD8-E606DF187FA2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="44" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8446294" y="1928812"/>
+            <a:ext cx="1850231" cy="1533526"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 100256"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="126" name="Connector: Elbow 125">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24ADCC6A-A336-40A3-952D-A8CAAD32FDA9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="44" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8446294" y="1928812"/>
+            <a:ext cx="4629150" cy="1514476"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 100000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="130" name="Connector: Elbow 129">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2134B77-EF39-4D49-920C-4BCE0D633126}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="44" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="7229474" y="3148012"/>
+            <a:ext cx="609604" cy="3"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 50000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>88891</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>42079</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>88891</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>156379</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="142" name="Group 141">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C52BA6-FC43-4646-B23E-7D9141CF726D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="10452091" y="6157129"/>
+          <a:ext cx="1828800" cy="1828800"/>
+          <a:chOff x="5353050" y="1009649"/>
+          <a:chExt cx="1828800" cy="1828800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="143" name="Group 142">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEBCF2D3-F95D-4D2E-86B2-910D7F5EA0D0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="5444490" y="1128712"/>
+            <a:ext cx="1645920" cy="1590675"/>
+            <a:chOff x="5396865" y="1084421"/>
+            <a:chExt cx="1645920" cy="1590675"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="145" name="Rectangle 144">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA49BB23-E295-4576-8000-E6DAB4B65D04}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5396865" y="2217896"/>
+              <a:ext cx="1645920" cy="457200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Environmental Factors</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="146" name="Rectangle 145">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF5FEFB4-16D8-4D59-A62A-59690049B6DE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5396865" y="1651159"/>
+              <a:ext cx="1645920" cy="457200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Organizational Factors</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="147" name="Rectangle 146">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A08F3ED7-02EC-40E8-8EE0-6BC4191D6964}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5396865" y="1084421"/>
+              <a:ext cx="1645920" cy="457200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Individual Factors</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="144" name="Rectangle 143">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FE487F7-7041-4684-B4EF-F0A4071BBCC5}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5353050" y="1009649"/>
+            <a:ext cx="1828800" cy="1828800"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>390526</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>393692</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>42079</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="149" name="Connector: Elbow 148">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA290536-ECB1-4F9B-981D-B2DA44F3F3AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="144" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="11058119" y="5848757"/>
+          <a:ext cx="613579" cy="3166"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>138112</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
@@ -10812,7 +13081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -10822,7 +13091,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="110" t="s">
         <v>338</v>
       </c>
     </row>
@@ -10840,6 +13109,34 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="110" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10850,7 +13147,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="110" t="s">
         <v>333</v>
       </c>
     </row>
@@ -11224,54 +13521,54 @@
       <c r="H20" s="109"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="110" t="s">
+      <c r="A21" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="110"/>
-      <c r="C21" s="110"/>
-      <c r="D21" s="110"/>
-      <c r="E21" s="110"/>
-      <c r="F21" s="110"/>
+      <c r="B21" s="111"/>
+      <c r="C21" s="111"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="111"/>
+      <c r="F21" s="111"/>
     </row>
     <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="111" t="s">
+      <c r="A22" s="112" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="111"/>
-      <c r="C22" s="111"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="111"/>
-      <c r="F22" s="111"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="112"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="112"/>
+      <c r="F22" s="112"/>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="110" t="s">
+      <c r="A23" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="110"/>
-      <c r="C23" s="110"/>
-      <c r="D23" s="110"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="110"/>
+      <c r="B23" s="111"/>
+      <c r="C23" s="111"/>
+      <c r="D23" s="111"/>
+      <c r="E23" s="111"/>
+      <c r="F23" s="111"/>
     </row>
     <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="110" t="s">
+      <c r="A24" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="110"/>
-      <c r="C24" s="110"/>
-      <c r="D24" s="110"/>
-      <c r="E24" s="110"/>
-      <c r="F24" s="110"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="111"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="111"/>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="110" t="s">
+      <c r="A25" s="111" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="110"/>
-      <c r="C25" s="110"/>
-      <c r="D25" s="110"/>
-      <c r="E25" s="110"/>
-      <c r="F25" s="110"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="111"/>
+      <c r="D25" s="111"/>
+      <c r="E25" s="111"/>
+      <c r="F25" s="111"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -11455,38 +13752,38 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="115" t="s">
+      <c r="E3" s="116" t="s">
         <v>276</v>
       </c>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="113"/>
-      <c r="I3" s="112" t="s">
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="114"/>
+      <c r="I3" s="113" t="s">
         <v>304</v>
       </c>
-      <c r="J3" s="113"/>
-      <c r="K3" s="112" t="s">
+      <c r="J3" s="114"/>
+      <c r="K3" s="113" t="s">
         <v>305</v>
       </c>
-      <c r="L3" s="114"/>
-      <c r="M3" s="115" t="s">
+      <c r="L3" s="115"/>
+      <c r="M3" s="116" t="s">
         <v>292</v>
       </c>
-      <c r="N3" s="116"/>
-      <c r="O3" s="113"/>
-      <c r="P3" s="117" t="s">
+      <c r="N3" s="117"/>
+      <c r="O3" s="114"/>
+      <c r="P3" s="118" t="s">
         <v>257</v>
       </c>
-      <c r="Q3" s="116"/>
-      <c r="R3" s="116"/>
-      <c r="S3" s="116"/>
-      <c r="T3" s="116"/>
-      <c r="U3" s="116"/>
-      <c r="V3" s="116"/>
-      <c r="W3" s="116"/>
-      <c r="X3" s="116"/>
-      <c r="Y3" s="116"/>
-      <c r="Z3" s="118"/>
+      <c r="Q3" s="117"/>
+      <c r="R3" s="117"/>
+      <c r="S3" s="117"/>
+      <c r="T3" s="117"/>
+      <c r="U3" s="117"/>
+      <c r="V3" s="117"/>
+      <c r="W3" s="117"/>
+      <c r="X3" s="117"/>
+      <c r="Y3" s="117"/>
+      <c r="Z3" s="119"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14762,10 +17059,10 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="116" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="113"/>
+      <c r="E3" s="114"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15025,32 +17322,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="110"/>
-      <c r="B24" s="110"/>
-      <c r="C24" s="110"/>
-      <c r="D24" s="110"/>
-      <c r="E24" s="110"/>
+      <c r="A24" s="111"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="111"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="111"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="110"/>
-      <c r="B25" s="110"/>
-      <c r="C25" s="110"/>
-      <c r="D25" s="110"/>
-      <c r="E25" s="110"/>
+      <c r="A25" s="111"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="111"/>
+      <c r="D25" s="111"/>
+      <c r="E25" s="111"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="110"/>
-      <c r="B26" s="110"/>
-      <c r="C26" s="110"/>
-      <c r="D26" s="110"/>
-      <c r="E26" s="110"/>
+      <c r="A26" s="111"/>
+      <c r="B26" s="111"/>
+      <c r="C26" s="111"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="111"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="110"/>
-      <c r="B27" s="110"/>
-      <c r="C27" s="110"/>
-      <c r="D27" s="110"/>
-      <c r="E27" s="110"/>
+      <c r="A27" s="111"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="111"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -15852,27 +18149,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="110"/>
-      <c r="B17" s="110"/>
-      <c r="C17" s="110"/>
+      <c r="A17" s="111"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="111"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="110"/>
-      <c r="B18" s="110"/>
-      <c r="C18" s="110"/>
+      <c r="A18" s="111"/>
+      <c r="B18" s="111"/>
+      <c r="C18" s="111"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="110"/>
-      <c r="B19" s="110"/>
-      <c r="C19" s="110"/>
+      <c r="A19" s="111"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="111"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -16311,30 +18608,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="119" t="s">
+      <c r="A42" s="120" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="119"/>
-      <c r="C42" s="119"/>
+      <c r="B42" s="120"/>
+      <c r="C42" s="120"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="120" t="s">
+      <c r="A43" s="121" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="120"/>
-      <c r="C43" s="120"/>
+      <c r="B43" s="121"/>
+      <c r="C43" s="121"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="119" t="s">
+      <c r="A44" s="120" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="119"/>
-      <c r="C44" s="119"/>
+      <c r="B44" s="120"/>
+      <c r="C44" s="120"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="110"/>
-      <c r="B45" s="110"/>
-      <c r="C45" s="110"/>
+      <c r="A45" s="111"/>
+      <c r="B45" s="111"/>
+      <c r="C45" s="111"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>
@@ -16410,7 +18707,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="110" t="s">
         <v>331</v>
       </c>
     </row>
@@ -16441,7 +18738,7 @@
       <c r="A2" s="108"/>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="110" t="s">
         <v>332</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added communication as mediator in figure of theory
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -8611,15 +8611,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>257177</xdr:colOff>
+      <xdr:colOff>514354</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>76203</xdr:rowOff>
+      <xdr:rowOff>47627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>314324</xdr:colOff>
+      <xdr:colOff>314326</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8636,8 +8636,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="804865" y="3776665"/>
-          <a:ext cx="790572" cy="666747"/>
+          <a:off x="919166" y="3890965"/>
+          <a:ext cx="819147" cy="409572"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -8671,13 +8671,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>142876</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:rowOff>42863</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>228601</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8695,8 +8695,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="752476" y="3681412"/>
-          <a:ext cx="6181725" cy="1843088"/>
+          <a:off x="752476" y="3681413"/>
+          <a:ext cx="6181725" cy="2328863"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -8789,11 +8789,11 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>445294</xdr:colOff>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -8808,13 +8808,12 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="4" idx="3"/>
-          <a:endCxn id="3" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2905125" y="3681412"/>
-          <a:ext cx="588169" cy="823913"/>
+          <a:off x="2905125" y="3676650"/>
+          <a:ext cx="390525" cy="828675"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -8846,15 +8845,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>381001</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8872,8 +8871,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="10472738" y="1509713"/>
-          <a:ext cx="1847850" cy="6181725"/>
+          <a:off x="10229851" y="1752600"/>
+          <a:ext cx="2333625" cy="6181725"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -8959,73 +8958,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>109538</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>166689</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>461963</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>52389</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="TextBox 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC8E44C7-8653-4DAF-A98D-6C82D9F6276A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="3714751" y="6715126"/>
-          <a:ext cx="457200" cy="352425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>. . .</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -9428,14 +9360,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -9450,7 +9382,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6934200" y="5295900"/>
+          <a:off x="6934200" y="5781675"/>
           <a:ext cx="1371600" cy="457200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10158,14 +10090,14 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>88891</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>42079</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>146854</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>88891</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>156379</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>70654</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -10180,7 +10112,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10452091" y="6157129"/>
+          <a:off x="10452091" y="6642904"/>
           <a:ext cx="1828800" cy="1828800"/>
           <a:chOff x="5353050" y="1009649"/>
           <a:chExt cx="1828800" cy="1828800"/>
@@ -10438,14 +10370,14 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>390526</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>393692</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>42079</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>146854</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -10462,13 +10394,402 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="11058119" y="5848757"/>
+          <a:off x="11058119" y="6334532"/>
           <a:ext cx="613579" cy="3166"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
             <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314323</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466723</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>157163</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Rectangle 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE0453F7-FF2B-43B2-8FD7-5646FC627E33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1533523" y="4862513"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Communication</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47627</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314323</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Connector: Elbow 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8354F54-6C08-4759-A94C-C35383918343}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="42" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="550069" y="4107658"/>
+          <a:ext cx="1404935" cy="561973"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466723</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>445294</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Connector: Elbow 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A8F5619-AF25-4A06-83F8-3BC52DD92A6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="42" idx="3"/>
+          <a:endCxn id="3" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2905123" y="3681412"/>
+          <a:ext cx="588171" cy="1409701"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209548</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>361948</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="Rectangle 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CE05044-F794-448C-A2F0-21C3C7FE2EAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6915148" y="4848226"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Communication</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209548</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Connector: Elbow 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A247CB47-38DC-45B9-A909-6F0DECD7DCF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="55" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5786435" y="3948113"/>
+          <a:ext cx="1409702" cy="847724"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>361948</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Connector: Elbow 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD489028-7AA7-4449-B6EE-8684493E9538}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="55" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8286748" y="3676650"/>
+          <a:ext cx="933452" cy="1400176"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
         </a:prstGeom>
         <a:ln w="25400">
           <a:solidFill>

</xml_diff>

<commit_message>
Annotation for Perkman, et al. (2013) and figure on applied research
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -25,8 +25,9 @@
     <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId11"/>
     <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId12"/>
     <sheet name="Figure - Experimental Situation" sheetId="9" r:id="rId13"/>
-    <sheet name="Figure - Theory" sheetId="15" r:id="rId14"/>
-    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId15"/>
+    <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId14"/>
+    <sheet name="Figure - Research" sheetId="16" r:id="rId15"/>
+    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Table - Determinants Examined'!$3:$4</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="341">
   <si>
     <t>Total</t>
   </si>
@@ -1313,6 +1314,9 @@
   </si>
   <si>
     <t>Conceptual Theory of Human Behavior in Organizational Contexts</t>
+  </si>
+  <si>
+    <t>Applied Research as a Mediating Variable</t>
   </si>
 </sst>
 </file>
@@ -9495,7 +9499,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Perceived Options</a:t>
+            <a:t>Options</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -10823,22 +10827,1020 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>138112</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>140017</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E986B7DC-01D2-42B9-B5AD-5E00930072DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190500" y="852487"/>
+          <a:ext cx="1371600" cy="640080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Curiosity-driven</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Basic Research</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>11906</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>164306</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB6CE6AB-EF54-4294-8361-356BD361C2B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4279106" y="2447925"/>
+          <a:ext cx="1371600" cy="640080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Applied Research</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>106679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>11906</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>81914</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Connector: Elbow 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{944C5D8A-09D2-404D-B62E-86369904C42E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="2"/>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="3566398" y="2055256"/>
+          <a:ext cx="737235" cy="688181"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>164306</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>273844</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>81915</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Connector: Elbow 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55EC332F-6B68-4502-8633-8227FDA270B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="6" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5650706" y="2030730"/>
+          <a:ext cx="719138" cy="737235"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>197644</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
+      <xdr:colOff>350044</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35456FC6-331E-4BF3-BF87-ECAB724FA2F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5684044" y="1390650"/>
+          <a:ext cx="1371600" cy="640080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Economic Productivity</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>197644</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52161E5F-F49F-4DCB-8DE4-1614A924A2F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="3"/>
+          <a:endCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4276725" y="1710690"/>
+          <a:ext cx="1407319" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA71DC0C-B14C-495B-9F38-970F91075C74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2905125" y="1390650"/>
+          <a:ext cx="1371600" cy="640080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Fundamental</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Knowledge</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>135255</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{917397A2-F98A-4899-A12F-D177BCAE38D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="180975" y="1990725"/>
+          <a:ext cx="1371600" cy="640080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Use-inspired</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Basic Research</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>10477</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Connector: Elbow 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1D9EC1D-93AD-4E4D-AC52-7CD313B06861}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1562100" y="1172527"/>
+          <a:ext cx="1343025" cy="538163"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Connector: Elbow 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD00A752-6D3F-4066-A3D5-EB329D3D0B6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="3"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1552575" y="1710690"/>
+          <a:ext cx="1352550" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>555625</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22E619F1-71AD-4CC5-9132-621D821EE49E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2365375" y="7480300"/>
+          <a:ext cx="1819275" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Supply-Side</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17F6B6C1-9C8C-4C36-8602-B1402047338C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5610225" y="7486650"/>
+          <a:ext cx="1838325" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Demand-Side</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>166688</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>176213</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FD3130E-F110-467E-827C-B7BBA17952B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="166688" y="5305425"/>
+          <a:ext cx="1838325" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Economic</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Theory</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>185738</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>195263</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1276320-DCDF-453E-8D71-B1F49995CD3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="185738" y="2276475"/>
+          <a:ext cx="1838325" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Organization</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Theory</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>217487</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="16" name="Group 15">
+        <xdr:cNvPr id="13" name="Group 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ABA0FA4-84FC-4CC8-93D9-F9995137D79D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C8E447B-EC35-45FE-B02D-B1754FAF62D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10846,390 +11848,12 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="138112" y="1447799"/>
-          <a:ext cx="6577013" cy="5305426"/>
-          <a:chOff x="585787" y="1447799"/>
-          <a:chExt cx="6577013" cy="5305426"/>
+          <a:off x="217487" y="823912"/>
+          <a:ext cx="7967663" cy="7240588"/>
+          <a:chOff x="138112" y="836612"/>
+          <a:chExt cx="7885113" cy="7240588"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="3" name="Straight Connector 2">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D052D879-FECA-4ED7-8CEE-F3EAA04FB3AD}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4876800" y="1447799"/>
-            <a:ext cx="0" cy="4572000"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="4" name="Straight Connector 3">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4150CF5C-937B-4CE7-9150-CE8938AF1378}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="16200000">
-            <a:off x="4876800" y="1447800"/>
-            <a:ext cx="0" cy="4572000"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="6" name="Straight Connector 5">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88A46163-3817-4B4C-9B32-F707056A5B8D}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2562225" y="1476375"/>
-            <a:ext cx="0" cy="4572000"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="7" name="Straight Connector 6">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{735397BA-0237-4A09-8C10-6BB614A2404C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="16200000">
-            <a:off x="4876800" y="3771900"/>
-            <a:ext cx="0" cy="4572000"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="TextBox 7">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22E619F1-71AD-4CC5-9132-621D821EE49E}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2771775" y="6229350"/>
-            <a:ext cx="1838325" cy="266700"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>Supply-Side</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="TextBox 9">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17F6B6C1-9C8C-4C36-8602-B1402047338C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5162550" y="6200775"/>
-            <a:ext cx="1838325" cy="266700"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>Demand-Side</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="TextBox 10">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FD3130E-F110-467E-827C-B7BBA17952B1}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="633413" y="4610100"/>
-            <a:ext cx="1838325" cy="266700"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>Economic</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" baseline="0"/>
-              <a:t> approach</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="12" name="TextBox 11">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1276320-DCDF-453E-8D71-B1F49995CD3F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="633413" y="2276475"/>
-            <a:ext cx="1838325" cy="266700"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>Sociological</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100" baseline="0"/>
-              <a:t> approach</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
           <xdr:cNvPr id="14" name="TextBox 13">
@@ -11243,8 +11867,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="3971925" y="6486525"/>
-            <a:ext cx="1838325" cy="266700"/>
+            <a:off x="3948113" y="7810500"/>
+            <a:ext cx="1819275" cy="266700"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -11300,7 +11924,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm rot="16200000">
-            <a:off x="-423863" y="3624263"/>
+            <a:off x="-871538" y="3903662"/>
             <a:ext cx="2286000" cy="266700"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -11339,6 +11963,191 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="9" name="Group 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95D76F0-DF02-4C8B-A70B-710F15E84147}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1692275" y="836612"/>
+            <a:ext cx="6330950" cy="6400800"/>
+            <a:chOff x="2038350" y="1309687"/>
+            <a:chExt cx="6400800" cy="6400800"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="3" name="Straight Connector 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D052D879-FECA-4ED7-8CEE-F3EAA04FB3AD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5133975" y="1309687"/>
+              <a:ext cx="0" cy="6400800"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="4" name="Straight Connector 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4150CF5C-937B-4CE7-9150-CE8938AF1378}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm rot="16200000">
+              <a:off x="5238750" y="1309688"/>
+              <a:ext cx="0" cy="6400800"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="Freeform: Shape 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA5A996-1E33-41F8-AA5F-AF4891FB8A2B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2038350" y="1309687"/>
+              <a:ext cx="6400800" cy="6400800"/>
+            </a:xfrm>
+            <a:custGeom>
+              <a:avLst/>
+              <a:gdLst>
+                <a:gd name="connsiteX0" fmla="*/ 0 w 4819650"/>
+                <a:gd name="connsiteY0" fmla="*/ 0 h 3143250"/>
+                <a:gd name="connsiteX1" fmla="*/ 0 w 4819650"/>
+                <a:gd name="connsiteY1" fmla="*/ 3143250 h 3143250"/>
+                <a:gd name="connsiteX2" fmla="*/ 4819650 w 4819650"/>
+                <a:gd name="connsiteY2" fmla="*/ 3143250 h 3143250"/>
+              </a:gdLst>
+              <a:ahLst/>
+              <a:cxnLst>
+                <a:cxn ang="0">
+                  <a:pos x="connsiteX0" y="connsiteY0"/>
+                </a:cxn>
+                <a:cxn ang="0">
+                  <a:pos x="connsiteX1" y="connsiteY1"/>
+                </a:cxn>
+                <a:cxn ang="0">
+                  <a:pos x="connsiteX2" y="connsiteY2"/>
+                </a:cxn>
+              </a:cxnLst>
+              <a:rect l="l" t="t" r="r" b="b"/>
+              <a:pathLst>
+                <a:path w="4819650" h="3143250">
+                  <a:moveTo>
+                    <a:pt x="0" y="0"/>
+                  </a:moveTo>
+                  <a:lnTo>
+                    <a:pt x="0" y="3143250"/>
+                  </a:lnTo>
+                  <a:lnTo>
+                    <a:pt x="4819650" y="3143250"/>
+                  </a:lnTo>
+                </a:path>
+              </a:pathLst>
+            </a:custGeom>
+            <a:noFill/>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -13469,6 +14278,34 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
+        <v>340</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="82" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="110" t="s">
         <v>333</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified figure on theory of research
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -24,9 +24,9 @@
     <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId10"/>
     <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId11"/>
     <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId12"/>
-    <sheet name="Figure - Experimental Situation" sheetId="9" r:id="rId13"/>
+    <sheet name="Figure - Research" sheetId="16" r:id="rId13"/>
     <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId14"/>
-    <sheet name="Figure - Research" sheetId="16" r:id="rId15"/>
+    <sheet name="Figure - Conceptual Framework" sheetId="9" r:id="rId15"/>
     <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId16"/>
   </sheets>
   <definedNames>
@@ -1310,13 +1310,13 @@
 Supply-side</t>
   </si>
   <si>
-    <t>Conceptual Model of Experimental Situation</t>
-  </si>
-  <si>
     <t>Conceptual Theory of Human Behavior in Organizational Contexts</t>
   </si>
   <si>
     <t>Applied Research as a Mediating Variable</t>
+  </si>
+  <si>
+    <t>Conceptual Framework</t>
   </si>
 </sst>
 </file>
@@ -7085,22 +7085,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>140017</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7FBD581-9132-4175-AC34-BD98A9A52BD0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E986B7DC-01D2-42B9-B5AD-5E00930072DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7108,8 +7108,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="485775" y="3224212"/>
-          <a:ext cx="1828800" cy="914400"/>
+          <a:off x="190500" y="852487"/>
+          <a:ext cx="1371600" cy="640080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7148,19 +7148,21 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Development stage of </a:t>
+            <a:t>Curiosity-driven</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1200">
+            <a:rPr lang="en-US" sz="1200" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>the  technology</a:t>
+            <a:t> Basic Research</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -7168,23 +7170,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>11906</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>164306</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectangle 7">
+        <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78775CEB-9626-4660-A44C-8F70D0A13B5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB6CE6AB-EF54-4294-8361-356BD361C2B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7192,8 +7194,204 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5562600" y="3224212"/>
-          <a:ext cx="1828800" cy="914400"/>
+          <a:off x="4279106" y="2447925"/>
+          <a:ext cx="1371600" cy="640080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Applied Research</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>106679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>11906</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>81914</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Connector: Elbow 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{944C5D8A-09D2-404D-B62E-86369904C42E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="2"/>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="3566398" y="2055256"/>
+          <a:ext cx="737235" cy="688181"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>164306</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>273844</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>81915</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Connector: Elbow 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55EC332F-6B68-4502-8633-8227FDA270B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="6" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5650706" y="2030730"/>
+          <a:ext cx="719138" cy="737235"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>197644</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>350044</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35456FC6-331E-4BF3-BF87-ECAB724FA2F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5684044" y="1390650"/>
+          <a:ext cx="1371600" cy="640080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7232,21 +7430,8 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Recommendation to</a:t>
+            <a:t>Societal Benefits</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> add the technology to the decision agenda</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -7254,23 +7439,82 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>197644</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52161E5F-F49F-4DCB-8DE4-1614A924A2F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="3"/>
+          <a:endCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4276725" y="1710690"/>
+          <a:ext cx="1407319" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 8">
+        <xdr:cNvPr id="8" name="Rectangle 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EDF8CFA-62CE-4CD9-A1E4-E2051F7B335E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA71DC0C-B14C-495B-9F38-970F91075C74}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7278,8 +7522,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3048000" y="2095500"/>
-          <a:ext cx="1828800" cy="914400"/>
+          <a:off x="2905125" y="1390650"/>
+          <a:ext cx="1371600" cy="640080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7318,16 +7562,21 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>DP</a:t>
+            <a:t>Fundamental</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="-25000">
+            <a:rPr lang="en-US" sz="1200" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>1</a:t>
+            <a:t> Knowledge</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -7335,23 +7584,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>135255</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="Rectangle 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0DC8DD-F6A6-40DC-831A-338DFA26E651}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{917397A2-F98A-4899-A12F-D177BCAE38D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7359,8 +7608,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3038475" y="3214687"/>
-          <a:ext cx="1828800" cy="914400"/>
+          <a:off x="180975" y="1990725"/>
+          <a:ext cx="1371600" cy="640080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7399,16 +7648,32 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>DP</a:t>
+            <a:t>Use-inspired</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="-25000">
+            <a:rPr lang="en-US" sz="1200" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>2</a:t>
+            <a:t> </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Basic Research</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -7416,23 +7681,141 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>10477</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Connector: Elbow 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1D9EC1D-93AD-4E4D-AC52-7CD313B06861}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1562100" y="1172527"/>
+          <a:ext cx="1343025" cy="538163"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Connector: Elbow 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD00A752-6D3F-4066-A3D5-EB329D3D0B6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="3"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1552575" y="1710690"/>
+          <a:ext cx="1352550" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1905</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 10">
+        <xdr:cNvPr id="12" name="Rectangle 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CB89335-6580-458F-8E57-39173AA7E02B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDF70D99-7556-4E0E-8B76-F515DE70741E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7440,8 +7823,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3048000" y="4733925"/>
-          <a:ext cx="1828800" cy="914400"/>
+          <a:off x="4267200" y="2133600"/>
+          <a:ext cx="1371600" cy="640080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7480,15 +7863,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>DP</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="-25000">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>n</a:t>
+            <a:t>Culture</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -7497,714 +7872,34 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1905</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA9B58F4-BE0E-4B02-98BA-EB1FC72D1482}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39826F15-D9C4-4DC7-8B7D-6BD493584CF3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="2" idx="3"/>
-          <a:endCxn id="8" idx="1"/>
+          <a:stCxn id="12" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2314575" y="3681412"/>
-          <a:ext cx="3248025" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Connector: Elbow 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BFF46A-19D4-4457-9D4F-D6C6E98861B2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="9" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1657350" y="4138612"/>
-          <a:ext cx="1390650" cy="909638"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>180976</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>52386</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="Connector: Elbow 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52FF6E3E-4187-43E2-8A05-5FF131F06074}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="2" idx="2"/>
-          <a:endCxn id="10" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="1204913" y="4333874"/>
-          <a:ext cx="2028825" cy="1638300"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>533401</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="Connector: Elbow 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BB21842-A987-4D88-A9C0-33EB2875A2D0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="11" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="319088" y="2462212"/>
-          <a:ext cx="3552825" cy="1905000"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="21" name="Connector: Elbow 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1206A40E-C509-4A7E-8F73-FB30DDBCCC48}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4867275" y="4148137"/>
-          <a:ext cx="1390650" cy="909638"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="23" name="Connector: Elbow 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CB449B0-6103-42E2-BE6D-DE4E2DD869CE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="10" idx="3"/>
-          <a:endCxn id="8" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4867275" y="4138612"/>
-          <a:ext cx="1609725" cy="2028825"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Connector: Elbow 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{703ADAEA-785F-4395-B619-4D90E53856D5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="11" idx="3"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4876800" y="1638300"/>
-          <a:ext cx="1847850" cy="3552825"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>109538</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>166689</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>461963</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>52389</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B7D077-5FD9-4402-9CB4-F8AAA2C8A7B5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="3714751" y="4219576"/>
-          <a:ext cx="457200" cy="352425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>. . .</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Rectangle 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{607722A7-0A06-44C0-835D-2088A6A4A6C3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="2409825" y="1171575"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Asborptive capacity</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Rectangle 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC4F0E75-89CB-4D8A-8F57-C110832D2580}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="3514725" y="1171575"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Organizational slack</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8CC71DE-30FA-4561-98F8-E7B24F9EBA13}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="16" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3324225" y="2543175"/>
-          <a:ext cx="0" cy="1133475"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>166688</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{927C467B-1531-4473-9834-ECF608E77259}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="18" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4429125" y="2543175"/>
-          <a:ext cx="4763" cy="1119187"/>
+          <a:off x="4953000" y="2773680"/>
+          <a:ext cx="0" cy="731520"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10827,22 +10522,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>140017</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E986B7DC-01D2-42B9-B5AD-5E00930072DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7FBD581-9132-4175-AC34-BD98A9A52BD0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10850,8 +10545,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="190500" y="852487"/>
-          <a:ext cx="1371600" cy="640080"/>
+          <a:off x="485775" y="3224212"/>
+          <a:ext cx="1828800" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10890,21 +10585,19 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Curiosity-driven</a:t>
+            <a:t>Development stage of </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
+            <a:rPr lang="en-US" sz="1200">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> Basic Research</a:t>
+            <a:t>the  technology</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -10912,23 +10605,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>11906</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>164306</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>20955</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2">
+        <xdr:cNvPr id="8" name="Rectangle 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB6CE6AB-EF54-4294-8361-356BD361C2B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78775CEB-9626-4660-A44C-8F70D0A13B5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10936,8 +10629,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4279106" y="2447925"/>
-          <a:ext cx="1371600" cy="640080"/>
+          <a:off x="5562600" y="3224212"/>
+          <a:ext cx="1828800" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10976,9 +10669,9 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Applied Research</a:t>
+            <a:t>Add the technology to the decision agenda</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+          <a:endParaRPr lang="en-US" sz="1200">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -10991,140 +10684,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>106679</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>11906</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>81914</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Connector: Elbow 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{944C5D8A-09D2-404D-B62E-86369904C42E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="8" idx="2"/>
-          <a:endCxn id="3" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="3566398" y="2055256"/>
-          <a:ext cx="737235" cy="688181"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>164306</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>273844</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>81915</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Connector: Elbow 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55EC332F-6B68-4502-8633-8227FDA270B7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="3" idx="3"/>
-          <a:endCxn id="6" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5650706" y="2030730"/>
-          <a:ext cx="719138" cy="737235"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>197644</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>350044</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 5">
+        <xdr:cNvPr id="9" name="Rectangle 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35456FC6-331E-4BF3-BF87-ECAB724FA2F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EDF8CFA-62CE-4CD9-A1E4-E2051F7B335E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11132,8 +10707,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5684044" y="1390650"/>
-          <a:ext cx="1371600" cy="640080"/>
+          <a:off x="3048000" y="2095500"/>
+          <a:ext cx="1828800" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11172,7 +10747,15 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Economic Productivity</a:t>
+            <a:t>DP</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="-25000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -11181,82 +10764,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>197644</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52161E5F-F49F-4DCB-8DE4-1614A924A2F5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="8" idx="3"/>
-          <a:endCxn id="6" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4276725" y="1710690"/>
-          <a:ext cx="1407319" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectangle 7">
+        <xdr:cNvPr id="10" name="Rectangle 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA71DC0C-B14C-495B-9F38-970F91075C74}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0DC8DD-F6A6-40DC-831A-338DFA26E651}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11264,8 +10788,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2905125" y="1390650"/>
-          <a:ext cx="1371600" cy="640080"/>
+          <a:off x="3038475" y="3214687"/>
+          <a:ext cx="1828800" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11304,21 +10828,16 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Fundamental</a:t>
+            <a:t>DP</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
+            <a:rPr lang="en-US" sz="1200" baseline="-25000">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> Knowledge</a:t>
+            <a:t>2</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -11326,23 +10845,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>135255</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 9">
+        <xdr:cNvPr id="11" name="Rectangle 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{917397A2-F98A-4899-A12F-D177BCAE38D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CB89335-6580-458F-8E57-39173AA7E02B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11350,8 +10869,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="180975" y="1990725"/>
-          <a:ext cx="1371600" cy="640080"/>
+          <a:off x="3048000" y="4733925"/>
+          <a:ext cx="1828800" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11390,32 +10909,16 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Use-inspired</a:t>
+            <a:t>DP</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
+            <a:rPr lang="en-US" sz="1200" baseline="-25000">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> </a:t>
+            <a:t>n</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Basic Research</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -11423,23 +10926,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>10477</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="Connector: Elbow 12">
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1D9EC1D-93AD-4E4D-AC52-7CD313B06861}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA9B58F4-BE0E-4B02-98BA-EB1FC72D1482}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11450,17 +10953,17 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1562100" y="1172527"/>
-          <a:ext cx="1343025" cy="538163"/>
+          <a:off x="2314575" y="3681412"/>
+          <a:ext cx="3248025" cy="0"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
+        <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="25400">
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="med"/>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -11483,43 +10986,663 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>5715</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Connector: Elbow 13">
+        <xdr:cNvPr id="15" name="Connector: Elbow 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD00A752-6D3F-4066-A3D5-EB329D3D0B6B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BFF46A-19D4-4457-9D4F-D6C6E98861B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="10" idx="3"/>
-          <a:endCxn id="8" idx="1"/>
+          <a:endCxn id="9" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="1552575" y="1710690"/>
-          <a:ext cx="1352550" cy="600075"/>
+        <a:xfrm>
+          <a:off x="1657350" y="4138612"/>
+          <a:ext cx="1390650" cy="909638"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119061</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Connector: Elbow 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52FF6E3E-4187-43E2-8A05-5FF131F06074}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="10" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1204913" y="4333874"/>
+          <a:ext cx="2028825" cy="1638300"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="25400">
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="med"/>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Connector: Elbow 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BB21842-A987-4D88-A9C0-33EB2875A2D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="11" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="319088" y="2462212"/>
+          <a:ext cx="3552825" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Connector: Elbow 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1206A40E-C509-4A7E-8F73-FB30DDBCCC48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4867275" y="4148137"/>
+          <a:ext cx="1390650" cy="909638"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Connector: Elbow 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CB449B0-6103-42E2-BE6D-DE4E2DD869CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="3"/>
+          <a:endCxn id="8" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4867275" y="4138612"/>
+          <a:ext cx="1609725" cy="2028825"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Connector: Elbow 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{703ADAEA-785F-4395-B619-4D90E53856D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4876800" y="1638300"/>
+          <a:ext cx="1847850" cy="3552825"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>109538</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>166689</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>461963</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>52389</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B7D077-5FD9-4402-9CB4-F8AAA2C8A7B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3714751" y="4219576"/>
+          <a:ext cx="457200" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>. . .</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rectangle 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{607722A7-0A06-44C0-835D-2088A6A4A6C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="2409825" y="1171575"/>
+          <a:ext cx="1828800" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Asborptive capacity</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rectangle 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC4F0E75-89CB-4D8A-8F57-C110832D2580}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="3514725" y="1171575"/>
+          <a:ext cx="1828800" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Organizational slack</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8CC71DE-30FA-4561-98F8-E7B24F9EBA13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="16" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3324225" y="2543175"/>
+          <a:ext cx="0" cy="1133475"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>166688</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{927C467B-1531-4473-9834-ECF608E77259}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="18" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4429125" y="2543175"/>
+          <a:ext cx="4763" cy="1119187"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -14209,9 +14332,12 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -14222,12 +14348,21 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>338</v>
-      </c>
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="110"/>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="110"/>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="110"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="82" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -14239,7 +14374,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -14250,7 +14385,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -14262,9 +14397,6 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -14283,7 +14415,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="82" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Modified figures of research and conceptual framework
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -20,11 +20,11 @@
     <sheet name="Table - NASA TRL Scale" sheetId="7" r:id="rId6"/>
     <sheet name="Table - Alt Readiness Scales" sheetId="8" r:id="rId7"/>
     <sheet name="Figure - Defining Technology" sheetId="12" r:id="rId8"/>
-    <sheet name="Figure - Dynamic Research Model" sheetId="13" r:id="rId9"/>
-    <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId10"/>
-    <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId11"/>
-    <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId12"/>
-    <sheet name="Figure - Research" sheetId="16" r:id="rId13"/>
+    <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId9"/>
+    <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId10"/>
+    <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId11"/>
+    <sheet name="Figure - Research Cycle" sheetId="13" r:id="rId12"/>
+    <sheet name="Figure - Research Model" sheetId="16" r:id="rId13"/>
     <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId14"/>
     <sheet name="Figure - Conceptual Framework" sheetId="9" r:id="rId15"/>
     <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId16"/>
@@ -1291,9 +1291,6 @@
     <t>The Narrowing Definition of Technology</t>
   </si>
   <si>
-    <t>Dynamic Model of Research</t>
-  </si>
-  <si>
     <t>Landscape of the Technology Transfer Literature</t>
   </si>
   <si>
@@ -1310,13 +1307,16 @@
 Supply-side</t>
   </si>
   <si>
-    <t>Conceptual Theory of Human Behavior in Organizational Contexts</t>
-  </si>
-  <si>
-    <t>Applied Research as a Mediating Variable</t>
-  </si>
-  <si>
     <t>Conceptual Framework</t>
+  </si>
+  <si>
+    <t>The Relationship Between Research and Societal Benefits</t>
+  </si>
+  <si>
+    <t>Theory of Human Behavior in Organizational Contexts</t>
+  </si>
+  <si>
+    <t>Research Cycle</t>
   </si>
 </sst>
 </file>
@@ -6314,6 +6314,129 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
+      <xdr:colOff>14286</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26F7D4F1-F364-4657-9D16-9F8E7A94596F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EF3FF4B-317E-4C31-9A51-7A6D86881DF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D659FB0-32AA-45AE-9E5C-A428E08AC8E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>221457</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6952,129 +7075,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>14286</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26F7D4F1-F364-4657-9D16-9F8E7A94596F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EF3FF4B-317E-4C31-9A51-7A6D86881DF7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D659FB0-32AA-45AE-9E5C-A428E08AC8E7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -7909,6 +7909,127 @@
             <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>135256</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>88106</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>20956</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Connector: Elbow 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42DC2956-7615-4D19-B6A0-79DCBB617F61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="10" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1">
+          <a:off x="2687241" y="1410415"/>
+          <a:ext cx="457200" cy="4098131"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>62864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Connector: Elbow 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1A8CA25-340B-4342-88F5-D1481BCDDA47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="2533650" y="1253489"/>
+          <a:ext cx="1733550" cy="1022985"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="med"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -10514,6 +10635,66 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>30861</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="Connector: Elbow 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAB35973-1A11-4FB9-BAFA-554FA922B9C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="47" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3733801" y="3669411"/>
+          <a:ext cx="3200400" cy="2340864"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100148"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -13031,465 +13212,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="19" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>1967</v>
-      </c>
-      <c r="B2" s="19">
-        <v>1454.3</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1968</v>
-      </c>
-      <c r="B3" s="19">
-        <v>1487.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>1969</v>
-      </c>
-      <c r="B4" s="19">
-        <v>1529.2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>1970</v>
-      </c>
-      <c r="B5" s="19">
-        <v>1475.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>1971</v>
-      </c>
-      <c r="B6" s="19">
-        <v>1644.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>1972</v>
-      </c>
-      <c r="B7" s="19">
-        <v>1903.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>1973</v>
-      </c>
-      <c r="B8" s="19">
-        <v>1916.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>1974</v>
-      </c>
-      <c r="B9" s="19">
-        <v>2214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>1975</v>
-      </c>
-      <c r="B10" s="19">
-        <v>2411.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>1976</v>
-      </c>
-      <c r="B11" s="19">
-        <v>2551.8000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>1977</v>
-      </c>
-      <c r="B12" s="19">
-        <v>2905.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>1978</v>
-      </c>
-      <c r="B13" s="19">
-        <v>3374.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>1979</v>
-      </c>
-      <c r="B14" s="19">
-        <v>3888.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>1980</v>
-      </c>
-      <c r="B15" s="19">
-        <v>4263.3999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>1981</v>
-      </c>
-      <c r="B16" s="19">
-        <v>4465.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>1982</v>
-      </c>
-      <c r="B17" s="19">
-        <v>4605.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>1983</v>
-      </c>
-      <c r="B18" s="19">
-        <v>4966.3999999999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>1984</v>
-      </c>
-      <c r="B19" s="19">
-        <v>5546.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>1985</v>
-      </c>
-      <c r="B20" s="19">
-        <v>6339.7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
-        <v>1986</v>
-      </c>
-      <c r="B21" s="19">
-        <v>6558.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>1987</v>
-      </c>
-      <c r="B22" s="19">
-        <v>7337.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
-        <v>1988</v>
-      </c>
-      <c r="B23" s="19">
-        <v>7827.7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
-        <v>1989</v>
-      </c>
-      <c r="B24" s="19">
-        <v>8672</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
-        <v>1990</v>
-      </c>
-      <c r="B25" s="19">
-        <v>9137.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
-        <v>1991</v>
-      </c>
-      <c r="B26" s="19">
-        <v>10168.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>1992</v>
-      </c>
-      <c r="B27" s="19">
-        <v>10271.200000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
-        <v>1993</v>
-      </c>
-      <c r="B28" s="19">
-        <v>11208.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
-        <v>1994</v>
-      </c>
-      <c r="B29" s="19">
-        <v>11796.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
-        <v>1995</v>
-      </c>
-      <c r="B30" s="19">
-        <v>11927.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
-        <v>1996</v>
-      </c>
-      <c r="B31" s="19">
-        <v>11977.8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
-        <v>1997</v>
-      </c>
-      <c r="B32" s="19">
-        <v>12559</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
-        <v>1998</v>
-      </c>
-      <c r="B33" s="19">
-        <v>13380.7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
-        <v>1999</v>
-      </c>
-      <c r="B34" s="19">
-        <v>14959.1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
-        <v>2000</v>
-      </c>
-      <c r="B35" s="19">
-        <v>16890.7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
-        <v>2001</v>
-      </c>
-      <c r="B36" s="19">
-        <v>20065.099999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
-        <v>2002</v>
-      </c>
-      <c r="B37" s="19">
-        <v>21620</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="10">
-        <v>2003</v>
-      </c>
-      <c r="B38" s="19">
-        <v>23005.8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="10">
-        <v>2004</v>
-      </c>
-      <c r="B39" s="19">
-        <v>24947</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="10">
-        <v>2005</v>
-      </c>
-      <c r="B40" s="19">
-        <v>25687.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="10">
-        <v>2006</v>
-      </c>
-      <c r="B41" s="19">
-        <v>24669.7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="10">
-        <v>2007</v>
-      </c>
-      <c r="B42" s="19">
-        <v>25547.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="10">
-        <v>2008</v>
-      </c>
-      <c r="B43" s="19">
-        <v>26026.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="10">
-        <v>2009</v>
-      </c>
-      <c r="B44" s="19">
-        <v>31557.8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="10">
-        <v>2010</v>
-      </c>
-      <c r="B45" s="19">
-        <v>31192.3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="10">
-        <v>2011</v>
-      </c>
-      <c r="B46" s="19">
-        <v>27680.3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="10">
-        <v>2012</v>
-      </c>
-      <c r="B47" s="19">
-        <v>27509.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="10">
-        <v>2013</v>
-      </c>
-      <c r="B48" s="19">
-        <v>25772</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="10">
-        <v>2014</v>
-      </c>
-      <c r="B49" s="19">
-        <v>27429.3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="10">
-        <v>2015</v>
-      </c>
-      <c r="B50" s="19">
-        <v>27414.7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="10">
-        <v>2016</v>
-      </c>
-      <c r="B51" s="19">
-        <v>28199.3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="10">
-        <v>2017</v>
-      </c>
-      <c r="B52" s="19">
-        <v>28963.200000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="10">
-        <v>2018</v>
-      </c>
-      <c r="B53" s="19">
-        <v>31534.1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B54" s="19">
-        <v>33359.199999999997</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13745,7 +13467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
@@ -14327,6 +14049,37 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="108"/>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="110" t="s">
+        <v>340</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="70" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14348,7 +14101,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -14385,7 +14138,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -14410,7 +14163,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -14438,7 +14191,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -14493,7 +14246,7 @@
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="34" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -14513,7 +14266,7 @@
       </c>
       <c r="G4" s="109"/>
       <c r="H4" s="109" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14533,7 +14286,7 @@
       </c>
       <c r="G5" s="109"/>
       <c r="H5" s="109" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -14553,7 +14306,7 @@
       </c>
       <c r="G6" s="109"/>
       <c r="H6" s="109" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -14573,7 +14326,7 @@
       </c>
       <c r="G7" s="109"/>
       <c r="H7" s="109" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14593,7 +14346,7 @@
       </c>
       <c r="G8" s="109"/>
       <c r="H8" s="109" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -14613,7 +14366,7 @@
       </c>
       <c r="G9" s="109"/>
       <c r="H9" s="109" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -14633,7 +14386,7 @@
       </c>
       <c r="G10" s="109"/>
       <c r="H10" s="109" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14653,7 +14406,7 @@
       </c>
       <c r="G11" s="109"/>
       <c r="H11" s="109" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14673,7 +14426,7 @@
       </c>
       <c r="G12" s="109"/>
       <c r="H12" s="109" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -14693,7 +14446,7 @@
       </c>
       <c r="G13" s="109"/>
       <c r="H13" s="109" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14713,7 +14466,7 @@
       </c>
       <c r="G14" s="109"/>
       <c r="H14" s="109" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14733,7 +14486,7 @@
       </c>
       <c r="G15" s="109"/>
       <c r="H15" s="109" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -14753,7 +14506,7 @@
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="38" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -14773,7 +14526,7 @@
       </c>
       <c r="G17" s="38"/>
       <c r="H17" s="38" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -20010,31 +19763,459 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="108"/>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="110" t="s">
-        <v>332</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1967</v>
+      </c>
+      <c r="B2" s="19">
+        <v>1454.3</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1968</v>
+      </c>
+      <c r="B3" s="19">
+        <v>1487.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>1969</v>
+      </c>
+      <c r="B4" s="19">
+        <v>1529.2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>1970</v>
+      </c>
+      <c r="B5" s="19">
+        <v>1475.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>1971</v>
+      </c>
+      <c r="B6" s="19">
+        <v>1644.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>1972</v>
+      </c>
+      <c r="B7" s="19">
+        <v>1903.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>1973</v>
+      </c>
+      <c r="B8" s="19">
+        <v>1916.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>1974</v>
+      </c>
+      <c r="B9" s="19">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>1975</v>
+      </c>
+      <c r="B10" s="19">
+        <v>2411.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>1976</v>
+      </c>
+      <c r="B11" s="19">
+        <v>2551.8000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>1977</v>
+      </c>
+      <c r="B12" s="19">
+        <v>2905.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>1978</v>
+      </c>
+      <c r="B13" s="19">
+        <v>3374.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>1979</v>
+      </c>
+      <c r="B14" s="19">
+        <v>3888.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>1980</v>
+      </c>
+      <c r="B15" s="19">
+        <v>4263.3999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>1981</v>
+      </c>
+      <c r="B16" s="19">
+        <v>4465.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>1982</v>
+      </c>
+      <c r="B17" s="19">
+        <v>4605.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>1983</v>
+      </c>
+      <c r="B18" s="19">
+        <v>4966.3999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>1984</v>
+      </c>
+      <c r="B19" s="19">
+        <v>5546.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>1985</v>
+      </c>
+      <c r="B20" s="19">
+        <v>6339.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>1986</v>
+      </c>
+      <c r="B21" s="19">
+        <v>6558.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>1987</v>
+      </c>
+      <c r="B22" s="19">
+        <v>7337.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>1988</v>
+      </c>
+      <c r="B23" s="19">
+        <v>7827.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>1989</v>
+      </c>
+      <c r="B24" s="19">
+        <v>8672</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>1990</v>
+      </c>
+      <c r="B25" s="19">
+        <v>9137.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>1991</v>
+      </c>
+      <c r="B26" s="19">
+        <v>10168.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>1992</v>
+      </c>
+      <c r="B27" s="19">
+        <v>10271.200000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>1993</v>
+      </c>
+      <c r="B28" s="19">
+        <v>11208.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>1994</v>
+      </c>
+      <c r="B29" s="19">
+        <v>11796.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>1995</v>
+      </c>
+      <c r="B30" s="19">
+        <v>11927.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>1996</v>
+      </c>
+      <c r="B31" s="19">
+        <v>11977.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>1997</v>
+      </c>
+      <c r="B32" s="19">
+        <v>12559</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>1998</v>
+      </c>
+      <c r="B33" s="19">
+        <v>13380.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>1999</v>
+      </c>
+      <c r="B34" s="19">
+        <v>14959.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>2000</v>
+      </c>
+      <c r="B35" s="19">
+        <v>16890.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>2001</v>
+      </c>
+      <c r="B36" s="19">
+        <v>20065.099999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>2002</v>
+      </c>
+      <c r="B37" s="19">
+        <v>21620</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>2003</v>
+      </c>
+      <c r="B38" s="19">
+        <v>23005.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>2004</v>
+      </c>
+      <c r="B39" s="19">
+        <v>24947</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>2005</v>
+      </c>
+      <c r="B40" s="19">
+        <v>25687.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>2006</v>
+      </c>
+      <c r="B41" s="19">
+        <v>24669.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
+        <v>2007</v>
+      </c>
+      <c r="B42" s="19">
+        <v>25547.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="10">
+        <v>2008</v>
+      </c>
+      <c r="B43" s="19">
+        <v>26026.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>2009</v>
+      </c>
+      <c r="B44" s="19">
+        <v>31557.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
+        <v>2010</v>
+      </c>
+      <c r="B45" s="19">
+        <v>31192.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>2011</v>
+      </c>
+      <c r="B46" s="19">
+        <v>27680.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
+        <v>2012</v>
+      </c>
+      <c r="B47" s="19">
+        <v>27509.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
+        <v>2013</v>
+      </c>
+      <c r="B48" s="19">
+        <v>25772</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>2014</v>
+      </c>
+      <c r="B49" s="19">
+        <v>27429.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
+        <v>2015</v>
+      </c>
+      <c r="B50" s="19">
+        <v>27414.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="10">
+        <v>2016</v>
+      </c>
+      <c r="B51" s="19">
+        <v>28199.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="10">
+        <v>2017</v>
+      </c>
+      <c r="B52" s="19">
+        <v>28963.200000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="10">
+        <v>2018</v>
+      </c>
+      <c r="B53" s="19">
+        <v>31534.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="19">
+        <v>33359.199999999997</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="70" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Annotation for Maslo (1943)
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -8120,7 +8120,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Motivation</a:t>
+            <a:t>Prompt</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -9908,346 +9908,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>88891</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>146854</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>88891</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>70654</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="142" name="Group 141">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C52BA6-FC43-4646-B23E-7D9141CF726D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="10452091" y="6642904"/>
-          <a:ext cx="1828800" cy="1828800"/>
-          <a:chOff x="5353050" y="1009649"/>
-          <a:chExt cx="1828800" cy="1828800"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="143" name="Group 142">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEBCF2D3-F95D-4D2E-86B2-910D7F5EA0D0}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="5444490" y="1128712"/>
-            <a:ext cx="1645920" cy="1590675"/>
-            <a:chOff x="5396865" y="1084421"/>
-            <a:chExt cx="1645920" cy="1590675"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="145" name="Rectangle 144">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA49BB23-E295-4576-8000-E6DAB4B65D04}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="5396865" y="2217896"/>
-              <a:ext cx="1645920" cy="457200"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
-                  </a:solidFill>
-                </a:rPr>
-                <a:t>Environmental Factors</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="146" name="Rectangle 145">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF5FEFB4-16D8-4D59-A62A-59690049B6DE}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="5396865" y="1651159"/>
-              <a:ext cx="1645920" cy="457200"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
-                  </a:solidFill>
-                </a:rPr>
-                <a:t>Organizational Factors</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="147" name="Rectangle 146">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A08F3ED7-02EC-40E8-8EE0-6BC4191D6964}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="5396865" y="1084421"/>
-              <a:ext cx="1645920" cy="457200"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
-                  </a:solidFill>
-                </a:rPr>
-                <a:t>Individual Factors</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="144" name="Rectangle 143">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FE487F7-7041-4684-B4EF-F0A4071BBCC5}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5353050" y="1009649"/>
-            <a:ext cx="1828800" cy="1828800"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="31750">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>390526</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>393692</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>146854</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="149" name="Connector: Elbow 148">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA290536-ECB1-4F9B-981D-B2DA44F3F3AD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="144" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipV="1">
-          <a:off x="11058119" y="6334532"/>
-          <a:ext cx="613579" cy="3166"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>314323</xdr:colOff>
       <xdr:row>25</xdr:row>
@@ -10669,6 +10329,66 @@
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
             <a:gd name="adj1" fmla="val 100148"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>553580</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Connector: Elbow 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3F3075E-D564-4AAF-AEC5-E87A922A21BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8478380" y="1924049"/>
+          <a:ext cx="6028195" cy="2857501"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 128056"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="25400">
@@ -14090,7 +13810,7 @@
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -14127,7 +13847,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -14143,7 +13863,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="49" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Modified figure on theory of org
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -8056,165 +8056,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{112D4868-B282-4C3E-93A6-7029C3F8EE2C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="66675" y="3224212"/>
-          <a:ext cx="1371600" cy="457200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Prompt</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>369094</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>521494</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6169B0DD-68CB-4FC2-A52E-A411FB8FEE39}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2807494" y="3224212"/>
-          <a:ext cx="1371600" cy="457200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Goal</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Decisions</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>22</xdr:row>
@@ -8431,15 +8272,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>514354</xdr:colOff>
+      <xdr:colOff>514349</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>47627</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>314326</xdr:colOff>
+      <xdr:colOff>314324</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8451,13 +8292,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:stCxn id="73" idx="2"/>
           <a:endCxn id="4" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="919166" y="3890965"/>
-          <a:ext cx="819147" cy="409572"/>
+          <a:off x="909637" y="3881437"/>
+          <a:ext cx="838200" cy="409575"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -8489,15 +8331,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>142876</xdr:colOff>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>42863</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>228601</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8509,17 +8351,19 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="47" idx="1"/>
+          <a:stCxn id="96" idx="2"/>
           <a:endCxn id="2" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="752476" y="3681413"/>
-          <a:ext cx="6181725" cy="2328863"/>
+        <a:xfrm rot="5400000">
+          <a:off x="9098757" y="-4688681"/>
+          <a:ext cx="23812" cy="16716375"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 9260192"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln w="25400">
           <a:solidFill>
@@ -8609,7 +8453,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
@@ -8628,71 +8472,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="77" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2905125" y="3676650"/>
-          <a:ext cx="390525" cy="828675"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>381001</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>466726</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="Connector: Elbow 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{178BF1B2-5124-4AFF-9876-37D1AA50280C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="40" idx="2"/>
-          <a:endCxn id="47" idx="3"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="10229851" y="1752600"/>
-          <a:ext cx="2333625" cy="6181725"/>
+          <a:off x="2905125" y="3667125"/>
+          <a:ext cx="390525" cy="838200"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -8778,79 +8564,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>395288</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>547688</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Rectangle 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{222E1D97-B053-4F72-B79C-FCF721309183}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8320088" y="3219450"/>
-          <a:ext cx="1371600" cy="457200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Action Decisions</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -9046,79 +8759,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="Rectangle 39">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34280298-5C2E-4C59-B30A-2BD06D9D6EDB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13801725" y="3219450"/>
-          <a:ext cx="1371600" cy="457200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Outcomes</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>240507</xdr:colOff>
       <xdr:row>18</xdr:row>
@@ -9174,152 +8814,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="Rectangle 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7732693-81E6-4C04-921A-9F7D33823AAB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6934200" y="5781675"/>
-          <a:ext cx="1371600" cy="457200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Assessment</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>54769</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>207169</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Rectangle 49">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBB14082-7FD4-4E35-9392-EEC6D5D32D82}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5541169" y="3219450"/>
-          <a:ext cx="1371600" cy="457200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Options</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -9383,23 +8877,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>180976</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>153613</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>153520</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="157" name="Group 156">
+        <xdr:cNvPr id="120" name="Group 119">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0728202-5D9E-4DFF-9D8D-1A6E81A5045B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB187BE9-B15D-4332-85CE-8773AAA683A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9407,18 +8901,18 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2009776" y="1009649"/>
-          <a:ext cx="11115674" cy="2447926"/>
-          <a:chOff x="2002632" y="1014412"/>
-          <a:chExt cx="11072812" cy="2447926"/>
+          <a:off x="8078413" y="695324"/>
+          <a:ext cx="1828707" cy="1828800"/>
+          <a:chOff x="8078413" y="1009649"/>
+          <a:chExt cx="1828707" cy="1828800"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="45" name="Group 44">
+          <xdr:cNvPr id="43" name="Group 42">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{818FB88D-4680-48AD-8A12-7201248072B4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78DF7D60-F0A3-4C1C-B4B2-BEE4C1B91C67}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9426,212 +8920,18 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="6624638" y="1014412"/>
-            <a:ext cx="1821656" cy="1828800"/>
-            <a:chOff x="5353050" y="1009649"/>
-            <a:chExt cx="1828800" cy="1828800"/>
+            <a:off x="8169848" y="1128712"/>
+            <a:ext cx="1645836" cy="1590675"/>
+            <a:chOff x="6825668" y="1084421"/>
+            <a:chExt cx="1645920" cy="1590675"/>
           </a:xfrm>
         </xdr:grpSpPr>
-        <xdr:grpSp>
-          <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="43" name="Group 42">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="84" name="Rectangle 83">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78DF7D60-F0A3-4C1C-B4B2-BEE4C1B91C67}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGrpSpPr/>
-          </xdr:nvGrpSpPr>
-          <xdr:grpSpPr>
-            <a:xfrm>
-              <a:off x="5444490" y="1128712"/>
-              <a:ext cx="1645920" cy="1590675"/>
-              <a:chOff x="5396865" y="1084421"/>
-              <a:chExt cx="1645920" cy="1590675"/>
-            </a:xfrm>
-          </xdr:grpSpPr>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="84" name="Rectangle 83">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D1C0CA5-37D6-4047-8AE5-BC1F0AC3FB9E}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="5396865" y="2217896"/>
-                <a:ext cx="1645920" cy="457200"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="ctr"/>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1200">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>Environmental Factors</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="85" name="Rectangle 84">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA3A926B-81E6-4DBA-9BCD-82E23E39637A}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="5396865" y="1651159"/>
-                <a:ext cx="1645920" cy="457200"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="ctr"/>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1200">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>Organizational Factors</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="88" name="Rectangle 87">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEDF6A07-79AD-4608-8341-C909208EB683}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="5396865" y="1084421"/>
-                <a:ext cx="1645920" cy="457200"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="ctr"/>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1200">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>Individual Factors</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-        </xdr:grpSp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="44" name="Rectangle 43">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F65BFDC2-7932-4B76-B187-D70D5CDA7D65}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D1C0CA5-37D6-4047-8AE5-BC1F0AC3FB9E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9639,14 +8939,14 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5353050" y="1009649"/>
-              <a:ext cx="1828800" cy="1828800"/>
+              <a:off x="6825668" y="2217896"/>
+              <a:ext cx="1645920" cy="457200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
             <a:noFill/>
-            <a:ln w="31750">
+            <a:ln w="19050">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -9669,241 +8969,426 @@
             </a:fontRef>
           </xdr:style>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Environmental Factors</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="85" name="Rectangle 84">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA3A926B-81E6-4DBA-9BCD-82E23E39637A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6825668" y="1651159"/>
+              <a:ext cx="1645920" cy="457200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Organizational Factors</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="88" name="Rectangle 87">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEDF6A07-79AD-4608-8341-C909208EB683}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6825668" y="1084421"/>
+              <a:ext cx="1645920" cy="457200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Individual Factors</a:t>
+              </a:r>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
       </xdr:grpSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="111" name="Connector: Elbow 110">
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="44" name="Rectangle 43">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7AE589E-F38F-4650-8A0D-FC78B8CF6865}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F65BFDC2-7932-4B76-B187-D70D5CDA7D65}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="44" idx="1"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
         <xdr:spPr>
-          <a:xfrm rot="10800000" flipV="1">
-            <a:off x="2002632" y="1928812"/>
-            <a:ext cx="4622007" cy="1533526"/>
+          <a:xfrm>
+            <a:off x="8078413" y="1009649"/>
+            <a:ext cx="1828707" cy="1828800"/>
           </a:xfrm>
-          <a:prstGeom prst="bentConnector3">
-            <a:avLst>
-              <a:gd name="adj1" fmla="val 99897"/>
-            </a:avLst>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
           </a:prstGeom>
-          <a:ln w="25400">
+          <a:noFill/>
+          <a:ln w="31750">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
             </a:solidFill>
-            <a:tailEnd type="triangle" w="lg" len="lg"/>
           </a:ln>
         </xdr:spPr>
         <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
           </a:lnRef>
-          <a:fillRef idx="0">
+          <a:fillRef idx="1">
             <a:schemeClr val="accent1"/>
           </a:fillRef>
           <a:effectRef idx="0">
             <a:schemeClr val="accent1"/>
           </a:effectRef>
           <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
+            <a:schemeClr val="lt1"/>
           </a:fontRef>
         </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="116" name="Connector: Elbow 115">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BB9F9BF-953C-422B-AB92-216F0C93D0FA}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="44" idx="1"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="10800000" flipV="1">
-            <a:off x="4745831" y="1928812"/>
-            <a:ext cx="1878807" cy="1514476"/>
-          </a:xfrm>
-          <a:prstGeom prst="bentConnector3">
-            <a:avLst>
-              <a:gd name="adj1" fmla="val 100000"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:tailEnd type="triangle" w="lg" len="lg"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>222885</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66673</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>153613</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="111" name="Connector: Elbow 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7AE589E-F38F-4650-8A0D-FC78B8CF6865}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="1"/>
+          <a:endCxn id="63" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="2051685" y="1609723"/>
+          <a:ext cx="6026728" cy="1847851"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
             <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="121" name="Connector: Elbow 120">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDC9698B-739E-4491-9CD8-E606DF187FA2}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="44" idx="3"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8446294" y="1928812"/>
-            <a:ext cx="1850231" cy="1533526"/>
-          </a:xfrm>
-          <a:prstGeom prst="bentConnector3">
-            <a:avLst>
-              <a:gd name="adj1" fmla="val 100256"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:tailEnd type="triangle" w="lg" len="lg"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>537209</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>153613</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="116" name="Connector: Elbow 115">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BB9F9BF-953C-422B-AB92-216F0C93D0FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="1"/>
+          <a:endCxn id="35" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="4804409" y="1609724"/>
+          <a:ext cx="3274004" cy="1838326"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
             <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="126" name="Connector: Elbow 125">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24ADCC6A-A336-40A3-952D-A8CAAD32FDA9}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="44" idx="3"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8446294" y="1928812"/>
-            <a:ext cx="4629150" cy="1514476"/>
-          </a:xfrm>
-          <a:prstGeom prst="bentConnector3">
-            <a:avLst>
-              <a:gd name="adj1" fmla="val 100000"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:tailEnd type="triangle" w="lg" len="lg"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>153520</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="121" name="Connector: Elbow 120">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDC9698B-739E-4491-9CD8-E606DF187FA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="3"/>
+          <a:endCxn id="65" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9907120" y="1609724"/>
+          <a:ext cx="440840" cy="1847851"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
             <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="130" name="Connector: Elbow 129">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2134B77-EF39-4D49-920C-4BCE0D633126}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="44" idx="2"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="16200000" flipH="1">
-            <a:off x="7229474" y="3148012"/>
-            <a:ext cx="609604" cy="3"/>
-          </a:xfrm>
-          <a:prstGeom prst="bentConnector3">
-            <a:avLst>
-              <a:gd name="adj1" fmla="val 50000"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:ln w="25400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:tailEnd type="triangle" w="lg" len="lg"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>153520</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>280035</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="126" name="Connector: Elbow 125">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24ADCC6A-A336-40A3-952D-A8CAAD32FDA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="3"/>
+          <a:endCxn id="67" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9907120" y="1609724"/>
+          <a:ext cx="3174515" cy="1857376"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
             <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -9989,7 +9474,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>47627</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
@@ -10007,13 +9492,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:stCxn id="71" idx="2"/>
           <a:endCxn id="42" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="550069" y="4107658"/>
-          <a:ext cx="1404935" cy="561973"/>
+          <a:off x="545305" y="4102894"/>
+          <a:ext cx="1414463" cy="561973"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -10182,13 +9668,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>581024</xdr:colOff>
+      <xdr:colOff>523874</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>209548</xdr:colOff>
+      <xdr:colOff>209547</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
@@ -10202,13 +9688,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:stCxn id="81" idx="2"/>
           <a:endCxn id="55" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="5786435" y="3948113"/>
-          <a:ext cx="1409702" cy="847724"/>
+          <a:off x="5762623" y="3924301"/>
+          <a:ext cx="1400176" cy="904873"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -10261,6 +9748,7 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="55" idx="3"/>
+          <a:endCxn id="83" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -10298,15 +9786,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>76201</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>30861</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>228601</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -10318,17 +9806,18 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="47" idx="1"/>
+          <a:stCxn id="96" idx="2"/>
+          <a:endCxn id="118" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="3733801" y="3669411"/>
-          <a:ext cx="3200400" cy="2340864"/>
+        <a:xfrm rot="5400000">
+          <a:off x="10591800" y="-3200400"/>
+          <a:ext cx="19050" cy="13735050"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 100148"/>
+            <a:gd name="adj1" fmla="val 11600000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="25400">
@@ -10357,16 +9846,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>553580</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>153520</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -10379,17 +9868,16 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="44" idx="3"/>
+          <a:endCxn id="69" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8478380" y="1924049"/>
-          <a:ext cx="6028195" cy="2857501"/>
+          <a:off x="9907120" y="1609724"/>
+          <a:ext cx="5927240" cy="1847851"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 128056"/>
-          </a:avLst>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
         </a:prstGeom>
         <a:ln w="25400">
           <a:solidFill>
@@ -10413,6 +9901,1946 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Arrow Connector 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41E27AF9-2618-489F-8AA2-8EE8DAFA6964}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="40" idx="3"/>
+          <a:endCxn id="47" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="15173325" y="3438525"/>
+          <a:ext cx="1390650" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>64769</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Oval 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1240153B-0687-4180-BA5D-9C6BCEFF9744}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4667249" y="3448050"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>360045</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>93345</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="Oval 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B46FEB95-48DC-494F-9BE1-304868AB4DF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1914525" y="3457575"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>93345</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Oval 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84950C82-D5D1-4F7B-ACF1-942B74E7A534}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10210800" y="3457575"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>417195</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="Oval 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83D6F8BA-7A2C-4ABB-BE7E-F6F9D4A45DA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12944475" y="3467100"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>93345</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="Oval 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7C564E6-4630-41C2-A974-55E228D20DAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15697200" y="3457575"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="62" name="Group 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CD133BB-0E43-42C9-B521-50A7E39F3278}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="66675" y="3209925"/>
+          <a:ext cx="1371600" cy="471487"/>
+          <a:chOff x="66675" y="3209925"/>
+          <a:chExt cx="1371600" cy="471487"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Rectangle 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{112D4868-B282-4C3E-93A6-7029C3F8EE2C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="66675" y="3224212"/>
+            <a:ext cx="1371600" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Prompts</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="71" name="Rectangle 70">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2288CAEA-0248-4F75-AF9C-9D17BA4AB5B3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="742950" y="3219450"/>
+            <a:ext cx="457200" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="73" name="Rectangle 72">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AFED4D4-436C-4A51-A0B3-D5BD4A1C4D1C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="895350" y="3209925"/>
+            <a:ext cx="457200" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>54769</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>207169</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="123" name="Group 122">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7083277D-F072-481C-A703-3028025076D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5541169" y="3219450"/>
+          <a:ext cx="1371600" cy="457200"/>
+          <a:chOff x="5541169" y="3219450"/>
+          <a:chExt cx="1371600" cy="457200"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="50" name="Rectangle 49">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBB14082-7FD4-4E35-9392-EEC6D5D32D82}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5541169" y="3219450"/>
+            <a:ext cx="1371600" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Options</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="81" name="Rectangle 80">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF25FCCA-4F59-4880-A9C6-7F60FDED350B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5781675" y="3219450"/>
+            <a:ext cx="457200" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>395288</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>547688</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="74" name="Group 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34B85B75-1497-408B-9672-A6733D948C4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="8320088" y="3219450"/>
+          <a:ext cx="1371600" cy="457200"/>
+          <a:chOff x="8320088" y="3219450"/>
+          <a:chExt cx="1371600" cy="457200"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="Rectangle 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{222E1D97-B053-4F72-B79C-FCF721309183}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8320088" y="3219450"/>
+            <a:ext cx="1371600" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Action Decisions</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="83" name="Rectangle 82">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36C4369E-63EA-455C-866E-D1C0ED91C74E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8991600" y="3219450"/>
+            <a:ext cx="457200" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>379095</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="91" name="Oval 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06FCAF1D-7781-4EEA-A9C5-C20814949FB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7419975" y="3467100"/>
+          <a:ext cx="274320" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>241935</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>153613</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="93" name="Connector: Elbow 92">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3D1D079-3432-4F5A-B7C6-73D7DD7D7408}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="1"/>
+          <a:endCxn id="91" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="7557135" y="1609724"/>
+          <a:ext cx="521278" cy="1857376"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="117" name="Group 116">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C8BA594-9307-4F24-AA87-D85ACE2231DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="16563975" y="3200400"/>
+          <a:ext cx="1371600" cy="466725"/>
+          <a:chOff x="16563975" y="3200400"/>
+          <a:chExt cx="1371600" cy="466725"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="47" name="Rectangle 46">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7732693-81E6-4C04-921A-9F7D33823AAB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="16563975" y="3209925"/>
+            <a:ext cx="1371600" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Assessment</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="86" name="Rectangle 85">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F11F912-32D7-47A0-AFD5-B602C88B7338}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="16773525" y="3209925"/>
+            <a:ext cx="457200" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="96" name="Rectangle 95">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{494943A0-BD22-4D3C-8C23-3D9C4C34FD5D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="17240250" y="3200400"/>
+            <a:ext cx="457200" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="104" name="Rectangle 103">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D58F31E6-181A-4253-861A-8186E23A2D37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15173326" y="4286251"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Decision Premises</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>464345</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="105" name="Connector: Elbow 104">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32C2CF5E-8F64-4C34-B60F-1F2A9D1262AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="104" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="14414898" y="3756422"/>
+          <a:ext cx="828675" cy="688181"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="106" name="Connector: Elbow 105">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D170CC21-9202-4BF3-8E85-94333F8ABC09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="104" idx="3"/>
+          <a:endCxn id="86" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="16544926" y="3667125"/>
+          <a:ext cx="457199" cy="847726"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76202</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152402</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="107" name="Rectangle 106">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4FBCC66-BB18-4A13-8951-4F80346C24C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15173324" y="4857752"/>
+          <a:ext cx="1371600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Communication</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>542923</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114302</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="108" name="Connector: Elbow 107">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51A4F4CF-2B65-4309-AF09-B88C85073970}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="107" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="14020799" y="3933827"/>
+          <a:ext cx="1400176" cy="904873"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114302</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="109" name="Connector: Elbow 108">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DCB0C50-8CB7-4877-A72B-224992C332BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="107" idx="3"/>
+          <a:endCxn id="47" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="16544924" y="3667125"/>
+          <a:ext cx="704851" cy="1419227"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="119" name="Group 118">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F88E26F4-6E66-446A-9B8F-6729AF91F97E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13801725" y="3209925"/>
+          <a:ext cx="1371600" cy="466725"/>
+          <a:chOff x="13801725" y="3209925"/>
+          <a:chExt cx="1371600" cy="466725"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="40" name="Rectangle 39">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34280298-5C2E-4C59-B30A-2BD06D9D6EDB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="13801725" y="3219450"/>
+            <a:ext cx="1371600" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Consequences</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="110" name="Rectangle 109">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3607B353-7BA7-4C6D-9CDB-9D8415A46768}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="14030325" y="3209925"/>
+            <a:ext cx="457200" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369094</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>521494</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="122" name="Group 121">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1004301-E069-4F54-8CC3-3C429D079E7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2807494" y="3209925"/>
+          <a:ext cx="1371600" cy="471487"/>
+          <a:chOff x="2807494" y="3209925"/>
+          <a:chExt cx="1371600" cy="471487"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Rectangle 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6169B0DD-68CB-4FC2-A52E-A411FB8FEE39}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2807494" y="3224212"/>
+            <a:ext cx="1371600" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Goal</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Decisions</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="77" name="Rectangle 76">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEC65663-ECC7-4B24-9196-6FC9AB0A8E0D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3067050" y="3209925"/>
+            <a:ext cx="457200" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="118" name="Rectangle 117">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7109A442-CF21-4787-87FA-65ED156EA4DC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="3219450"/>
+            <a:ext cx="457200" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -13863,7 +15291,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="49" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>